<commit_message>
Ran a quick validation check on the literature files
</commit_message>
<xml_diff>
--- a/Literature/Literature.xlsx
+++ b/Literature/Literature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hso20\OneDrive\Plocha\IES\Diploma-Thesis\Literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745362C2-E045-4915-A894-E241B006629F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A88B19E3-01A6-4529-AE5C-3FB3D1BAD786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -189,7 +189,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -211,7 +211,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14191" uniqueCount="5037">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14191" uniqueCount="5046">
   <si>
     <t>Number</t>
   </si>
@@ -15322,6 +15322,33 @@
   </si>
   <si>
     <t>Riddell (2005)</t>
+  </si>
+  <si>
+    <t>Lillo-Bañuls &amp; Casado-Díaz (2010)</t>
+  </si>
+  <si>
+    <t>Wolfe &amp; Haveman (2002)</t>
+  </si>
+  <si>
+    <t>Bils &amp; Klenow (2000)</t>
+  </si>
+  <si>
+    <t>Arias &amp; McMahon (2001)</t>
+  </si>
+  <si>
+    <t>Mendiratta &amp; Gupt (2013)</t>
+  </si>
+  <si>
+    <t>De Brauw &amp; Rozelle (2007)</t>
+  </si>
+  <si>
+    <t>De Brauw &amp; Rozelle (2012)</t>
+  </si>
+  <si>
+    <t>Warunsiri &amp; McNown (2010)</t>
+  </si>
+  <si>
+    <t>van der Hoeven (2013)</t>
   </si>
 </sst>
 </file>
@@ -15646,63 +15673,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAACAC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBA8CDC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6161"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="22">
     <dxf>
       <fill>
         <patternFill>
@@ -15763,6 +15734,41 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFBA8CDC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6161"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -16107,7 +16113,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D4E9F8-720A-49C1-8678-F81C22E3A380}">
   <dimension ref="A1:W575"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="G81" sqref="G81"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -16647,7 +16655,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>4882</v>
+        <v>5040</v>
       </c>
       <c r="C12" t="s">
         <v>4747</v>
@@ -16708,7 +16716,7 @@
       <c r="G13">
         <v>295</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="32" t="s">
         <v>1087</v>
       </c>
       <c r="I13" t="s">
@@ -16779,7 +16787,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>4884</v>
+        <v>5037</v>
       </c>
       <c r="C15" t="s">
         <v>4749</v>
@@ -18319,7 +18327,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>3990</v>
+        <v>5045</v>
       </c>
       <c r="C50" t="s">
         <v>3991</v>
@@ -18935,7 +18943,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>4899</v>
+        <v>5044</v>
       </c>
       <c r="C64" t="s">
         <v>4763</v>
@@ -19067,7 +19075,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>4900</v>
+        <v>5038</v>
       </c>
       <c r="C67" t="s">
         <v>4764</v>
@@ -19155,7 +19163,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>4531</v>
+        <v>5041</v>
       </c>
       <c r="C69" t="s">
         <v>4765</v>
@@ -19419,7 +19427,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>4903</v>
+        <v>5039</v>
       </c>
       <c r="C75" t="s">
         <v>4768</v>
@@ -22667,7 +22675,7 @@
         <v>153</v>
       </c>
       <c r="B154" t="s">
-        <v>4100</v>
+        <v>5042</v>
       </c>
       <c r="C154" t="s">
         <v>4008</v>
@@ -28032,7 +28040,7 @@
         <v>284</v>
       </c>
       <c r="B285" t="s">
-        <v>4239</v>
+        <v>5043</v>
       </c>
       <c r="C285" t="s">
         <v>4008</v>
@@ -39909,23 +39917,23 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="R5">
-    <cfRule type="cellIs" dxfId="24" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="12" operator="notEqual">
+    <cfRule type="cellIs" dxfId="20" priority="12" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsBlanks" dxfId="22" priority="10">
+    <cfRule type="containsBlanks" dxfId="19" priority="10">
       <formula>LEN(TRIM(F1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R7">
-    <cfRule type="cellIs" dxfId="21" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="8" operator="notEqual">
+    <cfRule type="cellIs" dxfId="17" priority="8" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -39943,10 +39951,11 @@
   <hyperlinks>
     <hyperlink ref="I160" r:id="rId1" location="page=11" xr:uid="{326005DB-1117-49A2-A7CC-17E70B92D8E0}"/>
     <hyperlink ref="I9" r:id="rId2" xr:uid="{F2C21F12-D85B-40BA-8CE3-AFFE36F6C7EE}"/>
+    <hyperlink ref="H13" r:id="rId3" display="https://books.google.com/books?hl=en&amp;lr=&amp;id=xHdLezAGFFMC&amp;oi=fnd&amp;pg=PP13&amp;dq=(%22ability+bias%22+OR+%22intelligence+bias%22)+AND+(%22private+returns%22)+AND+(%22income%22+OR+%22earnings%22)+AND+(%22schooling%22+OR+%22education%22)&amp;ots=AMWBbfJpWa&amp;sig=HzNyY_GdLkNjo-PvjNkJ8XDbCMo" xr:uid="{2C3AEDA8-76A3-44C3-91BC-EED4714074A1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId3"/>
-  <legacyDrawing r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId4"/>
+  <legacyDrawing r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -63766,34 +63775,34 @@
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="R5">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="notEqual">
+    <cfRule type="cellIs" dxfId="12" priority="8" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsBlanks" dxfId="5" priority="6">
+    <cfRule type="containsBlanks" dxfId="11" priority="6">
       <formula>LEN(TRIM(F1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R7">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="notEqual">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:M601">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="PRIMARY STUDY">
+    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="PRIMARY STUDY">
       <formula>NOT(ISERROR(SEARCH("PRIMARY STUDY",L2)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="1" priority="2" operator="notContains" text="YES">
+    <cfRule type="notContainsText" dxfId="7" priority="2" operator="notContains" text="YES">
       <formula>ISERROR(SEARCH("YES",L2))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",L2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -72689,10 +72698,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:K251 L1">
-    <cfRule type="expression" dxfId="13" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>$K1=FALSE</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="9">
+    <cfRule type="expression" dxfId="4" priority="9">
       <formula>$J1=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -80635,10 +80644,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J259:J1048576 J257 J1:J253">
-    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="3" priority="12" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="13" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="2" priority="13" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J1)))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="14">
@@ -80653,10 +80662,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M17">
-    <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",M17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",M17)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Revamped the main R code, added source file
</commit_message>
<xml_diff>
--- a/Literature/Literature.xlsx
+++ b/Literature/Literature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hso20\OneDrive\Plocha\IES\Diploma-Thesis\Literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9232F9E-62E6-494A-B791-4B7CA3B4EA09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81CA18E3-6EF9-49BB-8CC9-1180CB127E90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -496,7 +496,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9797" uniqueCount="5160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9801" uniqueCount="5160">
   <si>
     <t>Number</t>
   </si>
@@ -16892,7 +16892,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O24" sqref="O24"/>
+      <selection pane="bottomLeft" activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16972,7 +16972,7 @@
       </c>
       <c r="S1" s="29">
         <f>COUNTIFS($N:$N, "YES", $F:$F, "&lt;&gt;") + Twins!S1</f>
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="U1" s="28" t="s">
         <v>5049</v>
@@ -17153,7 +17153,7 @@
       </c>
       <c r="V4">
         <f>COUNTIFS($N:$N, "YES", $M:$M, "&lt;&gt;PRIMARY STUDY", $Q:$Q, "&lt;&gt;Twins")</f>
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.3">
@@ -17217,7 +17217,7 @@
       </c>
       <c r="V5" s="38">
         <f>COUNTIFS($O:$O, "YES", $F:$F, "&lt;&gt;")</f>
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.3">
@@ -18387,7 +18387,12 @@
       <c r="N27" t="s">
         <v>963</v>
       </c>
-      <c r="P27" s="7"/>
+      <c r="O27" t="s">
+        <v>963</v>
+      </c>
+      <c r="P27" s="7">
+        <v>3</v>
+      </c>
       <c r="S27" t="s">
         <v>904</v>
       </c>
@@ -18430,12 +18435,17 @@
         <v>4872</v>
       </c>
       <c r="M28" t="s">
-        <v>963</v>
+        <v>966</v>
       </c>
       <c r="N28" t="s">
-        <v>963</v>
-      </c>
-      <c r="P28" s="7"/>
+        <v>966</v>
+      </c>
+      <c r="O28" t="s">
+        <v>966</v>
+      </c>
+      <c r="P28" s="7" t="s">
+        <v>5039</v>
+      </c>
       <c r="S28" t="s">
         <v>904</v>
       </c>
@@ -18589,7 +18599,12 @@
       <c r="N31" t="s">
         <v>963</v>
       </c>
-      <c r="P31" s="7"/>
+      <c r="O31" t="s">
+        <v>963</v>
+      </c>
+      <c r="P31" s="7">
+        <v>4</v>
+      </c>
       <c r="S31" t="s">
         <v>904</v>
       </c>

</xml_diff>

<commit_message>
Added more data, ran formula check for return calculation
</commit_message>
<xml_diff>
--- a/Literature/Literature.xlsx
+++ b/Literature/Literature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hso20\OneDrive\Plocha\IES\Diploma-Thesis\Literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81CA18E3-6EF9-49BB-8CC9-1180CB127E90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68DC402-555B-4919-8F3C-76566701B959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -496,7 +496,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9801" uniqueCount="5160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9828" uniqueCount="5161">
   <si>
     <t>Number</t>
   </si>
@@ -15976,6 +15976,9 @@
   </si>
   <si>
     <t>from main query</t>
+  </si>
+  <si>
+    <t>lwol</t>
   </si>
 </sst>
 </file>
@@ -16891,8 +16894,8 @@
   <dimension ref="A1:Z575"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O31" sqref="O31"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O43" sqref="O43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16972,14 +16975,14 @@
       </c>
       <c r="S1" s="29">
         <f>COUNTIFS($N:$N, "YES", $F:$F, "&lt;&gt;") + Twins!S1</f>
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="U1" s="28" t="s">
         <v>5049</v>
       </c>
       <c r="V1" s="29">
         <f>COUNTIF($M$2:$M$575, "&lt;&gt; ") +Twins!V1</f>
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="W1" s="31"/>
       <c r="X1" s="31"/>
@@ -17153,7 +17156,7 @@
       </c>
       <c r="V4">
         <f>COUNTIFS($N:$N, "YES", $M:$M, "&lt;&gt;PRIMARY STUDY", $Q:$Q, "&lt;&gt;Twins")</f>
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.3">
@@ -17217,7 +17220,7 @@
       </c>
       <c r="V5" s="38">
         <f>COUNTIFS($O:$O, "YES", $F:$F, "&lt;&gt;")</f>
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.3">
@@ -18700,12 +18703,17 @@
         <v>3963</v>
       </c>
       <c r="M33" t="s">
-        <v>963</v>
+        <v>966</v>
       </c>
       <c r="N33" t="s">
-        <v>963</v>
-      </c>
-      <c r="P33" s="7"/>
+        <v>966</v>
+      </c>
+      <c r="O33" t="s">
+        <v>966</v>
+      </c>
+      <c r="P33" s="7" t="s">
+        <v>5039</v>
+      </c>
       <c r="S33" t="s">
         <v>904</v>
       </c>
@@ -18753,7 +18761,12 @@
       <c r="N34" t="s">
         <v>963</v>
       </c>
-      <c r="P34" s="7"/>
+      <c r="O34" t="s">
+        <v>963</v>
+      </c>
+      <c r="P34" s="7">
+        <v>2</v>
+      </c>
       <c r="S34" t="s">
         <v>904</v>
       </c>
@@ -18796,12 +18809,17 @@
         <v>4875</v>
       </c>
       <c r="M35" t="s">
-        <v>963</v>
+        <v>974</v>
       </c>
       <c r="N35" t="s">
-        <v>963</v>
-      </c>
-      <c r="P35" s="7"/>
+        <v>966</v>
+      </c>
+      <c r="O35" t="s">
+        <v>966</v>
+      </c>
+      <c r="P35" s="7" t="s">
+        <v>5039</v>
+      </c>
       <c r="S35" t="s">
         <v>904</v>
       </c>
@@ -18849,7 +18867,12 @@
       <c r="N36" t="s">
         <v>963</v>
       </c>
-      <c r="P36" s="7"/>
+      <c r="O36" t="s">
+        <v>963</v>
+      </c>
+      <c r="P36" s="7">
+        <v>2</v>
+      </c>
       <c r="S36" t="s">
         <v>904</v>
       </c>
@@ -18897,46 +18920,51 @@
       <c r="N37" t="s">
         <v>963</v>
       </c>
-      <c r="P37" s="7"/>
+      <c r="O37" t="s">
+        <v>963</v>
+      </c>
+      <c r="P37" s="7">
+        <v>2</v>
+      </c>
       <c r="S37" t="s">
         <v>904</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A38">
+      <c r="A38" s="39">
         <v>37</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="39" t="s">
         <v>3969</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="39" t="s">
         <v>3970</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="39">
         <v>2003</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="39" t="s">
         <v>1212</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" s="39" t="s">
         <v>4605</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G38" s="39" t="s">
         <v>1214</v>
       </c>
-      <c r="H38">
+      <c r="H38" s="39">
         <v>265</v>
       </c>
-      <c r="I38" t="s">
+      <c r="I38" s="39" t="s">
         <v>1213</v>
       </c>
-      <c r="J38" t="s">
+      <c r="J38" s="39" t="s">
         <v>1215</v>
       </c>
-      <c r="K38" t="s">
+      <c r="K38" s="39" t="s">
         <v>1216</v>
       </c>
-      <c r="L38" t="s">
+      <c r="L38" s="39" t="s">
         <v>3969</v>
       </c>
       <c r="M38" t="s">
@@ -18945,7 +18973,15 @@
       <c r="N38" t="s">
         <v>963</v>
       </c>
-      <c r="P38" s="7"/>
+      <c r="O38" t="s">
+        <v>966</v>
+      </c>
+      <c r="P38" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>5157</v>
+      </c>
       <c r="S38" t="s">
         <v>904</v>
       </c>
@@ -18955,7 +18991,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>3971</v>
+        <v>5160</v>
       </c>
       <c r="C39" t="s">
         <v>3972</v>
@@ -18993,7 +19029,12 @@
       <c r="N39" t="s">
         <v>963</v>
       </c>
-      <c r="P39" s="7"/>
+      <c r="O39" t="s">
+        <v>963</v>
+      </c>
+      <c r="P39" s="7">
+        <v>3</v>
+      </c>
       <c r="S39" t="s">
         <v>904</v>
       </c>
@@ -19041,7 +19082,12 @@
       <c r="N40" t="s">
         <v>963</v>
       </c>
-      <c r="P40" s="7"/>
+      <c r="O40" t="s">
+        <v>963</v>
+      </c>
+      <c r="P40" s="7">
+        <v>4</v>
+      </c>
       <c r="S40" t="s">
         <v>904</v>
       </c>
@@ -19089,7 +19135,12 @@
       <c r="N41" t="s">
         <v>963</v>
       </c>
-      <c r="P41" s="7"/>
+      <c r="O41" t="s">
+        <v>963</v>
+      </c>
+      <c r="P41" s="7">
+        <v>2</v>
+      </c>
       <c r="S41" t="s">
         <v>904</v>
       </c>
@@ -19137,7 +19188,12 @@
       <c r="N42" s="27" t="s">
         <v>967</v>
       </c>
-      <c r="P42" s="33"/>
+      <c r="O42" s="27" t="s">
+        <v>966</v>
+      </c>
+      <c r="P42" s="33" t="s">
+        <v>5039</v>
+      </c>
       <c r="S42" s="27" t="s">
         <v>904</v>
       </c>
@@ -44710,10 +44766,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{749DD0D2-2E6A-40E6-8DF0-CDB0B0705093}">
-  <dimension ref="A1:Z16"/>
+  <dimension ref="A1:Z17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -44778,14 +44834,14 @@
       </c>
       <c r="S1" s="29">
         <f>COUNTIFS($N:$N, "YES", $F:$F, "&lt;&gt;")</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="U1" s="28" t="s">
         <v>5049</v>
       </c>
       <c r="V1" s="29">
         <f>COUNTIF($M$2:$M$573, "YES")</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="W1" s="31"/>
       <c r="X1" s="31"/>
@@ -45061,7 +45117,7 @@
       </c>
       <c r="S6">
         <f>COUNTIFS($N:$N, "YES", $M:$M, "&lt;&gt;PRIMARY STUDY")</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="X6" t="s">
         <v>5089</v>
@@ -45568,6 +45624,59 @@
         <v>1</v>
       </c>
       <c r="Q16" t="s">
+        <v>5159</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3969</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3970</v>
+      </c>
+      <c r="D17">
+        <v>2003</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1212</v>
+      </c>
+      <c r="F17" t="s">
+        <v>4605</v>
+      </c>
+      <c r="G17" t="s">
+        <v>1214</v>
+      </c>
+      <c r="H17">
+        <v>265</v>
+      </c>
+      <c r="I17" t="s">
+        <v>1213</v>
+      </c>
+      <c r="J17" t="s">
+        <v>1215</v>
+      </c>
+      <c r="K17" t="s">
+        <v>1216</v>
+      </c>
+      <c r="L17" t="s">
+        <v>3969</v>
+      </c>
+      <c r="M17" t="s">
+        <v>963</v>
+      </c>
+      <c r="N17" t="s">
+        <v>963</v>
+      </c>
+      <c r="O17" t="s">
+        <v>966</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="Q17" t="s">
         <v>5159</v>
       </c>
     </row>
@@ -45577,7 +45686,7 @@
       <formula>LEN(TRIM(F1))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:O16">
+  <conditionalFormatting sqref="M2:O17">
     <cfRule type="containsText" dxfId="15" priority="7" operator="containsText" text="PRIMARY STUDY">
       <formula>NOT(ISERROR(SEARCH("PRIMARY STUDY",M2)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Added more data, at almost 400 obs
</commit_message>
<xml_diff>
--- a/Literature/Literature.xlsx
+++ b/Literature/Literature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hso20\OneDrive\Plocha\IES\Diploma-Thesis\Literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D980C5F3-80BC-4FD5-BF01-815CE521860C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C51B92ED-61E0-4AEA-9166-15174B6B0872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -496,7 +496,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9840" uniqueCount="5161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9859" uniqueCount="5162">
   <si>
     <t>Number</t>
   </si>
@@ -15979,6 +15979,9 @@
   </si>
   <si>
     <t>lwol</t>
+  </si>
+  <si>
+    <t>ch4, well written theory</t>
   </si>
 </sst>
 </file>
@@ -16364,6 +16367,27 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAACAC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBA8CDC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
@@ -16547,27 +16571,6 @@
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAACAC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBA8CDC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -16894,8 +16897,8 @@
   <dimension ref="A1:Z575"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B49" sqref="B49"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q58" sqref="Q58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17220,7 +17223,7 @@
       </c>
       <c r="V5" s="38">
         <f>COUNTIFS($O:$O, "YES", $F:$F, "&lt;&gt;")</f>
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.3">
@@ -19612,7 +19615,12 @@
       <c r="N50" t="s">
         <v>963</v>
       </c>
-      <c r="P50" s="7"/>
+      <c r="O50" t="s">
+        <v>963</v>
+      </c>
+      <c r="P50" s="7">
+        <v>2</v>
+      </c>
       <c r="S50" t="s">
         <v>904</v>
       </c>
@@ -19766,7 +19774,12 @@
       <c r="N53" t="s">
         <v>963</v>
       </c>
-      <c r="P53" s="7"/>
+      <c r="O53" t="s">
+        <v>963</v>
+      </c>
+      <c r="P53" s="7">
+        <v>4</v>
+      </c>
       <c r="S53" t="s">
         <v>904</v>
       </c>
@@ -19867,7 +19880,12 @@
       <c r="N55" t="s">
         <v>963</v>
       </c>
-      <c r="P55" s="7"/>
+      <c r="O55" t="s">
+        <v>963</v>
+      </c>
+      <c r="P55" s="7">
+        <v>2</v>
+      </c>
       <c r="S55" t="s">
         <v>904</v>
       </c>
@@ -19915,6 +19933,9 @@
       <c r="N56" t="s">
         <v>966</v>
       </c>
+      <c r="O56" t="s">
+        <v>966</v>
+      </c>
       <c r="P56" s="7" t="s">
         <v>5039</v>
       </c>
@@ -19965,7 +19986,15 @@
       <c r="N57" t="s">
         <v>963</v>
       </c>
-      <c r="P57" s="7"/>
+      <c r="O57" t="s">
+        <v>963</v>
+      </c>
+      <c r="P57" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>5161</v>
+      </c>
       <c r="S57" t="s">
         <v>904</v>
       </c>
@@ -20013,6 +20042,9 @@
       <c r="N58" t="s">
         <v>966</v>
       </c>
+      <c r="O58" t="s">
+        <v>966</v>
+      </c>
       <c r="P58" s="7" t="s">
         <v>5039</v>
       </c>
@@ -20111,6 +20143,9 @@
       <c r="N60" t="s">
         <v>966</v>
       </c>
+      <c r="O60" t="s">
+        <v>966</v>
+      </c>
       <c r="P60" s="7" t="s">
         <v>5039</v>
       </c>
@@ -20161,6 +20196,9 @@
       <c r="N61" t="s">
         <v>966</v>
       </c>
+      <c r="O61" t="s">
+        <v>966</v>
+      </c>
       <c r="P61" s="7" t="s">
         <v>5039</v>
       </c>
@@ -20451,6 +20489,9 @@
       <c r="N67" t="s">
         <v>966</v>
       </c>
+      <c r="O67" t="s">
+        <v>966</v>
+      </c>
       <c r="P67" s="7" t="s">
         <v>5039</v>
       </c>
@@ -20597,6 +20638,9 @@
       <c r="N70" t="s">
         <v>966</v>
       </c>
+      <c r="O70" t="s">
+        <v>966</v>
+      </c>
       <c r="P70" s="7" t="s">
         <v>5039</v>
       </c>
@@ -20743,6 +20787,9 @@
       <c r="N73" t="s">
         <v>966</v>
       </c>
+      <c r="O73" t="s">
+        <v>966</v>
+      </c>
       <c r="P73" s="7" t="s">
         <v>5039</v>
       </c>
@@ -20793,6 +20840,9 @@
       <c r="N74" t="s">
         <v>966</v>
       </c>
+      <c r="O74" t="s">
+        <v>966</v>
+      </c>
       <c r="P74" s="7" t="s">
         <v>5039</v>
       </c>
@@ -20843,6 +20893,9 @@
       <c r="N75" t="s">
         <v>966</v>
       </c>
+      <c r="O75" t="s">
+        <v>966</v>
+      </c>
       <c r="P75" s="7" t="s">
         <v>5039</v>
       </c>
@@ -20893,6 +20946,9 @@
       <c r="N76" t="s">
         <v>966</v>
       </c>
+      <c r="O76" t="s">
+        <v>966</v>
+      </c>
       <c r="P76" s="7" t="s">
         <v>5039</v>
       </c>
@@ -20991,6 +21047,9 @@
       <c r="N78" t="s">
         <v>966</v>
       </c>
+      <c r="O78" t="s">
+        <v>966</v>
+      </c>
       <c r="P78" s="7" t="s">
         <v>5039</v>
       </c>
@@ -21233,6 +21292,9 @@
       <c r="N83" t="s">
         <v>966</v>
       </c>
+      <c r="O83" t="s">
+        <v>966</v>
+      </c>
       <c r="P83" s="7" t="s">
         <v>5039</v>
       </c>
@@ -21379,6 +21441,9 @@
       <c r="N86" t="s">
         <v>966</v>
       </c>
+      <c r="O86" t="s">
+        <v>966</v>
+      </c>
       <c r="P86" s="7" t="s">
         <v>5039</v>
       </c>
@@ -21475,6 +21540,9 @@
         <v>974</v>
       </c>
       <c r="N88" t="s">
+        <v>966</v>
+      </c>
+      <c r="O88" t="s">
         <v>966</v>
       </c>
       <c r="P88" s="7" t="s">
@@ -44762,36 +44830,36 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:O601">
-    <cfRule type="containsText" dxfId="25" priority="11" operator="containsText" text="PRIMARY STUDY">
+    <cfRule type="containsText" dxfId="2" priority="11" operator="containsText" text="PRIMARY STUDY">
       <formula>NOT(ISERROR(SEARCH("PRIMARY STUDY",M2)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="24" priority="12" operator="notContains" text="YES">
+    <cfRule type="notContainsText" dxfId="1" priority="12" operator="notContains" text="YES">
       <formula>ISERROR(SEARCH("YES",M2))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="13" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="0" priority="13" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",M2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="22" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:R10 R16:R1048576 S11:S15">
-    <cfRule type="duplicateValues" dxfId="21" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q131 Q136 Q139 Q146 Q151 Q161 Q163 Q177 Q187 Q189:Q190 P2:P601">
-    <cfRule type="containsBlanks" dxfId="20" priority="22">
+    <cfRule type="containsBlanks" dxfId="23" priority="22">
       <formula>LEN(TRIM(P2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1">
-    <cfRule type="duplicateValues" dxfId="19" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q177 Q187 Q189:Q190 P2:P601">
-    <cfRule type="cellIs" dxfId="18" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="21" priority="8" operator="between">
       <formula>1</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="9" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="20" priority="9" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",P2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -45724,44 +45792,44 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F2">
-    <cfRule type="containsBlanks" dxfId="16" priority="10">
+    <cfRule type="containsBlanks" dxfId="19" priority="10">
       <formula>LEN(TRIM(F1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:O17">
-    <cfRule type="containsText" dxfId="15" priority="7" operator="containsText" text="PRIMARY STUDY">
+    <cfRule type="containsText" dxfId="18" priority="7" operator="containsText" text="PRIMARY STUDY">
       <formula>NOT(ISERROR(SEARCH("PRIMARY STUDY",M2)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="14" priority="8" operator="notContains" text="YES">
+    <cfRule type="notContainsText" dxfId="17" priority="8" operator="notContains" text="YES">
       <formula>ISERROR(SEARCH("YES",M2))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="9" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="16" priority="9" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",M2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B2">
-    <cfRule type="duplicateValues" dxfId="12" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:R2">
-    <cfRule type="duplicateValues" dxfId="11" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="containsBlanks" dxfId="10" priority="11">
+    <cfRule type="containsBlanks" dxfId="13" priority="11">
       <formula>LEN(TRIM(H1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1">
-    <cfRule type="duplicateValues" dxfId="9" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2">
-    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q4 P1:P1048576 Q1">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="between">
       <formula>1</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",P1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -54655,10 +54723,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:K251 L1">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>$K1=FALSE</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="9">
+    <cfRule type="expression" dxfId="7" priority="9">
       <formula>$J1=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -62602,10 +62670,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J259:J1048576 J257 J1:J253">
-    <cfRule type="containsText" dxfId="3" priority="12" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="6" priority="12" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="13" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="5" priority="13" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J1)))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="14">
@@ -62620,10 +62688,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M17">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",M17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",M17)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Hierarchical model now runs silently
</commit_message>
<xml_diff>
--- a/Literature/Literature.xlsx
+++ b/Literature/Literature.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hso20\OneDrive\Plocha\IES\Diploma-Thesis\Literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{779B930E-9976-4A3B-BF69-DAEDCC567775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E6D82E2-FDEC-4D1A-8496-B52F21630CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Query literature" sheetId="5" r:id="rId1"/>
@@ -496,7 +496,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9868" uniqueCount="5162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9871" uniqueCount="5162">
   <si>
     <t>Number</t>
   </si>
@@ -16896,9 +16896,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D4E9F8-720A-49C1-8678-F81C22E3A380}">
   <dimension ref="A1:Z575"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I71" sqref="I71"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K75" sqref="K75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16978,7 +16978,7 @@
       </c>
       <c r="S1" s="29">
         <f>COUNTIFS($N:$N, "YES", $F:$F, "&lt;&gt;") + Twins!S1</f>
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="U1" s="28" t="s">
         <v>5049</v>
@@ -17159,7 +17159,7 @@
       </c>
       <c r="V4">
         <f>COUNTIFS($N:$N, "YES", $M:$M, "&lt;&gt;PRIMARY STUDY", $Q:$Q, "&lt;&gt;Twins")</f>
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.3">
@@ -17223,7 +17223,7 @@
       </c>
       <c r="V5" s="38">
         <f>COUNTIFS($O:$O, "YES", $F:$F, "&lt;&gt;")</f>
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.3">
@@ -20726,12 +20726,17 @@
         <v>3993</v>
       </c>
       <c r="M71" t="s">
-        <v>963</v>
+        <v>974</v>
       </c>
       <c r="N71" t="s">
-        <v>963</v>
-      </c>
-      <c r="P71" s="7"/>
+        <v>966</v>
+      </c>
+      <c r="O71" t="s">
+        <v>966</v>
+      </c>
+      <c r="P71" s="7" t="s">
+        <v>5039</v>
+      </c>
       <c r="S71" t="s">
         <v>904</v>
       </c>
@@ -21039,7 +21044,12 @@
       <c r="N77" t="s">
         <v>963</v>
       </c>
-      <c r="P77" s="7"/>
+      <c r="O77" t="s">
+        <v>963</v>
+      </c>
+      <c r="P77" s="7">
+        <v>2</v>
+      </c>
       <c r="S77" t="s">
         <v>904</v>
       </c>

</xml_diff>

<commit_message>
Added detailed data to the variable list
</commit_message>
<xml_diff>
--- a/Literature/Literature.xlsx
+++ b/Literature/Literature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hso20\OneDrive\Plocha\IES\Diploma-Thesis\Literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14055D3-74A7-4E7E-966A-23FB6840174B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D549F8F-7421-498B-B0E2-D7739C7BECC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -496,7 +496,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9891" uniqueCount="5162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9896" uniqueCount="5162">
   <si>
     <t>Number</t>
   </si>
@@ -16898,8 +16898,8 @@
   <dimension ref="A1:Z575"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B97" sqref="B97"/>
+      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I105" sqref="I105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17224,7 +17224,7 @@
       </c>
       <c r="V5" s="38">
         <f>COUNTIFS($O:$O, "YES", $F:$F, "&lt;&gt;")</f>
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
@@ -22166,6 +22166,9 @@
       <c r="N98" t="s">
         <v>966</v>
       </c>
+      <c r="O98" t="s">
+        <v>966</v>
+      </c>
       <c r="P98" s="7" t="s">
         <v>5037</v>
       </c>
@@ -22216,6 +22219,9 @@
       <c r="N99" t="s">
         <v>966</v>
       </c>
+      <c r="O99" t="s">
+        <v>966</v>
+      </c>
       <c r="P99" s="7" t="s">
         <v>5037</v>
       </c>
@@ -22266,6 +22272,9 @@
       <c r="N100" t="s">
         <v>966</v>
       </c>
+      <c r="O100" t="s">
+        <v>966</v>
+      </c>
       <c r="P100" s="7" t="s">
         <v>5037</v>
       </c>
@@ -22316,6 +22325,9 @@
       <c r="N101" t="s">
         <v>966</v>
       </c>
+      <c r="O101" t="s">
+        <v>966</v>
+      </c>
       <c r="P101" s="7" t="s">
         <v>5037</v>
       </c>
@@ -22366,7 +22378,12 @@
       <c r="N102" t="s">
         <v>963</v>
       </c>
-      <c r="P102" s="7"/>
+      <c r="O102" t="s">
+        <v>963</v>
+      </c>
+      <c r="P102" s="7">
+        <v>3</v>
+      </c>
       <c r="S102" t="s">
         <v>904</v>
       </c>

</xml_diff>

<commit_message>
Added winsorized variables to summary statistics
</commit_message>
<xml_diff>
--- a/Literature/Literature.xlsx
+++ b/Literature/Literature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hso20\OneDrive\Plocha\IES\Diploma-Thesis\Literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D549F8F-7421-498B-B0E2-D7739C7BECC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0197798D-578C-4A4D-A3F7-A18B2F22CEFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -496,7 +496,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9896" uniqueCount="5162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9901" uniqueCount="5162">
   <si>
     <t>Number</t>
   </si>
@@ -16899,7 +16899,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I105" sqref="I105"/>
+      <selection pane="bottomLeft" activeCell="O92" sqref="O92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16979,7 +16979,7 @@
       </c>
       <c r="S1" s="29">
         <f>COUNTIFS($N:$N, "YES", $F:$F, "&lt;&gt;") + Twins!S1</f>
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="U1" s="28" t="s">
         <v>5047</v>
@@ -17160,7 +17160,7 @@
       </c>
       <c r="V4">
         <f>COUNTIFS($N:$N, "YES", $M:$M, "&lt;&gt;PRIMARY STUDY", $Q:$Q, "&lt;&gt;Twins")</f>
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
@@ -17224,7 +17224,7 @@
       </c>
       <c r="V5" s="38">
         <f>COUNTIFS($O:$O, "YES", $F:$F, "&lt;&gt;")</f>
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
@@ -22426,12 +22426,17 @@
         <v>4035</v>
       </c>
       <c r="M103" t="s">
-        <v>963</v>
+        <v>966</v>
       </c>
       <c r="N103" t="s">
-        <v>963</v>
-      </c>
-      <c r="P103" s="7"/>
+        <v>966</v>
+      </c>
+      <c r="O103" t="s">
+        <v>966</v>
+      </c>
+      <c r="P103" s="7" t="s">
+        <v>5037</v>
+      </c>
       <c r="S103" t="s">
         <v>904</v>
       </c>
@@ -22479,7 +22484,12 @@
       <c r="N104" t="s">
         <v>963</v>
       </c>
-      <c r="P104" s="7"/>
+      <c r="O104" t="s">
+        <v>963</v>
+      </c>
+      <c r="P104" s="7">
+        <v>4</v>
+      </c>
       <c r="S104" t="s">
         <v>904</v>
       </c>
@@ -22527,6 +22537,9 @@
       <c r="N105" t="s">
         <v>966</v>
       </c>
+      <c r="O105" t="s">
+        <v>966</v>
+      </c>
       <c r="P105" s="7" t="s">
         <v>5037</v>
       </c>
@@ -22576,6 +22589,9 @@
       </c>
       <c r="N106" t="s">
         <v>964</v>
+      </c>
+      <c r="O106" t="s">
+        <v>966</v>
       </c>
       <c r="P106" s="7" t="s">
         <v>5037</v>

</xml_diff>

<commit_message>
Added subsetting to one study only, more data, cleaner output
</commit_message>
<xml_diff>
--- a/Literature/Literature.xlsx
+++ b/Literature/Literature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hso20\OneDrive\Plocha\IES\Diploma-Thesis\Literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0197798D-578C-4A4D-A3F7-A18B2F22CEFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F5EB82C-3D37-40DA-AD50-9E6D56F6C7F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -496,7 +496,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9901" uniqueCount="5162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9906" uniqueCount="5163">
   <si>
     <t>Number</t>
   </si>
@@ -15982,6 +15982,9 @@
   </si>
   <si>
     <t>Lillo (2006)</t>
+  </si>
+  <si>
+    <t>in-depth</t>
   </si>
 </sst>
 </file>
@@ -16898,8 +16901,8 @@
   <dimension ref="A1:Z575"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O92" sqref="O92"/>
+      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O107" sqref="O107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17224,7 +17227,7 @@
       </c>
       <c r="V5" s="38">
         <f>COUNTIFS($O:$O, "YES", $F:$F, "&lt;&gt;")</f>
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
@@ -22643,7 +22646,12 @@
       <c r="N107" t="s">
         <v>963</v>
       </c>
-      <c r="P107" s="7"/>
+      <c r="O107" t="s">
+        <v>963</v>
+      </c>
+      <c r="P107" s="7">
+        <v>2</v>
+      </c>
       <c r="S107" t="s">
         <v>904</v>
       </c>
@@ -22691,6 +22699,9 @@
       <c r="N108" t="s">
         <v>966</v>
       </c>
+      <c r="O108" t="s">
+        <v>966</v>
+      </c>
       <c r="P108" s="7" t="s">
         <v>5037</v>
       </c>
@@ -22741,6 +22752,9 @@
       <c r="N109" t="s">
         <v>966</v>
       </c>
+      <c r="O109" t="s">
+        <v>966</v>
+      </c>
       <c r="P109" s="7" t="s">
         <v>5037</v>
       </c>
@@ -22791,7 +22805,15 @@
       <c r="N110" t="s">
         <v>963</v>
       </c>
-      <c r="P110" s="7"/>
+      <c r="O110" t="s">
+        <v>963</v>
+      </c>
+      <c r="P110" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q110" t="s">
+        <v>5162</v>
+      </c>
       <c r="S110" t="s">
         <v>904</v>
       </c>

</xml_diff>

<commit_message>
Added Selection Model to the non-linear tests, added docstrings
</commit_message>
<xml_diff>
--- a/Literature/Literature.xlsx
+++ b/Literature/Literature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hso20\OneDrive\Plocha\IES\Diploma-Thesis\Literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F5EB82C-3D37-40DA-AD50-9E6D56F6C7F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C744F9C-D9C3-49AC-B5C7-53099D29E8B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -496,7 +496,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9906" uniqueCount="5163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9908" uniqueCount="5163">
   <si>
     <t>Number</t>
   </si>
@@ -16902,7 +16902,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O107" sqref="O107"/>
+      <selection pane="bottomLeft" activeCell="O113" sqref="O113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22650,7 +22650,7 @@
         <v>963</v>
       </c>
       <c r="P107" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S107" t="s">
         <v>904</v>
@@ -22861,6 +22861,9 @@
       <c r="N111" t="s">
         <v>966</v>
       </c>
+      <c r="O111" t="s">
+        <v>966</v>
+      </c>
       <c r="P111" s="7" t="s">
         <v>5037</v>
       </c>
@@ -22909,6 +22912,9 @@
         <v>974</v>
       </c>
       <c r="N112" t="s">
+        <v>966</v>
+      </c>
+      <c r="O112" t="s">
         <v>966</v>
       </c>
       <c r="P112" s="7" t="s">

</xml_diff>

<commit_message>
Fixed the Endogenous Kink model, put the source code in a separate script
</commit_message>
<xml_diff>
--- a/Literature/Literature.xlsx
+++ b/Literature/Literature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hso20\OneDrive\Plocha\IES\Diploma-Thesis\Literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C744F9C-D9C3-49AC-B5C7-53099D29E8B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B02FE18-F340-482B-9B6B-ED473BFEF459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -496,7 +496,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9908" uniqueCount="5163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9909" uniqueCount="5163">
   <si>
     <t>Number</t>
   </si>
@@ -16902,7 +16902,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O113" sqref="O113"/>
+      <selection pane="bottomLeft" activeCell="N113" sqref="N113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17227,7 +17227,7 @@
       </c>
       <c r="V5" s="38">
         <f>COUNTIFS($O:$O, "YES", $F:$F, "&lt;&gt;")</f>
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
@@ -22967,7 +22967,12 @@
       <c r="N113" t="s">
         <v>963</v>
       </c>
-      <c r="P113" s="7"/>
+      <c r="O113" t="s">
+        <v>963</v>
+      </c>
+      <c r="P113" s="7">
+        <v>3</v>
+      </c>
       <c r="S113" t="s">
         <v>904</v>
       </c>

</xml_diff>

<commit_message>
Added the MAIVE estimator, exo tests coef handling/output
</commit_message>
<xml_diff>
--- a/Literature/Literature.xlsx
+++ b/Literature/Literature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hso20\OneDrive\Plocha\IES\Diploma-Thesis\Literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B02FE18-F340-482B-9B6B-ED473BFEF459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12962AA-26F3-4CBB-81D7-66ECBE5F00B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16902,7 +16902,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N113" sqref="N113"/>
+      <selection pane="bottomLeft" activeCell="N110" sqref="N110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added more data, crested 800 observations
</commit_message>
<xml_diff>
--- a/Literature/Literature.xlsx
+++ b/Literature/Literature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hso20\OneDrive\Plocha\IES\Diploma-Thesis\Literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12962AA-26F3-4CBB-81D7-66ECBE5F00B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9414EC0-F6EA-4B03-9594-099A9B45DF82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -496,7 +496,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9909" uniqueCount="5163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9913" uniqueCount="5163">
   <si>
     <t>Number</t>
   </si>
@@ -16901,8 +16901,8 @@
   <dimension ref="A1:Z575"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N110" sqref="N110"/>
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17227,7 +17227,7 @@
       </c>
       <c r="V5" s="38">
         <f>COUNTIFS($O:$O, "YES", $F:$F, "&lt;&gt;")</f>
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
@@ -23020,7 +23020,12 @@
       <c r="N114" t="s">
         <v>963</v>
       </c>
-      <c r="P114" s="7"/>
+      <c r="O114" t="s">
+        <v>963</v>
+      </c>
+      <c r="P114" s="7">
+        <v>3</v>
+      </c>
       <c r="S114" t="s">
         <v>904</v>
       </c>
@@ -23068,7 +23073,12 @@
       <c r="N115" t="s">
         <v>963</v>
       </c>
-      <c r="P115" s="7"/>
+      <c r="O115" t="s">
+        <v>963</v>
+      </c>
+      <c r="P115" s="7">
+        <v>2</v>
+      </c>
       <c r="S115" t="s">
         <v>904</v>
       </c>
@@ -23116,8 +23126,11 @@
       <c r="N116" t="s">
         <v>963</v>
       </c>
+      <c r="O116" t="s">
+        <v>963</v>
+      </c>
       <c r="P116" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S116" t="s">
         <v>904</v>
@@ -23165,6 +23178,9 @@
       </c>
       <c r="N117" t="s">
         <v>966</v>
+      </c>
+      <c r="O117" t="s">
+        <v>5037</v>
       </c>
       <c r="P117" s="7" t="s">
         <v>5037</v>

</xml_diff>

<commit_message>
Added p-uni to the exogenous methods
</commit_message>
<xml_diff>
--- a/Literature/Literature.xlsx
+++ b/Literature/Literature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hso20\OneDrive\Plocha\IES\Diploma-Thesis\Literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCC270B-E994-4C12-8CAF-F0603A473C5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63138BE2-13B7-4E9C-8069-8593DDA20B32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -496,7 +496,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9923" uniqueCount="5165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9924" uniqueCount="5165">
   <si>
     <t>Number</t>
   </si>
@@ -16907,8 +16907,8 @@
   <dimension ref="A1:Z575"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K117" sqref="K117"/>
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O128" sqref="O128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23720,6 +23720,9 @@
       </c>
       <c r="N127" t="s">
         <v>963</v>
+      </c>
+      <c r="O127" t="s">
+        <v>966</v>
       </c>
       <c r="P127" s="7">
         <v>1</v>

</xml_diff>

<commit_message>
Added a clever validation function, data type preprocessing
</commit_message>
<xml_diff>
--- a/Literature/Literature.xlsx
+++ b/Literature/Literature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hso20\OneDrive\Plocha\IES\Diploma-Thesis\Literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63138BE2-13B7-4E9C-8069-8593DDA20B32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED85B85-9EDA-4CCD-A590-9D63A16086AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -496,7 +496,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9924" uniqueCount="5165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9927" uniqueCount="5164">
   <si>
     <t>Number</t>
   </si>
@@ -15640,9 +15640,6 @@
   </si>
   <si>
     <t>IDENTIFIED</t>
-  </si>
-  <si>
-    <t>Not sure if years of schooling are used properly, otherwise good theory</t>
   </si>
   <si>
     <t>Too granular focus of dep var</t>
@@ -16907,8 +16904,8 @@
   <dimension ref="A1:Z575"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O128" sqref="O128"/>
+      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P132" sqref="P132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16975,13 +16972,13 @@
         <v>962</v>
       </c>
       <c r="O1" s="24" t="s">
-        <v>5150</v>
+        <v>5149</v>
       </c>
       <c r="P1" s="25" t="s">
-        <v>5148</v>
+        <v>5147</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>5156</v>
+        <v>5155</v>
       </c>
       <c r="R1" s="28" t="s">
         <v>5046</v>
@@ -17165,7 +17162,7 @@
         <v>574</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>5154</v>
+        <v>5153</v>
       </c>
       <c r="V4">
         <f>COUNTIFS($N:$N, "YES", $M:$M, "&lt;&gt;PRIMARY STUDY", $Q:$Q, "&lt;&gt;Twins")</f>
@@ -17229,11 +17226,11 @@
         <v>574</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>5151</v>
+        <v>5150</v>
       </c>
       <c r="V5" s="38">
         <f>COUNTIFS($O:$O, "YES", $F:$F, "&lt;&gt;")</f>
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
@@ -17550,10 +17547,10 @@
         <v>1</v>
       </c>
       <c r="Q11" t="s">
-        <v>5155</v>
+        <v>5154</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>5149</v>
+        <v>5148</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
@@ -17609,7 +17606,7 @@
         <v>1</v>
       </c>
       <c r="S12" t="s">
-        <v>5152</v>
+        <v>5151</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
@@ -17665,7 +17662,7 @@
         <v>2</v>
       </c>
       <c r="S13" t="s">
-        <v>5153</v>
+        <v>5152</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
@@ -18993,7 +18990,7 @@
         <v>1</v>
       </c>
       <c r="Q38" t="s">
-        <v>5155</v>
+        <v>5154</v>
       </c>
       <c r="S38" t="s">
         <v>904</v>
@@ -19004,7 +19001,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>5158</v>
+        <v>5157</v>
       </c>
       <c r="C39" t="s">
         <v>3972</v>
@@ -20003,7 +20000,7 @@
         <v>2</v>
       </c>
       <c r="Q57" t="s">
-        <v>5159</v>
+        <v>5158</v>
       </c>
       <c r="S57" t="s">
         <v>904</v>
@@ -21755,7 +21752,7 @@
         <v>1</v>
       </c>
       <c r="Q90" t="s">
-        <v>5160</v>
+        <v>5159</v>
       </c>
       <c r="S90" t="s">
         <v>904</v>
@@ -21766,7 +21763,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>5161</v>
+        <v>5160</v>
       </c>
       <c r="C91" t="s">
         <v>4019</v>
@@ -21796,7 +21793,7 @@
         <v>1491</v>
       </c>
       <c r="L91" t="s">
-        <v>5161</v>
+        <v>5160</v>
       </c>
       <c r="M91" t="s">
         <v>963</v>
@@ -22818,7 +22815,7 @@
         <v>1</v>
       </c>
       <c r="Q110" t="s">
-        <v>5162</v>
+        <v>5161</v>
       </c>
       <c r="S110" t="s">
         <v>904</v>
@@ -23286,7 +23283,7 @@
         <v>4055</v>
       </c>
       <c r="M119" t="s">
-        <v>5164</v>
+        <v>5163</v>
       </c>
       <c r="N119" t="s">
         <v>963</v>
@@ -23298,7 +23295,7 @@
         <v>4</v>
       </c>
       <c r="Q119" t="s">
-        <v>5163</v>
+        <v>5162</v>
       </c>
       <c r="S119" t="s">
         <v>904</v>
@@ -23774,6 +23771,9 @@
       <c r="N128" t="s">
         <v>966</v>
       </c>
+      <c r="O128" t="s">
+        <v>966</v>
+      </c>
       <c r="P128" s="7" t="s">
         <v>5037</v>
       </c>
@@ -23824,6 +23824,9 @@
       <c r="N129" t="s">
         <v>966</v>
       </c>
+      <c r="O129" t="s">
+        <v>966</v>
+      </c>
       <c r="P129" s="7" t="s">
         <v>5037</v>
       </c>
@@ -23874,6 +23877,9 @@
       <c r="N130" t="s">
         <v>966</v>
       </c>
+      <c r="O130" t="s">
+        <v>966</v>
+      </c>
       <c r="P130" s="7" t="s">
         <v>5037</v>
       </c>
@@ -23924,11 +23930,11 @@
       <c r="N131" t="s">
         <v>963</v>
       </c>
+      <c r="O131" t="s">
+        <v>963</v>
+      </c>
       <c r="P131" s="7">
-        <v>1</v>
-      </c>
-      <c r="Q131" t="s">
-        <v>5048</v>
+        <v>2</v>
       </c>
       <c r="S131" t="s">
         <v>904</v>
@@ -24178,7 +24184,7 @@
         <v>2</v>
       </c>
       <c r="Q136" t="s">
-        <v>5049</v>
+        <v>5048</v>
       </c>
       <c r="S136" t="s">
         <v>904</v>
@@ -24331,7 +24337,7 @@
         <v>1</v>
       </c>
       <c r="Q139" t="s">
-        <v>5050</v>
+        <v>5049</v>
       </c>
       <c r="S139" t="s">
         <v>904</v>
@@ -24419,7 +24425,7 @@
         <v>2027</v>
       </c>
       <c r="K141" t="s">
-        <v>5051</v>
+        <v>5050</v>
       </c>
       <c r="L141" t="s">
         <v>4900</v>
@@ -24681,7 +24687,7 @@
         <v>1</v>
       </c>
       <c r="Q146" t="s">
-        <v>5052</v>
+        <v>5051</v>
       </c>
       <c r="S146" t="s">
         <v>904</v>
@@ -24931,7 +24937,7 @@
         <v>3</v>
       </c>
       <c r="Q151" t="s">
-        <v>5053</v>
+        <v>5052</v>
       </c>
       <c r="S151" t="s">
         <v>904</v>
@@ -25434,7 +25440,7 @@
         <v>2</v>
       </c>
       <c r="Q161" t="s">
-        <v>5054</v>
+        <v>5053</v>
       </c>
       <c r="S161" t="s">
         <v>904</v>
@@ -25537,7 +25543,7 @@
         <v>2</v>
       </c>
       <c r="Q163" t="s">
-        <v>5055</v>
+        <v>5054</v>
       </c>
       <c r="S163" t="s">
         <v>904</v>
@@ -26249,7 +26255,7 @@
         <v>5037</v>
       </c>
       <c r="Q177" t="s">
-        <v>5056</v>
+        <v>5055</v>
       </c>
       <c r="S177" t="s">
         <v>904</v>
@@ -26752,7 +26758,7 @@
         <v>1</v>
       </c>
       <c r="Q187" t="s">
-        <v>5057</v>
+        <v>5056</v>
       </c>
       <c r="S187" t="s">
         <v>904</v>
@@ -26855,7 +26861,7 @@
         <v>1</v>
       </c>
       <c r="Q189" t="s">
-        <v>5079</v>
+        <v>5078</v>
       </c>
       <c r="S189" t="s">
         <v>904</v>
@@ -26908,7 +26914,7 @@
         <v>5037</v>
       </c>
       <c r="Q190" t="s">
-        <v>5080</v>
+        <v>5079</v>
       </c>
       <c r="S190" t="s">
         <v>904</v>
@@ -29255,7 +29261,7 @@
         <v>239</v>
       </c>
       <c r="B240" t="s">
-        <v>5081</v>
+        <v>5080</v>
       </c>
       <c r="C240" t="s">
         <v>4792</v>
@@ -45099,7 +45105,7 @@
   <conditionalFormatting sqref="R1:R10 R16:R1048576 S11:S15">
     <cfRule type="duplicateValues" dxfId="21" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q131 Q136 Q139 Q146 Q151 Q161 Q163 Q177 Q187 Q189:Q190 P2:P601">
+  <conditionalFormatting sqref="Q136 Q139 Q146 Q151 Q161 Q163 Q177 Q187 Q189:Q190 P2:P601">
     <cfRule type="containsBlanks" dxfId="20" priority="22">
       <formula>LEN(TRIM(P2))=0</formula>
     </cfRule>
@@ -45185,13 +45191,13 @@
         <v>962</v>
       </c>
       <c r="O1" s="24" t="s">
-        <v>5150</v>
+        <v>5149</v>
       </c>
       <c r="P1" s="25" t="s">
         <v>5034</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>5156</v>
+        <v>5155</v>
       </c>
       <c r="R1" s="28" t="s">
         <v>5046</v>
@@ -45217,19 +45223,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5063</v>
+        <v>5062</v>
       </c>
       <c r="C2" t="s">
-        <v>5062</v>
+        <v>5061</v>
       </c>
       <c r="D2">
         <v>1998</v>
       </c>
       <c r="E2" t="s">
-        <v>5070</v>
+        <v>5069</v>
       </c>
       <c r="F2" t="s">
-        <v>5061</v>
+        <v>5060</v>
       </c>
       <c r="G2" t="s">
         <v>5038</v>
@@ -45238,16 +45244,16 @@
         <v>908</v>
       </c>
       <c r="I2" t="s">
-        <v>5065</v>
+        <v>5064</v>
       </c>
       <c r="J2" t="s">
-        <v>5064</v>
+        <v>5063</v>
       </c>
       <c r="K2" t="s">
-        <v>5064</v>
+        <v>5063</v>
       </c>
       <c r="L2" t="s">
-        <v>5063</v>
+        <v>5062</v>
       </c>
       <c r="M2" t="s">
         <v>963</v>
@@ -45265,7 +45271,7 @@
         <v>904</v>
       </c>
       <c r="X2" t="s">
-        <v>5058</v>
+        <v>5057</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
@@ -45273,19 +45279,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5072</v>
+        <v>5071</v>
       </c>
       <c r="C3" t="s">
-        <v>5071</v>
+        <v>5070</v>
       </c>
       <c r="D3">
         <v>1994</v>
       </c>
       <c r="E3" t="s">
-        <v>5069</v>
+        <v>5068</v>
       </c>
       <c r="F3" t="s">
-        <v>5066</v>
+        <v>5065</v>
       </c>
       <c r="G3" t="s">
         <v>5038</v>
@@ -45294,16 +45300,16 @@
         <v>1812</v>
       </c>
       <c r="I3" t="s">
+        <v>5066</v>
+      </c>
+      <c r="J3" t="s">
         <v>5067</v>
       </c>
-      <c r="J3" t="s">
-        <v>5068</v>
-      </c>
       <c r="K3" t="s">
-        <v>5068</v>
+        <v>5067</v>
       </c>
       <c r="L3" t="s">
-        <v>5072</v>
+        <v>5071</v>
       </c>
       <c r="M3" t="s">
         <v>963</v>
@@ -45318,7 +45324,7 @@
         <v>1</v>
       </c>
       <c r="X3" t="s">
-        <v>5059</v>
+        <v>5058</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
@@ -45335,10 +45341,10 @@
         <v>1999</v>
       </c>
       <c r="E4" t="s">
-        <v>5077</v>
+        <v>5076</v>
       </c>
       <c r="F4" t="s">
-        <v>5073</v>
+        <v>5072</v>
       </c>
       <c r="G4" t="s">
         <v>5038</v>
@@ -45347,13 +45353,13 @@
         <v>188</v>
       </c>
       <c r="I4" t="s">
+        <v>5073</v>
+      </c>
+      <c r="J4" t="s">
+        <v>5075</v>
+      </c>
+      <c r="K4" t="s">
         <v>5074</v>
-      </c>
-      <c r="J4" t="s">
-        <v>5076</v>
-      </c>
-      <c r="K4" t="s">
-        <v>5075</v>
       </c>
       <c r="L4" t="s">
         <v>727</v>
@@ -45371,10 +45377,10 @@
         <v>1</v>
       </c>
       <c r="Q4" t="s">
-        <v>5078</v>
+        <v>5077</v>
       </c>
       <c r="X4" t="s">
-        <v>5060</v>
+        <v>5059</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
@@ -45382,19 +45388,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5082</v>
+        <v>5081</v>
       </c>
       <c r="C5" t="s">
-        <v>5090</v>
+        <v>5089</v>
       </c>
       <c r="D5">
         <v>2003</v>
       </c>
       <c r="E5" t="s">
+        <v>5093</v>
+      </c>
+      <c r="F5" t="s">
         <v>5094</v>
-      </c>
-      <c r="F5" t="s">
-        <v>5095</v>
       </c>
       <c r="G5" t="s">
         <v>5038</v>
@@ -45403,16 +45409,16 @@
         <v>158</v>
       </c>
       <c r="I5" t="s">
+        <v>5087</v>
+      </c>
+      <c r="J5" t="s">
         <v>5088</v>
       </c>
-      <c r="J5" t="s">
-        <v>5089</v>
-      </c>
       <c r="K5" t="s">
-        <v>5089</v>
+        <v>5088</v>
       </c>
       <c r="L5" t="s">
-        <v>5082</v>
+        <v>5081</v>
       </c>
       <c r="M5" t="s">
         <v>963</v>
@@ -45432,19 +45438,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>5083</v>
+        <v>5082</v>
       </c>
       <c r="C6" t="s">
-        <v>5091</v>
+        <v>5090</v>
       </c>
       <c r="D6">
         <v>2012</v>
       </c>
       <c r="E6" t="s">
-        <v>5097</v>
+        <v>5096</v>
       </c>
       <c r="F6" t="s">
-        <v>5096</v>
+        <v>5095</v>
       </c>
       <c r="G6" t="s">
         <v>5038</v>
@@ -45453,16 +45459,16 @@
         <v>176</v>
       </c>
       <c r="I6" t="s">
+        <v>5097</v>
+      </c>
+      <c r="J6" t="s">
         <v>5098</v>
       </c>
-      <c r="J6" t="s">
-        <v>5099</v>
-      </c>
       <c r="K6" t="s">
-        <v>5099</v>
+        <v>5098</v>
       </c>
       <c r="L6" t="s">
-        <v>5083</v>
+        <v>5082</v>
       </c>
       <c r="M6" t="s">
         <v>963</v>
@@ -45477,14 +45483,14 @@
         <v>1</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>5154</v>
+        <v>5153</v>
       </c>
       <c r="S6">
         <f>COUNTIFS($N:$N, "YES", $M:$M, "&lt;&gt;PRIMARY STUDY")</f>
         <v>16</v>
       </c>
       <c r="X6" t="s">
-        <v>5087</v>
+        <v>5086</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
@@ -45492,7 +45498,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>5084</v>
+        <v>5083</v>
       </c>
       <c r="C7" t="s">
         <v>4134</v>
@@ -45501,10 +45507,10 @@
         <v>1995</v>
       </c>
       <c r="E7" t="s">
+        <v>5099</v>
+      </c>
+      <c r="F7" t="s">
         <v>5100</v>
-      </c>
-      <c r="F7" t="s">
-        <v>5101</v>
       </c>
       <c r="G7" t="s">
         <v>5038</v>
@@ -45513,16 +45519,16 @@
         <v>372</v>
       </c>
       <c r="I7" t="s">
+        <v>5101</v>
+      </c>
+      <c r="J7" t="s">
         <v>5102</v>
       </c>
-      <c r="J7" t="s">
-        <v>5103</v>
-      </c>
       <c r="K7" t="s">
-        <v>5103</v>
+        <v>5102</v>
       </c>
       <c r="L7" t="s">
-        <v>5084</v>
+        <v>5083</v>
       </c>
       <c r="M7" t="s">
         <v>963</v>
@@ -45537,7 +45543,7 @@
         <v>1</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>5151</v>
+        <v>5150</v>
       </c>
       <c r="S7">
         <f>COUNTIFS($O:$O, "YES", $F:$F, "&lt;&gt;")</f>
@@ -45549,19 +45555,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>5104</v>
+        <v>5103</v>
       </c>
       <c r="C8" t="s">
-        <v>5092</v>
+        <v>5091</v>
       </c>
       <c r="D8">
         <v>1976</v>
       </c>
       <c r="E8" t="s">
+        <v>5104</v>
+      </c>
+      <c r="F8" t="s">
         <v>5105</v>
-      </c>
-      <c r="F8" t="s">
-        <v>5106</v>
       </c>
       <c r="G8" t="s">
         <v>5038</v>
@@ -45570,16 +45576,16 @@
         <v>382</v>
       </c>
       <c r="I8" t="s">
+        <v>5106</v>
+      </c>
+      <c r="J8" t="s">
         <v>5107</v>
       </c>
-      <c r="J8" t="s">
-        <v>5108</v>
-      </c>
       <c r="K8" t="s">
-        <v>5108</v>
+        <v>5107</v>
       </c>
       <c r="L8" t="s">
-        <v>5104</v>
+        <v>5103</v>
       </c>
       <c r="M8" t="s">
         <v>963</v>
@@ -45599,7 +45605,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>5085</v>
+        <v>5084</v>
       </c>
       <c r="C9" t="s">
         <v>4081</v>
@@ -45608,10 +45614,10 @@
         <v>1994</v>
       </c>
       <c r="E9" t="s">
-        <v>5112</v>
+        <v>5111</v>
       </c>
       <c r="F9" t="s">
-        <v>5111</v>
+        <v>5110</v>
       </c>
       <c r="G9" t="s">
         <v>5038</v>
@@ -45620,13 +45626,13 @@
         <v>616</v>
       </c>
       <c r="I9" t="s">
+        <v>5108</v>
+      </c>
+      <c r="J9" t="s">
         <v>5109</v>
       </c>
-      <c r="J9" t="s">
-        <v>5110</v>
-      </c>
       <c r="L9" t="s">
-        <v>5085</v>
+        <v>5084</v>
       </c>
       <c r="M9" t="s">
         <v>963</v>
@@ -45646,19 +45652,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>5086</v>
+        <v>5085</v>
       </c>
       <c r="C10" t="s">
-        <v>5093</v>
+        <v>5092</v>
       </c>
       <c r="D10">
         <v>1999</v>
       </c>
       <c r="E10" t="s">
+        <v>5114</v>
+      </c>
+      <c r="F10" t="s">
         <v>5115</v>
-      </c>
-      <c r="F10" t="s">
-        <v>5116</v>
       </c>
       <c r="G10" t="s">
         <v>5038</v>
@@ -45667,16 +45673,16 @@
         <v>196</v>
       </c>
       <c r="I10" t="s">
+        <v>5112</v>
+      </c>
+      <c r="J10" t="s">
         <v>5113</v>
       </c>
-      <c r="J10" t="s">
-        <v>5114</v>
-      </c>
       <c r="K10" t="s">
-        <v>5114</v>
+        <v>5113</v>
       </c>
       <c r="L10" t="s">
-        <v>5086</v>
+        <v>5085</v>
       </c>
       <c r="M10" t="s">
         <v>963</v>
@@ -45696,19 +45702,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>5119</v>
+      </c>
+      <c r="C11" t="s">
         <v>5120</v>
-      </c>
-      <c r="C11" t="s">
-        <v>5121</v>
       </c>
       <c r="D11">
         <v>1996</v>
       </c>
       <c r="E11" t="s">
-        <v>5122</v>
+        <v>5121</v>
       </c>
       <c r="F11" t="s">
-        <v>5117</v>
+        <v>5116</v>
       </c>
       <c r="G11" t="s">
         <v>5038</v>
@@ -45717,13 +45723,13 @@
         <v>218</v>
       </c>
       <c r="I11" t="s">
+        <v>5117</v>
+      </c>
+      <c r="J11" t="s">
         <v>5118</v>
       </c>
-      <c r="J11" t="s">
+      <c r="L11" t="s">
         <v>5119</v>
-      </c>
-      <c r="L11" t="s">
-        <v>5120</v>
       </c>
       <c r="M11" t="s">
         <v>963</v>
@@ -45743,19 +45749,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>5128</v>
+        <v>5127</v>
       </c>
       <c r="C12" t="s">
-        <v>5127</v>
+        <v>5126</v>
       </c>
       <c r="D12">
         <v>2002</v>
       </c>
       <c r="E12" t="s">
-        <v>5126</v>
+        <v>5125</v>
       </c>
       <c r="F12" t="s">
-        <v>5123</v>
+        <v>5122</v>
       </c>
       <c r="G12" t="s">
         <v>5038</v>
@@ -45764,16 +45770,16 @@
         <v>320</v>
       </c>
       <c r="I12" t="s">
+        <v>5123</v>
+      </c>
+      <c r="J12" t="s">
         <v>5124</v>
       </c>
-      <c r="J12" t="s">
-        <v>5125</v>
-      </c>
       <c r="K12" t="s">
-        <v>5125</v>
+        <v>5124</v>
       </c>
       <c r="L12" t="s">
-        <v>5128</v>
+        <v>5127</v>
       </c>
       <c r="M12" t="s">
         <v>963</v>
@@ -45793,19 +45799,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>5132</v>
+      </c>
+      <c r="C13" t="s">
         <v>5133</v>
-      </c>
-      <c r="C13" t="s">
-        <v>5134</v>
       </c>
       <c r="D13">
         <v>2018</v>
       </c>
       <c r="E13" t="s">
-        <v>5135</v>
+        <v>5134</v>
       </c>
       <c r="F13" t="s">
-        <v>5129</v>
+        <v>5128</v>
       </c>
       <c r="G13" t="s">
         <v>5038</v>
@@ -45814,16 +45820,16 @@
         <v>181</v>
       </c>
       <c r="I13" t="s">
+        <v>5129</v>
+      </c>
+      <c r="J13" t="s">
         <v>5130</v>
       </c>
-      <c r="J13" t="s">
-        <v>5131</v>
-      </c>
       <c r="K13" t="s">
-        <v>5131</v>
+        <v>5130</v>
       </c>
       <c r="L13" t="s">
-        <v>5133</v>
+        <v>5132</v>
       </c>
       <c r="M13" t="s">
         <v>963</v>
@@ -45835,7 +45841,7 @@
         <v>966</v>
       </c>
       <c r="P13" t="s">
-        <v>5132</v>
+        <v>5131</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
@@ -45843,19 +45849,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>5138</v>
+      </c>
+      <c r="C14" t="s">
         <v>5139</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5140</v>
       </c>
       <c r="D14">
         <v>2012</v>
       </c>
       <c r="E14" t="s">
-        <v>5141</v>
+        <v>5140</v>
       </c>
       <c r="F14" t="s">
-        <v>5136</v>
+        <v>5135</v>
       </c>
       <c r="G14" t="s">
         <v>5038</v>
@@ -45864,16 +45870,16 @@
         <v>18</v>
       </c>
       <c r="I14" t="s">
+        <v>5136</v>
+      </c>
+      <c r="J14" t="s">
         <v>5137</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
+        <v>5137</v>
+      </c>
+      <c r="L14" t="s">
         <v>5138</v>
-      </c>
-      <c r="K14" t="s">
-        <v>5138</v>
-      </c>
-      <c r="L14" t="s">
-        <v>5139</v>
       </c>
       <c r="M14" t="s">
         <v>963</v>
@@ -45893,19 +45899,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>5146</v>
+        <v>5145</v>
       </c>
       <c r="C15" t="s">
-        <v>5143</v>
+        <v>5142</v>
       </c>
       <c r="D15">
         <v>2020</v>
       </c>
       <c r="E15" t="s">
-        <v>5147</v>
+        <v>5146</v>
       </c>
       <c r="F15" t="s">
-        <v>5144</v>
+        <v>5143</v>
       </c>
       <c r="G15" t="s">
         <v>5038</v>
@@ -45914,16 +45920,16 @@
         <v>11</v>
       </c>
       <c r="I15" t="s">
+        <v>5144</v>
+      </c>
+      <c r="J15" t="s">
+        <v>5141</v>
+      </c>
+      <c r="K15" t="s">
+        <v>5141</v>
+      </c>
+      <c r="L15" t="s">
         <v>5145</v>
-      </c>
-      <c r="J15" t="s">
-        <v>5142</v>
-      </c>
-      <c r="K15" t="s">
-        <v>5142</v>
-      </c>
-      <c r="L15" t="s">
-        <v>5146</v>
       </c>
       <c r="M15" t="s">
         <v>963</v>
@@ -45988,7 +45994,7 @@
         <v>1</v>
       </c>
       <c r="Q16" t="s">
-        <v>5157</v>
+        <v>5156</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -46041,7 +46047,7 @@
         <v>1</v>
       </c>
       <c r="Q17" t="s">
-        <v>5157</v>
+        <v>5156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a function for automatic country info filling, added med_exp/min_wage data, AI generated
</commit_message>
<xml_diff>
--- a/Literature/Literature.xlsx
+++ b/Literature/Literature.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hso20\OneDrive\Plocha\IES\Diploma-Thesis\Literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED9A6F50-93F2-4D65-A24E-08364C221C8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7706826-902A-4225-A0BC-6BEA8CF3FED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Query literature" sheetId="5" r:id="rId1"/>
@@ -642,7 +642,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16527" uniqueCount="5162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16530" uniqueCount="5162">
   <si>
     <t>Number</t>
   </si>
@@ -16513,66 +16513,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFAACAC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAACAC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAACAC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBA8CDC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6161"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
@@ -16663,6 +16603,66 @@
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAACAC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBA8CDC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6161"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAACAC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAACAC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -17104,8 +17104,8 @@
   <dimension ref="A1:Z575"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E49" sqref="E49"/>
+      <pane ySplit="1" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O135" sqref="O135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17430,7 +17430,7 @@
       </c>
       <c r="V5" s="38">
         <f>COUNTIFS($O:$O, "YES", $F:$F, "&lt;&gt;")</f>
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
@@ -24183,8 +24183,11 @@
       <c r="N132" t="s">
         <v>963</v>
       </c>
+      <c r="O132" t="s">
+        <v>963</v>
+      </c>
       <c r="P132" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="S132" t="s">
         <v>904</v>
@@ -24230,6 +24233,9 @@
       <c r="N133" t="s">
         <v>966</v>
       </c>
+      <c r="O133" t="s">
+        <v>966</v>
+      </c>
       <c r="P133" s="7" t="s">
         <v>5037</v>
       </c>
@@ -24278,6 +24284,9 @@
         <v>972</v>
       </c>
       <c r="N134" t="s">
+        <v>966</v>
+      </c>
+      <c r="O134" t="s">
         <v>966</v>
       </c>
       <c r="P134" s="7" t="s">
@@ -71681,35 +71690,35 @@
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsBlanks" dxfId="7" priority="7">
+    <cfRule type="containsBlanks" dxfId="24" priority="7">
       <formula>LEN(TRIM(F1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:O601">
-    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="PRIMARY STUDY">
+    <cfRule type="containsText" dxfId="23" priority="4" operator="containsText" text="PRIMARY STUDY">
       <formula>NOT(ISERROR(SEARCH("PRIMARY STUDY",M2)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="5" priority="5" operator="notContains" text="YES">
+    <cfRule type="notContainsText" dxfId="22" priority="5" operator="notContains" text="YES">
       <formula>ISERROR(SEARCH("YES",M2))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="21" priority="6" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",M2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B38 B40:B1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P601">
-    <cfRule type="containsBlanks" dxfId="2" priority="8">
+    <cfRule type="containsBlanks" dxfId="19" priority="8">
       <formula>LEN(TRIM(P2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P601">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="between">
       <formula>1</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="17" priority="3" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",P2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -72642,44 +72651,44 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F2">
-    <cfRule type="containsBlanks" dxfId="24" priority="10">
+    <cfRule type="containsBlanks" dxfId="16" priority="10">
       <formula>LEN(TRIM(F1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:O17">
-    <cfRule type="containsText" dxfId="23" priority="7" operator="containsText" text="PRIMARY STUDY">
+    <cfRule type="containsText" dxfId="15" priority="7" operator="containsText" text="PRIMARY STUDY">
       <formula>NOT(ISERROR(SEARCH("PRIMARY STUDY",M2)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="22" priority="8" operator="notContains" text="YES">
+    <cfRule type="notContainsText" dxfId="14" priority="8" operator="notContains" text="YES">
       <formula>ISERROR(SEARCH("YES",M2))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="9" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="13" priority="9" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",M2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B2">
-    <cfRule type="duplicateValues" dxfId="20" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:R2">
-    <cfRule type="duplicateValues" dxfId="19" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="containsBlanks" dxfId="18" priority="11">
+    <cfRule type="containsBlanks" dxfId="10" priority="11">
       <formula>LEN(TRIM(H1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1">
-    <cfRule type="duplicateValues" dxfId="17" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2">
-    <cfRule type="duplicateValues" dxfId="16" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q4 P1:P1048576 Q1">
-    <cfRule type="cellIs" dxfId="15" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="between">
       <formula>1</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="6" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",P1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -81574,10 +81583,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:K251 L1">
-    <cfRule type="expression" dxfId="13" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>$K1=FALSE</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="9">
+    <cfRule type="expression" dxfId="4" priority="9">
       <formula>$J1=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -89522,10 +89531,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J259:J1048576 J257 J1:J253">
-    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="3" priority="12" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="13" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="2" priority="13" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J1)))</formula>
     </cfRule>
     <cfRule type="colorScale" priority="14">
@@ -89540,10 +89549,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M17">
-    <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",M17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",M17)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Allowed for PCC sum stats to handle a 0-NA only vector. Added data
</commit_message>
<xml_diff>
--- a/Literature/Literature.xlsx
+++ b/Literature/Literature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hso20\OneDrive\Plocha\IES\Diploma-Thesis\Literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA4E1AE-578C-4257-BE62-395B5056A356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB6BE4C-1AFB-469B-9B68-46F84C7A2576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -499,7 +499,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9355" uniqueCount="5160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9359" uniqueCount="5159">
   <si>
     <t>Number</t>
   </si>
@@ -15640,9 +15640,6 @@
   </si>
   <si>
     <t>Too granular focus of dep var</t>
-  </si>
-  <si>
-    <t>Must use</t>
   </si>
   <si>
     <t>https://www.tandfonline.com/doi/pdf/10.1080/00036846.2015.1085642?download=true</t>
@@ -16894,9 +16891,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Y575"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N139" sqref="N139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16959,20 +16956,20 @@
         <v>962</v>
       </c>
       <c r="N1" s="24" t="s">
-        <v>5147</v>
+        <v>5146</v>
       </c>
       <c r="O1" s="25" t="s">
-        <v>5145</v>
+        <v>5144</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>5153</v>
+        <v>5152</v>
       </c>
       <c r="Q1" s="28" t="s">
         <v>5044</v>
       </c>
       <c r="R1" s="29">
         <f>COUNTIFS($M:$M, "YES", $F:$F, "&lt;&gt;") + Twins!S1</f>
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="T1" s="28" t="s">
         <v>5045</v>
@@ -17140,11 +17137,11 @@
         <v>574</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>5151</v>
+        <v>5150</v>
       </c>
       <c r="U4">
         <f>COUNTIFS($M:$M, "YES", $L:$L, "&lt;&gt;PRIMARY STUDY", $P:$P, "&lt;&gt;Twins")</f>
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -17201,11 +17198,11 @@
         <v>574</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>5148</v>
+        <v>5147</v>
       </c>
       <c r="U5" s="38">
         <f>COUNTIFS($N:$N, "YES", $F:$F, "&lt;&gt;")</f>
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
@@ -17504,10 +17501,10 @@
         <v>1</v>
       </c>
       <c r="P11" t="s">
-        <v>5152</v>
+        <v>5151</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>5146</v>
+        <v>5145</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
@@ -17560,7 +17557,7 @@
         <v>1</v>
       </c>
       <c r="R12" t="s">
-        <v>5149</v>
+        <v>5148</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
@@ -17613,7 +17610,7 @@
         <v>2</v>
       </c>
       <c r="R13" t="s">
-        <v>5150</v>
+        <v>5149</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
@@ -18866,7 +18863,7 @@
         <v>1</v>
       </c>
       <c r="P38" t="s">
-        <v>5152</v>
+        <v>5151</v>
       </c>
       <c r="R38" t="s">
         <v>904</v>
@@ -19819,7 +19816,7 @@
         <v>2</v>
       </c>
       <c r="P57" t="s">
-        <v>5155</v>
+        <v>5154</v>
       </c>
       <c r="R57" t="s">
         <v>904</v>
@@ -21472,7 +21469,7 @@
         <v>1</v>
       </c>
       <c r="P90" t="s">
-        <v>5156</v>
+        <v>5155</v>
       </c>
       <c r="R90" t="s">
         <v>904</v>
@@ -21483,7 +21480,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>5157</v>
+        <v>5156</v>
       </c>
       <c r="C91" t="s">
         <v>4019</v>
@@ -22475,7 +22472,7 @@
         <v>1</v>
       </c>
       <c r="P110" t="s">
-        <v>5158</v>
+        <v>5157</v>
       </c>
       <c r="R110" t="s">
         <v>904</v>
@@ -22928,7 +22925,7 @@
         <v>4</v>
       </c>
       <c r="P119" t="s">
-        <v>5159</v>
+        <v>5158</v>
       </c>
       <c r="R119" t="s">
         <v>904</v>
@@ -23719,10 +23716,13 @@
         <v>1716</v>
       </c>
       <c r="L135" t="s">
-        <v>963</v>
+        <v>974</v>
       </c>
       <c r="M135" t="s">
-        <v>963</v>
+        <v>966</v>
+      </c>
+      <c r="N135" t="s">
+        <v>966</v>
       </c>
       <c r="O135" s="7">
         <v>3</v>
@@ -23771,6 +23771,9 @@
       <c r="M136" t="s">
         <v>966</v>
       </c>
+      <c r="N136" t="s">
+        <v>966</v>
+      </c>
       <c r="O136" s="7">
         <v>2</v>
       </c>
@@ -23816,10 +23819,13 @@
         <v>1728</v>
       </c>
       <c r="L137" t="s">
-        <v>963</v>
+        <v>974</v>
       </c>
       <c r="M137" t="s">
-        <v>963</v>
+        <v>966</v>
+      </c>
+      <c r="N137" t="s">
+        <v>966</v>
       </c>
       <c r="O137" s="7">
         <v>1</v>
@@ -23868,6 +23874,9 @@
       <c r="M138" t="s">
         <v>966</v>
       </c>
+      <c r="N138" t="s">
+        <v>966</v>
+      </c>
       <c r="O138" s="7" t="s">
         <v>5035</v>
       </c>
@@ -23915,11 +23924,11 @@
       <c r="M139" t="s">
         <v>963</v>
       </c>
+      <c r="N139" t="s">
+        <v>963</v>
+      </c>
       <c r="O139" s="7">
-        <v>1</v>
-      </c>
-      <c r="P139" t="s">
-        <v>5047</v>
+        <v>2</v>
       </c>
       <c r="R139" t="s">
         <v>904</v>
@@ -24004,7 +24013,7 @@
         <v>2027</v>
       </c>
       <c r="K141" t="s">
-        <v>5048</v>
+        <v>5047</v>
       </c>
       <c r="L141" t="s">
         <v>963</v>
@@ -24248,7 +24257,7 @@
         <v>1</v>
       </c>
       <c r="P146" t="s">
-        <v>5049</v>
+        <v>5048</v>
       </c>
       <c r="R146" t="s">
         <v>904</v>
@@ -24483,7 +24492,7 @@
         <v>3</v>
       </c>
       <c r="P151" t="s">
-        <v>5050</v>
+        <v>5049</v>
       </c>
       <c r="R151" t="s">
         <v>904</v>
@@ -24956,7 +24965,7 @@
         <v>2</v>
       </c>
       <c r="P161" t="s">
-        <v>5051</v>
+        <v>5050</v>
       </c>
       <c r="R161" t="s">
         <v>904</v>
@@ -25053,7 +25062,7 @@
         <v>2</v>
       </c>
       <c r="P163" t="s">
-        <v>5052</v>
+        <v>5051</v>
       </c>
       <c r="R163" t="s">
         <v>904</v>
@@ -25723,7 +25732,7 @@
         <v>5035</v>
       </c>
       <c r="P177" t="s">
-        <v>5053</v>
+        <v>5052</v>
       </c>
       <c r="R177" t="s">
         <v>904</v>
@@ -26196,7 +26205,7 @@
         <v>1</v>
       </c>
       <c r="P187" t="s">
-        <v>5054</v>
+        <v>5053</v>
       </c>
       <c r="R187" t="s">
         <v>904</v>
@@ -26293,7 +26302,7 @@
         <v>1</v>
       </c>
       <c r="P189" t="s">
-        <v>5076</v>
+        <v>5075</v>
       </c>
       <c r="R189" t="s">
         <v>904</v>
@@ -26343,7 +26352,7 @@
         <v>5035</v>
       </c>
       <c r="P190" t="s">
-        <v>5077</v>
+        <v>5076</v>
       </c>
       <c r="R190" t="s">
         <v>904</v>
@@ -28543,7 +28552,7 @@
         <v>239</v>
       </c>
       <c r="B240" t="s">
-        <v>5078</v>
+        <v>5077</v>
       </c>
       <c r="C240" t="s">
         <v>4792</v>
@@ -43379,7 +43388,7 @@
   <conditionalFormatting sqref="Q1:Q10 Q16:Q1048576 R11:R15">
     <cfRule type="duplicateValues" dxfId="21" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P136 P139 P146 P151 P161 P163 P177 P187 P189:P190 O2:O601">
+  <conditionalFormatting sqref="P136 P146 P151 P161 P163 P177 P187 P189:P190 O2:O601">
     <cfRule type="containsBlanks" dxfId="20" priority="22">
       <formula>LEN(TRIM(O2))=0</formula>
     </cfRule>
@@ -43465,13 +43474,13 @@
         <v>962</v>
       </c>
       <c r="O1" s="24" t="s">
-        <v>5147</v>
+        <v>5146</v>
       </c>
       <c r="P1" s="25" t="s">
         <v>5032</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>5153</v>
+        <v>5152</v>
       </c>
       <c r="R1" s="28" t="s">
         <v>5044</v>
@@ -43497,19 +43506,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5060</v>
+        <v>5059</v>
       </c>
       <c r="C2" t="s">
-        <v>5059</v>
+        <v>5058</v>
       </c>
       <c r="D2">
         <v>1998</v>
       </c>
       <c r="E2" t="s">
-        <v>5067</v>
+        <v>5066</v>
       </c>
       <c r="F2" t="s">
-        <v>5058</v>
+        <v>5057</v>
       </c>
       <c r="G2" t="s">
         <v>5036</v>
@@ -43518,16 +43527,16 @@
         <v>908</v>
       </c>
       <c r="I2" t="s">
-        <v>5062</v>
+        <v>5061</v>
       </c>
       <c r="J2" t="s">
-        <v>5061</v>
+        <v>5060</v>
       </c>
       <c r="K2" t="s">
-        <v>5061</v>
+        <v>5060</v>
       </c>
       <c r="L2" t="s">
-        <v>5060</v>
+        <v>5059</v>
       </c>
       <c r="M2" t="s">
         <v>963</v>
@@ -43545,7 +43554,7 @@
         <v>904</v>
       </c>
       <c r="X2" t="s">
-        <v>5055</v>
+        <v>5054</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
@@ -43553,19 +43562,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5069</v>
+        <v>5068</v>
       </c>
       <c r="C3" t="s">
-        <v>5068</v>
+        <v>5067</v>
       </c>
       <c r="D3">
         <v>1994</v>
       </c>
       <c r="E3" t="s">
-        <v>5066</v>
+        <v>5065</v>
       </c>
       <c r="F3" t="s">
-        <v>5063</v>
+        <v>5062</v>
       </c>
       <c r="G3" t="s">
         <v>5036</v>
@@ -43574,16 +43583,16 @@
         <v>1812</v>
       </c>
       <c r="I3" t="s">
+        <v>5063</v>
+      </c>
+      <c r="J3" t="s">
         <v>5064</v>
       </c>
-      <c r="J3" t="s">
-        <v>5065</v>
-      </c>
       <c r="K3" t="s">
-        <v>5065</v>
+        <v>5064</v>
       </c>
       <c r="L3" t="s">
-        <v>5069</v>
+        <v>5068</v>
       </c>
       <c r="M3" t="s">
         <v>963</v>
@@ -43598,7 +43607,7 @@
         <v>1</v>
       </c>
       <c r="X3" t="s">
-        <v>5056</v>
+        <v>5055</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
@@ -43615,10 +43624,10 @@
         <v>1999</v>
       </c>
       <c r="E4" t="s">
-        <v>5074</v>
+        <v>5073</v>
       </c>
       <c r="F4" t="s">
-        <v>5070</v>
+        <v>5069</v>
       </c>
       <c r="G4" t="s">
         <v>5036</v>
@@ -43627,13 +43636,13 @@
         <v>188</v>
       </c>
       <c r="I4" t="s">
+        <v>5070</v>
+      </c>
+      <c r="J4" t="s">
+        <v>5072</v>
+      </c>
+      <c r="K4" t="s">
         <v>5071</v>
-      </c>
-      <c r="J4" t="s">
-        <v>5073</v>
-      </c>
-      <c r="K4" t="s">
-        <v>5072</v>
       </c>
       <c r="L4" t="s">
         <v>727</v>
@@ -43651,10 +43660,10 @@
         <v>1</v>
       </c>
       <c r="Q4" t="s">
-        <v>5075</v>
+        <v>5074</v>
       </c>
       <c r="X4" t="s">
-        <v>5057</v>
+        <v>5056</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
@@ -43662,19 +43671,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5079</v>
+        <v>5078</v>
       </c>
       <c r="C5" t="s">
-        <v>5087</v>
+        <v>5086</v>
       </c>
       <c r="D5">
         <v>2003</v>
       </c>
       <c r="E5" t="s">
+        <v>5090</v>
+      </c>
+      <c r="F5" t="s">
         <v>5091</v>
-      </c>
-      <c r="F5" t="s">
-        <v>5092</v>
       </c>
       <c r="G5" t="s">
         <v>5036</v>
@@ -43683,16 +43692,16 @@
         <v>158</v>
       </c>
       <c r="I5" t="s">
+        <v>5084</v>
+      </c>
+      <c r="J5" t="s">
         <v>5085</v>
       </c>
-      <c r="J5" t="s">
-        <v>5086</v>
-      </c>
       <c r="K5" t="s">
-        <v>5086</v>
+        <v>5085</v>
       </c>
       <c r="L5" t="s">
-        <v>5079</v>
+        <v>5078</v>
       </c>
       <c r="M5" t="s">
         <v>963</v>
@@ -43712,19 +43721,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>5080</v>
+        <v>5079</v>
       </c>
       <c r="C6" t="s">
-        <v>5088</v>
+        <v>5087</v>
       </c>
       <c r="D6">
         <v>2012</v>
       </c>
       <c r="E6" t="s">
-        <v>5094</v>
+        <v>5093</v>
       </c>
       <c r="F6" t="s">
-        <v>5093</v>
+        <v>5092</v>
       </c>
       <c r="G6" t="s">
         <v>5036</v>
@@ -43733,16 +43742,16 @@
         <v>176</v>
       </c>
       <c r="I6" t="s">
+        <v>5094</v>
+      </c>
+      <c r="J6" t="s">
         <v>5095</v>
       </c>
-      <c r="J6" t="s">
-        <v>5096</v>
-      </c>
       <c r="K6" t="s">
-        <v>5096</v>
+        <v>5095</v>
       </c>
       <c r="L6" t="s">
-        <v>5080</v>
+        <v>5079</v>
       </c>
       <c r="M6" t="s">
         <v>963</v>
@@ -43757,14 +43766,14 @@
         <v>1</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>5151</v>
+        <v>5150</v>
       </c>
       <c r="S6">
         <f>COUNTIFS($N:$N, "YES", $M:$M, "&lt;&gt;PRIMARY STUDY")</f>
         <v>16</v>
       </c>
       <c r="X6" t="s">
-        <v>5084</v>
+        <v>5083</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
@@ -43772,7 +43781,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>5081</v>
+        <v>5080</v>
       </c>
       <c r="C7" t="s">
         <v>4134</v>
@@ -43781,10 +43790,10 @@
         <v>1995</v>
       </c>
       <c r="E7" t="s">
+        <v>5096</v>
+      </c>
+      <c r="F7" t="s">
         <v>5097</v>
-      </c>
-      <c r="F7" t="s">
-        <v>5098</v>
       </c>
       <c r="G7" t="s">
         <v>5036</v>
@@ -43793,16 +43802,16 @@
         <v>372</v>
       </c>
       <c r="I7" t="s">
+        <v>5098</v>
+      </c>
+      <c r="J7" t="s">
         <v>5099</v>
       </c>
-      <c r="J7" t="s">
-        <v>5100</v>
-      </c>
       <c r="K7" t="s">
-        <v>5100</v>
+        <v>5099</v>
       </c>
       <c r="L7" t="s">
-        <v>5081</v>
+        <v>5080</v>
       </c>
       <c r="M7" t="s">
         <v>963</v>
@@ -43817,7 +43826,7 @@
         <v>1</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>5148</v>
+        <v>5147</v>
       </c>
       <c r="S7">
         <f>COUNTIFS($O:$O, "YES", $F:$F, "&lt;&gt;")</f>
@@ -43829,19 +43838,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>5101</v>
+        <v>5100</v>
       </c>
       <c r="C8" t="s">
-        <v>5089</v>
+        <v>5088</v>
       </c>
       <c r="D8">
         <v>1976</v>
       </c>
       <c r="E8" t="s">
+        <v>5101</v>
+      </c>
+      <c r="F8" t="s">
         <v>5102</v>
-      </c>
-      <c r="F8" t="s">
-        <v>5103</v>
       </c>
       <c r="G8" t="s">
         <v>5036</v>
@@ -43850,16 +43859,16 @@
         <v>382</v>
       </c>
       <c r="I8" t="s">
+        <v>5103</v>
+      </c>
+      <c r="J8" t="s">
         <v>5104</v>
       </c>
-      <c r="J8" t="s">
-        <v>5105</v>
-      </c>
       <c r="K8" t="s">
-        <v>5105</v>
+        <v>5104</v>
       </c>
       <c r="L8" t="s">
-        <v>5101</v>
+        <v>5100</v>
       </c>
       <c r="M8" t="s">
         <v>963</v>
@@ -43879,7 +43888,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>5082</v>
+        <v>5081</v>
       </c>
       <c r="C9" t="s">
         <v>4081</v>
@@ -43888,10 +43897,10 @@
         <v>1994</v>
       </c>
       <c r="E9" t="s">
-        <v>5109</v>
+        <v>5108</v>
       </c>
       <c r="F9" t="s">
-        <v>5108</v>
+        <v>5107</v>
       </c>
       <c r="G9" t="s">
         <v>5036</v>
@@ -43900,13 +43909,13 @@
         <v>616</v>
       </c>
       <c r="I9" t="s">
+        <v>5105</v>
+      </c>
+      <c r="J9" t="s">
         <v>5106</v>
       </c>
-      <c r="J9" t="s">
-        <v>5107</v>
-      </c>
       <c r="L9" t="s">
-        <v>5082</v>
+        <v>5081</v>
       </c>
       <c r="M9" t="s">
         <v>963</v>
@@ -43926,19 +43935,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>5083</v>
+        <v>5082</v>
       </c>
       <c r="C10" t="s">
-        <v>5090</v>
+        <v>5089</v>
       </c>
       <c r="D10">
         <v>1999</v>
       </c>
       <c r="E10" t="s">
+        <v>5111</v>
+      </c>
+      <c r="F10" t="s">
         <v>5112</v>
-      </c>
-      <c r="F10" t="s">
-        <v>5113</v>
       </c>
       <c r="G10" t="s">
         <v>5036</v>
@@ -43947,16 +43956,16 @@
         <v>196</v>
       </c>
       <c r="I10" t="s">
+        <v>5109</v>
+      </c>
+      <c r="J10" t="s">
         <v>5110</v>
       </c>
-      <c r="J10" t="s">
-        <v>5111</v>
-      </c>
       <c r="K10" t="s">
-        <v>5111</v>
+        <v>5110</v>
       </c>
       <c r="L10" t="s">
-        <v>5083</v>
+        <v>5082</v>
       </c>
       <c r="M10" t="s">
         <v>963</v>
@@ -43976,19 +43985,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>5116</v>
+      </c>
+      <c r="C11" t="s">
         <v>5117</v>
-      </c>
-      <c r="C11" t="s">
-        <v>5118</v>
       </c>
       <c r="D11">
         <v>1996</v>
       </c>
       <c r="E11" t="s">
-        <v>5119</v>
+        <v>5118</v>
       </c>
       <c r="F11" t="s">
-        <v>5114</v>
+        <v>5113</v>
       </c>
       <c r="G11" t="s">
         <v>5036</v>
@@ -43997,13 +44006,13 @@
         <v>218</v>
       </c>
       <c r="I11" t="s">
+        <v>5114</v>
+      </c>
+      <c r="J11" t="s">
         <v>5115</v>
       </c>
-      <c r="J11" t="s">
+      <c r="L11" t="s">
         <v>5116</v>
-      </c>
-      <c r="L11" t="s">
-        <v>5117</v>
       </c>
       <c r="M11" t="s">
         <v>963</v>
@@ -44023,19 +44032,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>5125</v>
+        <v>5124</v>
       </c>
       <c r="C12" t="s">
-        <v>5124</v>
+        <v>5123</v>
       </c>
       <c r="D12">
         <v>2002</v>
       </c>
       <c r="E12" t="s">
-        <v>5123</v>
+        <v>5122</v>
       </c>
       <c r="F12" t="s">
-        <v>5120</v>
+        <v>5119</v>
       </c>
       <c r="G12" t="s">
         <v>5036</v>
@@ -44044,16 +44053,16 @@
         <v>320</v>
       </c>
       <c r="I12" t="s">
+        <v>5120</v>
+      </c>
+      <c r="J12" t="s">
         <v>5121</v>
       </c>
-      <c r="J12" t="s">
-        <v>5122</v>
-      </c>
       <c r="K12" t="s">
-        <v>5122</v>
+        <v>5121</v>
       </c>
       <c r="L12" t="s">
-        <v>5125</v>
+        <v>5124</v>
       </c>
       <c r="M12" t="s">
         <v>963</v>
@@ -44073,19 +44082,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>5129</v>
+      </c>
+      <c r="C13" t="s">
         <v>5130</v>
-      </c>
-      <c r="C13" t="s">
-        <v>5131</v>
       </c>
       <c r="D13">
         <v>2018</v>
       </c>
       <c r="E13" t="s">
-        <v>5132</v>
+        <v>5131</v>
       </c>
       <c r="F13" t="s">
-        <v>5126</v>
+        <v>5125</v>
       </c>
       <c r="G13" t="s">
         <v>5036</v>
@@ -44094,16 +44103,16 @@
         <v>181</v>
       </c>
       <c r="I13" t="s">
+        <v>5126</v>
+      </c>
+      <c r="J13" t="s">
         <v>5127</v>
       </c>
-      <c r="J13" t="s">
-        <v>5128</v>
-      </c>
       <c r="K13" t="s">
-        <v>5128</v>
+        <v>5127</v>
       </c>
       <c r="L13" t="s">
-        <v>5130</v>
+        <v>5129</v>
       </c>
       <c r="M13" t="s">
         <v>963</v>
@@ -44115,7 +44124,7 @@
         <v>966</v>
       </c>
       <c r="P13" t="s">
-        <v>5129</v>
+        <v>5128</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
@@ -44123,19 +44132,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>5135</v>
+      </c>
+      <c r="C14" t="s">
         <v>5136</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5137</v>
       </c>
       <c r="D14">
         <v>2012</v>
       </c>
       <c r="E14" t="s">
-        <v>5138</v>
+        <v>5137</v>
       </c>
       <c r="F14" t="s">
-        <v>5133</v>
+        <v>5132</v>
       </c>
       <c r="G14" t="s">
         <v>5036</v>
@@ -44144,16 +44153,16 @@
         <v>18</v>
       </c>
       <c r="I14" t="s">
+        <v>5133</v>
+      </c>
+      <c r="J14" t="s">
         <v>5134</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
+        <v>5134</v>
+      </c>
+      <c r="L14" t="s">
         <v>5135</v>
-      </c>
-      <c r="K14" t="s">
-        <v>5135</v>
-      </c>
-      <c r="L14" t="s">
-        <v>5136</v>
       </c>
       <c r="M14" t="s">
         <v>963</v>
@@ -44173,19 +44182,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>5143</v>
+        <v>5142</v>
       </c>
       <c r="C15" t="s">
-        <v>5140</v>
+        <v>5139</v>
       </c>
       <c r="D15">
         <v>2020</v>
       </c>
       <c r="E15" t="s">
-        <v>5144</v>
+        <v>5143</v>
       </c>
       <c r="F15" t="s">
-        <v>5141</v>
+        <v>5140</v>
       </c>
       <c r="G15" t="s">
         <v>5036</v>
@@ -44194,16 +44203,16 @@
         <v>11</v>
       </c>
       <c r="I15" t="s">
+        <v>5141</v>
+      </c>
+      <c r="J15" t="s">
+        <v>5138</v>
+      </c>
+      <c r="K15" t="s">
+        <v>5138</v>
+      </c>
+      <c r="L15" t="s">
         <v>5142</v>
-      </c>
-      <c r="J15" t="s">
-        <v>5139</v>
-      </c>
-      <c r="K15" t="s">
-        <v>5139</v>
-      </c>
-      <c r="L15" t="s">
-        <v>5143</v>
       </c>
       <c r="M15" t="s">
         <v>963</v>
@@ -44268,7 +44277,7 @@
         <v>1</v>
       </c>
       <c r="Q16" t="s">
-        <v>5154</v>
+        <v>5153</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -44321,7 +44330,7 @@
         <v>1</v>
       </c>
       <c r="Q17" t="s">
-        <v>5154</v>
+        <v>5153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Bayesian Model Averaging, along with plots, customization
</commit_message>
<xml_diff>
--- a/Literature/Literature.xlsx
+++ b/Literature/Literature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hso20\OneDrive\Plocha\IES\Diploma-Thesis\Literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB6BE4C-1AFB-469B-9B68-46F84C7A2576}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C55E8F-F30F-4BB0-9012-C319A6729A3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -499,7 +499,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9359" uniqueCount="5159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9364" uniqueCount="5159">
   <si>
     <t>Number</t>
   </si>
@@ -16891,9 +16891,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Y575"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N139" sqref="N139"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A136" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N142" sqref="N142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17202,7 +17202,7 @@
       </c>
       <c r="U5" s="38">
         <f>COUNTIFS($N:$N, "YES", $F:$F, "&lt;&gt;")</f>
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
@@ -23974,8 +23974,11 @@
       <c r="M140" t="s">
         <v>963</v>
       </c>
+      <c r="N140" t="s">
+        <v>963</v>
+      </c>
       <c r="O140" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R140" t="s">
         <v>904</v>
@@ -24021,6 +24024,9 @@
       <c r="M141" t="s">
         <v>963</v>
       </c>
+      <c r="N141" t="s">
+        <v>963</v>
+      </c>
       <c r="O141" s="7">
         <v>2</v>
       </c>
@@ -24068,6 +24074,9 @@
       <c r="M142" t="s">
         <v>966</v>
       </c>
+      <c r="N142" t="s">
+        <v>966</v>
+      </c>
       <c r="O142" s="7" t="s">
         <v>5035</v>
       </c>
@@ -24115,6 +24124,9 @@
       <c r="M143" t="s">
         <v>966</v>
       </c>
+      <c r="N143" t="s">
+        <v>966</v>
+      </c>
       <c r="O143" s="7" t="s">
         <v>5035</v>
       </c>
@@ -24160,6 +24172,9 @@
         <v>969</v>
       </c>
       <c r="M144" t="s">
+        <v>966</v>
+      </c>
+      <c r="N144" t="s">
         <v>966</v>
       </c>
       <c r="O144" s="7" t="s">
@@ -43422,7 +43437,7 @@
   <dimension ref="A1:Z17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Master dataset is finished with 1115 observations across 74 studies
</commit_message>
<xml_diff>
--- a/Literature/Literature.xlsx
+++ b/Literature/Literature.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-23145" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
   </bookViews>
   <sheets>
     <sheet name="Query literature" sheetId="5" r:id="rId1"/>
@@ -498,7 +498,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9404" uniqueCount="5161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9432" uniqueCount="5160">
   <si>
     <t>Number</t>
   </si>
@@ -15639,9 +15639,6 @@
   </si>
   <si>
     <t>Can be disregarded, possibly</t>
-  </si>
-  <si>
-    <t>Deals with twins, read thoroughly to confirm categorization</t>
   </si>
   <si>
     <t>A list of studies that were identified as relevant</t>
@@ -16362,7 +16359,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="31">
+  <dxfs count="43">
     <dxf>
       <fill>
         <patternFill>
@@ -16402,6 +16399,98 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC5C5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAACAC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAACAC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAACAC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAACAC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAACAC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBA8CDC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6161"/>
         </patternFill>
       </fill>
     </dxf>
@@ -16897,8 +16986,8 @@
   <dimension ref="A1:Y575"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A182" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N187" sqref="N187"/>
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16961,27 +17050,27 @@
         <v>962</v>
       </c>
       <c r="N1" s="24" t="s">
-        <v>5140</v>
+        <v>5139</v>
       </c>
       <c r="O1" s="25" t="s">
-        <v>5138</v>
+        <v>5137</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>5146</v>
+        <v>5145</v>
       </c>
       <c r="Q1" s="28" t="s">
         <v>5038</v>
       </c>
       <c r="R1" s="29">
         <f>COUNTIFS($M:$M, "YES", $F:$F, "&lt;&gt;") + Twins!S1</f>
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="T1" s="28" t="s">
         <v>5039</v>
       </c>
       <c r="U1" s="29">
         <f>COUNTIF($L$2:$L$575, "&lt;&gt; ") +Twins!V1</f>
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="V1" s="31"/>
       <c r="W1" s="31"/>
@@ -17142,11 +17231,11 @@
         <v>574</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>5144</v>
+        <v>5143</v>
       </c>
       <c r="U4">
         <f>COUNTIFS($M:$M, "YES", $L:$L, "&lt;&gt;PRIMARY STUDY", $P:$P, "&lt;&gt;Twins")</f>
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -17203,11 +17292,11 @@
         <v>574</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>5141</v>
+        <v>5140</v>
       </c>
       <c r="U5" s="38">
         <f>COUNTIFS($N:$N, "YES", $F:$F, "&lt;&gt;")</f>
-        <v>68</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
@@ -17506,10 +17595,10 @@
         <v>1</v>
       </c>
       <c r="P11" t="s">
-        <v>5145</v>
+        <v>5144</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>5139</v>
+        <v>5138</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
@@ -17562,7 +17651,7 @@
         <v>1</v>
       </c>
       <c r="R12" t="s">
-        <v>5142</v>
+        <v>5141</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
@@ -17615,7 +17704,7 @@
         <v>2</v>
       </c>
       <c r="R13" t="s">
-        <v>5143</v>
+        <v>5142</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
@@ -18868,7 +18957,7 @@
         <v>1</v>
       </c>
       <c r="P38" t="s">
-        <v>5145</v>
+        <v>5144</v>
       </c>
       <c r="R38" t="s">
         <v>904</v>
@@ -19021,7 +19110,7 @@
         <v>2</v>
       </c>
       <c r="P41" t="s">
-        <v>5156</v>
+        <v>5155</v>
       </c>
       <c r="R41" t="s">
         <v>904</v>
@@ -19824,7 +19913,7 @@
         <v>2</v>
       </c>
       <c r="P57" t="s">
-        <v>5148</v>
+        <v>5147</v>
       </c>
       <c r="R57" t="s">
         <v>904</v>
@@ -21477,7 +21566,7 @@
         <v>1</v>
       </c>
       <c r="P90" t="s">
-        <v>5149</v>
+        <v>5148</v>
       </c>
       <c r="R90" t="s">
         <v>904</v>
@@ -21488,7 +21577,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>5150</v>
+        <v>5149</v>
       </c>
       <c r="C91" t="s">
         <v>4015</v>
@@ -22480,7 +22569,7 @@
         <v>1</v>
       </c>
       <c r="P110" t="s">
-        <v>5151</v>
+        <v>5150</v>
       </c>
       <c r="R110" t="s">
         <v>904</v>
@@ -22933,7 +23022,7 @@
         <v>4</v>
       </c>
       <c r="P119" t="s">
-        <v>5152</v>
+        <v>5151</v>
       </c>
       <c r="R119" t="s">
         <v>904</v>
@@ -23333,7 +23422,7 @@
         <v>963</v>
       </c>
       <c r="N127" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
       <c r="O127" s="7">
         <v>1</v>
@@ -24227,7 +24316,7 @@
         <v>1765</v>
       </c>
       <c r="L145" t="s">
-        <v>5153</v>
+        <v>5152</v>
       </c>
       <c r="M145" t="s">
         <v>966</v>
@@ -24247,7 +24336,7 @@
         <v>145</v>
       </c>
       <c r="B146" t="s">
-        <v>5154</v>
+        <v>5153</v>
       </c>
       <c r="C146" t="s">
         <v>4080</v>
@@ -24259,7 +24348,7 @@
         <v>1766</v>
       </c>
       <c r="F146" t="s">
-        <v>5155</v>
+        <v>5154</v>
       </c>
       <c r="G146" t="s">
         <v>1768</v>
@@ -24450,7 +24539,7 @@
         <v>149</v>
       </c>
       <c r="B150" t="s">
-        <v>5157</v>
+        <v>5156</v>
       </c>
       <c r="C150" t="s">
         <v>4085</v>
@@ -24459,13 +24548,13 @@
         <v>2012</v>
       </c>
       <c r="E150" t="s">
+        <v>5157</v>
+      </c>
+      <c r="F150" t="s">
         <v>5158</v>
       </c>
-      <c r="F150" t="s">
+      <c r="G150" t="s">
         <v>5159</v>
-      </c>
-      <c r="G150" t="s">
-        <v>5160</v>
       </c>
       <c r="H150">
         <v>0</v>
@@ -26347,11 +26436,14 @@
       <c r="M187" t="s">
         <v>963</v>
       </c>
+      <c r="N187" t="s">
+        <v>966</v>
+      </c>
       <c r="O187" s="7">
         <v>1</v>
       </c>
       <c r="P187" t="s">
-        <v>5047</v>
+        <v>5144</v>
       </c>
       <c r="R187" t="s">
         <v>904</v>
@@ -26397,6 +26489,9 @@
       <c r="M188" t="s">
         <v>966</v>
       </c>
+      <c r="N188" t="s">
+        <v>966</v>
+      </c>
       <c r="O188" s="7" t="s">
         <v>5029</v>
       </c>
@@ -26444,11 +26539,14 @@
       <c r="M189" t="s">
         <v>969</v>
       </c>
+      <c r="N189" t="s">
+        <v>966</v>
+      </c>
       <c r="O189" s="7">
         <v>1</v>
       </c>
       <c r="P189" t="s">
-        <v>5069</v>
+        <v>5068</v>
       </c>
       <c r="R189" t="s">
         <v>904</v>
@@ -26494,11 +26592,14 @@
       <c r="M190" t="s">
         <v>966</v>
       </c>
+      <c r="N190" t="s">
+        <v>966</v>
+      </c>
       <c r="O190" s="7" t="s">
         <v>5029</v>
       </c>
       <c r="P190" t="s">
-        <v>5070</v>
+        <v>5069</v>
       </c>
       <c r="R190" t="s">
         <v>904</v>
@@ -26544,6 +26645,9 @@
       <c r="M191" t="s">
         <v>963</v>
       </c>
+      <c r="N191" t="s">
+        <v>963</v>
+      </c>
       <c r="O191" s="7">
         <v>2</v>
       </c>
@@ -26591,6 +26695,9 @@
       <c r="M192" t="s">
         <v>963</v>
       </c>
+      <c r="N192" t="s">
+        <v>963</v>
+      </c>
       <c r="O192" s="7">
         <v>3</v>
       </c>
@@ -26638,6 +26745,9 @@
       <c r="M193" t="s">
         <v>966</v>
       </c>
+      <c r="N193" t="s">
+        <v>966</v>
+      </c>
       <c r="O193" s="7" t="s">
         <v>5029</v>
       </c>
@@ -26685,6 +26795,9 @@
       <c r="M194" t="s">
         <v>966</v>
       </c>
+      <c r="N194" t="s">
+        <v>966</v>
+      </c>
       <c r="O194" s="7">
         <v>2</v>
       </c>
@@ -26732,6 +26845,9 @@
       <c r="M195" t="s">
         <v>963</v>
       </c>
+      <c r="N195" t="s">
+        <v>963</v>
+      </c>
       <c r="O195" s="7">
         <v>3</v>
       </c>
@@ -26779,6 +26895,9 @@
       <c r="M196" t="s">
         <v>963</v>
       </c>
+      <c r="N196" t="s">
+        <v>963</v>
+      </c>
       <c r="O196" s="7">
         <v>3</v>
       </c>
@@ -26826,6 +26945,9 @@
       <c r="M197" t="s">
         <v>966</v>
       </c>
+      <c r="N197" t="s">
+        <v>966</v>
+      </c>
       <c r="O197" s="7" t="s">
         <v>5029</v>
       </c>
@@ -26873,6 +26995,9 @@
       <c r="M198" t="s">
         <v>966</v>
       </c>
+      <c r="N198" t="s">
+        <v>966</v>
+      </c>
       <c r="O198" s="7" t="s">
         <v>5029</v>
       </c>
@@ -26920,6 +27045,9 @@
       <c r="M199" t="s">
         <v>966</v>
       </c>
+      <c r="N199" t="s">
+        <v>966</v>
+      </c>
       <c r="O199" s="7" t="s">
         <v>5029</v>
       </c>
@@ -26967,6 +27095,9 @@
       <c r="M200" t="s">
         <v>963</v>
       </c>
+      <c r="N200" t="s">
+        <v>963</v>
+      </c>
       <c r="O200" s="7">
         <v>2</v>
       </c>
@@ -27014,6 +27145,9 @@
       <c r="M201" s="36" t="s">
         <v>966</v>
       </c>
+      <c r="N201" s="36" t="s">
+        <v>966</v>
+      </c>
       <c r="O201" s="37" t="s">
         <v>5029</v>
       </c>
@@ -28698,7 +28832,7 @@
         <v>239</v>
       </c>
       <c r="B240" t="s">
-        <v>5071</v>
+        <v>5070</v>
       </c>
       <c r="C240" t="s">
         <v>4786</v>
@@ -43497,57 +43631,57 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="R6">
-    <cfRule type="cellIs" dxfId="30" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="21" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="29" priority="23">
+    <cfRule type="containsBlanks" dxfId="41" priority="23">
       <formula>LEN(TRIM(R6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsBlanks" dxfId="28" priority="20">
+    <cfRule type="containsBlanks" dxfId="40" priority="20">
       <formula>LEN(TRIM(F1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8">
-    <cfRule type="cellIs" dxfId="27" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="17" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="18" operator="notEqual">
+    <cfRule type="cellIs" dxfId="38" priority="18" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:N601">
-    <cfRule type="containsText" dxfId="25" priority="11" operator="containsText" text="PRIMARY STUDY">
+    <cfRule type="containsText" dxfId="37" priority="11" operator="containsText" text="PRIMARY STUDY">
       <formula>NOT(ISERROR(SEARCH("PRIMARY STUDY",L2)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="24" priority="12" operator="notContains" text="YES">
+    <cfRule type="notContainsText" dxfId="36" priority="12" operator="notContains" text="YES">
       <formula>ISERROR(SEARCH("YES",L2))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="13" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="35" priority="13" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",L2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B38 B40:B1048576">
-    <cfRule type="duplicateValues" dxfId="22" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q10 Q16:Q1048576 R11:R15">
-    <cfRule type="duplicateValues" dxfId="21" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P136 P146 P151 P161 P163 P177 P187 P189:P190 O2:O601">
-    <cfRule type="containsBlanks" dxfId="20" priority="22">
+    <cfRule type="containsBlanks" dxfId="32" priority="22">
       <formula>LEN(TRIM(O2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1">
-    <cfRule type="duplicateValues" dxfId="19" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="P177 P187 P189:P190 O2:O601">
-    <cfRule type="cellIs" dxfId="18" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="30" priority="8" operator="between">
       <formula>1</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="9" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="29" priority="9" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",O2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -43565,10 +43699,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:Z17"/>
+  <dimension ref="A1:Z18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43620,27 +43754,27 @@
         <v>962</v>
       </c>
       <c r="O1" s="24" t="s">
-        <v>5140</v>
+        <v>5139</v>
       </c>
       <c r="P1" s="25" t="s">
         <v>5026</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>5146</v>
+        <v>5145</v>
       </c>
       <c r="R1" s="28" t="s">
         <v>5038</v>
       </c>
       <c r="S1" s="29">
         <f>COUNTIFS($N:$N, "YES", $F:$F, "&lt;&gt;")</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="U1" s="28" t="s">
         <v>5039</v>
       </c>
       <c r="V1" s="29">
         <f>COUNTIF($M$2:$M$573, "YES")</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="W1" s="31"/>
       <c r="X1" s="31"/>
@@ -43652,19 +43786,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5053</v>
+        <v>5052</v>
       </c>
       <c r="C2" t="s">
-        <v>5052</v>
+        <v>5051</v>
       </c>
       <c r="D2">
         <v>1998</v>
       </c>
       <c r="E2" t="s">
-        <v>5060</v>
+        <v>5059</v>
       </c>
       <c r="F2" t="s">
-        <v>5051</v>
+        <v>5050</v>
       </c>
       <c r="G2" t="s">
         <v>5030</v>
@@ -43673,16 +43807,16 @@
         <v>908</v>
       </c>
       <c r="I2" t="s">
-        <v>5055</v>
+        <v>5054</v>
       </c>
       <c r="J2" t="s">
-        <v>5054</v>
+        <v>5053</v>
       </c>
       <c r="K2" t="s">
-        <v>5054</v>
+        <v>5053</v>
       </c>
       <c r="L2" t="s">
-        <v>5053</v>
+        <v>5052</v>
       </c>
       <c r="M2" t="s">
         <v>963</v>
@@ -43700,7 +43834,7 @@
         <v>904</v>
       </c>
       <c r="X2" t="s">
-        <v>5048</v>
+        <v>5047</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
@@ -43708,19 +43842,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5062</v>
+        <v>5061</v>
       </c>
       <c r="C3" t="s">
-        <v>5061</v>
+        <v>5060</v>
       </c>
       <c r="D3">
         <v>1994</v>
       </c>
       <c r="E3" t="s">
-        <v>5059</v>
+        <v>5058</v>
       </c>
       <c r="F3" t="s">
-        <v>5056</v>
+        <v>5055</v>
       </c>
       <c r="G3" t="s">
         <v>5030</v>
@@ -43729,16 +43863,16 @@
         <v>1812</v>
       </c>
       <c r="I3" t="s">
+        <v>5056</v>
+      </c>
+      <c r="J3" t="s">
         <v>5057</v>
       </c>
-      <c r="J3" t="s">
-        <v>5058</v>
-      </c>
       <c r="K3" t="s">
-        <v>5058</v>
+        <v>5057</v>
       </c>
       <c r="L3" t="s">
-        <v>5062</v>
+        <v>5061</v>
       </c>
       <c r="M3" t="s">
         <v>963</v>
@@ -43753,7 +43887,7 @@
         <v>1</v>
       </c>
       <c r="X3" t="s">
-        <v>5049</v>
+        <v>5048</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
@@ -43770,10 +43904,10 @@
         <v>1999</v>
       </c>
       <c r="E4" t="s">
-        <v>5067</v>
+        <v>5066</v>
       </c>
       <c r="F4" t="s">
-        <v>5063</v>
+        <v>5062</v>
       </c>
       <c r="G4" t="s">
         <v>5030</v>
@@ -43782,13 +43916,13 @@
         <v>188</v>
       </c>
       <c r="I4" t="s">
+        <v>5063</v>
+      </c>
+      <c r="J4" t="s">
+        <v>5065</v>
+      </c>
+      <c r="K4" t="s">
         <v>5064</v>
-      </c>
-      <c r="J4" t="s">
-        <v>5066</v>
-      </c>
-      <c r="K4" t="s">
-        <v>5065</v>
       </c>
       <c r="L4" t="s">
         <v>727</v>
@@ -43806,10 +43940,10 @@
         <v>1</v>
       </c>
       <c r="Q4" t="s">
-        <v>5068</v>
+        <v>5067</v>
       </c>
       <c r="X4" t="s">
-        <v>5050</v>
+        <v>5049</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
@@ -43817,19 +43951,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5072</v>
+        <v>5071</v>
       </c>
       <c r="C5" t="s">
-        <v>5080</v>
+        <v>5079</v>
       </c>
       <c r="D5">
         <v>2003</v>
       </c>
       <c r="E5" t="s">
+        <v>5083</v>
+      </c>
+      <c r="F5" t="s">
         <v>5084</v>
-      </c>
-      <c r="F5" t="s">
-        <v>5085</v>
       </c>
       <c r="G5" t="s">
         <v>5030</v>
@@ -43838,16 +43972,16 @@
         <v>158</v>
       </c>
       <c r="I5" t="s">
+        <v>5077</v>
+      </c>
+      <c r="J5" t="s">
         <v>5078</v>
       </c>
-      <c r="J5" t="s">
-        <v>5079</v>
-      </c>
       <c r="K5" t="s">
-        <v>5079</v>
+        <v>5078</v>
       </c>
       <c r="L5" t="s">
-        <v>5072</v>
+        <v>5071</v>
       </c>
       <c r="M5" t="s">
         <v>963</v>
@@ -43867,19 +44001,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>5073</v>
+        <v>5072</v>
       </c>
       <c r="C6" t="s">
-        <v>5081</v>
+        <v>5080</v>
       </c>
       <c r="D6">
         <v>2012</v>
       </c>
       <c r="E6" t="s">
-        <v>5087</v>
+        <v>5086</v>
       </c>
       <c r="F6" t="s">
-        <v>5086</v>
+        <v>5085</v>
       </c>
       <c r="G6" t="s">
         <v>5030</v>
@@ -43888,16 +44022,16 @@
         <v>176</v>
       </c>
       <c r="I6" t="s">
+        <v>5087</v>
+      </c>
+      <c r="J6" t="s">
         <v>5088</v>
       </c>
-      <c r="J6" t="s">
-        <v>5089</v>
-      </c>
       <c r="K6" t="s">
-        <v>5089</v>
+        <v>5088</v>
       </c>
       <c r="L6" t="s">
-        <v>5073</v>
+        <v>5072</v>
       </c>
       <c r="M6" t="s">
         <v>963</v>
@@ -43912,14 +44046,14 @@
         <v>1</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>5144</v>
+        <v>5143</v>
       </c>
       <c r="S6">
         <f>COUNTIFS($N:$N, "YES", $M:$M, "&lt;&gt;PRIMARY STUDY")</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="X6" t="s">
-        <v>5077</v>
+        <v>5076</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
@@ -43927,7 +44061,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>5074</v>
+        <v>5073</v>
       </c>
       <c r="C7" t="s">
         <v>4128</v>
@@ -43936,10 +44070,10 @@
         <v>1995</v>
       </c>
       <c r="E7" t="s">
+        <v>5089</v>
+      </c>
+      <c r="F7" t="s">
         <v>5090</v>
-      </c>
-      <c r="F7" t="s">
-        <v>5091</v>
       </c>
       <c r="G7" t="s">
         <v>5030</v>
@@ -43948,16 +44082,16 @@
         <v>372</v>
       </c>
       <c r="I7" t="s">
+        <v>5091</v>
+      </c>
+      <c r="J7" t="s">
         <v>5092</v>
       </c>
-      <c r="J7" t="s">
-        <v>5093</v>
-      </c>
       <c r="K7" t="s">
-        <v>5093</v>
+        <v>5092</v>
       </c>
       <c r="L7" t="s">
-        <v>5074</v>
+        <v>5073</v>
       </c>
       <c r="M7" t="s">
         <v>963</v>
@@ -43972,7 +44106,7 @@
         <v>1</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>5141</v>
+        <v>5140</v>
       </c>
       <c r="S7">
         <f>COUNTIFS($O:$O, "YES", $F:$F, "&lt;&gt;")</f>
@@ -43984,19 +44118,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>5094</v>
+        <v>5093</v>
       </c>
       <c r="C8" t="s">
-        <v>5082</v>
+        <v>5081</v>
       </c>
       <c r="D8">
         <v>1976</v>
       </c>
       <c r="E8" t="s">
+        <v>5094</v>
+      </c>
+      <c r="F8" t="s">
         <v>5095</v>
-      </c>
-      <c r="F8" t="s">
-        <v>5096</v>
       </c>
       <c r="G8" t="s">
         <v>5030</v>
@@ -44005,16 +44139,16 @@
         <v>382</v>
       </c>
       <c r="I8" t="s">
+        <v>5096</v>
+      </c>
+      <c r="J8" t="s">
         <v>5097</v>
       </c>
-      <c r="J8" t="s">
-        <v>5098</v>
-      </c>
       <c r="K8" t="s">
-        <v>5098</v>
+        <v>5097</v>
       </c>
       <c r="L8" t="s">
-        <v>5094</v>
+        <v>5093</v>
       </c>
       <c r="M8" t="s">
         <v>963</v>
@@ -44034,7 +44168,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>5075</v>
+        <v>5074</v>
       </c>
       <c r="C9" t="s">
         <v>4077</v>
@@ -44043,10 +44177,10 @@
         <v>1994</v>
       </c>
       <c r="E9" t="s">
-        <v>5102</v>
+        <v>5101</v>
       </c>
       <c r="F9" t="s">
-        <v>5101</v>
+        <v>5100</v>
       </c>
       <c r="G9" t="s">
         <v>5030</v>
@@ -44055,13 +44189,13 @@
         <v>616</v>
       </c>
       <c r="I9" t="s">
+        <v>5098</v>
+      </c>
+      <c r="J9" t="s">
         <v>5099</v>
       </c>
-      <c r="J9" t="s">
-        <v>5100</v>
-      </c>
       <c r="L9" t="s">
-        <v>5075</v>
+        <v>5074</v>
       </c>
       <c r="M9" t="s">
         <v>963</v>
@@ -44081,19 +44215,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>5076</v>
+        <v>5075</v>
       </c>
       <c r="C10" t="s">
-        <v>5083</v>
+        <v>5082</v>
       </c>
       <c r="D10">
         <v>1999</v>
       </c>
       <c r="E10" t="s">
+        <v>5104</v>
+      </c>
+      <c r="F10" t="s">
         <v>5105</v>
-      </c>
-      <c r="F10" t="s">
-        <v>5106</v>
       </c>
       <c r="G10" t="s">
         <v>5030</v>
@@ -44102,16 +44236,16 @@
         <v>196</v>
       </c>
       <c r="I10" t="s">
+        <v>5102</v>
+      </c>
+      <c r="J10" t="s">
         <v>5103</v>
       </c>
-      <c r="J10" t="s">
-        <v>5104</v>
-      </c>
       <c r="K10" t="s">
-        <v>5104</v>
+        <v>5103</v>
       </c>
       <c r="L10" t="s">
-        <v>5076</v>
+        <v>5075</v>
       </c>
       <c r="M10" t="s">
         <v>963</v>
@@ -44131,19 +44265,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>5109</v>
+      </c>
+      <c r="C11" t="s">
         <v>5110</v>
-      </c>
-      <c r="C11" t="s">
-        <v>5111</v>
       </c>
       <c r="D11">
         <v>1996</v>
       </c>
       <c r="E11" t="s">
-        <v>5112</v>
+        <v>5111</v>
       </c>
       <c r="F11" t="s">
-        <v>5107</v>
+        <v>5106</v>
       </c>
       <c r="G11" t="s">
         <v>5030</v>
@@ -44152,13 +44286,13 @@
         <v>218</v>
       </c>
       <c r="I11" t="s">
+        <v>5107</v>
+      </c>
+      <c r="J11" t="s">
         <v>5108</v>
       </c>
-      <c r="J11" t="s">
+      <c r="L11" t="s">
         <v>5109</v>
-      </c>
-      <c r="L11" t="s">
-        <v>5110</v>
       </c>
       <c r="M11" t="s">
         <v>963</v>
@@ -44178,19 +44312,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>5118</v>
+        <v>5117</v>
       </c>
       <c r="C12" t="s">
-        <v>5117</v>
+        <v>5116</v>
       </c>
       <c r="D12">
         <v>2002</v>
       </c>
       <c r="E12" t="s">
-        <v>5116</v>
+        <v>5115</v>
       </c>
       <c r="F12" t="s">
-        <v>5113</v>
+        <v>5112</v>
       </c>
       <c r="G12" t="s">
         <v>5030</v>
@@ -44199,16 +44333,16 @@
         <v>320</v>
       </c>
       <c r="I12" t="s">
+        <v>5113</v>
+      </c>
+      <c r="J12" t="s">
         <v>5114</v>
       </c>
-      <c r="J12" t="s">
-        <v>5115</v>
-      </c>
       <c r="K12" t="s">
-        <v>5115</v>
+        <v>5114</v>
       </c>
       <c r="L12" t="s">
-        <v>5118</v>
+        <v>5117</v>
       </c>
       <c r="M12" t="s">
         <v>963</v>
@@ -44228,19 +44362,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>5122</v>
+      </c>
+      <c r="C13" t="s">
         <v>5123</v>
-      </c>
-      <c r="C13" t="s">
-        <v>5124</v>
       </c>
       <c r="D13">
         <v>2018</v>
       </c>
       <c r="E13" t="s">
-        <v>5125</v>
+        <v>5124</v>
       </c>
       <c r="F13" t="s">
-        <v>5119</v>
+        <v>5118</v>
       </c>
       <c r="G13" t="s">
         <v>5030</v>
@@ -44249,16 +44383,16 @@
         <v>181</v>
       </c>
       <c r="I13" t="s">
+        <v>5119</v>
+      </c>
+      <c r="J13" t="s">
         <v>5120</v>
       </c>
-      <c r="J13" t="s">
-        <v>5121</v>
-      </c>
       <c r="K13" t="s">
-        <v>5121</v>
+        <v>5120</v>
       </c>
       <c r="L13" t="s">
-        <v>5123</v>
+        <v>5122</v>
       </c>
       <c r="M13" t="s">
         <v>963</v>
@@ -44270,7 +44404,7 @@
         <v>966</v>
       </c>
       <c r="P13" t="s">
-        <v>5122</v>
+        <v>5121</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
@@ -44278,19 +44412,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>5128</v>
+      </c>
+      <c r="C14" t="s">
         <v>5129</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5130</v>
       </c>
       <c r="D14">
         <v>2012</v>
       </c>
       <c r="E14" t="s">
-        <v>5131</v>
+        <v>5130</v>
       </c>
       <c r="F14" t="s">
-        <v>5126</v>
+        <v>5125</v>
       </c>
       <c r="G14" t="s">
         <v>5030</v>
@@ -44299,16 +44433,16 @@
         <v>18</v>
       </c>
       <c r="I14" t="s">
+        <v>5126</v>
+      </c>
+      <c r="J14" t="s">
         <v>5127</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
+        <v>5127</v>
+      </c>
+      <c r="L14" t="s">
         <v>5128</v>
-      </c>
-      <c r="K14" t="s">
-        <v>5128</v>
-      </c>
-      <c r="L14" t="s">
-        <v>5129</v>
       </c>
       <c r="M14" t="s">
         <v>963</v>
@@ -44328,19 +44462,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>5136</v>
+        <v>5135</v>
       </c>
       <c r="C15" t="s">
-        <v>5133</v>
+        <v>5132</v>
       </c>
       <c r="D15">
         <v>2020</v>
       </c>
       <c r="E15" t="s">
-        <v>5137</v>
+        <v>5136</v>
       </c>
       <c r="F15" t="s">
-        <v>5134</v>
+        <v>5133</v>
       </c>
       <c r="G15" t="s">
         <v>5030</v>
@@ -44349,16 +44483,16 @@
         <v>11</v>
       </c>
       <c r="I15" t="s">
+        <v>5134</v>
+      </c>
+      <c r="J15" t="s">
+        <v>5131</v>
+      </c>
+      <c r="K15" t="s">
+        <v>5131</v>
+      </c>
+      <c r="L15" t="s">
         <v>5135</v>
-      </c>
-      <c r="J15" t="s">
-        <v>5132</v>
-      </c>
-      <c r="K15" t="s">
-        <v>5132</v>
-      </c>
-      <c r="L15" t="s">
-        <v>5136</v>
       </c>
       <c r="M15" t="s">
         <v>963</v>
@@ -44423,7 +44557,7 @@
         <v>1</v>
       </c>
       <c r="Q16" t="s">
-        <v>5147</v>
+        <v>5146</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -44476,51 +44610,154 @@
         <v>1</v>
       </c>
       <c r="Q17" t="s">
-        <v>5147</v>
+        <v>5146</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4127</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4128</v>
+      </c>
+      <c r="D18">
+        <v>2004</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1957</v>
+      </c>
+      <c r="F18" t="s">
+        <v>1962</v>
+      </c>
+      <c r="G18" t="s">
+        <v>1959</v>
+      </c>
+      <c r="H18">
+        <v>19</v>
+      </c>
+      <c r="I18" t="s">
+        <v>1958</v>
+      </c>
+      <c r="J18" t="s">
+        <v>1960</v>
+      </c>
+      <c r="K18" t="s">
+        <v>1961</v>
+      </c>
+      <c r="L18" t="s">
+        <v>4127</v>
+      </c>
+      <c r="M18" t="s">
+        <v>963</v>
+      </c>
+      <c r="N18" t="s">
+        <v>963</v>
+      </c>
+      <c r="O18" t="s">
+        <v>966</v>
+      </c>
+      <c r="P18" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>5146</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:F2">
-    <cfRule type="containsBlanks" dxfId="16" priority="10">
+    <cfRule type="containsBlanks" dxfId="28" priority="22">
       <formula>LEN(TRIM(F1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:O17">
-    <cfRule type="containsText" dxfId="15" priority="7" operator="containsText" text="PRIMARY STUDY">
+    <cfRule type="containsText" dxfId="27" priority="19" operator="containsText" text="PRIMARY STUDY">
       <formula>NOT(ISERROR(SEARCH("PRIMARY STUDY",M2)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="14" priority="8" operator="notContains" text="YES">
+    <cfRule type="notContainsText" dxfId="26" priority="20" operator="notContains" text="YES">
       <formula>ISERROR(SEARCH("YES",M2))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="9" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="25" priority="21" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",M2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B2">
-    <cfRule type="duplicateValues" dxfId="12" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:R2">
-    <cfRule type="duplicateValues" dxfId="11" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="16"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="containsBlanks" dxfId="10" priority="11">
+  <conditionalFormatting sqref="H1:H17 H19:H1048576">
+    <cfRule type="containsBlanks" dxfId="22" priority="23">
       <formula>LEN(TRIM(H1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1">
-    <cfRule type="duplicateValues" dxfId="9" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2">
-    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q4 P1:P1048576 Q1">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="19" priority="17" operator="between">
       <formula>1</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",P1)))</formula>
     </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F18">
+    <cfRule type="containsBlanks" dxfId="17" priority="11">
+      <formula>LEN(TRIM(F18))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M18:O18">
+    <cfRule type="containsText" dxfId="16" priority="8" operator="containsText" text="PRIMARY STUDY">
+      <formula>NOT(ISERROR(SEARCH("PRIMARY STUDY",M18)))</formula>
+    </cfRule>
+    <cfRule type="notContainsText" dxfId="15" priority="9" operator="notContains" text="YES">
+      <formula>ISERROR(SEARCH("YES",M18))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="10" operator="containsText" text="YES">
+      <formula>NOT(ISERROR(SEARCH("YES",M18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18">
+    <cfRule type="duplicateValues" dxfId="13" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O18">
+    <cfRule type="containsBlanks" dxfId="12" priority="12">
+      <formula>LEN(TRIM(O18))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O18">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="between">
+      <formula>1</formula>
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="7" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",O18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P18">
+    <cfRule type="containsBlanks" dxfId="9" priority="4">
+      <formula>LEN(TRIM(P18))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P18">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="between">
+      <formula>1</formula>
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",P18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L18">
+    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Unified all schooling level effects to the same formula
</commit_message>
<xml_diff>
--- a/Literature/Literature.xlsx
+++ b/Literature/Literature.xlsx
@@ -16986,8 +16986,8 @@
   <dimension ref="A1:Y575"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B52" sqref="B52"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changed the snowballing data frame to master data frame. Moved old master to backup.
</commit_message>
<xml_diff>
--- a/Literature/Literature.xlsx
+++ b/Literature/Literature.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hso20\OneDrive\Plocha\IES\Diploma-Thesis\Literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C454236-CAA7-4624-A062-FF875F6DC4F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2E02EF-29CA-4747-863E-88FD6C53DEBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Query literature" sheetId="5" r:id="rId1"/>
@@ -292,7 +292,7 @@
     <author>Petr Čala</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{AF9AAD2B-1DAE-4AFF-8795-41070BDA5303}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -318,7 +318,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{CD062C54-5659-481F-BE24-852459D90489}">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -344,7 +344,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{59C8AD7A-E480-4151-A614-B7660055D9A0}">
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -371,7 +371,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{F7068529-54B9-48DC-B4A2-F9131D1185FD}">
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -397,7 +397,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{142D23B3-C19A-4A32-A578-4735D120524A}">
+    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -423,7 +423,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{4256AAE2-AA64-4E19-AC6D-839929BA83F4}">
+    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
         <r>
           <rPr>
@@ -449,7 +449,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U6" authorId="0" shapeId="0" xr:uid="{B680C59F-6BD6-45E1-B89E-FBFC10B4AA42}">
+    <comment ref="U6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
       <text>
         <r>
           <rPr>
@@ -485,7 +485,7 @@
     <author>Petr Čala</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -511,7 +511,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -537,7 +537,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -564,7 +564,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
         <r>
           <rPr>
@@ -590,7 +590,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
       <text>
         <r>
           <rPr>
@@ -616,7 +616,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
+    <comment ref="R6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000006000000}">
       <text>
         <r>
           <rPr>
@@ -652,7 +652,7 @@
     <author>Petr Čala</author>
   </authors>
   <commentList>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -694,7 +694,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10116" uniqueCount="5364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10275" uniqueCount="5374">
   <si>
     <t>Number</t>
   </si>
@@ -16602,12 +16602,6 @@
     <t>Light, A. and Strayer, W. (2004): "Who Receives the College Wage Premium Assessing the Labor Market Returns to Degrees and College Transfer Patterns." The Journal of Human Resources, 39(3), pp. 746-773.</t>
   </si>
   <si>
-    <t>Miller, &amp; Nmartin(1995): (1995)</t>
-  </si>
-  <si>
-    <t>Miller, &amp; Nmartin(1995):</t>
-  </si>
-  <si>
     <t>What do Twins Studies Reveal About the Economic Returns to Education?</t>
   </si>
   <si>
@@ -16786,13 +16780,49 @@
   </si>
   <si>
     <t>Journal of Econometrics</t>
+  </si>
+  <si>
+    <t>much theory</t>
+  </si>
+  <si>
+    <t>DISCONTINUITY</t>
+  </si>
+  <si>
+    <t>PART OF MAIN QUERY</t>
+  </si>
+  <si>
+    <t>IQ ONLY</t>
+  </si>
+  <si>
+    <t>Focuses purely on ability, no returns to schooling (except for meta data)</t>
+  </si>
+  <si>
+    <t>Effect of a reform on years of schooling / immigration</t>
+  </si>
+  <si>
+    <t>Math reform instead of years of schooling</t>
+  </si>
+  <si>
+    <t>wrong flag, collected later as a part of snowballing literature, also brilliant for literature, primary study also</t>
+  </si>
+  <si>
+    <t>cool theory on abiliity bias, so really 1, but no data for 1, only 3</t>
+  </si>
+  <si>
+    <t>TWINS</t>
+  </si>
+  <si>
+    <t>from snowballing query</t>
+  </si>
+  <si>
+    <t>REPLICATION OF CARD(1995)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -16857,6 +16887,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -17075,15 +17113,6 @@
     <border>
       <left/>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -17110,12 +17139,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -17156,43 +17196,19 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="49">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="51">
     <dxf>
       <fill>
         <patternFill>
@@ -17350,6 +17366,17 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFAACAC"/>
@@ -17393,6 +17420,46 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAACAC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFAACAC"/>
@@ -17403,13 +17470,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAACAC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -17850,9 +17910,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Y575"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J15" sqref="J15"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17928,14 +17988,14 @@
       </c>
       <c r="R1" s="29">
         <f>COUNTIFS($M:$M, "YES", $F:$F, "&lt;&gt;") + Twins!S1</f>
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="T1" s="28" t="s">
         <v>5039</v>
       </c>
       <c r="U1" s="29">
         <f>COUNTIF($L$2:$L$575, "&lt;&gt; ") +Twins!V1</f>
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="V1" s="31"/>
       <c r="W1" s="31"/>
@@ -18159,7 +18219,7 @@
       <c r="T5" s="2" t="s">
         <v>5140</v>
       </c>
-      <c r="U5" s="38">
+      <c r="U5" s="37">
         <f>COUNTIFS($N:$N, "YES", $F:$F, "&lt;&gt;")</f>
         <v>74</v>
       </c>
@@ -18264,6 +18324,12 @@
       <c r="O7" s="7" t="s">
         <v>5029</v>
       </c>
+      <c r="P7" t="s">
+        <v>5369</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>904</v>
+      </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -18414,37 +18480,37 @@
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A11" s="39">
+      <c r="A11" s="38">
         <v>10</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="38" t="s">
         <v>3935</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="38" t="s">
         <v>3936</v>
       </c>
-      <c r="D11" s="39">
+      <c r="D11" s="38">
         <v>2005</v>
       </c>
-      <c r="E11" s="39" t="s">
+      <c r="E11" s="38" t="s">
         <v>1072</v>
       </c>
-      <c r="F11" s="39" t="s">
+      <c r="F11" s="38" t="s">
         <v>970</v>
       </c>
-      <c r="G11" s="39" t="s">
+      <c r="G11" s="38" t="s">
         <v>1074</v>
       </c>
-      <c r="H11" s="39">
-        <v>1</v>
-      </c>
-      <c r="I11" s="39" t="s">
+      <c r="H11" s="38">
+        <v>1</v>
+      </c>
+      <c r="I11" s="38" t="s">
         <v>1073</v>
       </c>
-      <c r="J11" s="39" t="s">
+      <c r="J11" s="38" t="s">
         <v>1075</v>
       </c>
-      <c r="K11" s="39" t="s">
+      <c r="K11" s="38" t="s">
         <v>1075</v>
       </c>
       <c r="L11" t="s">
@@ -19776,37 +19842,37 @@
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A38" s="39">
+      <c r="A38" s="38">
         <v>37</v>
       </c>
-      <c r="B38" s="39" t="s">
+      <c r="B38" s="38" t="s">
         <v>3965</v>
       </c>
-      <c r="C38" s="39" t="s">
+      <c r="C38" s="38" t="s">
         <v>3966</v>
       </c>
-      <c r="D38" s="39">
+      <c r="D38" s="38">
         <v>2003</v>
       </c>
-      <c r="E38" s="39" t="s">
+      <c r="E38" s="38" t="s">
         <v>1211</v>
       </c>
-      <c r="F38" s="39" t="s">
+      <c r="F38" s="38" t="s">
         <v>4598</v>
       </c>
-      <c r="G38" s="39" t="s">
+      <c r="G38" s="38" t="s">
         <v>1213</v>
       </c>
-      <c r="H38" s="39">
+      <c r="H38" s="38">
         <v>265</v>
       </c>
-      <c r="I38" s="39" t="s">
+      <c r="I38" s="38" t="s">
         <v>1212</v>
       </c>
-      <c r="J38" s="39" t="s">
+      <c r="J38" s="38" t="s">
         <v>1214</v>
       </c>
-      <c r="K38" s="39" t="s">
+      <c r="K38" s="38" t="s">
         <v>1215</v>
       </c>
       <c r="L38" t="s">
@@ -27970,53 +28036,53 @@
         <v>904</v>
       </c>
     </row>
-    <row r="201" spans="1:18" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A201" s="36">
+    <row r="201" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A201" s="35">
         <v>200</v>
       </c>
-      <c r="B201" s="36" t="s">
+      <c r="B201" s="35" t="s">
         <v>4141</v>
       </c>
-      <c r="C201" s="36" t="s">
+      <c r="C201" s="35" t="s">
         <v>4142</v>
       </c>
-      <c r="D201" s="36">
+      <c r="D201" s="35">
         <v>4903</v>
       </c>
-      <c r="E201" s="36" t="s">
+      <c r="E201" s="35" t="s">
         <v>2025</v>
       </c>
-      <c r="F201" s="36" t="s">
+      <c r="F201" s="35" t="s">
         <v>4621</v>
       </c>
-      <c r="G201" s="36" t="s">
+      <c r="G201" s="35" t="s">
         <v>2027</v>
       </c>
-      <c r="H201" s="36">
+      <c r="H201" s="35">
         <v>7</v>
       </c>
-      <c r="I201" s="36" t="s">
+      <c r="I201" s="35" t="s">
         <v>2026</v>
       </c>
-      <c r="J201" s="36" t="s">
+      <c r="J201" s="35" t="s">
         <v>2028</v>
       </c>
-      <c r="K201" s="36" t="s">
+      <c r="K201" s="35" t="s">
         <v>2028</v>
       </c>
-      <c r="L201" s="36" t="s">
+      <c r="L201" s="35" t="s">
         <v>974</v>
       </c>
-      <c r="M201" s="36" t="s">
+      <c r="M201" s="35" t="s">
         <v>966</v>
       </c>
-      <c r="N201" s="36" t="s">
+      <c r="N201" s="35" t="s">
         <v>966</v>
       </c>
-      <c r="O201" s="37" t="s">
-        <v>5029</v>
-      </c>
-      <c r="R201" s="36" t="s">
+      <c r="O201" s="36" t="s">
+        <v>5029</v>
+      </c>
+      <c r="R201" s="35" t="s">
         <v>904</v>
       </c>
     </row>
@@ -44496,59 +44562,59 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B38 B40:B1048576">
-    <cfRule type="duplicateValues" dxfId="48" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="50" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsBlanks" dxfId="47" priority="20">
+    <cfRule type="containsBlanks" dxfId="49" priority="20">
       <formula>LEN(TRIM(F1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:N601">
-    <cfRule type="containsText" dxfId="46" priority="11" operator="containsText" text="PRIMARY STUDY">
+    <cfRule type="containsText" dxfId="48" priority="11" operator="containsText" text="PRIMARY STUDY">
       <formula>NOT(ISERROR(SEARCH("PRIMARY STUDY",L2)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="45" priority="12" operator="notContains" text="YES">
+    <cfRule type="notContainsText" dxfId="47" priority="12" operator="notContains" text="YES">
       <formula>ISERROR(SEARCH("YES",L2))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="13" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="46" priority="13" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",L2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O601 P136 P146 P151 P161 P163 P177 P187 P189:P190">
-    <cfRule type="containsBlanks" dxfId="43" priority="22">
+    <cfRule type="containsBlanks" dxfId="45" priority="22">
       <formula>LEN(TRIM(O2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O601 P177 P187 P189:P190">
-    <cfRule type="cellIs" dxfId="42" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="44" priority="8" operator="between">
       <formula>1</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="9" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="43" priority="9" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",O2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q10 Q16:Q1048576 R11:R15">
-    <cfRule type="duplicateValues" dxfId="40" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R6">
-    <cfRule type="cellIs" dxfId="39" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="21" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="38" priority="23">
+    <cfRule type="containsBlanks" dxfId="40" priority="23">
       <formula>LEN(TRIM(R6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8">
-    <cfRule type="cellIs" dxfId="37" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="17" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="18" operator="notEqual">
+    <cfRule type="cellIs" dxfId="38" priority="18" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1">
-    <cfRule type="duplicateValues" dxfId="35" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="5"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="K160" r:id="rId1" location="page=11" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -44562,12 +44628,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E591E98B-02D7-41E1-8C44-6E84A040E0B9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC575"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S10" sqref="S10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44644,20 +44710,22 @@
       <c r="S1" s="25" t="s">
         <v>5137</v>
       </c>
-      <c r="T1" s="31"/>
+      <c r="T1" s="39" t="s">
+        <v>5145</v>
+      </c>
       <c r="U1" s="28" t="s">
         <v>5038</v>
       </c>
       <c r="V1" s="29">
         <f>COUNTIFS($Q:$Q, "YES", $F:$F, "&lt;&gt;")</f>
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="X1" s="28" t="s">
         <v>5039</v>
       </c>
       <c r="Y1" s="29">
         <f>COUNTIF($P:$P, "YES")</f>
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="Z1" s="31"/>
       <c r="AA1" s="31"/>
@@ -44693,10 +44761,10 @@
         <v>1</v>
       </c>
       <c r="J2" s="34" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K2" s="34" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L2" s="34">
         <v>289</v>
@@ -44710,10 +44778,18 @@
       <c r="O2" s="34" t="s">
         <v>5029</v>
       </c>
+      <c r="P2" s="34" t="s">
+        <v>963</v>
+      </c>
       <c r="Q2" s="34" t="s">
         <v>963</v>
       </c>
-      <c r="S2" s="9"/>
+      <c r="R2" s="34" t="s">
+        <v>963</v>
+      </c>
+      <c r="S2" s="9">
+        <v>2</v>
+      </c>
       <c r="U2"/>
       <c r="V2" t="s">
         <v>904</v>
@@ -44745,16 +44821,16 @@
         <v>5029</v>
       </c>
       <c r="H3" t="s">
-        <v>5350</v>
+        <v>5348</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K3" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L3">
         <v>1486</v>
@@ -44768,10 +44844,18 @@
       <c r="O3" t="s">
         <v>5029</v>
       </c>
-      <c r="Q3" s="42" t="s">
+      <c r="P3" t="s">
+        <v>5364</v>
+      </c>
+      <c r="Q3" t="s">
         <v>963</v>
       </c>
-      <c r="S3" s="7"/>
+      <c r="R3" t="s">
+        <v>966</v>
+      </c>
+      <c r="S3" s="7" t="s">
+        <v>5029</v>
+      </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -44802,10 +44886,10 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K4" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L4">
         <v>321</v>
@@ -44819,10 +44903,18 @@
       <c r="O4" t="s">
         <v>5029</v>
       </c>
-      <c r="Q4" s="42" t="s">
+      <c r="P4" t="s">
         <v>963</v>
       </c>
-      <c r="S4" s="7"/>
+      <c r="Q4" t="s">
+        <v>963</v>
+      </c>
+      <c r="R4" t="s">
+        <v>963</v>
+      </c>
+      <c r="S4" s="7">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -44847,16 +44939,16 @@
         <v>5029</v>
       </c>
       <c r="H5" t="s">
-        <v>5351</v>
+        <v>5349</v>
       </c>
       <c r="I5" t="b">
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K5" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L5">
         <v>3590</v>
@@ -44870,10 +44962,18 @@
       <c r="O5" t="s">
         <v>5029</v>
       </c>
-      <c r="Q5" s="42" t="s">
+      <c r="P5" t="s">
         <v>963</v>
       </c>
-      <c r="S5" s="7"/>
+      <c r="Q5" t="s">
+        <v>963</v>
+      </c>
+      <c r="R5" t="s">
+        <v>963</v>
+      </c>
+      <c r="S5" s="7">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -44904,10 +45004,10 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K6" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L6">
         <v>1510</v>
@@ -44921,16 +45021,27 @@
       <c r="O6" t="s">
         <v>5029</v>
       </c>
-      <c r="Q6" s="42" t="s">
-        <v>963</v>
-      </c>
-      <c r="S6" s="7"/>
+      <c r="P6" t="s">
+        <v>967</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>967</v>
+      </c>
+      <c r="R6" t="s">
+        <v>966</v>
+      </c>
+      <c r="S6" s="7" t="s">
+        <v>5029</v>
+      </c>
+      <c r="T6" t="s">
+        <v>5362</v>
+      </c>
       <c r="U6" s="2" t="s">
         <v>5143</v>
       </c>
       <c r="V6">
         <f>COUNTIF($P:$P, "YES")</f>
-        <v>0</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
@@ -44956,16 +45067,16 @@
         <v>5029</v>
       </c>
       <c r="H7" t="s">
-        <v>5352</v>
+        <v>5350</v>
       </c>
       <c r="I7" t="b">
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K7" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L7">
         <v>321</v>
@@ -44979,16 +45090,24 @@
       <c r="O7" t="s">
         <v>5029</v>
       </c>
-      <c r="Q7" s="42" t="s">
+      <c r="P7" t="s">
         <v>963</v>
       </c>
-      <c r="S7" s="7"/>
+      <c r="Q7" t="s">
+        <v>963</v>
+      </c>
+      <c r="R7" t="s">
+        <v>963</v>
+      </c>
+      <c r="S7" s="7">
+        <v>1</v>
+      </c>
       <c r="U7" s="2" t="s">
         <v>5140</v>
       </c>
       <c r="V7">
         <f>COUNTIFS($R:$R, "YES", $F:$F, "&lt;&gt;")</f>
-        <v>0</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
@@ -45020,10 +45139,10 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K8" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L8">
         <v>588</v>
@@ -45037,10 +45156,18 @@
       <c r="O8" t="s">
         <v>5029</v>
       </c>
-      <c r="Q8" s="42" t="s">
+      <c r="P8" t="s">
         <v>963</v>
       </c>
-      <c r="S8" s="7"/>
+      <c r="Q8" t="s">
+        <v>963</v>
+      </c>
+      <c r="R8" t="s">
+        <v>963</v>
+      </c>
+      <c r="S8" s="7">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -45065,16 +45192,16 @@
         <v>5029</v>
       </c>
       <c r="H9" t="s">
-        <v>5353</v>
+        <v>5351</v>
       </c>
       <c r="I9" t="b">
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K9" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L9">
         <v>73</v>
@@ -45088,10 +45215,18 @@
       <c r="O9" t="s">
         <v>5029</v>
       </c>
-      <c r="Q9" s="42" t="s">
+      <c r="P9" t="s">
         <v>963</v>
       </c>
-      <c r="S9" s="7"/>
+      <c r="Q9" t="s">
+        <v>963</v>
+      </c>
+      <c r="R9" t="s">
+        <v>963</v>
+      </c>
+      <c r="S9" s="7">
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -45116,16 +45251,16 @@
         <v>5029</v>
       </c>
       <c r="H10" t="s">
-        <v>5354</v>
+        <v>5352</v>
       </c>
       <c r="I10" t="b">
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K10" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L10">
         <v>74</v>
@@ -45139,61 +45274,77 @@
       <c r="O10" t="s">
         <v>5029</v>
       </c>
-      <c r="Q10" s="42" t="s">
+      <c r="P10" t="s">
+        <v>5363</v>
+      </c>
+      <c r="Q10" t="s">
         <v>963</v>
       </c>
-      <c r="S10" s="7"/>
-    </row>
-    <row r="11" spans="1:29" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="40">
+      <c r="R10" t="s">
+        <v>966</v>
+      </c>
+      <c r="S10" s="7" t="s">
+        <v>5029</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" t="s">
         <v>5199</v>
       </c>
-      <c r="C11" s="40" t="s">
+      <c r="C11" t="s">
         <v>5200</v>
       </c>
-      <c r="D11" s="40">
+      <c r="D11">
         <v>2014</v>
       </c>
-      <c r="E11" s="40" t="s">
+      <c r="E11" t="s">
         <v>5201</v>
       </c>
-      <c r="F11" s="40" t="s">
+      <c r="F11" t="s">
         <v>5202</v>
       </c>
-      <c r="G11" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="H11" s="40" t="s">
+      <c r="G11" t="s">
+        <v>5029</v>
+      </c>
+      <c r="H11" t="s">
         <v>253</v>
       </c>
-      <c r="I11" s="40" t="b">
-        <v>1</v>
-      </c>
-      <c r="J11" s="40" t="s">
-        <v>5349</v>
-      </c>
-      <c r="K11" s="40" t="s">
-        <v>5349</v>
-      </c>
-      <c r="L11" s="40">
+      <c r="I11" t="b">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>5347</v>
+      </c>
+      <c r="K11" t="s">
+        <v>5347</v>
+      </c>
+      <c r="L11">
         <v>17</v>
       </c>
-      <c r="M11" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="N11" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="O11" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="Q11" s="42" t="s">
+      <c r="M11" t="s">
+        <v>5029</v>
+      </c>
+      <c r="N11" t="s">
+        <v>5029</v>
+      </c>
+      <c r="O11" t="s">
+        <v>5029</v>
+      </c>
+      <c r="P11" t="s">
         <v>963</v>
       </c>
-      <c r="S11" s="41"/>
+      <c r="Q11" t="s">
+        <v>963</v>
+      </c>
+      <c r="R11" t="s">
+        <v>963</v>
+      </c>
+      <c r="S11" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -45218,16 +45369,16 @@
         <v>5029</v>
       </c>
       <c r="H12" t="s">
-        <v>5355</v>
+        <v>5353</v>
       </c>
       <c r="I12" t="b">
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K12" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L12">
         <v>1789</v>
@@ -45241,10 +45392,18 @@
       <c r="O12" t="s">
         <v>5029</v>
       </c>
-      <c r="Q12" s="42" t="s">
+      <c r="P12" t="s">
         <v>963</v>
       </c>
-      <c r="S12" s="7"/>
+      <c r="Q12" t="s">
+        <v>963</v>
+      </c>
+      <c r="R12" t="s">
+        <v>963</v>
+      </c>
+      <c r="S12" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -45269,16 +45428,16 @@
         <v>5029</v>
       </c>
       <c r="H13" t="s">
-        <v>5352</v>
+        <v>5350</v>
       </c>
       <c r="I13" t="b">
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K13" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L13">
         <v>2928</v>
@@ -45292,10 +45451,21 @@
       <c r="O13" t="s">
         <v>5029</v>
       </c>
-      <c r="Q13" s="42" t="s">
+      <c r="P13" t="s">
+        <v>5365</v>
+      </c>
+      <c r="Q13" t="s">
         <v>963</v>
       </c>
-      <c r="S13" s="7"/>
+      <c r="R13" t="s">
+        <v>966</v>
+      </c>
+      <c r="S13" s="7">
+        <v>1</v>
+      </c>
+      <c r="T13" t="s">
+        <v>5366</v>
+      </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -45320,16 +45490,16 @@
         <v>5029</v>
       </c>
       <c r="H14" t="s">
-        <v>5356</v>
+        <v>5354</v>
       </c>
       <c r="I14" t="b">
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K14" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L14">
         <v>783</v>
@@ -45343,10 +45513,18 @@
       <c r="O14" t="s">
         <v>5029</v>
       </c>
-      <c r="Q14" s="42" t="s">
+      <c r="P14" t="s">
         <v>963</v>
       </c>
-      <c r="S14" s="7"/>
+      <c r="Q14" t="s">
+        <v>963</v>
+      </c>
+      <c r="R14" t="s">
+        <v>963</v>
+      </c>
+      <c r="S14" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -45371,16 +45549,16 @@
         <v>5029</v>
       </c>
       <c r="H15" t="s">
-        <v>5357</v>
+        <v>5355</v>
       </c>
       <c r="I15" t="b">
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K15" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L15">
         <v>141</v>
@@ -45394,10 +45572,21 @@
       <c r="O15" t="s">
         <v>5029</v>
       </c>
-      <c r="Q15" s="42" t="s">
+      <c r="P15" t="s">
+        <v>966</v>
+      </c>
+      <c r="Q15" t="s">
         <v>963</v>
       </c>
-      <c r="S15" s="7"/>
+      <c r="R15" t="s">
+        <v>966</v>
+      </c>
+      <c r="S15" s="7" t="s">
+        <v>5029</v>
+      </c>
+      <c r="T15" t="s">
+        <v>5367</v>
+      </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -45428,10 +45617,10 @@
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K16" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L16">
         <v>284</v>
@@ -45445,12 +45634,20 @@
       <c r="O16" t="s">
         <v>5029</v>
       </c>
-      <c r="Q16" s="42" t="s">
+      <c r="P16" t="s">
         <v>963</v>
       </c>
-      <c r="S16" s="7"/>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q16" t="s">
+        <v>963</v>
+      </c>
+      <c r="R16" t="s">
+        <v>963</v>
+      </c>
+      <c r="S16" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -45473,16 +45670,16 @@
         <v>5029</v>
       </c>
       <c r="H17" t="s">
-        <v>5358</v>
+        <v>5356</v>
       </c>
       <c r="I17" t="b">
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K17" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L17">
         <v>252</v>
@@ -45496,12 +45693,20 @@
       <c r="O17" t="s">
         <v>5029</v>
       </c>
-      <c r="Q17" s="42" t="s">
+      <c r="P17" t="s">
         <v>963</v>
       </c>
-      <c r="S17" s="7"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q17" t="s">
+        <v>963</v>
+      </c>
+      <c r="R17" t="s">
+        <v>963</v>
+      </c>
+      <c r="S17" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -45530,10 +45735,10 @@
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K18" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L18">
         <v>88</v>
@@ -45547,12 +45752,20 @@
       <c r="O18" t="s">
         <v>5029</v>
       </c>
-      <c r="Q18" s="42" t="s">
+      <c r="P18" t="s">
         <v>963</v>
       </c>
-      <c r="S18" s="7"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q18" t="s">
+        <v>963</v>
+      </c>
+      <c r="R18" t="s">
+        <v>963</v>
+      </c>
+      <c r="S18" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -45581,10 +45794,10 @@
         <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K19" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L19">
         <v>2852</v>
@@ -45598,12 +45811,20 @@
       <c r="O19" t="s">
         <v>5029</v>
       </c>
-      <c r="Q19" s="42" t="s">
+      <c r="P19" t="s">
         <v>963</v>
       </c>
-      <c r="S19" s="7"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q19" t="s">
+        <v>963</v>
+      </c>
+      <c r="R19" t="s">
+        <v>963</v>
+      </c>
+      <c r="S19" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -45632,10 +45853,10 @@
         <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K20" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L20">
         <v>386</v>
@@ -45649,12 +45870,20 @@
       <c r="O20" t="s">
         <v>5029</v>
       </c>
-      <c r="Q20" s="42" t="s">
+      <c r="P20" t="s">
         <v>963</v>
       </c>
-      <c r="S20" s="7"/>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q20" t="s">
+        <v>963</v>
+      </c>
+      <c r="R20" t="s">
+        <v>963</v>
+      </c>
+      <c r="S20" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -45677,16 +45906,16 @@
         <v>5029</v>
       </c>
       <c r="H21" t="s">
-        <v>5359</v>
+        <v>5357</v>
       </c>
       <c r="I21" t="b">
         <v>1</v>
       </c>
       <c r="J21" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K21" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L21">
         <v>494</v>
@@ -45700,12 +45929,20 @@
       <c r="O21" t="s">
         <v>5029</v>
       </c>
-      <c r="Q21" s="42" t="s">
+      <c r="P21" t="s">
         <v>963</v>
       </c>
-      <c r="S21" s="7"/>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q21" t="s">
+        <v>963</v>
+      </c>
+      <c r="R21" t="s">
+        <v>963</v>
+      </c>
+      <c r="S21" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -45728,16 +45965,16 @@
         <v>5029</v>
       </c>
       <c r="H22" t="s">
-        <v>167</v>
+        <v>253</v>
       </c>
       <c r="I22" t="b">
         <v>1</v>
       </c>
       <c r="J22" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K22" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L22">
         <v>101</v>
@@ -45751,12 +45988,20 @@
       <c r="O22" t="s">
         <v>5029</v>
       </c>
-      <c r="Q22" s="42" t="s">
+      <c r="P22" t="s">
         <v>963</v>
       </c>
-      <c r="S22" s="7"/>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q22" t="s">
+        <v>963</v>
+      </c>
+      <c r="R22" t="s">
+        <v>963</v>
+      </c>
+      <c r="S22" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -45779,16 +46024,16 @@
         <v>5029</v>
       </c>
       <c r="H23" t="s">
-        <v>5354</v>
+        <v>5352</v>
       </c>
       <c r="I23" t="b">
         <v>1</v>
       </c>
       <c r="J23" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K23" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L23">
         <v>92</v>
@@ -45802,12 +46047,23 @@
       <c r="O23" t="s">
         <v>5029</v>
       </c>
-      <c r="Q23" s="42" t="s">
+      <c r="P23" t="s">
+        <v>966</v>
+      </c>
+      <c r="Q23" t="s">
         <v>963</v>
       </c>
-      <c r="S23" s="7"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R23" t="s">
+        <v>966</v>
+      </c>
+      <c r="S23" s="7" t="s">
+        <v>5029</v>
+      </c>
+      <c r="T23" t="s">
+        <v>5368</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -45836,10 +46092,10 @@
         <v>1</v>
       </c>
       <c r="J24" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K24" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L24">
         <v>171</v>
@@ -45853,12 +46109,20 @@
       <c r="O24" t="s">
         <v>5029</v>
       </c>
-      <c r="Q24" s="42" t="s">
+      <c r="P24" t="s">
         <v>963</v>
       </c>
-      <c r="S24" s="7"/>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q24" t="s">
+        <v>963</v>
+      </c>
+      <c r="R24" t="s">
+        <v>963</v>
+      </c>
+      <c r="S24" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -45881,16 +46145,16 @@
         <v>5029</v>
       </c>
       <c r="H25" t="s">
-        <v>5359</v>
+        <v>5357</v>
       </c>
       <c r="I25" t="b">
         <v>1</v>
       </c>
       <c r="J25" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K25" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L25">
         <v>662</v>
@@ -45904,12 +46168,20 @@
       <c r="O25" t="s">
         <v>5029</v>
       </c>
-      <c r="Q25" s="42" t="s">
+      <c r="P25" t="s">
         <v>963</v>
       </c>
-      <c r="S25" s="7"/>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q25" t="s">
+        <v>963</v>
+      </c>
+      <c r="R25" t="s">
+        <v>963</v>
+      </c>
+      <c r="S25" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -45938,10 +46210,10 @@
         <v>1</v>
       </c>
       <c r="J26" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K26" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L26">
         <v>888</v>
@@ -45955,12 +46227,20 @@
       <c r="O26" t="s">
         <v>5029</v>
       </c>
-      <c r="Q26" s="42" t="s">
+      <c r="P26" t="s">
         <v>963</v>
       </c>
-      <c r="S26" s="7"/>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q26" t="s">
+        <v>963</v>
+      </c>
+      <c r="R26" t="s">
+        <v>963</v>
+      </c>
+      <c r="S26" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -45989,10 +46269,10 @@
         <v>1</v>
       </c>
       <c r="J27" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K27" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L27">
         <v>100</v>
@@ -46006,12 +46286,20 @@
       <c r="O27" t="s">
         <v>5029</v>
       </c>
-      <c r="Q27" s="42" t="s">
+      <c r="P27" t="s">
         <v>963</v>
       </c>
-      <c r="S27" s="7"/>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q27" t="s">
+        <v>963</v>
+      </c>
+      <c r="R27" t="s">
+        <v>963</v>
+      </c>
+      <c r="S27" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -46034,16 +46322,16 @@
         <v>5029</v>
       </c>
       <c r="H28" t="s">
-        <v>5354</v>
+        <v>5352</v>
       </c>
       <c r="I28" t="b">
         <v>1</v>
       </c>
       <c r="J28" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K28" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L28">
         <v>860</v>
@@ -46057,12 +46345,20 @@
       <c r="O28" t="s">
         <v>5029</v>
       </c>
-      <c r="Q28" s="42" t="s">
+      <c r="P28" t="s">
         <v>963</v>
       </c>
-      <c r="S28" s="7"/>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q28" t="s">
+        <v>963</v>
+      </c>
+      <c r="R28" t="s">
+        <v>963</v>
+      </c>
+      <c r="S28" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -46091,10 +46387,10 @@
         <v>1</v>
       </c>
       <c r="J29" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K29" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L29">
         <v>27</v>
@@ -46108,12 +46404,20 @@
       <c r="O29" t="s">
         <v>5029</v>
       </c>
-      <c r="Q29" s="42" t="s">
+      <c r="P29" t="s">
+        <v>966</v>
+      </c>
+      <c r="Q29" t="s">
         <v>963</v>
       </c>
-      <c r="S29" s="7"/>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R29" t="s">
+        <v>966</v>
+      </c>
+      <c r="S29" s="7" t="s">
+        <v>5029</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -46136,16 +46440,16 @@
         <v>5029</v>
       </c>
       <c r="H30" t="s">
-        <v>5360</v>
+        <v>5358</v>
       </c>
       <c r="I30" t="b">
         <v>1</v>
       </c>
       <c r="J30" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K30" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L30">
         <v>1427</v>
@@ -46159,12 +46463,23 @@
       <c r="O30" t="s">
         <v>5029</v>
       </c>
-      <c r="Q30" s="42" t="s">
+      <c r="P30" t="s">
         <v>963</v>
       </c>
-      <c r="S30" s="7"/>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q30" t="s">
+        <v>963</v>
+      </c>
+      <c r="R30" t="s">
+        <v>963</v>
+      </c>
+      <c r="S30" s="7">
+        <v>3</v>
+      </c>
+      <c r="T30" t="s">
+        <v>5370</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -46187,16 +46502,16 @@
         <v>5029</v>
       </c>
       <c r="H31" t="s">
-        <v>5359</v>
+        <v>5357</v>
       </c>
       <c r="I31" t="b">
         <v>1</v>
       </c>
       <c r="J31" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K31" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L31">
         <v>80</v>
@@ -46210,12 +46525,20 @@
       <c r="O31" t="s">
         <v>5029</v>
       </c>
-      <c r="Q31" s="42" t="s">
+      <c r="P31" t="s">
         <v>963</v>
       </c>
-      <c r="S31" s="7"/>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q31" t="s">
+        <v>963</v>
+      </c>
+      <c r="R31" t="s">
+        <v>963</v>
+      </c>
+      <c r="S31" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -46244,10 +46567,10 @@
         <v>1</v>
       </c>
       <c r="J32" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K32" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L32">
         <v>182</v>
@@ -46261,10 +46584,18 @@
       <c r="O32" t="s">
         <v>5029</v>
       </c>
-      <c r="Q32" s="42" t="s">
+      <c r="P32" t="s">
         <v>963</v>
       </c>
-      <c r="S32" s="7"/>
+      <c r="Q32" t="s">
+        <v>963</v>
+      </c>
+      <c r="R32" t="s">
+        <v>963</v>
+      </c>
+      <c r="S32" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33">
@@ -46289,16 +46620,16 @@
         <v>5029</v>
       </c>
       <c r="H33" t="s">
-        <v>5354</v>
+        <v>5352</v>
       </c>
       <c r="I33" t="b">
         <v>1</v>
       </c>
       <c r="J33" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K33" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L33">
         <v>389</v>
@@ -46312,10 +46643,18 @@
       <c r="O33" t="s">
         <v>5029</v>
       </c>
-      <c r="Q33" s="42" t="s">
+      <c r="P33" t="s">
         <v>963</v>
       </c>
-      <c r="S33" s="7"/>
+      <c r="Q33" t="s">
+        <v>963</v>
+      </c>
+      <c r="R33" t="s">
+        <v>963</v>
+      </c>
+      <c r="S33" s="7">
+        <v>4</v>
+      </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34">
@@ -46346,10 +46685,10 @@
         <v>1</v>
       </c>
       <c r="J34" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K34" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L34">
         <v>177</v>
@@ -46363,10 +46702,18 @@
       <c r="O34" t="s">
         <v>5029</v>
       </c>
-      <c r="Q34" s="42" t="s">
+      <c r="P34" t="s">
+        <v>5371</v>
+      </c>
+      <c r="Q34" t="s">
         <v>963</v>
       </c>
-      <c r="S34" s="7"/>
+      <c r="R34" t="s">
+        <v>966</v>
+      </c>
+      <c r="S34" s="7" t="s">
+        <v>5029</v>
+      </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35">
@@ -46397,10 +46744,10 @@
         <v>1</v>
       </c>
       <c r="J35" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K35" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L35">
         <v>217</v>
@@ -46414,401 +46761,465 @@
       <c r="O35" t="s">
         <v>5029</v>
       </c>
-      <c r="Q35" s="42" t="s">
+      <c r="P35" t="s">
         <v>963</v>
       </c>
-      <c r="S35" s="7"/>
-    </row>
-    <row r="36" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="40">
+      <c r="Q35" t="s">
+        <v>963</v>
+      </c>
+      <c r="R35" t="s">
+        <v>963</v>
+      </c>
+      <c r="S35" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" s="40" t="s">
+      <c r="B36" t="s">
         <v>5282</v>
       </c>
-      <c r="C36" s="40" t="s">
+      <c r="C36" t="s">
         <v>5283</v>
       </c>
-      <c r="D36" s="40">
+      <c r="D36">
         <v>1993</v>
       </c>
-      <c r="E36" s="40" t="s">
+      <c r="E36" t="s">
         <v>5284</v>
       </c>
-      <c r="F36" s="40" t="s">
+      <c r="F36" t="s">
         <v>5285</v>
       </c>
-      <c r="G36" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="H36" s="40" t="s">
+      <c r="G36" t="s">
+        <v>5029</v>
+      </c>
+      <c r="H36" t="s">
         <v>99</v>
       </c>
-      <c r="I36" s="40" t="b">
-        <v>1</v>
-      </c>
-      <c r="J36" s="40" t="s">
-        <v>5349</v>
-      </c>
-      <c r="K36" s="40" t="s">
-        <v>5349</v>
-      </c>
-      <c r="L36" s="40">
+      <c r="I36" t="b">
+        <v>1</v>
+      </c>
+      <c r="J36" t="s">
+        <v>5347</v>
+      </c>
+      <c r="K36" t="s">
+        <v>5347</v>
+      </c>
+      <c r="L36">
         <v>1442</v>
       </c>
-      <c r="M36" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="N36" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="O36" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="Q36" s="42" t="s">
+      <c r="M36" t="s">
+        <v>5029</v>
+      </c>
+      <c r="N36" t="s">
+        <v>5029</v>
+      </c>
+      <c r="O36" t="s">
+        <v>5029</v>
+      </c>
+      <c r="P36" t="s">
         <v>963</v>
       </c>
-      <c r="S36" s="41"/>
-    </row>
-    <row r="37" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="40">
+      <c r="Q36" t="s">
+        <v>963</v>
+      </c>
+      <c r="R36" t="s">
+        <v>963</v>
+      </c>
+      <c r="S36" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" s="40" t="s">
+      <c r="B37" t="s">
         <v>469</v>
       </c>
-      <c r="C37" s="40" t="s">
+      <c r="C37" t="s">
         <v>470</v>
       </c>
-      <c r="D37" s="40">
+      <c r="D37">
         <v>2006</v>
       </c>
-      <c r="E37" s="40" t="s">
+      <c r="E37" t="s">
         <v>5286</v>
       </c>
-      <c r="F37" s="40" t="s">
+      <c r="F37" t="s">
         <v>5287</v>
       </c>
-      <c r="G37" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="H37" s="40" t="s">
+      <c r="G37" t="s">
+        <v>5029</v>
+      </c>
+      <c r="H37" t="s">
         <v>477</v>
       </c>
-      <c r="I37" s="40" t="b">
-        <v>1</v>
-      </c>
-      <c r="J37" s="40" t="s">
-        <v>5349</v>
-      </c>
-      <c r="K37" s="40" t="s">
-        <v>5349</v>
-      </c>
-      <c r="L37" s="40">
+      <c r="I37" t="b">
+        <v>1</v>
+      </c>
+      <c r="J37" t="s">
+        <v>5347</v>
+      </c>
+      <c r="K37" t="s">
+        <v>5347</v>
+      </c>
+      <c r="L37">
         <v>254</v>
       </c>
-      <c r="M37" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="N37" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="O37" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="Q37" s="42" t="s">
+      <c r="M37" t="s">
+        <v>5029</v>
+      </c>
+      <c r="N37" t="s">
+        <v>5029</v>
+      </c>
+      <c r="O37" t="s">
+        <v>5029</v>
+      </c>
+      <c r="P37" t="s">
         <v>963</v>
       </c>
-      <c r="S37" s="41"/>
-    </row>
-    <row r="38" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="40">
+      <c r="Q37" t="s">
+        <v>963</v>
+      </c>
+      <c r="R37" t="s">
+        <v>963</v>
+      </c>
+      <c r="S37" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" s="40" t="s">
+      <c r="B38" t="s">
         <v>472</v>
       </c>
-      <c r="C38" s="40" t="s">
+      <c r="C38" t="s">
         <v>473</v>
       </c>
-      <c r="D38" s="40">
+      <c r="D38">
         <v>1998</v>
       </c>
-      <c r="E38" s="40" t="s">
+      <c r="E38" t="s">
         <v>5288</v>
       </c>
-      <c r="F38" s="40" t="s">
+      <c r="F38" t="s">
         <v>5289</v>
       </c>
-      <c r="G38" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="H38" s="40" t="s">
+      <c r="G38" t="s">
+        <v>5029</v>
+      </c>
+      <c r="H38" t="s">
         <v>19</v>
       </c>
-      <c r="I38" s="40" t="b">
-        <v>1</v>
-      </c>
-      <c r="J38" s="40" t="s">
-        <v>5349</v>
-      </c>
-      <c r="K38" s="40" t="s">
-        <v>5349</v>
-      </c>
-      <c r="L38" s="40">
+      <c r="I38" t="b">
+        <v>1</v>
+      </c>
+      <c r="J38" t="s">
+        <v>5347</v>
+      </c>
+      <c r="K38" t="s">
+        <v>5347</v>
+      </c>
+      <c r="L38">
         <v>301</v>
       </c>
-      <c r="M38" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="N38" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="O38" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="Q38" s="42" t="s">
+      <c r="M38" t="s">
+        <v>5029</v>
+      </c>
+      <c r="N38" t="s">
+        <v>5029</v>
+      </c>
+      <c r="O38" t="s">
+        <v>5029</v>
+      </c>
+      <c r="P38" t="s">
         <v>963</v>
       </c>
-      <c r="S38" s="41"/>
-    </row>
-    <row r="39" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="40">
+      <c r="Q38" t="s">
+        <v>963</v>
+      </c>
+      <c r="R38" t="s">
+        <v>963</v>
+      </c>
+      <c r="S38" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" s="40" t="s">
+      <c r="B39" t="s">
         <v>475</v>
       </c>
-      <c r="C39" s="40" t="s">
+      <c r="C39" t="s">
         <v>476</v>
       </c>
-      <c r="D39" s="40">
+      <c r="D39">
         <v>2001</v>
       </c>
-      <c r="E39" s="40" t="s">
+      <c r="E39" t="s">
         <v>5290</v>
       </c>
-      <c r="F39" s="40" t="s">
+      <c r="F39" t="s">
         <v>5291</v>
       </c>
-      <c r="G39" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="H39" s="40" t="s">
-        <v>5361</v>
-      </c>
-      <c r="I39" s="40" t="b">
-        <v>1</v>
-      </c>
-      <c r="J39" s="40" t="s">
-        <v>5349</v>
-      </c>
-      <c r="K39" s="40" t="s">
-        <v>5349</v>
-      </c>
-      <c r="L39" s="40">
+      <c r="G39" t="s">
+        <v>5029</v>
+      </c>
+      <c r="H39" t="s">
+        <v>5359</v>
+      </c>
+      <c r="I39" t="b">
+        <v>1</v>
+      </c>
+      <c r="J39" t="s">
+        <v>5347</v>
+      </c>
+      <c r="K39" t="s">
+        <v>5347</v>
+      </c>
+      <c r="L39">
         <v>293</v>
       </c>
-      <c r="M39" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="N39" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="O39" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="Q39" s="42" t="s">
+      <c r="M39" t="s">
+        <v>5029</v>
+      </c>
+      <c r="N39" t="s">
+        <v>5029</v>
+      </c>
+      <c r="O39" t="s">
+        <v>5029</v>
+      </c>
+      <c r="P39" t="s">
+        <v>5373</v>
+      </c>
+      <c r="Q39" t="s">
         <v>963</v>
       </c>
-      <c r="S39" s="41"/>
-    </row>
-    <row r="40" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="40">
+      <c r="R39" t="s">
+        <v>966</v>
+      </c>
+      <c r="S39" s="7" t="s">
+        <v>5029</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40" s="40" t="s">
+      <c r="B40" t="s">
         <v>3923</v>
       </c>
-      <c r="C40" s="40" t="s">
+      <c r="C40" t="s">
         <v>3924</v>
       </c>
-      <c r="D40" s="40">
+      <c r="D40">
         <v>2008</v>
       </c>
-      <c r="E40" s="40" t="s">
+      <c r="E40" t="s">
         <v>5292</v>
       </c>
-      <c r="F40" s="40" t="s">
+      <c r="F40" t="s">
         <v>5293</v>
       </c>
-      <c r="G40" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="H40" s="40" t="s">
-        <v>5359</v>
-      </c>
-      <c r="I40" s="40" t="b">
-        <v>1</v>
-      </c>
-      <c r="J40" s="40" t="s">
-        <v>5349</v>
-      </c>
-      <c r="K40" s="40" t="s">
-        <v>5349</v>
-      </c>
-      <c r="L40" s="40">
+      <c r="G40" t="s">
+        <v>5029</v>
+      </c>
+      <c r="H40" t="s">
+        <v>5357</v>
+      </c>
+      <c r="I40" t="b">
+        <v>1</v>
+      </c>
+      <c r="J40" t="s">
+        <v>5347</v>
+      </c>
+      <c r="K40" t="s">
+        <v>5347</v>
+      </c>
+      <c r="L40">
         <v>153</v>
       </c>
-      <c r="M40" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="N40" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="O40" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="Q40" s="42" t="s">
+      <c r="M40" t="s">
+        <v>5029</v>
+      </c>
+      <c r="N40" t="s">
+        <v>5029</v>
+      </c>
+      <c r="O40" t="s">
+        <v>5029</v>
+      </c>
+      <c r="P40" t="s">
         <v>963</v>
       </c>
-      <c r="S40" s="41"/>
-    </row>
-    <row r="41" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="40">
+      <c r="Q40" t="s">
+        <v>963</v>
+      </c>
+      <c r="R40" t="s">
+        <v>963</v>
+      </c>
+      <c r="S40" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A41">
         <v>40</v>
       </c>
-      <c r="B41" s="40" t="s">
+      <c r="B41" t="s">
         <v>5294</v>
       </c>
-      <c r="C41" s="40" t="s">
+      <c r="C41" t="s">
         <v>5295</v>
       </c>
-      <c r="D41" s="40">
+      <c r="D41">
         <v>2001</v>
       </c>
-      <c r="E41" s="40" t="s">
+      <c r="E41" t="s">
         <v>5296</v>
       </c>
-      <c r="F41" s="40" t="s">
+      <c r="F41" t="s">
         <v>5297</v>
       </c>
-      <c r="G41" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="H41" s="40" t="s">
+      <c r="G41" t="s">
+        <v>5029</v>
+      </c>
+      <c r="H41" t="s">
         <v>42</v>
       </c>
-      <c r="I41" s="40" t="b">
-        <v>1</v>
-      </c>
-      <c r="J41" s="40" t="s">
-        <v>5349</v>
-      </c>
-      <c r="K41" s="40" t="s">
-        <v>5349</v>
-      </c>
-      <c r="L41" s="40">
+      <c r="I41" t="b">
+        <v>1</v>
+      </c>
+      <c r="J41" t="s">
+        <v>5347</v>
+      </c>
+      <c r="K41" t="s">
+        <v>5347</v>
+      </c>
+      <c r="L41">
         <v>188</v>
       </c>
-      <c r="M41" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="N41" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="O41" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="Q41" s="42" t="s">
+      <c r="M41" t="s">
+        <v>5029</v>
+      </c>
+      <c r="N41" t="s">
+        <v>5029</v>
+      </c>
+      <c r="O41" t="s">
+        <v>5029</v>
+      </c>
+      <c r="P41" t="s">
         <v>963</v>
       </c>
-      <c r="S41" s="41"/>
-    </row>
-    <row r="42" spans="1:19" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="40">
+      <c r="Q41" t="s">
+        <v>963</v>
+      </c>
+      <c r="R41" t="s">
+        <v>963</v>
+      </c>
+      <c r="S41" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A42">
         <v>41</v>
       </c>
-      <c r="B42" s="40" t="s">
+      <c r="B42" t="s">
         <v>5298</v>
       </c>
-      <c r="C42" s="40" t="s">
+      <c r="C42" t="s">
         <v>5299</v>
       </c>
-      <c r="D42" s="40">
+      <c r="D42">
         <v>2004</v>
       </c>
-      <c r="E42" s="40" t="s">
+      <c r="E42" t="s">
         <v>5300</v>
       </c>
-      <c r="F42" s="40" t="s">
+      <c r="F42" t="s">
         <v>5301</v>
       </c>
-      <c r="G42" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="H42" s="40" t="s">
-        <v>5354</v>
-      </c>
-      <c r="I42" s="40" t="b">
-        <v>1</v>
-      </c>
-      <c r="J42" s="40" t="s">
-        <v>5349</v>
-      </c>
-      <c r="K42" s="40" t="s">
-        <v>5349</v>
-      </c>
-      <c r="L42" s="40">
+      <c r="G42" t="s">
+        <v>5029</v>
+      </c>
+      <c r="H42" t="s">
+        <v>5352</v>
+      </c>
+      <c r="I42" t="b">
+        <v>1</v>
+      </c>
+      <c r="J42" t="s">
+        <v>5347</v>
+      </c>
+      <c r="K42" t="s">
+        <v>5347</v>
+      </c>
+      <c r="L42">
         <v>93</v>
       </c>
-      <c r="M42" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="N42" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="O42" s="40" t="s">
-        <v>5029</v>
-      </c>
-      <c r="Q42" s="42" t="s">
+      <c r="M42" t="s">
+        <v>5029</v>
+      </c>
+      <c r="N42" t="s">
+        <v>5029</v>
+      </c>
+      <c r="O42" t="s">
+        <v>5029</v>
+      </c>
+      <c r="P42" t="s">
         <v>963</v>
       </c>
-      <c r="S42" s="41"/>
+      <c r="Q42" t="s">
+        <v>963</v>
+      </c>
+      <c r="R42" t="s">
+        <v>963</v>
+      </c>
+      <c r="S42" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>5302</v>
+        <v>5073</v>
       </c>
       <c r="C43" t="s">
-        <v>5303</v>
+        <v>4128</v>
       </c>
       <c r="D43">
         <v>1995</v>
       </c>
       <c r="E43" t="s">
-        <v>5304</v>
+        <v>5302</v>
       </c>
       <c r="F43" t="s">
-        <v>5305</v>
+        <v>5303</v>
       </c>
       <c r="G43" t="s">
         <v>5029</v>
       </c>
       <c r="H43" t="s">
-        <v>5362</v>
+        <v>5360</v>
       </c>
       <c r="I43" t="b">
         <v>1</v>
       </c>
       <c r="J43" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K43" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L43">
         <v>372</v>
@@ -46822,29 +47233,37 @@
       <c r="O43" t="s">
         <v>5029</v>
       </c>
-      <c r="Q43" s="42" t="s">
+      <c r="P43" t="s">
+        <v>5371</v>
+      </c>
+      <c r="Q43" t="s">
         <v>963</v>
       </c>
-      <c r="S43" s="7"/>
+      <c r="R43" t="s">
+        <v>966</v>
+      </c>
+      <c r="S43" s="7" t="s">
+        <v>5029</v>
+      </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>5306</v>
+        <v>5304</v>
       </c>
       <c r="C44" t="s">
-        <v>5307</v>
+        <v>5305</v>
       </c>
       <c r="D44">
         <v>2004</v>
       </c>
       <c r="E44" t="s">
-        <v>5308</v>
+        <v>5306</v>
       </c>
       <c r="F44" t="s">
-        <v>5309</v>
+        <v>5307</v>
       </c>
       <c r="G44" t="s">
         <v>5029</v>
@@ -46856,10 +47275,10 @@
         <v>1</v>
       </c>
       <c r="J44" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K44" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L44">
         <v>1830</v>
@@ -46873,29 +47292,37 @@
       <c r="O44" t="s">
         <v>5029</v>
       </c>
-      <c r="Q44" s="42" t="s">
+      <c r="P44" t="s">
         <v>963</v>
       </c>
-      <c r="S44" s="7"/>
+      <c r="Q44" t="s">
+        <v>963</v>
+      </c>
+      <c r="R44" t="s">
+        <v>963</v>
+      </c>
+      <c r="S44" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>5310</v>
+        <v>5308</v>
       </c>
       <c r="C45" t="s">
-        <v>5311</v>
+        <v>5309</v>
       </c>
       <c r="D45">
         <v>2005</v>
       </c>
       <c r="E45" t="s">
-        <v>5312</v>
+        <v>5310</v>
       </c>
       <c r="F45" t="s">
-        <v>5313</v>
+        <v>5311</v>
       </c>
       <c r="G45" t="s">
         <v>5029</v>
@@ -46907,10 +47334,10 @@
         <v>1</v>
       </c>
       <c r="J45" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K45" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L45">
         <v>345</v>
@@ -46924,44 +47351,52 @@
       <c r="O45" t="s">
         <v>5029</v>
       </c>
-      <c r="Q45" s="42" t="s">
+      <c r="P45" t="s">
         <v>963</v>
       </c>
-      <c r="S45" s="7"/>
+      <c r="Q45" t="s">
+        <v>963</v>
+      </c>
+      <c r="R45" t="s">
+        <v>963</v>
+      </c>
+      <c r="S45" s="7">
+        <v>3</v>
+      </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>5314</v>
+        <v>5312</v>
       </c>
       <c r="C46" t="s">
-        <v>5315</v>
+        <v>5313</v>
       </c>
       <c r="D46">
         <v>2006</v>
       </c>
       <c r="E46" t="s">
-        <v>5316</v>
+        <v>5314</v>
       </c>
       <c r="F46" t="s">
-        <v>5317</v>
+        <v>5315</v>
       </c>
       <c r="G46" t="s">
         <v>5029</v>
       </c>
       <c r="H46" t="s">
-        <v>5363</v>
+        <v>5361</v>
       </c>
       <c r="I46" t="b">
         <v>1</v>
       </c>
       <c r="J46" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K46" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L46">
         <v>1005</v>
@@ -46975,29 +47410,37 @@
       <c r="O46" t="s">
         <v>5029</v>
       </c>
-      <c r="Q46" s="42" t="s">
+      <c r="P46" t="s">
+        <v>5363</v>
+      </c>
+      <c r="Q46" t="s">
         <v>963</v>
       </c>
-      <c r="S46" s="7"/>
+      <c r="R46" t="s">
+        <v>966</v>
+      </c>
+      <c r="S46" s="7" t="s">
+        <v>5029</v>
+      </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>5318</v>
+        <v>5316</v>
       </c>
       <c r="C47" t="s">
-        <v>5319</v>
+        <v>5317</v>
       </c>
       <c r="D47">
         <v>2006</v>
       </c>
       <c r="E47" t="s">
-        <v>5320</v>
+        <v>5318</v>
       </c>
       <c r="F47" t="s">
-        <v>5321</v>
+        <v>5319</v>
       </c>
       <c r="G47" t="s">
         <v>5029</v>
@@ -47009,10 +47452,10 @@
         <v>1</v>
       </c>
       <c r="J47" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K47" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L47">
         <v>596</v>
@@ -47026,26 +47469,34 @@
       <c r="O47" t="s">
         <v>5029</v>
       </c>
-      <c r="Q47" s="42" t="s">
+      <c r="P47" t="s">
+        <v>5363</v>
+      </c>
+      <c r="Q47" t="s">
         <v>963</v>
       </c>
-      <c r="S47" s="7"/>
+      <c r="R47" t="s">
+        <v>966</v>
+      </c>
+      <c r="S47" s="7" t="s">
+        <v>5029</v>
+      </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>5322</v>
+        <v>5320</v>
       </c>
       <c r="C48" t="s">
-        <v>5323</v>
+        <v>5321</v>
       </c>
       <c r="D48">
         <v>2005</v>
       </c>
       <c r="E48" t="s">
-        <v>5324</v>
+        <v>5322</v>
       </c>
       <c r="F48" t="s">
         <v>5164</v>
@@ -47060,10 +47511,10 @@
         <v>1</v>
       </c>
       <c r="J48" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K48" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L48">
         <v>386</v>
@@ -47077,10 +47528,18 @@
       <c r="O48" t="s">
         <v>5029</v>
       </c>
-      <c r="Q48" s="42" t="s">
+      <c r="P48" t="s">
         <v>963</v>
       </c>
-      <c r="S48" s="7"/>
+      <c r="Q48" t="s">
+        <v>963</v>
+      </c>
+      <c r="R48" t="s">
+        <v>963</v>
+      </c>
+      <c r="S48" s="7">
+        <v>3</v>
+      </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49">
@@ -47096,7 +47555,7 @@
         <v>1982</v>
       </c>
       <c r="E49" t="s">
-        <v>5325</v>
+        <v>5323</v>
       </c>
       <c r="F49" t="s">
         <v>5165</v>
@@ -47105,16 +47564,16 @@
         <v>5029</v>
       </c>
       <c r="H49" t="s">
-        <v>5362</v>
+        <v>5360</v>
       </c>
       <c r="I49" t="b">
         <v>1</v>
       </c>
       <c r="J49" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K49" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L49">
         <v>55</v>
@@ -47128,10 +47587,18 @@
       <c r="O49" t="s">
         <v>5029</v>
       </c>
-      <c r="Q49" s="42" t="s">
+      <c r="P49" t="s">
         <v>963</v>
       </c>
-      <c r="S49" s="7"/>
+      <c r="Q49" t="s">
+        <v>963</v>
+      </c>
+      <c r="R49" t="s">
+        <v>963</v>
+      </c>
+      <c r="S49" s="7">
+        <v>4</v>
+      </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50">
@@ -47147,7 +47614,7 @@
         <v>1985</v>
       </c>
       <c r="E50" t="s">
-        <v>5326</v>
+        <v>5324</v>
       </c>
       <c r="F50" t="s">
         <v>5166</v>
@@ -47162,10 +47629,10 @@
         <v>1</v>
       </c>
       <c r="J50" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K50" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L50">
         <v>2143</v>
@@ -47179,17 +47646,25 @@
       <c r="O50" t="s">
         <v>5029</v>
       </c>
-      <c r="Q50" s="42" t="s">
+      <c r="P50" t="s">
+        <v>974</v>
+      </c>
+      <c r="Q50" t="s">
         <v>963</v>
       </c>
-      <c r="S50" s="7"/>
+      <c r="R50" t="s">
+        <v>966</v>
+      </c>
+      <c r="S50" s="7" t="s">
+        <v>5029</v>
+      </c>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>5327</v>
+        <v>5325</v>
       </c>
       <c r="C51" t="s">
         <v>674</v>
@@ -47198,7 +47673,7 @@
         <v>1979</v>
       </c>
       <c r="E51" t="s">
-        <v>5328</v>
+        <v>5326</v>
       </c>
       <c r="F51" t="s">
         <v>5167</v>
@@ -47213,10 +47688,10 @@
         <v>1</v>
       </c>
       <c r="J51" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K51" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L51">
         <v>251</v>
@@ -47230,29 +47705,37 @@
       <c r="O51" t="s">
         <v>5029</v>
       </c>
-      <c r="Q51" s="42" t="s">
+      <c r="P51" t="s">
         <v>963</v>
       </c>
-      <c r="S51" s="7"/>
+      <c r="Q51" t="s">
+        <v>963</v>
+      </c>
+      <c r="R51" t="s">
+        <v>963</v>
+      </c>
+      <c r="S51" s="7">
+        <v>3</v>
+      </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>5329</v>
+        <v>5327</v>
       </c>
       <c r="C52" t="s">
-        <v>5330</v>
+        <v>5328</v>
       </c>
       <c r="D52">
         <v>1997</v>
       </c>
       <c r="E52" t="s">
-        <v>5331</v>
+        <v>5329</v>
       </c>
       <c r="F52" t="s">
-        <v>5332</v>
+        <v>5330</v>
       </c>
       <c r="G52" t="s">
         <v>5029</v>
@@ -47264,10 +47747,10 @@
         <v>1</v>
       </c>
       <c r="J52" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K52" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L52">
         <v>9699</v>
@@ -47281,44 +47764,52 @@
       <c r="O52" t="s">
         <v>5029</v>
       </c>
-      <c r="Q52" s="42" t="s">
+      <c r="P52" t="s">
         <v>963</v>
       </c>
-      <c r="S52" s="7"/>
+      <c r="Q52" t="s">
+        <v>963</v>
+      </c>
+      <c r="R52" t="s">
+        <v>963</v>
+      </c>
+      <c r="S52" s="7">
+        <v>4</v>
+      </c>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>5333</v>
+        <v>5331</v>
       </c>
       <c r="C53" t="s">
-        <v>5334</v>
+        <v>5332</v>
       </c>
       <c r="D53">
         <v>2014</v>
       </c>
       <c r="E53" t="s">
-        <v>5335</v>
+        <v>5333</v>
       </c>
       <c r="F53" t="s">
-        <v>5336</v>
+        <v>5334</v>
       </c>
       <c r="G53" t="s">
         <v>5029</v>
       </c>
       <c r="H53" t="s">
-        <v>5352</v>
+        <v>5350</v>
       </c>
       <c r="I53" t="b">
         <v>1</v>
       </c>
       <c r="J53" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K53" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L53">
         <v>264</v>
@@ -47332,29 +47823,37 @@
       <c r="O53" t="s">
         <v>5029</v>
       </c>
-      <c r="Q53" s="42" t="s">
+      <c r="P53" t="s">
         <v>963</v>
       </c>
-      <c r="S53" s="7"/>
+      <c r="Q53" t="s">
+        <v>963</v>
+      </c>
+      <c r="R53" t="s">
+        <v>963</v>
+      </c>
+      <c r="S53" s="7">
+        <v>4</v>
+      </c>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>5337</v>
+        <v>5335</v>
       </c>
       <c r="C54" t="s">
-        <v>5338</v>
+        <v>5336</v>
       </c>
       <c r="D54">
         <v>2001</v>
       </c>
       <c r="E54" t="s">
-        <v>5339</v>
+        <v>5337</v>
       </c>
       <c r="F54" t="s">
-        <v>5340</v>
+        <v>5338</v>
       </c>
       <c r="G54" t="s">
         <v>5029</v>
@@ -47366,10 +47865,10 @@
         <v>1</v>
       </c>
       <c r="J54" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K54" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L54">
         <v>261</v>
@@ -47383,29 +47882,37 @@
       <c r="O54" t="s">
         <v>5029</v>
       </c>
-      <c r="Q54" s="42" t="s">
+      <c r="P54" t="s">
         <v>963</v>
       </c>
-      <c r="S54" s="7"/>
+      <c r="Q54" t="s">
+        <v>963</v>
+      </c>
+      <c r="R54" t="s">
+        <v>963</v>
+      </c>
+      <c r="S54" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>5341</v>
+        <v>5339</v>
       </c>
       <c r="C55" t="s">
-        <v>5342</v>
+        <v>5340</v>
       </c>
       <c r="D55">
         <v>1999</v>
       </c>
       <c r="E55" t="s">
-        <v>5343</v>
+        <v>5341</v>
       </c>
       <c r="F55" t="s">
-        <v>5344</v>
+        <v>5342</v>
       </c>
       <c r="G55" t="s">
         <v>5029</v>
@@ -47417,10 +47924,10 @@
         <v>1</v>
       </c>
       <c r="J55" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K55" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L55">
         <v>423</v>
@@ -47434,29 +47941,37 @@
       <c r="O55" t="s">
         <v>5029</v>
       </c>
-      <c r="Q55" s="42" t="s">
+      <c r="P55" t="s">
         <v>963</v>
       </c>
-      <c r="S55" s="7"/>
+      <c r="Q55" t="s">
+        <v>963</v>
+      </c>
+      <c r="R55" t="s">
+        <v>963</v>
+      </c>
+      <c r="S55" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>5345</v>
+        <v>5343</v>
       </c>
       <c r="C56" t="s">
-        <v>5346</v>
+        <v>5344</v>
       </c>
       <c r="D56">
         <v>2011</v>
       </c>
       <c r="E56" t="s">
-        <v>5347</v>
+        <v>5345</v>
       </c>
       <c r="F56" t="s">
-        <v>5348</v>
+        <v>5346</v>
       </c>
       <c r="G56" t="s">
         <v>5029</v>
@@ -47468,10 +47983,10 @@
         <v>1</v>
       </c>
       <c r="J56" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="K56" t="s">
-        <v>5349</v>
+        <v>5347</v>
       </c>
       <c r="L56">
         <v>197</v>
@@ -47485,10 +48000,18 @@
       <c r="O56" t="s">
         <v>5029</v>
       </c>
-      <c r="Q56" s="42" t="s">
+      <c r="P56" t="s">
+        <v>966</v>
+      </c>
+      <c r="Q56" t="s">
         <v>963</v>
       </c>
-      <c r="S56" s="7"/>
+      <c r="R56" t="s">
+        <v>966</v>
+      </c>
+      <c r="S56" s="7" t="s">
+        <v>5029</v>
+      </c>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="S57" s="7"/>
@@ -47923,8 +48446,8 @@
     <row r="200" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S200" s="7"/>
     </row>
-    <row r="201" spans="19:19" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="S201" s="37"/>
+    <row r="201" spans="19:19" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S201" s="36"/>
     </row>
     <row r="202" spans="19:19" x14ac:dyDescent="0.25">
       <c r="S202" s="7"/>
@@ -49050,43 +49573,41 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B38 B40:B1048576">
-    <cfRule type="duplicateValues" dxfId="34" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsBlanks" dxfId="33" priority="13">
+    <cfRule type="containsBlanks" dxfId="35" priority="13">
       <formula>LEN(TRIM(F1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:R601">
-    <cfRule type="containsText" dxfId="32" priority="8" operator="containsText" text="PRIMARY STUDY">
+    <cfRule type="containsText" dxfId="34" priority="8" operator="containsText" text="PRIMARY STUDY">
       <formula>NOT(ISERROR(SEARCH("PRIMARY STUDY",P2)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="31" priority="9" operator="notContains" text="YES">
+    <cfRule type="notContainsText" dxfId="33" priority="9" operator="notContains" text="YES">
       <formula>ISERROR(SEARCH("YES",P2))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="10" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="32" priority="10" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",P2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S601">
+    <cfRule type="cellIs" dxfId="31" priority="6" operator="between">
+      <formula>1</formula>
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="7" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",S2)))</formula>
+    </cfRule>
     <cfRule type="containsBlanks" dxfId="29" priority="15">
       <formula>LEN(TRIM(S2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S2:S601">
-    <cfRule type="cellIs" dxfId="28" priority="6" operator="between">
-      <formula>1</formula>
-      <formula>4</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="7" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH("X",S2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="U1:U2">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="X1">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
@@ -49095,12 +49616,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:Z18"/>
+  <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="V1" sqref="V1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49165,14 +49686,14 @@
       </c>
       <c r="S1" s="29">
         <f>COUNTIFS($N:$N, "YES", $F:$F, "&lt;&gt;")</f>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="U1" s="28" t="s">
         <v>5039</v>
       </c>
       <c r="V1" s="29">
         <f>COUNTIF($M$2:$M$573, "YES")</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="W1" s="31"/>
       <c r="X1" s="31"/>
@@ -49225,7 +49746,7 @@
       <c r="O2" t="s">
         <v>966</v>
       </c>
-      <c r="P2" s="35">
+      <c r="P2" s="40">
         <v>1</v>
       </c>
       <c r="S2" t="s">
@@ -49281,7 +49802,7 @@
       <c r="O3" t="s">
         <v>966</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="7">
         <v>1</v>
       </c>
       <c r="X3" t="s">
@@ -49334,7 +49855,7 @@
       <c r="O4" t="s">
         <v>966</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="7">
         <v>1</v>
       </c>
       <c r="Q4" t="s">
@@ -49390,7 +49911,7 @@
       <c r="O5" t="s">
         <v>966</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="7">
         <v>1</v>
       </c>
     </row>
@@ -49440,7 +49961,7 @@
       <c r="O6" t="s">
         <v>966</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="7">
         <v>1</v>
       </c>
       <c r="R6" s="2" t="s">
@@ -49448,7 +49969,7 @@
       </c>
       <c r="S6">
         <f>COUNTIFS($N:$N, "YES", $M:$M, "&lt;&gt;PRIMARY STUDY")</f>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="X6" t="s">
         <v>5076</v>
@@ -49500,7 +50021,7 @@
       <c r="O7" t="s">
         <v>966</v>
       </c>
-      <c r="P7">
+      <c r="P7" s="7">
         <v>1</v>
       </c>
       <c r="R7" s="2" t="s">
@@ -49557,7 +50078,7 @@
       <c r="O8" t="s">
         <v>966</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="7">
         <v>1</v>
       </c>
     </row>
@@ -49604,7 +50125,7 @@
       <c r="O9" t="s">
         <v>966</v>
       </c>
-      <c r="P9">
+      <c r="P9" s="7">
         <v>1</v>
       </c>
     </row>
@@ -49654,7 +50175,7 @@
       <c r="O10" t="s">
         <v>966</v>
       </c>
-      <c r="P10">
+      <c r="P10" s="7">
         <v>1</v>
       </c>
     </row>
@@ -49701,7 +50222,7 @@
       <c r="O11" t="s">
         <v>966</v>
       </c>
-      <c r="P11">
+      <c r="P11" s="7">
         <v>1</v>
       </c>
     </row>
@@ -49751,7 +50272,7 @@
       <c r="O12" t="s">
         <v>966</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="7">
         <v>1</v>
       </c>
     </row>
@@ -49801,7 +50322,7 @@
       <c r="O13" t="s">
         <v>966</v>
       </c>
-      <c r="P13" t="s">
+      <c r="P13" s="7" t="s">
         <v>5121</v>
       </c>
     </row>
@@ -49851,7 +50372,7 @@
       <c r="O14" t="s">
         <v>966</v>
       </c>
-      <c r="P14">
+      <c r="P14" s="7">
         <v>1</v>
       </c>
     </row>
@@ -49901,7 +50422,7 @@
       <c r="O15" t="s">
         <v>966</v>
       </c>
-      <c r="P15">
+      <c r="P15" s="7">
         <v>1</v>
       </c>
     </row>
@@ -49951,7 +50472,7 @@
       <c r="O16" t="s">
         <v>966</v>
       </c>
-      <c r="P16">
+      <c r="P16" s="7">
         <v>1</v>
       </c>
       <c r="Q16" t="s">
@@ -50004,7 +50525,7 @@
       <c r="O17" t="s">
         <v>966</v>
       </c>
-      <c r="P17">
+      <c r="P17" s="7">
         <v>1</v>
       </c>
       <c r="Q17" t="s">
@@ -50064,82 +50585,194 @@
         <v>5146</v>
       </c>
     </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>399</v>
+      </c>
+      <c r="C19" t="s">
+        <v>400</v>
+      </c>
+      <c r="D19">
+        <v>1999</v>
+      </c>
+      <c r="E19" t="s">
+        <v>5278</v>
+      </c>
+      <c r="F19" t="s">
+        <v>5279</v>
+      </c>
+      <c r="G19" t="s">
+        <v>5029</v>
+      </c>
+      <c r="H19">
+        <v>177</v>
+      </c>
+      <c r="I19" t="s">
+        <v>5029</v>
+      </c>
+      <c r="J19" t="s">
+        <v>5029</v>
+      </c>
+      <c r="K19" t="s">
+        <v>5029</v>
+      </c>
+      <c r="L19" t="s">
+        <v>399</v>
+      </c>
+      <c r="M19" t="s">
+        <v>963</v>
+      </c>
+      <c r="N19" t="s">
+        <v>963</v>
+      </c>
+      <c r="O19" t="s">
+        <v>966</v>
+      </c>
+      <c r="P19" s="7" t="s">
+        <v>5029</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>5372</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5073</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4128</v>
+      </c>
+      <c r="D20">
+        <v>1995</v>
+      </c>
+      <c r="E20" t="s">
+        <v>5302</v>
+      </c>
+      <c r="F20" t="s">
+        <v>5303</v>
+      </c>
+      <c r="G20" t="s">
+        <v>5029</v>
+      </c>
+      <c r="H20">
+        <v>372</v>
+      </c>
+      <c r="I20" t="s">
+        <v>5029</v>
+      </c>
+      <c r="J20" t="s">
+        <v>5029</v>
+      </c>
+      <c r="K20" t="s">
+        <v>5029</v>
+      </c>
+      <c r="L20" t="s">
+        <v>5073</v>
+      </c>
+      <c r="M20" t="s">
+        <v>5371</v>
+      </c>
+      <c r="N20" t="s">
+        <v>963</v>
+      </c>
+      <c r="O20" t="s">
+        <v>966</v>
+      </c>
+      <c r="P20" s="7" t="s">
+        <v>5029</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>5372</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B2">
-    <cfRule type="duplicateValues" dxfId="26" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="25" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="20"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19">
+    <cfRule type="duplicateValues" dxfId="24" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F2">
-    <cfRule type="containsBlanks" dxfId="24" priority="22">
+    <cfRule type="containsBlanks" dxfId="23" priority="37">
       <formula>LEN(TRIM(F1))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F18">
-    <cfRule type="containsBlanks" dxfId="23" priority="11">
+  <conditionalFormatting sqref="F18:F19">
+    <cfRule type="containsBlanks" dxfId="22" priority="15">
       <formula>LEN(TRIM(F18))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H17 H19:H1048576">
-    <cfRule type="containsBlanks" dxfId="22" priority="23">
+  <conditionalFormatting sqref="H1:H17 H20:H1048576">
+    <cfRule type="containsBlanks" dxfId="21" priority="38">
       <formula>LEN(TRIM(H1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2">
-    <cfRule type="duplicateValues" dxfId="21" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L18">
-    <cfRule type="duplicateValues" dxfId="20" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="16"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:O18">
-    <cfRule type="containsText" dxfId="19" priority="8" operator="containsText" text="PRIMARY STUDY">
+  <conditionalFormatting sqref="L19">
+    <cfRule type="duplicateValues" dxfId="18" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2:O20">
+    <cfRule type="containsText" dxfId="17" priority="2" operator="containsText" text="PRIMARY STUDY">
       <formula>NOT(ISERROR(SEARCH("PRIMARY STUDY",M2)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="18" priority="9" operator="notContains" text="YES">
+    <cfRule type="notContainsText" dxfId="16" priority="3" operator="notContains" text="YES">
       <formula>ISERROR(SEARCH("YES",M2))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="10" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="15" priority="4" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",M2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O18">
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="between">
+  <conditionalFormatting sqref="O18:O20">
+    <cfRule type="cellIs" dxfId="14" priority="10" operator="between">
       <formula>1</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="7" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",O18)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O18:P18">
-    <cfRule type="containsBlanks" dxfId="14" priority="4">
+  <conditionalFormatting sqref="O18:P20">
+    <cfRule type="containsBlanks" dxfId="12" priority="1">
       <formula>LEN(TRIM(O18))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1:P1048576">
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="between">
       <formula>1</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="3" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="10" priority="7" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",P1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1 Q4">
-    <cfRule type="cellIs" dxfId="11" priority="17" operator="between">
+    <cfRule type="cellIs" dxfId="9" priority="32" operator="between">
       <formula>1</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="18" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="8" priority="33" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",Q1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:R2">
-    <cfRule type="duplicateValues" dxfId="9" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1">
-    <cfRule type="duplicateValues" dxfId="8" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="29"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
@@ -50148,7 +50781,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:L251"/>
   <sheetViews>
@@ -59032,10 +59665,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L1 A1:K251">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>$K1=FALSE</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="9">
+    <cfRule type="expression" dxfId="4" priority="9">
       <formula>$J1=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -59046,7 +59679,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:M293"/>
   <sheetViews>
@@ -66980,10 +67613,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J1:J253 J257 J259:J1048576">
-    <cfRule type="containsText" dxfId="5" priority="12" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="3" priority="12" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="13" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="2" priority="13" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -67000,10 +67633,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M17">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",M17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",M17)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -67012,7 +67645,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Modified funnel plot precision measure. Now defaults to sqrt(DoF)
</commit_message>
<xml_diff>
--- a/Literature/Literature.xlsx
+++ b/Literature/Literature.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hso20\OneDrive\Plocha\IES\Diploma-Thesis\Literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2E02EF-29CA-4747-863E-88FD6C53DEBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A047345-A63F-45C6-88AA-BD32C313A873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Query literature" sheetId="5" r:id="rId1"/>
@@ -17910,9 +17910,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Y575"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A200" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44631,9 +44631,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC575"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Modified the proposal, added twin studies sheet into main data frame
</commit_message>
<xml_diff>
--- a/Literature/Literature.xlsx
+++ b/Literature/Literature.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hso20\OneDrive\Plocha\IES\Diploma-Thesis\Literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A047345-A63F-45C6-88AA-BD32C313A873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF931D5-9DDF-418B-B7C1-2267838073B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Query literature" sheetId="5" r:id="rId1"/>
@@ -694,7 +694,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10275" uniqueCount="5374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10262" uniqueCount="5375">
   <si>
     <t>Number</t>
   </si>
@@ -16816,6 +16816,9 @@
   </si>
   <si>
     <t>REPLICATION OF CARD(1995)</t>
+  </si>
+  <si>
+    <t>Already identified during twins snowballing</t>
   </si>
 </sst>
 </file>
@@ -17208,7 +17211,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="51">
+  <dxfs count="49">
     <dxf>
       <fill>
         <patternFill>
@@ -17270,20 +17273,6 @@
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAACAC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -17910,8 +17899,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Y575"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A200" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -17988,7 +17977,7 @@
       </c>
       <c r="R1" s="29">
         <f>COUNTIFS($M:$M, "YES", $F:$F, "&lt;&gt;") + Twins!S1</f>
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="T1" s="28" t="s">
         <v>5039</v>
@@ -44562,59 +44551,59 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B38 B40:B1048576">
-    <cfRule type="duplicateValues" dxfId="50" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="48" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsBlanks" dxfId="49" priority="20">
+    <cfRule type="containsBlanks" dxfId="47" priority="20">
       <formula>LEN(TRIM(F1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:N601">
-    <cfRule type="containsText" dxfId="48" priority="11" operator="containsText" text="PRIMARY STUDY">
+    <cfRule type="containsText" dxfId="46" priority="11" operator="containsText" text="PRIMARY STUDY">
       <formula>NOT(ISERROR(SEARCH("PRIMARY STUDY",L2)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="47" priority="12" operator="notContains" text="YES">
+    <cfRule type="notContainsText" dxfId="45" priority="12" operator="notContains" text="YES">
       <formula>ISERROR(SEARCH("YES",L2))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="13" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="44" priority="13" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",L2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O2:O601 P136 P146 P151 P161 P163 P177 P187 P189:P190">
-    <cfRule type="containsBlanks" dxfId="45" priority="22">
+  <conditionalFormatting sqref="O2:O601 P177 P187 P189:P190 P136 P146 P151 P161 P163">
+    <cfRule type="containsBlanks" dxfId="43" priority="22">
       <formula>LEN(TRIM(O2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O601 P177 P187 P189:P190">
-    <cfRule type="cellIs" dxfId="44" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="42" priority="8" operator="between">
       <formula>1</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="9" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="41" priority="9" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",O2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q10 Q16:Q1048576 R11:R15">
-    <cfRule type="duplicateValues" dxfId="42" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R6">
-    <cfRule type="cellIs" dxfId="41" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="21" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="40" priority="23">
+    <cfRule type="containsBlanks" dxfId="38" priority="23">
       <formula>LEN(TRIM(R6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R8">
-    <cfRule type="cellIs" dxfId="39" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="17" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="18" operator="notEqual">
+    <cfRule type="cellIs" dxfId="36" priority="18" operator="notEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1">
-    <cfRule type="duplicateValues" dxfId="37" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="5"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="K160" r:id="rId1" location="page=11" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -44631,9 +44620,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC575"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46597,7 +46586,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -46656,7 +46645,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -46715,7 +46704,7 @@
         <v>5029</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -46774,7 +46763,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -46833,7 +46822,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -46892,7 +46881,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -46951,7 +46940,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -47010,7 +46999,7 @@
         <v>5029</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -47069,7 +47058,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -47128,7 +47117,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -47187,7 +47176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -47245,8 +47234,11 @@
       <c r="S43" s="7" t="s">
         <v>5029</v>
       </c>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T43" t="s">
+        <v>5374</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -47305,7 +47297,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -47364,7 +47356,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -47423,7 +47415,7 @@
         <v>5029</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -47482,7 +47474,7 @@
         <v>5029</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -49573,41 +49565,41 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B38 B40:B1048576">
-    <cfRule type="duplicateValues" dxfId="36" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsBlanks" dxfId="35" priority="13">
+    <cfRule type="containsBlanks" dxfId="33" priority="13">
       <formula>LEN(TRIM(F1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:R601">
-    <cfRule type="containsText" dxfId="34" priority="8" operator="containsText" text="PRIMARY STUDY">
+    <cfRule type="containsText" dxfId="32" priority="8" operator="containsText" text="PRIMARY STUDY">
       <formula>NOT(ISERROR(SEARCH("PRIMARY STUDY",P2)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="33" priority="9" operator="notContains" text="YES">
+    <cfRule type="notContainsText" dxfId="31" priority="9" operator="notContains" text="YES">
       <formula>ISERROR(SEARCH("YES",P2))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="10" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="30" priority="10" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",P2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S601">
-    <cfRule type="cellIs" dxfId="31" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="29" priority="6" operator="between">
       <formula>1</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="7" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="28" priority="7" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",S2)))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="29" priority="15">
+    <cfRule type="containsBlanks" dxfId="27" priority="15">
       <formula>LEN(TRIM(S2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U1:U2">
-    <cfRule type="duplicateValues" dxfId="28" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="X1">
-    <cfRule type="duplicateValues" dxfId="27" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
@@ -49618,10 +49610,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:Z20"/>
+  <dimension ref="A1:Z19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49686,13 +49678,13 @@
       </c>
       <c r="S1" s="29">
         <f>COUNTIFS($N:$N, "YES", $F:$F, "&lt;&gt;")</f>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="U1" s="28" t="s">
         <v>5039</v>
       </c>
       <c r="V1" s="29">
-        <f>COUNTIF($M$2:$M$573, "YES")</f>
+        <f>COUNTIF($M$2:$M$572, "YES")</f>
         <v>18</v>
       </c>
       <c r="W1" s="31"/>
@@ -49969,7 +49961,7 @@
       </c>
       <c r="S6">
         <f>COUNTIFS($N:$N, "YES", $M:$M, "&lt;&gt;PRIMARY STUDY")</f>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="X6" t="s">
         <v>5076</v>
@@ -50638,125 +50630,63 @@
         <v>5372</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>5073</v>
-      </c>
-      <c r="C20" t="s">
-        <v>4128</v>
-      </c>
-      <c r="D20">
-        <v>1995</v>
-      </c>
-      <c r="E20" t="s">
-        <v>5302</v>
-      </c>
-      <c r="F20" t="s">
-        <v>5303</v>
-      </c>
-      <c r="G20" t="s">
-        <v>5029</v>
-      </c>
-      <c r="H20">
-        <v>372</v>
-      </c>
-      <c r="I20" t="s">
-        <v>5029</v>
-      </c>
-      <c r="J20" t="s">
-        <v>5029</v>
-      </c>
-      <c r="K20" t="s">
-        <v>5029</v>
-      </c>
-      <c r="L20" t="s">
-        <v>5073</v>
-      </c>
-      <c r="M20" t="s">
-        <v>5371</v>
-      </c>
-      <c r="N20" t="s">
-        <v>963</v>
-      </c>
-      <c r="O20" t="s">
-        <v>966</v>
-      </c>
-      <c r="P20" s="7" t="s">
-        <v>5029</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>5372</v>
-      </c>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B2">
-    <cfRule type="duplicateValues" dxfId="26" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="25" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="duplicateValues" dxfId="24" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F2">
-    <cfRule type="containsBlanks" dxfId="23" priority="37">
+    <cfRule type="containsBlanks" dxfId="21" priority="37">
       <formula>LEN(TRIM(F1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18:F19">
-    <cfRule type="containsBlanks" dxfId="22" priority="15">
+    <cfRule type="containsBlanks" dxfId="20" priority="15">
       <formula>LEN(TRIM(F18))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:H17 H20:H1048576">
-    <cfRule type="containsBlanks" dxfId="21" priority="38">
+    <cfRule type="containsBlanks" dxfId="19" priority="38">
       <formula>LEN(TRIM(H1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2">
-    <cfRule type="duplicateValues" dxfId="20" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L18">
-    <cfRule type="duplicateValues" dxfId="19" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L19">
-    <cfRule type="duplicateValues" dxfId="18" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:O20">
-    <cfRule type="containsText" dxfId="17" priority="2" operator="containsText" text="PRIMARY STUDY">
+  <conditionalFormatting sqref="M2:O19">
+    <cfRule type="containsText" dxfId="15" priority="2" operator="containsText" text="PRIMARY STUDY">
       <formula>NOT(ISERROR(SEARCH("PRIMARY STUDY",M2)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="16" priority="3" operator="notContains" text="YES">
+    <cfRule type="notContainsText" dxfId="14" priority="3" operator="notContains" text="YES">
       <formula>ISERROR(SEARCH("YES",M2))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="4" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="13" priority="4" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",M2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O18:O20">
-    <cfRule type="cellIs" dxfId="14" priority="10" operator="between">
+  <conditionalFormatting sqref="O18:O19 P1:P1048576">
+    <cfRule type="cellIs" dxfId="12" priority="10" operator="between">
       <formula>1</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH("X",O18)))</formula>
+    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",O1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O18:P20">
-    <cfRule type="containsBlanks" dxfId="12" priority="1">
+  <conditionalFormatting sqref="O18:P19">
+    <cfRule type="containsBlanks" dxfId="10" priority="1">
       <formula>LEN(TRIM(O18))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P1:P1048576">
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="between">
-      <formula>1</formula>
-      <formula>4</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="7" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH("X",P1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1 Q4">

</xml_diff>

<commit_message>
Finished the 5th chapter of the main text
</commit_message>
<xml_diff>
--- a/Literature/Literature.xlsx
+++ b/Literature/Literature.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hso20\OneDrive\Plocha\IES\Diploma-Thesis\Literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF931D5-9DDF-418B-B7C1-2267838073B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716267EF-05B1-4B0E-996C-517D07DA0F00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Query literature" sheetId="5" r:id="rId1"/>
@@ -694,7 +694,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10262" uniqueCount="5375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10250" uniqueCount="5369">
   <si>
     <t>Number</t>
   </si>
@@ -16030,24 +16030,6 @@
   </si>
   <si>
     <t>Using siblings to estimate the effect of school quality on wages</t>
-  </si>
-  <si>
-    <t>Belzil, Christian, and Jörgen Hansen. "Unobserved ability and the return to schooling." Econometrica 70, no. 5 (2002): 2075-2091.</t>
-  </si>
-  <si>
-    <t>ezQKpLmXhosJ</t>
-  </si>
-  <si>
-    <t>https://www.econstor.eu/bitstream/10419/21433/1/dp508.pdf</t>
-  </si>
-  <si>
-    <t>Unobserved ability and the return to schooling</t>
-  </si>
-  <si>
-    <t>Belzil &amp; Hansen</t>
-  </si>
-  <si>
-    <t>Belzil &amp; Hansen (2002)</t>
   </si>
   <si>
     <t>Gensowski, Miriam. "Personality, IQ, and lifetime earnings." Labour Economics 51 (2018): 170-183.</t>
@@ -17964,27 +17946,27 @@
         <v>962</v>
       </c>
       <c r="N1" s="24" t="s">
+        <v>5133</v>
+      </c>
+      <c r="O1" s="25" t="s">
+        <v>5131</v>
+      </c>
+      <c r="P1" s="5" t="s">
         <v>5139</v>
-      </c>
-      <c r="O1" s="25" t="s">
-        <v>5137</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>5145</v>
       </c>
       <c r="Q1" s="28" t="s">
         <v>5038</v>
       </c>
       <c r="R1" s="29">
         <f>COUNTIFS($M:$M, "YES", $F:$F, "&lt;&gt;") + Twins!S1</f>
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="T1" s="28" t="s">
         <v>5039</v>
       </c>
       <c r="U1" s="29">
         <f>COUNTIF($L$2:$L$575, "&lt;&gt; ") +Twins!V1</f>
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="V1" s="31"/>
       <c r="W1" s="31"/>
@@ -18145,7 +18127,7 @@
         <v>574</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>5143</v>
+        <v>5137</v>
       </c>
       <c r="U4">
         <f>COUNTIFS($M:$M, "YES", $L:$L, "&lt;&gt;PRIMARY STUDY", $P:$P, "&lt;&gt;Twins")</f>
@@ -18206,7 +18188,7 @@
         <v>574</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>5140</v>
+        <v>5134</v>
       </c>
       <c r="U5" s="37">
         <f>COUNTIFS($N:$N, "YES", $F:$F, "&lt;&gt;")</f>
@@ -18314,7 +18296,7 @@
         <v>5029</v>
       </c>
       <c r="P7" t="s">
-        <v>5369</v>
+        <v>5363</v>
       </c>
       <c r="Q7" s="2" t="s">
         <v>904</v>
@@ -18515,10 +18497,10 @@
         <v>1</v>
       </c>
       <c r="P11" t="s">
-        <v>5144</v>
+        <v>5138</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>5138</v>
+        <v>5132</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
@@ -18571,7 +18553,7 @@
         <v>1</v>
       </c>
       <c r="R12" t="s">
-        <v>5141</v>
+        <v>5135</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
@@ -18624,7 +18606,7 @@
         <v>2</v>
       </c>
       <c r="R13" t="s">
-        <v>5142</v>
+        <v>5136</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
@@ -19877,7 +19859,7 @@
         <v>1</v>
       </c>
       <c r="P38" t="s">
-        <v>5144</v>
+        <v>5138</v>
       </c>
       <c r="R38" t="s">
         <v>904</v>
@@ -20030,7 +20012,7 @@
         <v>2</v>
       </c>
       <c r="P41" t="s">
-        <v>5155</v>
+        <v>5149</v>
       </c>
       <c r="R41" t="s">
         <v>904</v>
@@ -20833,7 +20815,7 @@
         <v>2</v>
       </c>
       <c r="P57" t="s">
-        <v>5147</v>
+        <v>5141</v>
       </c>
       <c r="R57" t="s">
         <v>904</v>
@@ -22486,7 +22468,7 @@
         <v>1</v>
       </c>
       <c r="P90" t="s">
-        <v>5148</v>
+        <v>5142</v>
       </c>
       <c r="R90" t="s">
         <v>904</v>
@@ -22497,7 +22479,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>5149</v>
+        <v>5143</v>
       </c>
       <c r="C91" t="s">
         <v>4015</v>
@@ -23489,7 +23471,7 @@
         <v>1</v>
       </c>
       <c r="P110" t="s">
-        <v>5150</v>
+        <v>5144</v>
       </c>
       <c r="R110" t="s">
         <v>904</v>
@@ -23942,7 +23924,7 @@
         <v>4</v>
       </c>
       <c r="P119" t="s">
-        <v>5151</v>
+        <v>5145</v>
       </c>
       <c r="R119" t="s">
         <v>904</v>
@@ -25236,7 +25218,7 @@
         <v>1765</v>
       </c>
       <c r="L145" t="s">
-        <v>5152</v>
+        <v>5146</v>
       </c>
       <c r="M145" t="s">
         <v>966</v>
@@ -25256,7 +25238,7 @@
         <v>145</v>
       </c>
       <c r="B146" t="s">
-        <v>5153</v>
+        <v>5147</v>
       </c>
       <c r="C146" t="s">
         <v>4080</v>
@@ -25268,7 +25250,7 @@
         <v>1766</v>
       </c>
       <c r="F146" t="s">
-        <v>5154</v>
+        <v>5148</v>
       </c>
       <c r="G146" t="s">
         <v>1768</v>
@@ -25459,7 +25441,7 @@
         <v>149</v>
       </c>
       <c r="B150" t="s">
-        <v>5156</v>
+        <v>5150</v>
       </c>
       <c r="C150" t="s">
         <v>4085</v>
@@ -25468,13 +25450,13 @@
         <v>2012</v>
       </c>
       <c r="E150" t="s">
-        <v>5157</v>
+        <v>5151</v>
       </c>
       <c r="F150" t="s">
-        <v>5158</v>
+        <v>5152</v>
       </c>
       <c r="G150" t="s">
-        <v>5159</v>
+        <v>5153</v>
       </c>
       <c r="H150">
         <v>0</v>
@@ -27363,7 +27345,7 @@
         <v>1</v>
       </c>
       <c r="P187" t="s">
-        <v>5144</v>
+        <v>5138</v>
       </c>
       <c r="R187" t="s">
         <v>904</v>
@@ -44620,9 +44602,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC575"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44664,16 +44646,16 @@
         <v>3907</v>
       </c>
       <c r="H1" s="23" t="s">
-        <v>5160</v>
+        <v>5154</v>
       </c>
       <c r="I1" s="23" t="s">
-        <v>5161</v>
+        <v>5155</v>
       </c>
       <c r="J1" s="23" t="s">
-        <v>5162</v>
+        <v>5156</v>
       </c>
       <c r="K1" s="23" t="s">
-        <v>5163</v>
+        <v>5157</v>
       </c>
       <c r="L1" s="23" t="s">
         <v>3902</v>
@@ -44694,13 +44676,13 @@
         <v>962</v>
       </c>
       <c r="R1" s="24" t="s">
+        <v>5133</v>
+      </c>
+      <c r="S1" s="25" t="s">
+        <v>5131</v>
+      </c>
+      <c r="T1" s="39" t="s">
         <v>5139</v>
-      </c>
-      <c r="S1" s="25" t="s">
-        <v>5137</v>
-      </c>
-      <c r="T1" s="39" t="s">
-        <v>5145</v>
       </c>
       <c r="U1" s="28" t="s">
         <v>5038</v>
@@ -44726,7 +44708,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>5168</v>
+        <v>5162</v>
       </c>
       <c r="C2" s="34" t="s">
         <v>4157</v>
@@ -44735,10 +44717,10 @@
         <v>2010</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>5169</v>
+        <v>5163</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>5170</v>
+        <v>5164</v>
       </c>
       <c r="G2" s="34" t="s">
         <v>5029</v>
@@ -44750,10 +44732,10 @@
         <v>1</v>
       </c>
       <c r="J2" s="34" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K2" s="34" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L2" s="34">
         <v>289</v>
@@ -44792,34 +44774,34 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5171</v>
+        <v>5165</v>
       </c>
       <c r="C3" t="s">
-        <v>5172</v>
+        <v>5166</v>
       </c>
       <c r="D3">
         <v>2000</v>
       </c>
       <c r="E3" t="s">
-        <v>5173</v>
+        <v>5167</v>
       </c>
       <c r="F3" t="s">
-        <v>5174</v>
+        <v>5168</v>
       </c>
       <c r="G3" t="s">
         <v>5029</v>
       </c>
       <c r="H3" t="s">
-        <v>5348</v>
+        <v>5342</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K3" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L3">
         <v>1486</v>
@@ -44834,7 +44816,7 @@
         <v>5029</v>
       </c>
       <c r="P3" t="s">
-        <v>5364</v>
+        <v>5358</v>
       </c>
       <c r="Q3" t="s">
         <v>963</v>
@@ -44860,10 +44842,10 @@
         <v>1995</v>
       </c>
       <c r="E4" t="s">
-        <v>5175</v>
+        <v>5169</v>
       </c>
       <c r="F4" t="s">
-        <v>5176</v>
+        <v>5170</v>
       </c>
       <c r="G4" t="s">
         <v>5029</v>
@@ -44875,10 +44857,10 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K4" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L4">
         <v>321</v>
@@ -44910,34 +44892,34 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5177</v>
+        <v>5171</v>
       </c>
       <c r="C5" t="s">
-        <v>5178</v>
+        <v>5172</v>
       </c>
       <c r="D5">
         <v>1991</v>
       </c>
       <c r="E5" t="s">
-        <v>5179</v>
+        <v>5173</v>
       </c>
       <c r="F5" t="s">
-        <v>5180</v>
+        <v>5174</v>
       </c>
       <c r="G5" t="s">
         <v>5029</v>
       </c>
       <c r="H5" t="s">
-        <v>5349</v>
+        <v>5343</v>
       </c>
       <c r="I5" t="b">
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K5" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L5">
         <v>3590</v>
@@ -44969,19 +44951,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>5181</v>
+        <v>5175</v>
       </c>
       <c r="C6" t="s">
-        <v>5182</v>
+        <v>5176</v>
       </c>
       <c r="D6">
         <v>2005</v>
       </c>
       <c r="E6" t="s">
-        <v>5183</v>
+        <v>5177</v>
       </c>
       <c r="F6" t="s">
-        <v>5184</v>
+        <v>5178</v>
       </c>
       <c r="G6" t="s">
         <v>5029</v>
@@ -44993,10 +44975,10 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K6" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L6">
         <v>1510</v>
@@ -45023,10 +45005,10 @@
         <v>5029</v>
       </c>
       <c r="T6" t="s">
-        <v>5362</v>
+        <v>5356</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>5143</v>
+        <v>5137</v>
       </c>
       <c r="V6">
         <f>COUNTIF($P:$P, "YES")</f>
@@ -45038,34 +45020,34 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>5185</v>
+        <v>5179</v>
       </c>
       <c r="C7" t="s">
-        <v>5186</v>
+        <v>5180</v>
       </c>
       <c r="D7">
         <v>2002</v>
       </c>
       <c r="E7" t="s">
-        <v>5187</v>
+        <v>5181</v>
       </c>
       <c r="F7" t="s">
-        <v>5188</v>
+        <v>5182</v>
       </c>
       <c r="G7" t="s">
         <v>5029</v>
       </c>
       <c r="H7" t="s">
-        <v>5350</v>
+        <v>5344</v>
       </c>
       <c r="I7" t="b">
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K7" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L7">
         <v>321</v>
@@ -45092,7 +45074,7 @@
         <v>1</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>5140</v>
+        <v>5134</v>
       </c>
       <c r="V7">
         <f>COUNTIFS($R:$R, "YES", $F:$F, "&lt;&gt;")</f>
@@ -45113,10 +45095,10 @@
         <v>1998</v>
       </c>
       <c r="E8" t="s">
-        <v>5189</v>
+        <v>5183</v>
       </c>
       <c r="F8" t="s">
-        <v>5190</v>
+        <v>5184</v>
       </c>
       <c r="G8" t="s">
         <v>5029</v>
@@ -45128,10 +45110,10 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K8" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L8">
         <v>588</v>
@@ -45163,34 +45145,34 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>5191</v>
+        <v>5185</v>
       </c>
       <c r="C9" t="s">
-        <v>5192</v>
+        <v>5186</v>
       </c>
       <c r="D9">
         <v>2014</v>
       </c>
       <c r="E9" t="s">
-        <v>5193</v>
+        <v>5187</v>
       </c>
       <c r="F9" t="s">
-        <v>5194</v>
+        <v>5188</v>
       </c>
       <c r="G9" t="s">
         <v>5029</v>
       </c>
       <c r="H9" t="s">
-        <v>5351</v>
+        <v>5345</v>
       </c>
       <c r="I9" t="b">
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K9" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L9">
         <v>73</v>
@@ -45222,34 +45204,34 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>5195</v>
+        <v>5189</v>
       </c>
       <c r="C10" t="s">
-        <v>5196</v>
+        <v>5190</v>
       </c>
       <c r="D10">
         <v>2018</v>
       </c>
       <c r="E10" t="s">
-        <v>5197</v>
+        <v>5191</v>
       </c>
       <c r="F10" t="s">
-        <v>5198</v>
+        <v>5192</v>
       </c>
       <c r="G10" t="s">
         <v>5029</v>
       </c>
       <c r="H10" t="s">
-        <v>5352</v>
+        <v>5346</v>
       </c>
       <c r="I10" t="b">
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K10" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L10">
         <v>74</v>
@@ -45264,7 +45246,7 @@
         <v>5029</v>
       </c>
       <c r="P10" t="s">
-        <v>5363</v>
+        <v>5357</v>
       </c>
       <c r="Q10" t="s">
         <v>963</v>
@@ -45281,19 +45263,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>5199</v>
+        <v>5193</v>
       </c>
       <c r="C11" t="s">
-        <v>5200</v>
+        <v>5194</v>
       </c>
       <c r="D11">
         <v>2014</v>
       </c>
       <c r="E11" t="s">
-        <v>5201</v>
+        <v>5195</v>
       </c>
       <c r="F11" t="s">
-        <v>5202</v>
+        <v>5196</v>
       </c>
       <c r="G11" t="s">
         <v>5029</v>
@@ -45305,10 +45287,10 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K11" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L11">
         <v>17</v>
@@ -45340,7 +45322,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>5203</v>
+        <v>5197</v>
       </c>
       <c r="C12" t="s">
         <v>3928</v>
@@ -45349,25 +45331,25 @@
         <v>1995</v>
       </c>
       <c r="E12" t="s">
-        <v>5204</v>
+        <v>5198</v>
       </c>
       <c r="F12" t="s">
-        <v>5205</v>
+        <v>5199</v>
       </c>
       <c r="G12" t="s">
         <v>5029</v>
       </c>
       <c r="H12" t="s">
-        <v>5353</v>
+        <v>5347</v>
       </c>
       <c r="I12" t="b">
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K12" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L12">
         <v>1789</v>
@@ -45399,7 +45381,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>5206</v>
+        <v>5200</v>
       </c>
       <c r="C13" t="s">
         <v>3928</v>
@@ -45408,25 +45390,25 @@
         <v>2001</v>
       </c>
       <c r="E13" t="s">
-        <v>5207</v>
+        <v>5201</v>
       </c>
       <c r="F13" t="s">
-        <v>5208</v>
+        <v>5202</v>
       </c>
       <c r="G13" t="s">
         <v>5029</v>
       </c>
       <c r="H13" t="s">
-        <v>5350</v>
+        <v>5344</v>
       </c>
       <c r="I13" t="b">
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K13" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L13">
         <v>2928</v>
@@ -45441,7 +45423,7 @@
         <v>5029</v>
       </c>
       <c r="P13" t="s">
-        <v>5365</v>
+        <v>5359</v>
       </c>
       <c r="Q13" t="s">
         <v>963</v>
@@ -45453,7 +45435,7 @@
         <v>1</v>
       </c>
       <c r="T13" t="s">
-        <v>5366</v>
+        <v>5360</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
@@ -45461,7 +45443,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>5209</v>
+        <v>5203</v>
       </c>
       <c r="C14" t="s">
         <v>4356</v>
@@ -45470,25 +45452,25 @@
         <v>2011</v>
       </c>
       <c r="E14" t="s">
-        <v>5210</v>
+        <v>5204</v>
       </c>
       <c r="F14" t="s">
-        <v>5211</v>
+        <v>5205</v>
       </c>
       <c r="G14" t="s">
         <v>5029</v>
       </c>
       <c r="H14" t="s">
-        <v>5354</v>
+        <v>5348</v>
       </c>
       <c r="I14" t="b">
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K14" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L14">
         <v>783</v>
@@ -45520,34 +45502,34 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>5212</v>
+        <v>5206</v>
       </c>
       <c r="C15" t="s">
-        <v>5213</v>
+        <v>5207</v>
       </c>
       <c r="D15">
         <v>2019</v>
       </c>
       <c r="E15" t="s">
-        <v>5214</v>
+        <v>5208</v>
       </c>
       <c r="F15" t="s">
-        <v>5215</v>
+        <v>5209</v>
       </c>
       <c r="G15" t="s">
         <v>5029</v>
       </c>
       <c r="H15" t="s">
-        <v>5355</v>
+        <v>5349</v>
       </c>
       <c r="I15" t="b">
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K15" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L15">
         <v>141</v>
@@ -45574,7 +45556,7 @@
         <v>5029</v>
       </c>
       <c r="T15" t="s">
-        <v>5367</v>
+        <v>5361</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
@@ -45591,10 +45573,10 @@
         <v>1998</v>
       </c>
       <c r="E16" t="s">
-        <v>5216</v>
+        <v>5210</v>
       </c>
       <c r="F16" t="s">
-        <v>5217</v>
+        <v>5211</v>
       </c>
       <c r="G16" t="s">
         <v>5029</v>
@@ -45606,10 +45588,10 @@
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K16" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L16">
         <v>284</v>
@@ -45641,34 +45623,34 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>5218</v>
+        <v>5212</v>
       </c>
       <c r="C17" t="s">
-        <v>5219</v>
+        <v>5213</v>
       </c>
       <c r="D17">
         <v>2010</v>
       </c>
       <c r="E17" t="s">
-        <v>5220</v>
+        <v>5214</v>
       </c>
       <c r="F17" t="s">
-        <v>5221</v>
+        <v>5215</v>
       </c>
       <c r="G17" t="s">
         <v>5029</v>
       </c>
       <c r="H17" t="s">
-        <v>5356</v>
+        <v>5350</v>
       </c>
       <c r="I17" t="b">
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K17" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L17">
         <v>252</v>
@@ -45700,19 +45682,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>5222</v>
+        <v>5216</v>
       </c>
       <c r="C18" t="s">
-        <v>5223</v>
+        <v>5217</v>
       </c>
       <c r="D18">
         <v>1991</v>
       </c>
       <c r="E18" t="s">
-        <v>5224</v>
+        <v>5218</v>
       </c>
       <c r="F18" t="s">
-        <v>5225</v>
+        <v>5219</v>
       </c>
       <c r="G18" t="s">
         <v>5029</v>
@@ -45724,10 +45706,10 @@
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K18" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L18">
         <v>88</v>
@@ -45768,10 +45750,10 @@
         <v>2001</v>
       </c>
       <c r="E19" t="s">
-        <v>5226</v>
+        <v>5220</v>
       </c>
       <c r="F19" t="s">
-        <v>5227</v>
+        <v>5221</v>
       </c>
       <c r="G19" t="s">
         <v>5029</v>
@@ -45783,10 +45765,10 @@
         <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K19" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L19">
         <v>2852</v>
@@ -45827,10 +45809,10 @@
         <v>2002</v>
       </c>
       <c r="E20" t="s">
-        <v>5228</v>
+        <v>5222</v>
       </c>
       <c r="F20" t="s">
-        <v>5229</v>
+        <v>5223</v>
       </c>
       <c r="G20" t="s">
         <v>5029</v>
@@ -45842,10 +45824,10 @@
         <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K20" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L20">
         <v>386</v>
@@ -45877,34 +45859,34 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>5230</v>
+        <v>5224</v>
       </c>
       <c r="C21" t="s">
-        <v>5231</v>
+        <v>5225</v>
       </c>
       <c r="D21">
         <v>2008</v>
       </c>
       <c r="E21" t="s">
-        <v>5232</v>
+        <v>5226</v>
       </c>
       <c r="F21" t="s">
-        <v>5233</v>
+        <v>5227</v>
       </c>
       <c r="G21" t="s">
         <v>5029</v>
       </c>
       <c r="H21" t="s">
-        <v>5357</v>
+        <v>5351</v>
       </c>
       <c r="I21" t="b">
         <v>1</v>
       </c>
       <c r="J21" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K21" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L21">
         <v>494</v>
@@ -45936,19 +45918,19 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>5234</v>
+        <v>5228</v>
       </c>
       <c r="C22" t="s">
-        <v>5235</v>
+        <v>5229</v>
       </c>
       <c r="D22">
         <v>2000</v>
       </c>
       <c r="E22" t="s">
-        <v>5236</v>
+        <v>5230</v>
       </c>
       <c r="F22" t="s">
-        <v>5237</v>
+        <v>5231</v>
       </c>
       <c r="G22" t="s">
         <v>5029</v>
@@ -45960,10 +45942,10 @@
         <v>1</v>
       </c>
       <c r="J22" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K22" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L22">
         <v>101</v>
@@ -45995,34 +45977,34 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>5238</v>
+        <v>5232</v>
       </c>
       <c r="C23" t="s">
-        <v>5239</v>
+        <v>5233</v>
       </c>
       <c r="D23">
         <v>2019</v>
       </c>
       <c r="E23" t="s">
-        <v>5240</v>
+        <v>5234</v>
       </c>
       <c r="F23" t="s">
-        <v>5241</v>
+        <v>5235</v>
       </c>
       <c r="G23" t="s">
         <v>5029</v>
       </c>
       <c r="H23" t="s">
-        <v>5352</v>
+        <v>5346</v>
       </c>
       <c r="I23" t="b">
         <v>1</v>
       </c>
       <c r="J23" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K23" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L23">
         <v>92</v>
@@ -46049,7 +46031,7 @@
         <v>5029</v>
       </c>
       <c r="T23" t="s">
-        <v>5368</v>
+        <v>5362</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
@@ -46057,19 +46039,19 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>5242</v>
+        <v>5236</v>
       </c>
       <c r="C24" t="s">
-        <v>5243</v>
+        <v>5237</v>
       </c>
       <c r="D24">
         <v>2005</v>
       </c>
       <c r="E24" t="s">
-        <v>5244</v>
+        <v>5238</v>
       </c>
       <c r="F24" t="s">
-        <v>5245</v>
+        <v>5239</v>
       </c>
       <c r="G24" t="s">
         <v>5029</v>
@@ -46081,10 +46063,10 @@
         <v>1</v>
       </c>
       <c r="J24" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K24" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L24">
         <v>171</v>
@@ -46116,34 +46098,34 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>5246</v>
+        <v>5240</v>
       </c>
       <c r="C25" t="s">
-        <v>5247</v>
+        <v>5241</v>
       </c>
       <c r="D25">
         <v>1995</v>
       </c>
       <c r="E25" t="s">
-        <v>5248</v>
+        <v>5242</v>
       </c>
       <c r="F25" t="s">
-        <v>5249</v>
+        <v>5243</v>
       </c>
       <c r="G25" t="s">
         <v>5029</v>
       </c>
       <c r="H25" t="s">
-        <v>5357</v>
+        <v>5351</v>
       </c>
       <c r="I25" t="b">
         <v>1</v>
       </c>
       <c r="J25" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K25" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L25">
         <v>662</v>
@@ -46175,7 +46157,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>5250</v>
+        <v>5244</v>
       </c>
       <c r="C26" t="s">
         <v>3930</v>
@@ -46184,10 +46166,10 @@
         <v>1995</v>
       </c>
       <c r="E26" t="s">
-        <v>5251</v>
+        <v>5245</v>
       </c>
       <c r="F26" t="s">
-        <v>5252</v>
+        <v>5246</v>
       </c>
       <c r="G26" t="s">
         <v>5029</v>
@@ -46199,10 +46181,10 @@
         <v>1</v>
       </c>
       <c r="J26" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K26" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L26">
         <v>888</v>
@@ -46234,7 +46216,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>5253</v>
+        <v>5247</v>
       </c>
       <c r="C27" t="s">
         <v>3930</v>
@@ -46243,10 +46225,10 @@
         <v>1999</v>
       </c>
       <c r="E27" t="s">
-        <v>5254</v>
+        <v>5248</v>
       </c>
       <c r="F27" t="s">
-        <v>5255</v>
+        <v>5249</v>
       </c>
       <c r="G27" t="s">
         <v>5029</v>
@@ -46258,10 +46240,10 @@
         <v>1</v>
       </c>
       <c r="J27" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K27" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L27">
         <v>100</v>
@@ -46302,25 +46284,25 @@
         <v>2003</v>
       </c>
       <c r="E28" t="s">
-        <v>5256</v>
+        <v>5250</v>
       </c>
       <c r="F28" t="s">
-        <v>5257</v>
+        <v>5251</v>
       </c>
       <c r="G28" t="s">
         <v>5029</v>
       </c>
       <c r="H28" t="s">
-        <v>5352</v>
+        <v>5346</v>
       </c>
       <c r="I28" t="b">
         <v>1</v>
       </c>
       <c r="J28" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K28" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L28">
         <v>860</v>
@@ -46352,19 +46334,19 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>5258</v>
+        <v>5252</v>
       </c>
       <c r="C29" t="s">
-        <v>5259</v>
+        <v>5253</v>
       </c>
       <c r="D29">
         <v>2007</v>
       </c>
       <c r="E29" t="s">
-        <v>5260</v>
+        <v>5254</v>
       </c>
       <c r="F29" t="s">
-        <v>5261</v>
+        <v>5255</v>
       </c>
       <c r="G29" t="s">
         <v>5029</v>
@@ -46376,10 +46358,10 @@
         <v>1</v>
       </c>
       <c r="J29" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K29" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L29">
         <v>27</v>
@@ -46411,34 +46393,34 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>5262</v>
+        <v>5256</v>
       </c>
       <c r="C30" t="s">
-        <v>5263</v>
+        <v>5257</v>
       </c>
       <c r="D30">
         <v>2006</v>
       </c>
       <c r="E30" t="s">
-        <v>5264</v>
+        <v>5258</v>
       </c>
       <c r="F30" t="s">
-        <v>5265</v>
+        <v>5259</v>
       </c>
       <c r="G30" t="s">
         <v>5029</v>
       </c>
       <c r="H30" t="s">
-        <v>5358</v>
+        <v>5352</v>
       </c>
       <c r="I30" t="b">
         <v>1</v>
       </c>
       <c r="J30" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K30" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L30">
         <v>1427</v>
@@ -46465,7 +46447,7 @@
         <v>3</v>
       </c>
       <c r="T30" t="s">
-        <v>5370</v>
+        <v>5364</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
@@ -46473,34 +46455,34 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>5266</v>
+        <v>5260</v>
       </c>
       <c r="C31" t="s">
-        <v>5267</v>
+        <v>5261</v>
       </c>
       <c r="D31">
         <v>2011</v>
       </c>
       <c r="E31" t="s">
-        <v>5268</v>
+        <v>5262</v>
       </c>
       <c r="F31" t="s">
-        <v>5269</v>
+        <v>5263</v>
       </c>
       <c r="G31" t="s">
         <v>5029</v>
       </c>
       <c r="H31" t="s">
-        <v>5357</v>
+        <v>5351</v>
       </c>
       <c r="I31" t="b">
         <v>1</v>
       </c>
       <c r="J31" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K31" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L31">
         <v>80</v>
@@ -46532,19 +46514,19 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>5270</v>
+        <v>5264</v>
       </c>
       <c r="C32" t="s">
-        <v>5271</v>
+        <v>5265</v>
       </c>
       <c r="D32">
         <v>1999</v>
       </c>
       <c r="E32" t="s">
-        <v>5272</v>
+        <v>5266</v>
       </c>
       <c r="F32" t="s">
-        <v>5273</v>
+        <v>5267</v>
       </c>
       <c r="G32" t="s">
         <v>5029</v>
@@ -46556,10 +46538,10 @@
         <v>1</v>
       </c>
       <c r="J32" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K32" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L32">
         <v>182</v>
@@ -46591,34 +46573,34 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>5274</v>
+        <v>5268</v>
       </c>
       <c r="C33" t="s">
-        <v>5275</v>
+        <v>5269</v>
       </c>
       <c r="D33">
         <v>2004</v>
       </c>
       <c r="E33" t="s">
-        <v>5276</v>
+        <v>5270</v>
       </c>
       <c r="F33" t="s">
-        <v>5277</v>
+        <v>5271</v>
       </c>
       <c r="G33" t="s">
         <v>5029</v>
       </c>
       <c r="H33" t="s">
-        <v>5352</v>
+        <v>5346</v>
       </c>
       <c r="I33" t="b">
         <v>1</v>
       </c>
       <c r="J33" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K33" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L33">
         <v>389</v>
@@ -46659,10 +46641,10 @@
         <v>1999</v>
       </c>
       <c r="E34" t="s">
-        <v>5278</v>
+        <v>5272</v>
       </c>
       <c r="F34" t="s">
-        <v>5279</v>
+        <v>5273</v>
       </c>
       <c r="G34" t="s">
         <v>5029</v>
@@ -46674,10 +46656,10 @@
         <v>1</v>
       </c>
       <c r="J34" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K34" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L34">
         <v>177</v>
@@ -46692,7 +46674,7 @@
         <v>5029</v>
       </c>
       <c r="P34" t="s">
-        <v>5371</v>
+        <v>5365</v>
       </c>
       <c r="Q34" t="s">
         <v>963</v>
@@ -46718,10 +46700,10 @@
         <v>2001</v>
       </c>
       <c r="E35" t="s">
-        <v>5280</v>
+        <v>5274</v>
       </c>
       <c r="F35" t="s">
-        <v>5281</v>
+        <v>5275</v>
       </c>
       <c r="G35" t="s">
         <v>5029</v>
@@ -46733,10 +46715,10 @@
         <v>1</v>
       </c>
       <c r="J35" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K35" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L35">
         <v>217</v>
@@ -46768,19 +46750,19 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>5282</v>
+        <v>5276</v>
       </c>
       <c r="C36" t="s">
-        <v>5283</v>
+        <v>5277</v>
       </c>
       <c r="D36">
         <v>1993</v>
       </c>
       <c r="E36" t="s">
-        <v>5284</v>
+        <v>5278</v>
       </c>
       <c r="F36" t="s">
-        <v>5285</v>
+        <v>5279</v>
       </c>
       <c r="G36" t="s">
         <v>5029</v>
@@ -46792,10 +46774,10 @@
         <v>1</v>
       </c>
       <c r="J36" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K36" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L36">
         <v>1442</v>
@@ -46836,10 +46818,10 @@
         <v>2006</v>
       </c>
       <c r="E37" t="s">
-        <v>5286</v>
+        <v>5280</v>
       </c>
       <c r="F37" t="s">
-        <v>5287</v>
+        <v>5281</v>
       </c>
       <c r="G37" t="s">
         <v>5029</v>
@@ -46851,10 +46833,10 @@
         <v>1</v>
       </c>
       <c r="J37" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K37" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L37">
         <v>254</v>
@@ -46895,10 +46877,10 @@
         <v>1998</v>
       </c>
       <c r="E38" t="s">
-        <v>5288</v>
+        <v>5282</v>
       </c>
       <c r="F38" t="s">
-        <v>5289</v>
+        <v>5283</v>
       </c>
       <c r="G38" t="s">
         <v>5029</v>
@@ -46910,10 +46892,10 @@
         <v>1</v>
       </c>
       <c r="J38" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K38" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L38">
         <v>301</v>
@@ -46954,25 +46936,25 @@
         <v>2001</v>
       </c>
       <c r="E39" t="s">
-        <v>5290</v>
+        <v>5284</v>
       </c>
       <c r="F39" t="s">
-        <v>5291</v>
+        <v>5285</v>
       </c>
       <c r="G39" t="s">
         <v>5029</v>
       </c>
       <c r="H39" t="s">
-        <v>5359</v>
+        <v>5353</v>
       </c>
       <c r="I39" t="b">
         <v>1</v>
       </c>
       <c r="J39" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K39" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L39">
         <v>293</v>
@@ -46987,7 +46969,7 @@
         <v>5029</v>
       </c>
       <c r="P39" t="s">
-        <v>5373</v>
+        <v>5367</v>
       </c>
       <c r="Q39" t="s">
         <v>963</v>
@@ -47013,25 +46995,25 @@
         <v>2008</v>
       </c>
       <c r="E40" t="s">
-        <v>5292</v>
+        <v>5286</v>
       </c>
       <c r="F40" t="s">
-        <v>5293</v>
+        <v>5287</v>
       </c>
       <c r="G40" t="s">
         <v>5029</v>
       </c>
       <c r="H40" t="s">
-        <v>5357</v>
+        <v>5351</v>
       </c>
       <c r="I40" t="b">
         <v>1</v>
       </c>
       <c r="J40" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K40" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L40">
         <v>153</v>
@@ -47063,19 +47045,19 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>5294</v>
+        <v>5288</v>
       </c>
       <c r="C41" t="s">
-        <v>5295</v>
+        <v>5289</v>
       </c>
       <c r="D41">
         <v>2001</v>
       </c>
       <c r="E41" t="s">
-        <v>5296</v>
+        <v>5290</v>
       </c>
       <c r="F41" t="s">
-        <v>5297</v>
+        <v>5291</v>
       </c>
       <c r="G41" t="s">
         <v>5029</v>
@@ -47087,10 +47069,10 @@
         <v>1</v>
       </c>
       <c r="J41" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K41" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L41">
         <v>188</v>
@@ -47122,34 +47104,34 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>5298</v>
+        <v>5292</v>
       </c>
       <c r="C42" t="s">
-        <v>5299</v>
+        <v>5293</v>
       </c>
       <c r="D42">
         <v>2004</v>
       </c>
       <c r="E42" t="s">
-        <v>5300</v>
+        <v>5294</v>
       </c>
       <c r="F42" t="s">
-        <v>5301</v>
+        <v>5295</v>
       </c>
       <c r="G42" t="s">
         <v>5029</v>
       </c>
       <c r="H42" t="s">
-        <v>5352</v>
+        <v>5346</v>
       </c>
       <c r="I42" t="b">
         <v>1</v>
       </c>
       <c r="J42" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K42" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L42">
         <v>93</v>
@@ -47190,25 +47172,25 @@
         <v>1995</v>
       </c>
       <c r="E43" t="s">
-        <v>5302</v>
+        <v>5296</v>
       </c>
       <c r="F43" t="s">
-        <v>5303</v>
+        <v>5297</v>
       </c>
       <c r="G43" t="s">
         <v>5029</v>
       </c>
       <c r="H43" t="s">
-        <v>5360</v>
+        <v>5354</v>
       </c>
       <c r="I43" t="b">
         <v>1</v>
       </c>
       <c r="J43" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K43" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L43">
         <v>372</v>
@@ -47223,7 +47205,7 @@
         <v>5029</v>
       </c>
       <c r="P43" t="s">
-        <v>5371</v>
+        <v>5365</v>
       </c>
       <c r="Q43" t="s">
         <v>963</v>
@@ -47235,7 +47217,7 @@
         <v>5029</v>
       </c>
       <c r="T43" t="s">
-        <v>5374</v>
+        <v>5368</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
@@ -47243,19 +47225,19 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>5304</v>
+        <v>5298</v>
       </c>
       <c r="C44" t="s">
-        <v>5305</v>
+        <v>5299</v>
       </c>
       <c r="D44">
         <v>2004</v>
       </c>
       <c r="E44" t="s">
-        <v>5306</v>
+        <v>5300</v>
       </c>
       <c r="F44" t="s">
-        <v>5307</v>
+        <v>5301</v>
       </c>
       <c r="G44" t="s">
         <v>5029</v>
@@ -47267,10 +47249,10 @@
         <v>1</v>
       </c>
       <c r="J44" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K44" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L44">
         <v>1830</v>
@@ -47302,19 +47284,19 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>5308</v>
+        <v>5302</v>
       </c>
       <c r="C45" t="s">
-        <v>5309</v>
+        <v>5303</v>
       </c>
       <c r="D45">
         <v>2005</v>
       </c>
       <c r="E45" t="s">
-        <v>5310</v>
+        <v>5304</v>
       </c>
       <c r="F45" t="s">
-        <v>5311</v>
+        <v>5305</v>
       </c>
       <c r="G45" t="s">
         <v>5029</v>
@@ -47326,10 +47308,10 @@
         <v>1</v>
       </c>
       <c r="J45" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K45" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L45">
         <v>345</v>
@@ -47361,34 +47343,34 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>5312</v>
+        <v>5306</v>
       </c>
       <c r="C46" t="s">
-        <v>5313</v>
+        <v>5307</v>
       </c>
       <c r="D46">
         <v>2006</v>
       </c>
       <c r="E46" t="s">
-        <v>5314</v>
+        <v>5308</v>
       </c>
       <c r="F46" t="s">
-        <v>5315</v>
+        <v>5309</v>
       </c>
       <c r="G46" t="s">
         <v>5029</v>
       </c>
       <c r="H46" t="s">
-        <v>5361</v>
+        <v>5355</v>
       </c>
       <c r="I46" t="b">
         <v>1</v>
       </c>
       <c r="J46" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K46" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L46">
         <v>1005</v>
@@ -47403,7 +47385,7 @@
         <v>5029</v>
       </c>
       <c r="P46" t="s">
-        <v>5363</v>
+        <v>5357</v>
       </c>
       <c r="Q46" t="s">
         <v>963</v>
@@ -47420,19 +47402,19 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>5316</v>
+        <v>5310</v>
       </c>
       <c r="C47" t="s">
-        <v>5317</v>
+        <v>5311</v>
       </c>
       <c r="D47">
         <v>2006</v>
       </c>
       <c r="E47" t="s">
-        <v>5318</v>
+        <v>5312</v>
       </c>
       <c r="F47" t="s">
-        <v>5319</v>
+        <v>5313</v>
       </c>
       <c r="G47" t="s">
         <v>5029</v>
@@ -47444,10 +47426,10 @@
         <v>1</v>
       </c>
       <c r="J47" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K47" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L47">
         <v>596</v>
@@ -47462,7 +47444,7 @@
         <v>5029</v>
       </c>
       <c r="P47" t="s">
-        <v>5363</v>
+        <v>5357</v>
       </c>
       <c r="Q47" t="s">
         <v>963</v>
@@ -47479,19 +47461,19 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>5320</v>
+        <v>5314</v>
       </c>
       <c r="C48" t="s">
-        <v>5321</v>
+        <v>5315</v>
       </c>
       <c r="D48">
         <v>2005</v>
       </c>
       <c r="E48" t="s">
-        <v>5322</v>
+        <v>5316</v>
       </c>
       <c r="F48" t="s">
-        <v>5164</v>
+        <v>5158</v>
       </c>
       <c r="G48" t="s">
         <v>5029</v>
@@ -47503,10 +47485,10 @@
         <v>1</v>
       </c>
       <c r="J48" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K48" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L48">
         <v>386</v>
@@ -47547,25 +47529,25 @@
         <v>1982</v>
       </c>
       <c r="E49" t="s">
-        <v>5323</v>
+        <v>5317</v>
       </c>
       <c r="F49" t="s">
-        <v>5165</v>
+        <v>5159</v>
       </c>
       <c r="G49" t="s">
         <v>5029</v>
       </c>
       <c r="H49" t="s">
-        <v>5360</v>
+        <v>5354</v>
       </c>
       <c r="I49" t="b">
         <v>1</v>
       </c>
       <c r="J49" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K49" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L49">
         <v>55</v>
@@ -47606,10 +47588,10 @@
         <v>1985</v>
       </c>
       <c r="E50" t="s">
-        <v>5324</v>
+        <v>5318</v>
       </c>
       <c r="F50" t="s">
-        <v>5166</v>
+        <v>5160</v>
       </c>
       <c r="G50" t="s">
         <v>5029</v>
@@ -47621,10 +47603,10 @@
         <v>1</v>
       </c>
       <c r="J50" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K50" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L50">
         <v>2143</v>
@@ -47656,7 +47638,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>5325</v>
+        <v>5319</v>
       </c>
       <c r="C51" t="s">
         <v>674</v>
@@ -47665,10 +47647,10 @@
         <v>1979</v>
       </c>
       <c r="E51" t="s">
-        <v>5326</v>
+        <v>5320</v>
       </c>
       <c r="F51" t="s">
-        <v>5167</v>
+        <v>5161</v>
       </c>
       <c r="G51" t="s">
         <v>5029</v>
@@ -47680,10 +47662,10 @@
         <v>1</v>
       </c>
       <c r="J51" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K51" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L51">
         <v>251</v>
@@ -47715,19 +47697,19 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="C52" t="s">
-        <v>5328</v>
+        <v>5322</v>
       </c>
       <c r="D52">
         <v>1997</v>
       </c>
       <c r="E52" t="s">
-        <v>5329</v>
+        <v>5323</v>
       </c>
       <c r="F52" t="s">
-        <v>5330</v>
+        <v>5324</v>
       </c>
       <c r="G52" t="s">
         <v>5029</v>
@@ -47739,10 +47721,10 @@
         <v>1</v>
       </c>
       <c r="J52" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K52" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L52">
         <v>9699</v>
@@ -47774,34 +47756,34 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>5331</v>
+        <v>5325</v>
       </c>
       <c r="C53" t="s">
-        <v>5332</v>
+        <v>5326</v>
       </c>
       <c r="D53">
         <v>2014</v>
       </c>
       <c r="E53" t="s">
-        <v>5333</v>
+        <v>5327</v>
       </c>
       <c r="F53" t="s">
-        <v>5334</v>
+        <v>5328</v>
       </c>
       <c r="G53" t="s">
         <v>5029</v>
       </c>
       <c r="H53" t="s">
-        <v>5350</v>
+        <v>5344</v>
       </c>
       <c r="I53" t="b">
         <v>1</v>
       </c>
       <c r="J53" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K53" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L53">
         <v>264</v>
@@ -47833,19 +47815,19 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>5335</v>
+        <v>5329</v>
       </c>
       <c r="C54" t="s">
-        <v>5336</v>
+        <v>5330</v>
       </c>
       <c r="D54">
         <v>2001</v>
       </c>
       <c r="E54" t="s">
-        <v>5337</v>
+        <v>5331</v>
       </c>
       <c r="F54" t="s">
-        <v>5338</v>
+        <v>5332</v>
       </c>
       <c r="G54" t="s">
         <v>5029</v>
@@ -47857,10 +47839,10 @@
         <v>1</v>
       </c>
       <c r="J54" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K54" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L54">
         <v>261</v>
@@ -47892,19 +47874,19 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>5339</v>
+        <v>5333</v>
       </c>
       <c r="C55" t="s">
-        <v>5340</v>
+        <v>5334</v>
       </c>
       <c r="D55">
         <v>1999</v>
       </c>
       <c r="E55" t="s">
-        <v>5341</v>
+        <v>5335</v>
       </c>
       <c r="F55" t="s">
-        <v>5342</v>
+        <v>5336</v>
       </c>
       <c r="G55" t="s">
         <v>5029</v>
@@ -47916,10 +47898,10 @@
         <v>1</v>
       </c>
       <c r="J55" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K55" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L55">
         <v>423</v>
@@ -47951,19 +47933,19 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>5343</v>
+        <v>5337</v>
       </c>
       <c r="C56" t="s">
-        <v>5344</v>
+        <v>5338</v>
       </c>
       <c r="D56">
         <v>2011</v>
       </c>
       <c r="E56" t="s">
-        <v>5345</v>
+        <v>5339</v>
       </c>
       <c r="F56" t="s">
-        <v>5346</v>
+        <v>5340</v>
       </c>
       <c r="G56" t="s">
         <v>5029</v>
@@ -47975,10 +47957,10 @@
         <v>1</v>
       </c>
       <c r="J56" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="K56" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
       <c r="L56">
         <v>197</v>
@@ -49610,10 +49592,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:Z19"/>
+  <dimension ref="A1:Z18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I13" sqref="I12:I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49665,27 +49647,27 @@
         <v>962</v>
       </c>
       <c r="O1" s="24" t="s">
-        <v>5139</v>
+        <v>5133</v>
       </c>
       <c r="P1" s="25" t="s">
         <v>5026</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>5145</v>
+        <v>5139</v>
       </c>
       <c r="R1" s="28" t="s">
         <v>5038</v>
       </c>
       <c r="S1" s="29">
         <f>COUNTIFS($N:$N, "YES", $F:$F, "&lt;&gt;")</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="U1" s="28" t="s">
         <v>5039</v>
       </c>
       <c r="V1" s="29">
-        <f>COUNTIF($M$2:$M$572, "YES")</f>
-        <v>18</v>
+        <f>COUNTIF($M$2:$M$571, "YES")</f>
+        <v>17</v>
       </c>
       <c r="W1" s="31"/>
       <c r="X1" s="31"/>
@@ -49957,11 +49939,11 @@
         <v>1</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>5143</v>
+        <v>5137</v>
       </c>
       <c r="S6">
         <f>COUNTIFS($N:$N, "YES", $M:$M, "&lt;&gt;PRIMARY STUDY")</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="X6" t="s">
         <v>5076</v>
@@ -50017,7 +49999,7 @@
         <v>1</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>5140</v>
+        <v>5134</v>
       </c>
       <c r="S7">
         <f>COUNTIFS($O:$O, "YES", $F:$F, "&lt;&gt;")</f>
@@ -50223,16 +50205,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>5116</v>
+      </c>
+      <c r="C12" t="s">
         <v>5117</v>
       </c>
-      <c r="C12" t="s">
-        <v>5116</v>
-      </c>
       <c r="D12">
-        <v>2002</v>
+        <v>2018</v>
       </c>
       <c r="E12" t="s">
-        <v>5115</v>
+        <v>5118</v>
       </c>
       <c r="F12" t="s">
         <v>5112</v>
@@ -50241,7 +50223,7 @@
         <v>5030</v>
       </c>
       <c r="H12">
-        <v>320</v>
+        <v>181</v>
       </c>
       <c r="I12" t="s">
         <v>5113</v>
@@ -50253,7 +50235,7 @@
         <v>5114</v>
       </c>
       <c r="L12" t="s">
-        <v>5117</v>
+        <v>5116</v>
       </c>
       <c r="M12" t="s">
         <v>963</v>
@@ -50264,8 +50246,8 @@
       <c r="O12" t="s">
         <v>966</v>
       </c>
-      <c r="P12" s="7">
-        <v>1</v>
+      <c r="P12" s="7" t="s">
+        <v>5115</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
@@ -50279,28 +50261,28 @@
         <v>5123</v>
       </c>
       <c r="D13">
-        <v>2018</v>
+        <v>2012</v>
       </c>
       <c r="E13" t="s">
         <v>5124</v>
       </c>
       <c r="F13" t="s">
-        <v>5118</v>
+        <v>5119</v>
       </c>
       <c r="G13" t="s">
         <v>5030</v>
       </c>
       <c r="H13">
-        <v>181</v>
+        <v>18</v>
       </c>
       <c r="I13" t="s">
-        <v>5119</v>
+        <v>5120</v>
       </c>
       <c r="J13" t="s">
-        <v>5120</v>
+        <v>5121</v>
       </c>
       <c r="K13" t="s">
-        <v>5120</v>
+        <v>5121</v>
       </c>
       <c r="L13" t="s">
         <v>5122</v>
@@ -50314,8 +50296,8 @@
       <c r="O13" t="s">
         <v>966</v>
       </c>
-      <c r="P13" s="7" t="s">
-        <v>5121</v>
+      <c r="P13" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
@@ -50323,37 +50305,37 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>5128</v>
+        <v>5129</v>
       </c>
       <c r="C14" t="s">
-        <v>5129</v>
+        <v>5126</v>
       </c>
       <c r="D14">
-        <v>2012</v>
+        <v>2020</v>
       </c>
       <c r="E14" t="s">
         <v>5130</v>
       </c>
       <c r="F14" t="s">
-        <v>5125</v>
+        <v>5127</v>
       </c>
       <c r="G14" t="s">
         <v>5030</v>
       </c>
       <c r="H14">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I14" t="s">
-        <v>5126</v>
+        <v>5128</v>
       </c>
       <c r="J14" t="s">
-        <v>5127</v>
+        <v>5125</v>
       </c>
       <c r="K14" t="s">
-        <v>5127</v>
+        <v>5125</v>
       </c>
       <c r="L14" t="s">
-        <v>5128</v>
+        <v>5129</v>
       </c>
       <c r="M14" t="s">
         <v>963</v>
@@ -50373,37 +50355,37 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>5135</v>
+        <v>3935</v>
       </c>
       <c r="C15" t="s">
-        <v>5132</v>
+        <v>3936</v>
       </c>
       <c r="D15">
-        <v>2020</v>
+        <v>2005</v>
       </c>
       <c r="E15" t="s">
-        <v>5136</v>
+        <v>1072</v>
       </c>
       <c r="F15" t="s">
-        <v>5133</v>
+        <v>970</v>
       </c>
       <c r="G15" t="s">
-        <v>5030</v>
+        <v>1074</v>
       </c>
       <c r="H15">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="I15" t="s">
-        <v>5134</v>
+        <v>1073</v>
       </c>
       <c r="J15" t="s">
-        <v>5131</v>
+        <v>1075</v>
       </c>
       <c r="K15" t="s">
-        <v>5131</v>
+        <v>1075</v>
       </c>
       <c r="L15" t="s">
-        <v>5135</v>
+        <v>3935</v>
       </c>
       <c r="M15" t="s">
         <v>963</v>
@@ -50416,6 +50398,9 @@
       </c>
       <c r="P15" s="7">
         <v>1</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>5140</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
@@ -50423,37 +50408,37 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>3935</v>
+        <v>3965</v>
       </c>
       <c r="C16" t="s">
-        <v>3936</v>
+        <v>3966</v>
       </c>
       <c r="D16">
-        <v>2005</v>
+        <v>2003</v>
       </c>
       <c r="E16" t="s">
-        <v>1072</v>
+        <v>1211</v>
       </c>
       <c r="F16" t="s">
-        <v>970</v>
+        <v>4598</v>
       </c>
       <c r="G16" t="s">
-        <v>1074</v>
+        <v>1213</v>
       </c>
       <c r="H16">
-        <v>1</v>
+        <v>265</v>
       </c>
       <c r="I16" t="s">
-        <v>1073</v>
+        <v>1212</v>
       </c>
       <c r="J16" t="s">
-        <v>1075</v>
+        <v>1214</v>
       </c>
       <c r="K16" t="s">
-        <v>1075</v>
+        <v>1215</v>
       </c>
       <c r="L16" t="s">
-        <v>3935</v>
+        <v>3965</v>
       </c>
       <c r="M16" t="s">
         <v>963</v>
@@ -50468,7 +50453,7 @@
         <v>1</v>
       </c>
       <c r="Q16" t="s">
-        <v>5146</v>
+        <v>5140</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -50476,37 +50461,37 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>3965</v>
+        <v>4127</v>
       </c>
       <c r="C17" t="s">
-        <v>3966</v>
+        <v>4128</v>
       </c>
       <c r="D17">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="E17" t="s">
-        <v>1211</v>
+        <v>1957</v>
       </c>
       <c r="F17" t="s">
-        <v>4598</v>
+        <v>1962</v>
       </c>
       <c r="G17" t="s">
-        <v>1213</v>
+        <v>1959</v>
       </c>
       <c r="H17">
-        <v>265</v>
+        <v>19</v>
       </c>
       <c r="I17" t="s">
-        <v>1212</v>
+        <v>1958</v>
       </c>
       <c r="J17" t="s">
-        <v>1214</v>
+        <v>1960</v>
       </c>
       <c r="K17" t="s">
-        <v>1215</v>
+        <v>1961</v>
       </c>
       <c r="L17" t="s">
-        <v>3965</v>
+        <v>4127</v>
       </c>
       <c r="M17" t="s">
         <v>963</v>
@@ -50521,7 +50506,7 @@
         <v>1</v>
       </c>
       <c r="Q17" t="s">
-        <v>5146</v>
+        <v>5140</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -50529,37 +50514,37 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>4127</v>
+        <v>399</v>
       </c>
       <c r="C18" t="s">
-        <v>4128</v>
+        <v>400</v>
       </c>
       <c r="D18">
-        <v>2004</v>
+        <v>1999</v>
       </c>
       <c r="E18" t="s">
-        <v>1957</v>
+        <v>5272</v>
       </c>
       <c r="F18" t="s">
-        <v>1962</v>
+        <v>5273</v>
       </c>
       <c r="G18" t="s">
-        <v>1959</v>
+        <v>5029</v>
       </c>
       <c r="H18">
-        <v>19</v>
+        <v>177</v>
       </c>
       <c r="I18" t="s">
-        <v>1958</v>
+        <v>5029</v>
       </c>
       <c r="J18" t="s">
-        <v>1960</v>
+        <v>5029</v>
       </c>
       <c r="K18" t="s">
-        <v>1961</v>
+        <v>5029</v>
       </c>
       <c r="L18" t="s">
-        <v>4127</v>
+        <v>399</v>
       </c>
       <c r="M18" t="s">
         <v>963</v>
@@ -50570,74 +50555,21 @@
       <c r="O18" t="s">
         <v>966</v>
       </c>
-      <c r="P18" s="7">
-        <v>1</v>
+      <c r="P18" s="7" t="s">
+        <v>5029</v>
       </c>
       <c r="Q18" t="s">
-        <v>5146</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>399</v>
-      </c>
-      <c r="C19" t="s">
-        <v>400</v>
-      </c>
-      <c r="D19">
-        <v>1999</v>
-      </c>
-      <c r="E19" t="s">
-        <v>5278</v>
-      </c>
-      <c r="F19" t="s">
-        <v>5279</v>
-      </c>
-      <c r="G19" t="s">
-        <v>5029</v>
-      </c>
-      <c r="H19">
-        <v>177</v>
-      </c>
-      <c r="I19" t="s">
-        <v>5029</v>
-      </c>
-      <c r="J19" t="s">
-        <v>5029</v>
-      </c>
-      <c r="K19" t="s">
-        <v>5029</v>
-      </c>
-      <c r="L19" t="s">
-        <v>399</v>
-      </c>
-      <c r="M19" t="s">
-        <v>963</v>
-      </c>
-      <c r="N19" t="s">
-        <v>963</v>
-      </c>
-      <c r="O19" t="s">
-        <v>966</v>
-      </c>
-      <c r="P19" s="7" t="s">
-        <v>5029</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>5372</v>
+        <v>5366</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B2">
     <cfRule type="duplicateValues" dxfId="24" priority="30"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B18">
+  <conditionalFormatting sqref="B17">
     <cfRule type="duplicateValues" dxfId="23" priority="20"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B19">
+  <conditionalFormatting sqref="B18">
     <cfRule type="duplicateValues" dxfId="22" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F2">
@@ -50645,12 +50577,12 @@
       <formula>LEN(TRIM(F1))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F18:F19">
+  <conditionalFormatting sqref="F17:F18">
     <cfRule type="containsBlanks" dxfId="20" priority="15">
-      <formula>LEN(TRIM(F18))=0</formula>
+      <formula>LEN(TRIM(F17))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H17 H20:H1048576">
+  <conditionalFormatting sqref="H19:H1048576 H1:H16">
     <cfRule type="containsBlanks" dxfId="19" priority="38">
       <formula>LEN(TRIM(H1))=0</formula>
     </cfRule>
@@ -50658,13 +50590,13 @@
   <conditionalFormatting sqref="L2">
     <cfRule type="duplicateValues" dxfId="18" priority="28"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L18">
+  <conditionalFormatting sqref="L17">
     <cfRule type="duplicateValues" dxfId="17" priority="16"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L19">
+  <conditionalFormatting sqref="L18">
     <cfRule type="duplicateValues" dxfId="16" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:O19">
+  <conditionalFormatting sqref="M2:O18">
     <cfRule type="containsText" dxfId="15" priority="2" operator="containsText" text="PRIMARY STUDY">
       <formula>NOT(ISERROR(SEARCH("PRIMARY STUDY",M2)))</formula>
     </cfRule>
@@ -50675,18 +50607,20 @@
       <formula>NOT(ISERROR(SEARCH("YES",M2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O18:O19 P1:P1048576">
+  <conditionalFormatting sqref="O17:O18 P1:P1048576">
     <cfRule type="cellIs" dxfId="12" priority="10" operator="between">
       <formula>1</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH("X",O1)))</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O17:P18">
+    <cfRule type="containsBlanks" dxfId="11" priority="1">
+      <formula>LEN(TRIM(O17))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O18:P19">
-    <cfRule type="containsBlanks" dxfId="10" priority="1">
-      <formula>LEN(TRIM(O18))=0</formula>
+  <conditionalFormatting sqref="O17:O18 P1:P1048576">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",O1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1 Q4">

</xml_diff>

<commit_message>
Changed the BPE so that the functional form is now printed into the console when the data frame with results is
</commit_message>
<xml_diff>
--- a/Literature/Literature.xlsx
+++ b/Literature/Literature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hso20\OneDrive\Plocha\IES\Diploma-Thesis\Literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F59C4BC-1D8D-4185-866E-15E3AE35A458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C5C6E9-86CC-421E-B7CC-DE69CE96C238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49578,7 +49578,7 @@
   <dimension ref="A1:Y18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Removed several twin studies with insufficient data. Added more observations
</commit_message>
<xml_diff>
--- a/Literature/Literature.xlsx
+++ b/Literature/Literature.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hso20\OneDrive\Plocha\IES\Diploma-Thesis\Literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C5C6E9-86CC-421E-B7CC-DE69CE96C238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5790807-DFDD-4C9F-AECC-2EE0BADB10E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Query literature" sheetId="5" r:id="rId1"/>
@@ -694,7 +694,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10247" uniqueCount="5367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10224" uniqueCount="5355">
   <si>
     <t>Number</t>
   </si>
@@ -15936,9 +15936,6 @@
     <t>Li et al.</t>
   </si>
   <si>
-    <t>Taubman</t>
-  </si>
-  <si>
     <t>Behrman and Rosenzweig</t>
   </si>
   <si>
@@ -15972,21 +15969,6 @@
     <t>https://www.researchgate.net/profile/Charles-Mulvey/publication/4901303_What_Do_Twins_Studies_Reveal_About_the_Economic_Returns_to_Education_A_Comparison_of_Australian_and_US_Findings/links/5dcbc167458515143506df81/What-Do-Twins-Studies-Reveal-About-the-Economic-Returns-to-Education-A-Comparison-of-Australian-and-US-Findings.pdf</t>
   </si>
   <si>
-    <t>Taubman (1976)</t>
-  </si>
-  <si>
-    <t>The determinants of earnings: Genetics, family, and other environments: A study of white male twins</t>
-  </si>
-  <si>
-    <t>Taubman, Paul. "The determinants of earnings: Genetics, family, and other environments: A study of white male twins." The American Economic Review 66, no. 5 (1976): 858-870.</t>
-  </si>
-  <si>
-    <t>SS9rzvcuvZkJ</t>
-  </si>
-  <si>
-    <t>https://www.jstor.org/stable/pdf/1827497.pdf?refreqid=excelsior%3A65985ad5ad118aff33e2e8897703eed9&amp;ab_segments=&amp;origin=&amp;acceptTC=1</t>
-  </si>
-  <si>
     <t>zjHqohf8afwJ</t>
   </si>
   <si>
@@ -16009,24 +15991,6 @@
   </si>
   <si>
     <t>Behrman, Jere R., and Mark R. Rosenzweig. "“Ability” biases in schooling returns and twins: a test and new estimates." Economics of education review 18, no. 2 (1999): 159-167.</t>
-  </si>
-  <si>
-    <t>Altonji, Joseph G., and Thomas A. Dunn. "Using siblings to estimate the effect of school quality on wages." The Review of Economics and Statistics (1996): 665-671.</t>
-  </si>
-  <si>
-    <t>coRGeUocOSoJ</t>
-  </si>
-  <si>
-    <t>https://www.jstor.org/stable/2109953</t>
-  </si>
-  <si>
-    <t>Altonji &amp; Dunn (1996)</t>
-  </si>
-  <si>
-    <t>Altonji &amp; Dunn</t>
-  </si>
-  <si>
-    <t>Using siblings to estimate the effect of school quality on wages</t>
   </si>
   <si>
     <t>Gensowski, Miriam. "Personality, IQ, and lifetime earnings." Labour Economics 51 (2018): 170-183.</t>
@@ -16801,7 +16765,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -16874,6 +16838,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -17123,7 +17093,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -17170,13 +17140,54 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="49">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAACAC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAACAC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBA8CDC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAACAC"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -17263,41 +17274,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAACAC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAACAC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBA8CDC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <color theme="4" tint="-0.24994659260841701"/>
@@ -17327,13 +17303,6 @@
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAACAC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -17929,27 +17898,27 @@
         <v>962</v>
       </c>
       <c r="N1" s="24" t="s">
-        <v>5131</v>
+        <v>5119</v>
       </c>
       <c r="O1" s="25" t="s">
-        <v>5129</v>
+        <v>5117</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>5137</v>
+        <v>5125</v>
       </c>
       <c r="Q1" s="28" t="s">
         <v>5037</v>
       </c>
       <c r="R1" s="29">
         <f>COUNTIFS($M:$M, "YES", $F:$F, "&lt;&gt;") + Twins!R1</f>
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="T1" s="28" t="s">
         <v>5038</v>
       </c>
       <c r="U1" s="29">
         <f>COUNTIF($L$2:$L$575, "&lt;&gt; ") +Twins!U1</f>
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="V1" s="31"/>
       <c r="W1" s="31"/>
@@ -18110,7 +18079,7 @@
         <v>574</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>5135</v>
+        <v>5123</v>
       </c>
       <c r="U4">
         <f>COUNTIFS($M:$M, "YES", $L:$L, "&lt;&gt;PRIMARY STUDY", $P:$P, "&lt;&gt;Twins")</f>
@@ -18171,7 +18140,7 @@
         <v>574</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>5132</v>
+        <v>5120</v>
       </c>
       <c r="U5" s="37">
         <f>COUNTIFS($N:$N, "YES", $F:$F, "&lt;&gt;")</f>
@@ -18279,7 +18248,7 @@
         <v>5028</v>
       </c>
       <c r="P7" t="s">
-        <v>5361</v>
+        <v>5349</v>
       </c>
       <c r="Q7" s="2" t="s">
         <v>904</v>
@@ -18480,10 +18449,10 @@
         <v>1</v>
       </c>
       <c r="P11" t="s">
-        <v>5136</v>
+        <v>5124</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>5130</v>
+        <v>5118</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
@@ -18536,7 +18505,7 @@
         <v>1</v>
       </c>
       <c r="R12" t="s">
-        <v>5133</v>
+        <v>5121</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
@@ -18589,7 +18558,7 @@
         <v>2</v>
       </c>
       <c r="R13" t="s">
-        <v>5134</v>
+        <v>5122</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
@@ -19842,7 +19811,7 @@
         <v>1</v>
       </c>
       <c r="P38" t="s">
-        <v>5136</v>
+        <v>5124</v>
       </c>
       <c r="R38" t="s">
         <v>904</v>
@@ -19995,7 +19964,7 @@
         <v>2</v>
       </c>
       <c r="P41" t="s">
-        <v>5147</v>
+        <v>5135</v>
       </c>
       <c r="R41" t="s">
         <v>904</v>
@@ -20798,7 +20767,7 @@
         <v>2</v>
       </c>
       <c r="P57" t="s">
-        <v>5139</v>
+        <v>5127</v>
       </c>
       <c r="R57" t="s">
         <v>904</v>
@@ -22451,7 +22420,7 @@
         <v>1</v>
       </c>
       <c r="P90" t="s">
-        <v>5140</v>
+        <v>5128</v>
       </c>
       <c r="R90" t="s">
         <v>904</v>
@@ -22462,7 +22431,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>5141</v>
+        <v>5129</v>
       </c>
       <c r="C91" t="s">
         <v>4015</v>
@@ -23454,7 +23423,7 @@
         <v>1</v>
       </c>
       <c r="P110" t="s">
-        <v>5142</v>
+        <v>5130</v>
       </c>
       <c r="R110" t="s">
         <v>904</v>
@@ -23907,7 +23876,7 @@
         <v>4</v>
       </c>
       <c r="P119" t="s">
-        <v>5143</v>
+        <v>5131</v>
       </c>
       <c r="R119" t="s">
         <v>904</v>
@@ -25201,7 +25170,7 @@
         <v>1765</v>
       </c>
       <c r="L145" t="s">
-        <v>5144</v>
+        <v>5132</v>
       </c>
       <c r="M145" t="s">
         <v>966</v>
@@ -25221,7 +25190,7 @@
         <v>145</v>
       </c>
       <c r="B146" t="s">
-        <v>5145</v>
+        <v>5133</v>
       </c>
       <c r="C146" t="s">
         <v>4080</v>
@@ -25233,7 +25202,7 @@
         <v>1766</v>
       </c>
       <c r="F146" t="s">
-        <v>5146</v>
+        <v>5134</v>
       </c>
       <c r="G146" t="s">
         <v>1768</v>
@@ -25424,7 +25393,7 @@
         <v>149</v>
       </c>
       <c r="B150" t="s">
-        <v>5148</v>
+        <v>5136</v>
       </c>
       <c r="C150" t="s">
         <v>4085</v>
@@ -25433,13 +25402,13 @@
         <v>2012</v>
       </c>
       <c r="E150" t="s">
-        <v>5149</v>
+        <v>5137</v>
       </c>
       <c r="F150" t="s">
-        <v>5150</v>
+        <v>5138</v>
       </c>
       <c r="G150" t="s">
-        <v>5151</v>
+        <v>5139</v>
       </c>
       <c r="H150">
         <v>0</v>
@@ -27328,7 +27297,7 @@
         <v>1</v>
       </c>
       <c r="P187" t="s">
-        <v>5136</v>
+        <v>5124</v>
       </c>
       <c r="R187" t="s">
         <v>904</v>
@@ -44629,16 +44598,16 @@
         <v>3907</v>
       </c>
       <c r="H1" s="23" t="s">
-        <v>5152</v>
+        <v>5140</v>
       </c>
       <c r="I1" s="23" t="s">
-        <v>5153</v>
+        <v>5141</v>
       </c>
       <c r="J1" s="23" t="s">
-        <v>5154</v>
+        <v>5142</v>
       </c>
       <c r="K1" s="23" t="s">
-        <v>5155</v>
+        <v>5143</v>
       </c>
       <c r="L1" s="23" t="s">
         <v>3902</v>
@@ -44659,13 +44628,13 @@
         <v>962</v>
       </c>
       <c r="R1" s="24" t="s">
-        <v>5131</v>
+        <v>5119</v>
       </c>
       <c r="S1" s="25" t="s">
-        <v>5129</v>
+        <v>5117</v>
       </c>
       <c r="T1" s="39" t="s">
-        <v>5137</v>
+        <v>5125</v>
       </c>
       <c r="U1" s="28" t="s">
         <v>5037</v>
@@ -44691,7 +44660,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>5160</v>
+        <v>5148</v>
       </c>
       <c r="C2" s="34" t="s">
         <v>4157</v>
@@ -44700,10 +44669,10 @@
         <v>2010</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>5161</v>
+        <v>5149</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>5162</v>
+        <v>5150</v>
       </c>
       <c r="G2" s="34" t="s">
         <v>5028</v>
@@ -44715,10 +44684,10 @@
         <v>1</v>
       </c>
       <c r="J2" s="34" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K2" s="34" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L2" s="34">
         <v>289</v>
@@ -44757,34 +44726,34 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5163</v>
+        <v>5151</v>
       </c>
       <c r="C3" t="s">
-        <v>5164</v>
+        <v>5152</v>
       </c>
       <c r="D3">
         <v>2000</v>
       </c>
       <c r="E3" t="s">
-        <v>5165</v>
+        <v>5153</v>
       </c>
       <c r="F3" t="s">
-        <v>5166</v>
+        <v>5154</v>
       </c>
       <c r="G3" t="s">
         <v>5028</v>
       </c>
       <c r="H3" t="s">
-        <v>5340</v>
+        <v>5328</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K3" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L3">
         <v>1486</v>
@@ -44799,7 +44768,7 @@
         <v>5028</v>
       </c>
       <c r="P3" t="s">
-        <v>5356</v>
+        <v>5344</v>
       </c>
       <c r="Q3" t="s">
         <v>963</v>
@@ -44825,10 +44794,10 @@
         <v>1995</v>
       </c>
       <c r="E4" t="s">
-        <v>5167</v>
+        <v>5155</v>
       </c>
       <c r="F4" t="s">
-        <v>5168</v>
+        <v>5156</v>
       </c>
       <c r="G4" t="s">
         <v>5028</v>
@@ -44840,10 +44809,10 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K4" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L4">
         <v>321</v>
@@ -44875,34 +44844,34 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5169</v>
+        <v>5157</v>
       </c>
       <c r="C5" t="s">
-        <v>5170</v>
+        <v>5158</v>
       </c>
       <c r="D5">
         <v>1991</v>
       </c>
       <c r="E5" t="s">
-        <v>5171</v>
+        <v>5159</v>
       </c>
       <c r="F5" t="s">
-        <v>5172</v>
+        <v>5160</v>
       </c>
       <c r="G5" t="s">
         <v>5028</v>
       </c>
       <c r="H5" t="s">
-        <v>5341</v>
+        <v>5329</v>
       </c>
       <c r="I5" t="b">
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K5" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L5">
         <v>3590</v>
@@ -44934,19 +44903,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>5173</v>
+        <v>5161</v>
       </c>
       <c r="C6" t="s">
-        <v>5174</v>
+        <v>5162</v>
       </c>
       <c r="D6">
         <v>2005</v>
       </c>
       <c r="E6" t="s">
-        <v>5175</v>
+        <v>5163</v>
       </c>
       <c r="F6" t="s">
-        <v>5176</v>
+        <v>5164</v>
       </c>
       <c r="G6" t="s">
         <v>5028</v>
@@ -44958,10 +44927,10 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K6" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L6">
         <v>1510</v>
@@ -44988,10 +44957,10 @@
         <v>5028</v>
       </c>
       <c r="T6" t="s">
-        <v>5354</v>
+        <v>5342</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>5135</v>
+        <v>5123</v>
       </c>
       <c r="V6">
         <f>COUNTIF($P:$P, "YES")</f>
@@ -45003,34 +44972,34 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>5177</v>
+        <v>5165</v>
       </c>
       <c r="C7" t="s">
-        <v>5178</v>
+        <v>5166</v>
       </c>
       <c r="D7">
         <v>2002</v>
       </c>
       <c r="E7" t="s">
-        <v>5179</v>
+        <v>5167</v>
       </c>
       <c r="F7" t="s">
-        <v>5180</v>
+        <v>5168</v>
       </c>
       <c r="G7" t="s">
         <v>5028</v>
       </c>
       <c r="H7" t="s">
-        <v>5342</v>
+        <v>5330</v>
       </c>
       <c r="I7" t="b">
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K7" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L7">
         <v>321</v>
@@ -45057,7 +45026,7 @@
         <v>1</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>5132</v>
+        <v>5120</v>
       </c>
       <c r="V7">
         <f>COUNTIFS($R:$R, "YES", $F:$F, "&lt;&gt;")</f>
@@ -45078,10 +45047,10 @@
         <v>1998</v>
       </c>
       <c r="E8" t="s">
-        <v>5181</v>
+        <v>5169</v>
       </c>
       <c r="F8" t="s">
-        <v>5182</v>
+        <v>5170</v>
       </c>
       <c r="G8" t="s">
         <v>5028</v>
@@ -45093,10 +45062,10 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K8" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L8">
         <v>588</v>
@@ -45128,34 +45097,34 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>5183</v>
+        <v>5171</v>
       </c>
       <c r="C9" t="s">
-        <v>5184</v>
+        <v>5172</v>
       </c>
       <c r="D9">
         <v>2014</v>
       </c>
       <c r="E9" t="s">
-        <v>5185</v>
+        <v>5173</v>
       </c>
       <c r="F9" t="s">
-        <v>5186</v>
+        <v>5174</v>
       </c>
       <c r="G9" t="s">
         <v>5028</v>
       </c>
       <c r="H9" t="s">
-        <v>5343</v>
+        <v>5331</v>
       </c>
       <c r="I9" t="b">
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K9" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L9">
         <v>73</v>
@@ -45187,34 +45156,34 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>5187</v>
+        <v>5175</v>
       </c>
       <c r="C10" t="s">
-        <v>5188</v>
+        <v>5176</v>
       </c>
       <c r="D10">
         <v>2018</v>
       </c>
       <c r="E10" t="s">
-        <v>5189</v>
+        <v>5177</v>
       </c>
       <c r="F10" t="s">
-        <v>5190</v>
+        <v>5178</v>
       </c>
       <c r="G10" t="s">
         <v>5028</v>
       </c>
       <c r="H10" t="s">
-        <v>5344</v>
+        <v>5332</v>
       </c>
       <c r="I10" t="b">
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K10" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L10">
         <v>74</v>
@@ -45229,7 +45198,7 @@
         <v>5028</v>
       </c>
       <c r="P10" t="s">
-        <v>5355</v>
+        <v>5343</v>
       </c>
       <c r="Q10" t="s">
         <v>963</v>
@@ -45246,19 +45215,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>5191</v>
+        <v>5179</v>
       </c>
       <c r="C11" t="s">
-        <v>5192</v>
+        <v>5180</v>
       </c>
       <c r="D11">
         <v>2014</v>
       </c>
       <c r="E11" t="s">
-        <v>5193</v>
+        <v>5181</v>
       </c>
       <c r="F11" t="s">
-        <v>5194</v>
+        <v>5182</v>
       </c>
       <c r="G11" t="s">
         <v>5028</v>
@@ -45270,10 +45239,10 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K11" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L11">
         <v>17</v>
@@ -45305,7 +45274,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>5195</v>
+        <v>5183</v>
       </c>
       <c r="C12" t="s">
         <v>3928</v>
@@ -45314,25 +45283,25 @@
         <v>1995</v>
       </c>
       <c r="E12" t="s">
-        <v>5196</v>
+        <v>5184</v>
       </c>
       <c r="F12" t="s">
-        <v>5197</v>
+        <v>5185</v>
       </c>
       <c r="G12" t="s">
         <v>5028</v>
       </c>
       <c r="H12" t="s">
-        <v>5345</v>
+        <v>5333</v>
       </c>
       <c r="I12" t="b">
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K12" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L12">
         <v>1789</v>
@@ -45364,7 +45333,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>5198</v>
+        <v>5186</v>
       </c>
       <c r="C13" t="s">
         <v>3928</v>
@@ -45373,25 +45342,25 @@
         <v>2001</v>
       </c>
       <c r="E13" t="s">
-        <v>5199</v>
+        <v>5187</v>
       </c>
       <c r="F13" t="s">
-        <v>5200</v>
+        <v>5188</v>
       </c>
       <c r="G13" t="s">
         <v>5028</v>
       </c>
       <c r="H13" t="s">
-        <v>5342</v>
+        <v>5330</v>
       </c>
       <c r="I13" t="b">
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K13" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L13">
         <v>2928</v>
@@ -45406,7 +45375,7 @@
         <v>5028</v>
       </c>
       <c r="P13" t="s">
-        <v>5357</v>
+        <v>5345</v>
       </c>
       <c r="Q13" t="s">
         <v>963</v>
@@ -45418,7 +45387,7 @@
         <v>1</v>
       </c>
       <c r="T13" t="s">
-        <v>5358</v>
+        <v>5346</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
@@ -45426,7 +45395,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>5201</v>
+        <v>5189</v>
       </c>
       <c r="C14" t="s">
         <v>4356</v>
@@ -45435,25 +45404,25 @@
         <v>2011</v>
       </c>
       <c r="E14" t="s">
-        <v>5202</v>
+        <v>5190</v>
       </c>
       <c r="F14" t="s">
-        <v>5203</v>
+        <v>5191</v>
       </c>
       <c r="G14" t="s">
         <v>5028</v>
       </c>
       <c r="H14" t="s">
-        <v>5346</v>
+        <v>5334</v>
       </c>
       <c r="I14" t="b">
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K14" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L14">
         <v>783</v>
@@ -45485,34 +45454,34 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>5204</v>
+        <v>5192</v>
       </c>
       <c r="C15" t="s">
-        <v>5205</v>
+        <v>5193</v>
       </c>
       <c r="D15">
         <v>2019</v>
       </c>
       <c r="E15" t="s">
-        <v>5206</v>
+        <v>5194</v>
       </c>
       <c r="F15" t="s">
-        <v>5207</v>
+        <v>5195</v>
       </c>
       <c r="G15" t="s">
         <v>5028</v>
       </c>
       <c r="H15" t="s">
-        <v>5347</v>
+        <v>5335</v>
       </c>
       <c r="I15" t="b">
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K15" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L15">
         <v>141</v>
@@ -45539,7 +45508,7 @@
         <v>5028</v>
       </c>
       <c r="T15" t="s">
-        <v>5359</v>
+        <v>5347</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
@@ -45556,10 +45525,10 @@
         <v>1998</v>
       </c>
       <c r="E16" t="s">
-        <v>5208</v>
+        <v>5196</v>
       </c>
       <c r="F16" t="s">
-        <v>5209</v>
+        <v>5197</v>
       </c>
       <c r="G16" t="s">
         <v>5028</v>
@@ -45571,10 +45540,10 @@
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K16" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L16">
         <v>284</v>
@@ -45606,34 +45575,34 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>5210</v>
+        <v>5198</v>
       </c>
       <c r="C17" t="s">
-        <v>5211</v>
+        <v>5199</v>
       </c>
       <c r="D17">
         <v>2010</v>
       </c>
       <c r="E17" t="s">
-        <v>5212</v>
+        <v>5200</v>
       </c>
       <c r="F17" t="s">
-        <v>5213</v>
+        <v>5201</v>
       </c>
       <c r="G17" t="s">
         <v>5028</v>
       </c>
       <c r="H17" t="s">
-        <v>5348</v>
+        <v>5336</v>
       </c>
       <c r="I17" t="b">
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K17" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L17">
         <v>252</v>
@@ -45665,19 +45634,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>5214</v>
+        <v>5202</v>
       </c>
       <c r="C18" t="s">
-        <v>5215</v>
+        <v>5203</v>
       </c>
       <c r="D18">
         <v>1991</v>
       </c>
       <c r="E18" t="s">
-        <v>5216</v>
+        <v>5204</v>
       </c>
       <c r="F18" t="s">
-        <v>5217</v>
+        <v>5205</v>
       </c>
       <c r="G18" t="s">
         <v>5028</v>
@@ -45689,10 +45658,10 @@
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K18" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L18">
         <v>88</v>
@@ -45733,10 +45702,10 @@
         <v>2001</v>
       </c>
       <c r="E19" t="s">
-        <v>5218</v>
+        <v>5206</v>
       </c>
       <c r="F19" t="s">
-        <v>5219</v>
+        <v>5207</v>
       </c>
       <c r="G19" t="s">
         <v>5028</v>
@@ -45748,10 +45717,10 @@
         <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K19" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L19">
         <v>2852</v>
@@ -45792,10 +45761,10 @@
         <v>2002</v>
       </c>
       <c r="E20" t="s">
-        <v>5220</v>
+        <v>5208</v>
       </c>
       <c r="F20" t="s">
-        <v>5221</v>
+        <v>5209</v>
       </c>
       <c r="G20" t="s">
         <v>5028</v>
@@ -45807,10 +45776,10 @@
         <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K20" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L20">
         <v>386</v>
@@ -45842,34 +45811,34 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>5222</v>
+        <v>5210</v>
       </c>
       <c r="C21" t="s">
-        <v>5223</v>
+        <v>5211</v>
       </c>
       <c r="D21">
         <v>2008</v>
       </c>
       <c r="E21" t="s">
-        <v>5224</v>
+        <v>5212</v>
       </c>
       <c r="F21" t="s">
-        <v>5225</v>
+        <v>5213</v>
       </c>
       <c r="G21" t="s">
         <v>5028</v>
       </c>
       <c r="H21" t="s">
-        <v>5349</v>
+        <v>5337</v>
       </c>
       <c r="I21" t="b">
         <v>1</v>
       </c>
       <c r="J21" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K21" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L21">
         <v>494</v>
@@ -45901,19 +45870,19 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>5226</v>
+        <v>5214</v>
       </c>
       <c r="C22" t="s">
-        <v>5227</v>
+        <v>5215</v>
       </c>
       <c r="D22">
         <v>2000</v>
       </c>
       <c r="E22" t="s">
-        <v>5228</v>
+        <v>5216</v>
       </c>
       <c r="F22" t="s">
-        <v>5229</v>
+        <v>5217</v>
       </c>
       <c r="G22" t="s">
         <v>5028</v>
@@ -45925,10 +45894,10 @@
         <v>1</v>
       </c>
       <c r="J22" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K22" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L22">
         <v>101</v>
@@ -45960,34 +45929,34 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>5230</v>
+        <v>5218</v>
       </c>
       <c r="C23" t="s">
-        <v>5231</v>
+        <v>5219</v>
       </c>
       <c r="D23">
         <v>2019</v>
       </c>
       <c r="E23" t="s">
-        <v>5232</v>
+        <v>5220</v>
       </c>
       <c r="F23" t="s">
-        <v>5233</v>
+        <v>5221</v>
       </c>
       <c r="G23" t="s">
         <v>5028</v>
       </c>
       <c r="H23" t="s">
-        <v>5344</v>
+        <v>5332</v>
       </c>
       <c r="I23" t="b">
         <v>1</v>
       </c>
       <c r="J23" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K23" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L23">
         <v>92</v>
@@ -46014,7 +45983,7 @@
         <v>5028</v>
       </c>
       <c r="T23" t="s">
-        <v>5360</v>
+        <v>5348</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
@@ -46022,19 +45991,19 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>5234</v>
+        <v>5222</v>
       </c>
       <c r="C24" t="s">
-        <v>5235</v>
+        <v>5223</v>
       </c>
       <c r="D24">
         <v>2005</v>
       </c>
       <c r="E24" t="s">
-        <v>5236</v>
+        <v>5224</v>
       </c>
       <c r="F24" t="s">
-        <v>5237</v>
+        <v>5225</v>
       </c>
       <c r="G24" t="s">
         <v>5028</v>
@@ -46046,10 +46015,10 @@
         <v>1</v>
       </c>
       <c r="J24" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K24" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L24">
         <v>171</v>
@@ -46081,34 +46050,34 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>5238</v>
+        <v>5226</v>
       </c>
       <c r="C25" t="s">
-        <v>5239</v>
+        <v>5227</v>
       </c>
       <c r="D25">
         <v>1995</v>
       </c>
       <c r="E25" t="s">
-        <v>5240</v>
+        <v>5228</v>
       </c>
       <c r="F25" t="s">
-        <v>5241</v>
+        <v>5229</v>
       </c>
       <c r="G25" t="s">
         <v>5028</v>
       </c>
       <c r="H25" t="s">
-        <v>5349</v>
+        <v>5337</v>
       </c>
       <c r="I25" t="b">
         <v>1</v>
       </c>
       <c r="J25" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K25" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L25">
         <v>662</v>
@@ -46140,7 +46109,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>5242</v>
+        <v>5230</v>
       </c>
       <c r="C26" t="s">
         <v>3930</v>
@@ -46149,10 +46118,10 @@
         <v>1995</v>
       </c>
       <c r="E26" t="s">
-        <v>5243</v>
+        <v>5231</v>
       </c>
       <c r="F26" t="s">
-        <v>5244</v>
+        <v>5232</v>
       </c>
       <c r="G26" t="s">
         <v>5028</v>
@@ -46164,10 +46133,10 @@
         <v>1</v>
       </c>
       <c r="J26" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K26" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L26">
         <v>888</v>
@@ -46199,7 +46168,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>5245</v>
+        <v>5233</v>
       </c>
       <c r="C27" t="s">
         <v>3930</v>
@@ -46208,10 +46177,10 @@
         <v>1999</v>
       </c>
       <c r="E27" t="s">
-        <v>5246</v>
+        <v>5234</v>
       </c>
       <c r="F27" t="s">
-        <v>5247</v>
+        <v>5235</v>
       </c>
       <c r="G27" t="s">
         <v>5028</v>
@@ -46223,10 +46192,10 @@
         <v>1</v>
       </c>
       <c r="J27" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K27" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L27">
         <v>100</v>
@@ -46267,25 +46236,25 @@
         <v>2003</v>
       </c>
       <c r="E28" t="s">
-        <v>5248</v>
+        <v>5236</v>
       </c>
       <c r="F28" t="s">
-        <v>5249</v>
+        <v>5237</v>
       </c>
       <c r="G28" t="s">
         <v>5028</v>
       </c>
       <c r="H28" t="s">
-        <v>5344</v>
+        <v>5332</v>
       </c>
       <c r="I28" t="b">
         <v>1</v>
       </c>
       <c r="J28" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K28" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L28">
         <v>860</v>
@@ -46317,19 +46286,19 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>5250</v>
+        <v>5238</v>
       </c>
       <c r="C29" t="s">
-        <v>5251</v>
+        <v>5239</v>
       </c>
       <c r="D29">
         <v>2007</v>
       </c>
       <c r="E29" t="s">
-        <v>5252</v>
+        <v>5240</v>
       </c>
       <c r="F29" t="s">
-        <v>5253</v>
+        <v>5241</v>
       </c>
       <c r="G29" t="s">
         <v>5028</v>
@@ -46341,10 +46310,10 @@
         <v>1</v>
       </c>
       <c r="J29" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K29" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L29">
         <v>27</v>
@@ -46376,34 +46345,34 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>5254</v>
+        <v>5242</v>
       </c>
       <c r="C30" t="s">
-        <v>5255</v>
+        <v>5243</v>
       </c>
       <c r="D30">
         <v>2006</v>
       </c>
       <c r="E30" t="s">
-        <v>5256</v>
+        <v>5244</v>
       </c>
       <c r="F30" t="s">
-        <v>5257</v>
+        <v>5245</v>
       </c>
       <c r="G30" t="s">
         <v>5028</v>
       </c>
       <c r="H30" t="s">
-        <v>5350</v>
+        <v>5338</v>
       </c>
       <c r="I30" t="b">
         <v>1</v>
       </c>
       <c r="J30" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K30" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L30">
         <v>1427</v>
@@ -46430,7 +46399,7 @@
         <v>3</v>
       </c>
       <c r="T30" t="s">
-        <v>5362</v>
+        <v>5350</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
@@ -46438,34 +46407,34 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>5258</v>
+        <v>5246</v>
       </c>
       <c r="C31" t="s">
-        <v>5259</v>
+        <v>5247</v>
       </c>
       <c r="D31">
         <v>2011</v>
       </c>
       <c r="E31" t="s">
-        <v>5260</v>
+        <v>5248</v>
       </c>
       <c r="F31" t="s">
-        <v>5261</v>
+        <v>5249</v>
       </c>
       <c r="G31" t="s">
         <v>5028</v>
       </c>
       <c r="H31" t="s">
-        <v>5349</v>
+        <v>5337</v>
       </c>
       <c r="I31" t="b">
         <v>1</v>
       </c>
       <c r="J31" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K31" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L31">
         <v>80</v>
@@ -46497,19 +46466,19 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>5262</v>
+        <v>5250</v>
       </c>
       <c r="C32" t="s">
-        <v>5263</v>
+        <v>5251</v>
       </c>
       <c r="D32">
         <v>1999</v>
       </c>
       <c r="E32" t="s">
-        <v>5264</v>
+        <v>5252</v>
       </c>
       <c r="F32" t="s">
-        <v>5265</v>
+        <v>5253</v>
       </c>
       <c r="G32" t="s">
         <v>5028</v>
@@ -46521,10 +46490,10 @@
         <v>1</v>
       </c>
       <c r="J32" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K32" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L32">
         <v>182</v>
@@ -46556,34 +46525,34 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>5266</v>
+        <v>5254</v>
       </c>
       <c r="C33" t="s">
-        <v>5267</v>
+        <v>5255</v>
       </c>
       <c r="D33">
         <v>2004</v>
       </c>
       <c r="E33" t="s">
-        <v>5268</v>
+        <v>5256</v>
       </c>
       <c r="F33" t="s">
-        <v>5269</v>
+        <v>5257</v>
       </c>
       <c r="G33" t="s">
         <v>5028</v>
       </c>
       <c r="H33" t="s">
-        <v>5344</v>
+        <v>5332</v>
       </c>
       <c r="I33" t="b">
         <v>1</v>
       </c>
       <c r="J33" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K33" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L33">
         <v>389</v>
@@ -46624,10 +46593,10 @@
         <v>1999</v>
       </c>
       <c r="E34" t="s">
-        <v>5270</v>
+        <v>5258</v>
       </c>
       <c r="F34" t="s">
-        <v>5271</v>
+        <v>5259</v>
       </c>
       <c r="G34" t="s">
         <v>5028</v>
@@ -46639,10 +46608,10 @@
         <v>1</v>
       </c>
       <c r="J34" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K34" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L34">
         <v>177</v>
@@ -46657,7 +46626,7 @@
         <v>5028</v>
       </c>
       <c r="P34" t="s">
-        <v>5363</v>
+        <v>5351</v>
       </c>
       <c r="Q34" t="s">
         <v>963</v>
@@ -46683,10 +46652,10 @@
         <v>2001</v>
       </c>
       <c r="E35" t="s">
-        <v>5272</v>
+        <v>5260</v>
       </c>
       <c r="F35" t="s">
-        <v>5273</v>
+        <v>5261</v>
       </c>
       <c r="G35" t="s">
         <v>5028</v>
@@ -46698,10 +46667,10 @@
         <v>1</v>
       </c>
       <c r="J35" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K35" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L35">
         <v>217</v>
@@ -46733,19 +46702,19 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>5274</v>
+        <v>5262</v>
       </c>
       <c r="C36" t="s">
-        <v>5275</v>
+        <v>5263</v>
       </c>
       <c r="D36">
         <v>1993</v>
       </c>
       <c r="E36" t="s">
-        <v>5276</v>
+        <v>5264</v>
       </c>
       <c r="F36" t="s">
-        <v>5277</v>
+        <v>5265</v>
       </c>
       <c r="G36" t="s">
         <v>5028</v>
@@ -46757,10 +46726,10 @@
         <v>1</v>
       </c>
       <c r="J36" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K36" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L36">
         <v>1442</v>
@@ -46801,10 +46770,10 @@
         <v>2006</v>
       </c>
       <c r="E37" t="s">
-        <v>5278</v>
+        <v>5266</v>
       </c>
       <c r="F37" t="s">
-        <v>5279</v>
+        <v>5267</v>
       </c>
       <c r="G37" t="s">
         <v>5028</v>
@@ -46816,10 +46785,10 @@
         <v>1</v>
       </c>
       <c r="J37" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K37" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L37">
         <v>254</v>
@@ -46860,10 +46829,10 @@
         <v>1998</v>
       </c>
       <c r="E38" t="s">
-        <v>5280</v>
+        <v>5268</v>
       </c>
       <c r="F38" t="s">
-        <v>5281</v>
+        <v>5269</v>
       </c>
       <c r="G38" t="s">
         <v>5028</v>
@@ -46875,10 +46844,10 @@
         <v>1</v>
       </c>
       <c r="J38" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K38" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L38">
         <v>301</v>
@@ -46919,25 +46888,25 @@
         <v>2001</v>
       </c>
       <c r="E39" t="s">
-        <v>5282</v>
+        <v>5270</v>
       </c>
       <c r="F39" t="s">
-        <v>5283</v>
+        <v>5271</v>
       </c>
       <c r="G39" t="s">
         <v>5028</v>
       </c>
       <c r="H39" t="s">
-        <v>5351</v>
+        <v>5339</v>
       </c>
       <c r="I39" t="b">
         <v>1</v>
       </c>
       <c r="J39" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K39" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L39">
         <v>293</v>
@@ -46952,7 +46921,7 @@
         <v>5028</v>
       </c>
       <c r="P39" t="s">
-        <v>5365</v>
+        <v>5353</v>
       </c>
       <c r="Q39" t="s">
         <v>963</v>
@@ -46978,25 +46947,25 @@
         <v>2008</v>
       </c>
       <c r="E40" t="s">
-        <v>5284</v>
+        <v>5272</v>
       </c>
       <c r="F40" t="s">
-        <v>5285</v>
+        <v>5273</v>
       </c>
       <c r="G40" t="s">
         <v>5028</v>
       </c>
       <c r="H40" t="s">
-        <v>5349</v>
+        <v>5337</v>
       </c>
       <c r="I40" t="b">
         <v>1</v>
       </c>
       <c r="J40" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K40" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L40">
         <v>153</v>
@@ -47028,19 +46997,19 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>5286</v>
+        <v>5274</v>
       </c>
       <c r="C41" t="s">
-        <v>5287</v>
+        <v>5275</v>
       </c>
       <c r="D41">
         <v>2001</v>
       </c>
       <c r="E41" t="s">
-        <v>5288</v>
+        <v>5276</v>
       </c>
       <c r="F41" t="s">
-        <v>5289</v>
+        <v>5277</v>
       </c>
       <c r="G41" t="s">
         <v>5028</v>
@@ -47052,10 +47021,10 @@
         <v>1</v>
       </c>
       <c r="J41" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K41" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L41">
         <v>188</v>
@@ -47087,34 +47056,34 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>5290</v>
+        <v>5278</v>
       </c>
       <c r="C42" t="s">
-        <v>5291</v>
+        <v>5279</v>
       </c>
       <c r="D42">
         <v>2004</v>
       </c>
       <c r="E42" t="s">
-        <v>5292</v>
+        <v>5280</v>
       </c>
       <c r="F42" t="s">
-        <v>5293</v>
+        <v>5281</v>
       </c>
       <c r="G42" t="s">
         <v>5028</v>
       </c>
       <c r="H42" t="s">
-        <v>5344</v>
+        <v>5332</v>
       </c>
       <c r="I42" t="b">
         <v>1</v>
       </c>
       <c r="J42" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K42" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L42">
         <v>93</v>
@@ -47155,25 +47124,25 @@
         <v>1995</v>
       </c>
       <c r="E43" t="s">
-        <v>5294</v>
+        <v>5282</v>
       </c>
       <c r="F43" t="s">
-        <v>5295</v>
+        <v>5283</v>
       </c>
       <c r="G43" t="s">
         <v>5028</v>
       </c>
       <c r="H43" t="s">
-        <v>5352</v>
+        <v>5340</v>
       </c>
       <c r="I43" t="b">
         <v>1</v>
       </c>
       <c r="J43" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K43" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L43">
         <v>372</v>
@@ -47188,7 +47157,7 @@
         <v>5028</v>
       </c>
       <c r="P43" t="s">
-        <v>5363</v>
+        <v>5351</v>
       </c>
       <c r="Q43" t="s">
         <v>963</v>
@@ -47200,7 +47169,7 @@
         <v>5028</v>
       </c>
       <c r="T43" t="s">
-        <v>5366</v>
+        <v>5354</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
@@ -47208,19 +47177,19 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>5296</v>
+        <v>5284</v>
       </c>
       <c r="C44" t="s">
-        <v>5297</v>
+        <v>5285</v>
       </c>
       <c r="D44">
         <v>2004</v>
       </c>
       <c r="E44" t="s">
-        <v>5298</v>
+        <v>5286</v>
       </c>
       <c r="F44" t="s">
-        <v>5299</v>
+        <v>5287</v>
       </c>
       <c r="G44" t="s">
         <v>5028</v>
@@ -47232,10 +47201,10 @@
         <v>1</v>
       </c>
       <c r="J44" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K44" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L44">
         <v>1830</v>
@@ -47267,19 +47236,19 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>5300</v>
+        <v>5288</v>
       </c>
       <c r="C45" t="s">
-        <v>5301</v>
+        <v>5289</v>
       </c>
       <c r="D45">
         <v>2005</v>
       </c>
       <c r="E45" t="s">
-        <v>5302</v>
+        <v>5290</v>
       </c>
       <c r="F45" t="s">
-        <v>5303</v>
+        <v>5291</v>
       </c>
       <c r="G45" t="s">
         <v>5028</v>
@@ -47291,10 +47260,10 @@
         <v>1</v>
       </c>
       <c r="J45" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K45" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L45">
         <v>345</v>
@@ -47326,34 +47295,34 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>5304</v>
+        <v>5292</v>
       </c>
       <c r="C46" t="s">
-        <v>5305</v>
+        <v>5293</v>
       </c>
       <c r="D46">
         <v>2006</v>
       </c>
       <c r="E46" t="s">
-        <v>5306</v>
+        <v>5294</v>
       </c>
       <c r="F46" t="s">
-        <v>5307</v>
+        <v>5295</v>
       </c>
       <c r="G46" t="s">
         <v>5028</v>
       </c>
       <c r="H46" t="s">
-        <v>5353</v>
+        <v>5341</v>
       </c>
       <c r="I46" t="b">
         <v>1</v>
       </c>
       <c r="J46" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K46" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L46">
         <v>1005</v>
@@ -47368,7 +47337,7 @@
         <v>5028</v>
       </c>
       <c r="P46" t="s">
-        <v>5355</v>
+        <v>5343</v>
       </c>
       <c r="Q46" t="s">
         <v>963</v>
@@ -47385,19 +47354,19 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>5308</v>
+        <v>5296</v>
       </c>
       <c r="C47" t="s">
-        <v>5309</v>
+        <v>5297</v>
       </c>
       <c r="D47">
         <v>2006</v>
       </c>
       <c r="E47" t="s">
-        <v>5310</v>
+        <v>5298</v>
       </c>
       <c r="F47" t="s">
-        <v>5311</v>
+        <v>5299</v>
       </c>
       <c r="G47" t="s">
         <v>5028</v>
@@ -47409,10 +47378,10 @@
         <v>1</v>
       </c>
       <c r="J47" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K47" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L47">
         <v>596</v>
@@ -47427,7 +47396,7 @@
         <v>5028</v>
       </c>
       <c r="P47" t="s">
-        <v>5355</v>
+        <v>5343</v>
       </c>
       <c r="Q47" t="s">
         <v>963</v>
@@ -47444,19 +47413,19 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>5312</v>
+        <v>5300</v>
       </c>
       <c r="C48" t="s">
-        <v>5313</v>
+        <v>5301</v>
       </c>
       <c r="D48">
         <v>2005</v>
       </c>
       <c r="E48" t="s">
-        <v>5314</v>
+        <v>5302</v>
       </c>
       <c r="F48" t="s">
-        <v>5156</v>
+        <v>5144</v>
       </c>
       <c r="G48" t="s">
         <v>5028</v>
@@ -47468,10 +47437,10 @@
         <v>1</v>
       </c>
       <c r="J48" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K48" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L48">
         <v>386</v>
@@ -47512,25 +47481,25 @@
         <v>1982</v>
       </c>
       <c r="E49" t="s">
-        <v>5315</v>
+        <v>5303</v>
       </c>
       <c r="F49" t="s">
-        <v>5157</v>
+        <v>5145</v>
       </c>
       <c r="G49" t="s">
         <v>5028</v>
       </c>
       <c r="H49" t="s">
-        <v>5352</v>
+        <v>5340</v>
       </c>
       <c r="I49" t="b">
         <v>1</v>
       </c>
       <c r="J49" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K49" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L49">
         <v>55</v>
@@ -47571,10 +47540,10 @@
         <v>1985</v>
       </c>
       <c r="E50" t="s">
-        <v>5316</v>
+        <v>5304</v>
       </c>
       <c r="F50" t="s">
-        <v>5158</v>
+        <v>5146</v>
       </c>
       <c r="G50" t="s">
         <v>5028</v>
@@ -47586,10 +47555,10 @@
         <v>1</v>
       </c>
       <c r="J50" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K50" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L50">
         <v>2143</v>
@@ -47621,7 +47590,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>5317</v>
+        <v>5305</v>
       </c>
       <c r="C51" t="s">
         <v>674</v>
@@ -47630,10 +47599,10 @@
         <v>1979</v>
       </c>
       <c r="E51" t="s">
-        <v>5318</v>
+        <v>5306</v>
       </c>
       <c r="F51" t="s">
-        <v>5159</v>
+        <v>5147</v>
       </c>
       <c r="G51" t="s">
         <v>5028</v>
@@ -47645,10 +47614,10 @@
         <v>1</v>
       </c>
       <c r="J51" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K51" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L51">
         <v>251</v>
@@ -47680,19 +47649,19 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>5319</v>
+        <v>5307</v>
       </c>
       <c r="C52" t="s">
-        <v>5320</v>
+        <v>5308</v>
       </c>
       <c r="D52">
         <v>1997</v>
       </c>
       <c r="E52" t="s">
-        <v>5321</v>
+        <v>5309</v>
       </c>
       <c r="F52" t="s">
-        <v>5322</v>
+        <v>5310</v>
       </c>
       <c r="G52" t="s">
         <v>5028</v>
@@ -47704,10 +47673,10 @@
         <v>1</v>
       </c>
       <c r="J52" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K52" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L52">
         <v>9699</v>
@@ -47739,34 +47708,34 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>5323</v>
+        <v>5311</v>
       </c>
       <c r="C53" t="s">
-        <v>5324</v>
+        <v>5312</v>
       </c>
       <c r="D53">
         <v>2014</v>
       </c>
       <c r="E53" t="s">
-        <v>5325</v>
+        <v>5313</v>
       </c>
       <c r="F53" t="s">
-        <v>5326</v>
+        <v>5314</v>
       </c>
       <c r="G53" t="s">
         <v>5028</v>
       </c>
       <c r="H53" t="s">
-        <v>5342</v>
+        <v>5330</v>
       </c>
       <c r="I53" t="b">
         <v>1</v>
       </c>
       <c r="J53" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K53" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L53">
         <v>264</v>
@@ -47798,19 +47767,19 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>5327</v>
+        <v>5315</v>
       </c>
       <c r="C54" t="s">
-        <v>5328</v>
+        <v>5316</v>
       </c>
       <c r="D54">
         <v>2001</v>
       </c>
       <c r="E54" t="s">
-        <v>5329</v>
+        <v>5317</v>
       </c>
       <c r="F54" t="s">
-        <v>5330</v>
+        <v>5318</v>
       </c>
       <c r="G54" t="s">
         <v>5028</v>
@@ -47822,10 +47791,10 @@
         <v>1</v>
       </c>
       <c r="J54" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K54" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L54">
         <v>261</v>
@@ -47857,19 +47826,19 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>5331</v>
+        <v>5319</v>
       </c>
       <c r="C55" t="s">
-        <v>5332</v>
+        <v>5320</v>
       </c>
       <c r="D55">
         <v>1999</v>
       </c>
       <c r="E55" t="s">
-        <v>5333</v>
+        <v>5321</v>
       </c>
       <c r="F55" t="s">
-        <v>5334</v>
+        <v>5322</v>
       </c>
       <c r="G55" t="s">
         <v>5028</v>
@@ -47881,10 +47850,10 @@
         <v>1</v>
       </c>
       <c r="J55" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K55" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L55">
         <v>423</v>
@@ -47916,19 +47885,19 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>5335</v>
+        <v>5323</v>
       </c>
       <c r="C56" t="s">
-        <v>5336</v>
+        <v>5324</v>
       </c>
       <c r="D56">
         <v>2011</v>
       </c>
       <c r="E56" t="s">
-        <v>5337</v>
+        <v>5325</v>
       </c>
       <c r="F56" t="s">
-        <v>5338</v>
+        <v>5326</v>
       </c>
       <c r="G56" t="s">
         <v>5028</v>
@@ -47940,10 +47909,10 @@
         <v>1</v>
       </c>
       <c r="J56" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="K56" t="s">
-        <v>5339</v>
+        <v>5327</v>
       </c>
       <c r="L56">
         <v>197</v>
@@ -49575,10 +49544,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:Y18"/>
+  <dimension ref="A1:Y16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49630,24 +49599,24 @@
         <v>962</v>
       </c>
       <c r="O1" s="23" t="s">
-        <v>5131</v>
-      </c>
-      <c r="P1" s="40" t="s">
-        <v>5137</v>
+        <v>5119</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>5125</v>
       </c>
       <c r="Q1" s="28" t="s">
         <v>5037</v>
       </c>
       <c r="R1" s="29">
         <f>COUNTIFS($N:$N, "YES", $F:$F, "&lt;&gt;")</f>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="T1" s="28" t="s">
         <v>5038</v>
       </c>
       <c r="U1" s="29">
-        <f>COUNTIF($M$2:$M$571, "YES")</f>
-        <v>17</v>
+        <f>COUNTIF($M$2:$M$569, "YES")</f>
+        <v>15</v>
       </c>
       <c r="V1" s="31"/>
       <c r="W1" s="31"/>
@@ -49824,10 +49793,10 @@
         <v>2003</v>
       </c>
       <c r="E5" t="s">
+        <v>5081</v>
+      </c>
+      <c r="F5" t="s">
         <v>5082</v>
-      </c>
-      <c r="F5" t="s">
-        <v>5083</v>
       </c>
       <c r="G5" t="s">
         <v>5029</v>
@@ -49871,10 +49840,10 @@
         <v>2012</v>
       </c>
       <c r="E6" t="s">
-        <v>5085</v>
+        <v>5084</v>
       </c>
       <c r="F6" t="s">
-        <v>5084</v>
+        <v>5083</v>
       </c>
       <c r="G6" t="s">
         <v>5029</v>
@@ -49883,13 +49852,13 @@
         <v>176</v>
       </c>
       <c r="I6" t="s">
+        <v>5085</v>
+      </c>
+      <c r="J6" t="s">
         <v>5086</v>
       </c>
-      <c r="J6" t="s">
-        <v>5087</v>
-      </c>
       <c r="K6" t="s">
-        <v>5087</v>
+        <v>5086</v>
       </c>
       <c r="L6" t="s">
         <v>5071</v>
@@ -49904,11 +49873,11 @@
         <v>966</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>5135</v>
+        <v>5123</v>
       </c>
       <c r="R6">
         <f>COUNTIFS($N:$N, "YES", $M:$M, "&lt;&gt;PRIMARY STUDY")</f>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="W6" t="s">
         <v>5075</v>
@@ -49928,10 +49897,10 @@
         <v>1995</v>
       </c>
       <c r="E7" t="s">
+        <v>5087</v>
+      </c>
+      <c r="F7" t="s">
         <v>5088</v>
-      </c>
-      <c r="F7" t="s">
-        <v>5089</v>
       </c>
       <c r="G7" t="s">
         <v>5029</v>
@@ -49940,13 +49909,13 @@
         <v>372</v>
       </c>
       <c r="I7" t="s">
+        <v>5089</v>
+      </c>
+      <c r="J7" t="s">
         <v>5090</v>
       </c>
-      <c r="J7" t="s">
-        <v>5091</v>
-      </c>
       <c r="K7" t="s">
-        <v>5091</v>
+        <v>5090</v>
       </c>
       <c r="L7" t="s">
         <v>5072</v>
@@ -49961,7 +49930,7 @@
         <v>966</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>5132</v>
+        <v>5120</v>
       </c>
       <c r="R7">
         <f>COUNTIFS($O:$O, "YES", $F:$F, "&lt;&gt;")</f>
@@ -49973,37 +49942,34 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>5092</v>
+        <v>5073</v>
       </c>
       <c r="C8" t="s">
-        <v>5080</v>
+        <v>4077</v>
       </c>
       <c r="D8">
-        <v>1976</v>
+        <v>1994</v>
       </c>
       <c r="E8" t="s">
+        <v>5094</v>
+      </c>
+      <c r="F8" t="s">
         <v>5093</v>
-      </c>
-      <c r="F8" t="s">
-        <v>5094</v>
       </c>
       <c r="G8" t="s">
         <v>5029</v>
       </c>
       <c r="H8">
-        <v>382</v>
+        <v>616</v>
       </c>
       <c r="I8" t="s">
-        <v>5095</v>
+        <v>5091</v>
       </c>
       <c r="J8" t="s">
-        <v>5096</v>
-      </c>
-      <c r="K8" t="s">
-        <v>5096</v>
+        <v>5092</v>
       </c>
       <c r="L8" t="s">
-        <v>5092</v>
+        <v>5073</v>
       </c>
       <c r="M8" t="s">
         <v>963</v>
@@ -50020,34 +49986,37 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>5073</v>
+        <v>5074</v>
       </c>
       <c r="C9" t="s">
-        <v>4077</v>
+        <v>5080</v>
       </c>
       <c r="D9">
-        <v>1994</v>
+        <v>1999</v>
       </c>
       <c r="E9" t="s">
-        <v>5100</v>
+        <v>5097</v>
       </c>
       <c r="F9" t="s">
-        <v>5099</v>
+        <v>5098</v>
       </c>
       <c r="G9" t="s">
         <v>5029</v>
       </c>
       <c r="H9">
-        <v>616</v>
+        <v>196</v>
       </c>
       <c r="I9" t="s">
-        <v>5097</v>
+        <v>5095</v>
       </c>
       <c r="J9" t="s">
-        <v>5098</v>
+        <v>5096</v>
+      </c>
+      <c r="K9" t="s">
+        <v>5096</v>
       </c>
       <c r="L9" t="s">
-        <v>5073</v>
+        <v>5074</v>
       </c>
       <c r="M9" t="s">
         <v>963</v>
@@ -50064,37 +50033,37 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>5074</v>
+        <v>5102</v>
       </c>
       <c r="C10" t="s">
-        <v>5081</v>
+        <v>5103</v>
       </c>
       <c r="D10">
-        <v>1999</v>
+        <v>2018</v>
       </c>
       <c r="E10" t="s">
-        <v>5103</v>
+        <v>5104</v>
       </c>
       <c r="F10" t="s">
-        <v>5104</v>
+        <v>5099</v>
       </c>
       <c r="G10" t="s">
         <v>5029</v>
       </c>
       <c r="H10">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="I10" t="s">
+        <v>5100</v>
+      </c>
+      <c r="J10" t="s">
         <v>5101</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
+        <v>5101</v>
+      </c>
+      <c r="L10" t="s">
         <v>5102</v>
-      </c>
-      <c r="K10" t="s">
-        <v>5102</v>
-      </c>
-      <c r="L10" t="s">
-        <v>5074</v>
       </c>
       <c r="M10" t="s">
         <v>963</v>
@@ -50117,7 +50086,7 @@
         <v>5109</v>
       </c>
       <c r="D11">
-        <v>1996</v>
+        <v>2012</v>
       </c>
       <c r="E11" t="s">
         <v>5110</v>
@@ -50129,12 +50098,15 @@
         <v>5029</v>
       </c>
       <c r="H11">
-        <v>218</v>
+        <v>18</v>
       </c>
       <c r="I11" t="s">
         <v>5106</v>
       </c>
       <c r="J11" t="s">
+        <v>5107</v>
+      </c>
+      <c r="K11" t="s">
         <v>5107</v>
       </c>
       <c r="L11" t="s">
@@ -50155,37 +50127,37 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>5114</v>
+        <v>5115</v>
       </c>
       <c r="C12" t="s">
-        <v>5115</v>
+        <v>5112</v>
       </c>
       <c r="D12">
-        <v>2018</v>
+        <v>2020</v>
       </c>
       <c r="E12" t="s">
         <v>5116</v>
       </c>
       <c r="F12" t="s">
-        <v>5111</v>
+        <v>5113</v>
       </c>
       <c r="G12" t="s">
         <v>5029</v>
       </c>
       <c r="H12">
-        <v>181</v>
+        <v>11</v>
       </c>
       <c r="I12" t="s">
-        <v>5112</v>
+        <v>5114</v>
       </c>
       <c r="J12" t="s">
-        <v>5113</v>
+        <v>5111</v>
       </c>
       <c r="K12" t="s">
-        <v>5113</v>
+        <v>5111</v>
       </c>
       <c r="L12" t="s">
-        <v>5114</v>
+        <v>5115</v>
       </c>
       <c r="M12" t="s">
         <v>963</v>
@@ -50202,37 +50174,37 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>5120</v>
+        <v>3935</v>
       </c>
       <c r="C13" t="s">
-        <v>5121</v>
+        <v>3936</v>
       </c>
       <c r="D13">
-        <v>2012</v>
+        <v>2005</v>
       </c>
       <c r="E13" t="s">
-        <v>5122</v>
+        <v>1072</v>
       </c>
       <c r="F13" t="s">
-        <v>5117</v>
+        <v>970</v>
       </c>
       <c r="G13" t="s">
-        <v>5029</v>
+        <v>1074</v>
       </c>
       <c r="H13">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="I13" t="s">
-        <v>5118</v>
+        <v>1073</v>
       </c>
       <c r="J13" t="s">
-        <v>5119</v>
+        <v>1075</v>
       </c>
       <c r="K13" t="s">
-        <v>5119</v>
+        <v>1075</v>
       </c>
       <c r="L13" t="s">
-        <v>5120</v>
+        <v>3935</v>
       </c>
       <c r="M13" t="s">
         <v>963</v>
@@ -50242,6 +50214,9 @@
       </c>
       <c r="O13" s="7" t="s">
         <v>966</v>
+      </c>
+      <c r="P13" t="s">
+        <v>5126</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
@@ -50249,37 +50224,37 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>5127</v>
+        <v>3965</v>
       </c>
       <c r="C14" t="s">
-        <v>5124</v>
+        <v>3966</v>
       </c>
       <c r="D14">
-        <v>2020</v>
+        <v>2003</v>
       </c>
       <c r="E14" t="s">
-        <v>5128</v>
+        <v>1211</v>
       </c>
       <c r="F14" t="s">
-        <v>5125</v>
+        <v>4598</v>
       </c>
       <c r="G14" t="s">
-        <v>5029</v>
+        <v>1213</v>
       </c>
       <c r="H14">
-        <v>11</v>
+        <v>265</v>
       </c>
       <c r="I14" t="s">
-        <v>5126</v>
+        <v>1212</v>
       </c>
       <c r="J14" t="s">
-        <v>5123</v>
+        <v>1214</v>
       </c>
       <c r="K14" t="s">
-        <v>5123</v>
+        <v>1215</v>
       </c>
       <c r="L14" t="s">
-        <v>5127</v>
+        <v>3965</v>
       </c>
       <c r="M14" t="s">
         <v>963</v>
@@ -50289,6 +50264,9 @@
       </c>
       <c r="O14" s="7" t="s">
         <v>966</v>
+      </c>
+      <c r="P14" t="s">
+        <v>5126</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
@@ -50296,37 +50274,37 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>3935</v>
+        <v>4127</v>
       </c>
       <c r="C15" t="s">
-        <v>3936</v>
+        <v>4128</v>
       </c>
       <c r="D15">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="E15" t="s">
-        <v>1072</v>
+        <v>1957</v>
       </c>
       <c r="F15" t="s">
-        <v>970</v>
+        <v>1962</v>
       </c>
       <c r="G15" t="s">
-        <v>1074</v>
+        <v>1959</v>
       </c>
       <c r="H15">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="I15" t="s">
-        <v>1073</v>
+        <v>1958</v>
       </c>
       <c r="J15" t="s">
-        <v>1075</v>
+        <v>1960</v>
       </c>
       <c r="K15" t="s">
-        <v>1075</v>
+        <v>1961</v>
       </c>
       <c r="L15" t="s">
-        <v>3935</v>
+        <v>4127</v>
       </c>
       <c r="M15" t="s">
         <v>963</v>
@@ -50338,7 +50316,7 @@
         <v>966</v>
       </c>
       <c r="P15" t="s">
-        <v>5138</v>
+        <v>5126</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
@@ -50346,37 +50324,37 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>3965</v>
+        <v>399</v>
       </c>
       <c r="C16" t="s">
-        <v>3966</v>
+        <v>400</v>
       </c>
       <c r="D16">
-        <v>2003</v>
+        <v>1999</v>
       </c>
       <c r="E16" t="s">
-        <v>1211</v>
+        <v>5258</v>
       </c>
       <c r="F16" t="s">
-        <v>4598</v>
+        <v>5259</v>
       </c>
       <c r="G16" t="s">
-        <v>1213</v>
+        <v>5028</v>
       </c>
       <c r="H16">
-        <v>265</v>
+        <v>177</v>
       </c>
       <c r="I16" t="s">
-        <v>1212</v>
+        <v>5028</v>
       </c>
       <c r="J16" t="s">
-        <v>1214</v>
+        <v>5028</v>
       </c>
       <c r="K16" t="s">
-        <v>1215</v>
+        <v>5028</v>
       </c>
       <c r="L16" t="s">
-        <v>3965</v>
+        <v>399</v>
       </c>
       <c r="M16" t="s">
         <v>963</v>
@@ -50388,117 +50366,18 @@
         <v>966</v>
       </c>
       <c r="P16" t="s">
-        <v>5138</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>4127</v>
-      </c>
-      <c r="C17" t="s">
-        <v>4128</v>
-      </c>
-      <c r="D17">
-        <v>2004</v>
-      </c>
-      <c r="E17" t="s">
-        <v>1957</v>
-      </c>
-      <c r="F17" t="s">
-        <v>1962</v>
-      </c>
-      <c r="G17" t="s">
-        <v>1959</v>
-      </c>
-      <c r="H17">
-        <v>19</v>
-      </c>
-      <c r="I17" t="s">
-        <v>1958</v>
-      </c>
-      <c r="J17" t="s">
-        <v>1960</v>
-      </c>
-      <c r="K17" t="s">
-        <v>1961</v>
-      </c>
-      <c r="L17" t="s">
-        <v>4127</v>
-      </c>
-      <c r="M17" t="s">
-        <v>963</v>
-      </c>
-      <c r="N17" t="s">
-        <v>963</v>
-      </c>
-      <c r="O17" s="7" t="s">
-        <v>966</v>
-      </c>
-      <c r="P17" t="s">
-        <v>5138</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>399</v>
-      </c>
-      <c r="C18" t="s">
-        <v>400</v>
-      </c>
-      <c r="D18">
-        <v>1999</v>
-      </c>
-      <c r="E18" t="s">
-        <v>5270</v>
-      </c>
-      <c r="F18" t="s">
-        <v>5271</v>
-      </c>
-      <c r="G18" t="s">
-        <v>5028</v>
-      </c>
-      <c r="H18">
-        <v>177</v>
-      </c>
-      <c r="I18" t="s">
-        <v>5028</v>
-      </c>
-      <c r="J18" t="s">
-        <v>5028</v>
-      </c>
-      <c r="K18" t="s">
-        <v>5028</v>
-      </c>
-      <c r="L18" t="s">
-        <v>399</v>
-      </c>
-      <c r="M18" t="s">
-        <v>963</v>
-      </c>
-      <c r="N18" t="s">
-        <v>963</v>
-      </c>
-      <c r="O18" s="7" t="s">
-        <v>966</v>
-      </c>
-      <c r="P18" t="s">
-        <v>5364</v>
+        <v>5352</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="10" type="noConversion"/>
   <conditionalFormatting sqref="B1:B2">
     <cfRule type="duplicateValues" dxfId="24" priority="30"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B17">
+  <conditionalFormatting sqref="B15">
     <cfRule type="duplicateValues" dxfId="23" priority="20"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B18">
+  <conditionalFormatting sqref="B16">
     <cfRule type="duplicateValues" dxfId="22" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F2">
@@ -50506,66 +50385,62 @@
       <formula>LEN(TRIM(F1))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F17:F18">
+  <conditionalFormatting sqref="F15:F16">
     <cfRule type="containsBlanks" dxfId="20" priority="15">
-      <formula>LEN(TRIM(F17))=0</formula>
+      <formula>LEN(TRIM(F15))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H16 H19:H1048576">
-    <cfRule type="containsBlanks" dxfId="19" priority="38">
+  <conditionalFormatting sqref="H17:H1048576 H1:H14">
+    <cfRule type="containsBlanks" dxfId="5" priority="38">
       <formula>LEN(TRIM(H1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2">
-    <cfRule type="duplicateValues" dxfId="18" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="28"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L17">
-    <cfRule type="duplicateValues" dxfId="17" priority="16"/>
+  <conditionalFormatting sqref="L15">
+    <cfRule type="duplicateValues" dxfId="18" priority="16"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L18">
-    <cfRule type="duplicateValues" dxfId="16" priority="5"/>
+  <conditionalFormatting sqref="L16">
+    <cfRule type="duplicateValues" dxfId="17" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:O18">
-    <cfRule type="containsText" dxfId="15" priority="2" operator="containsText" text="PRIMARY STUDY">
+  <conditionalFormatting sqref="M2:O16">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="PRIMARY STUDY">
       <formula>NOT(ISERROR(SEARCH("PRIMARY STUDY",M2)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="14" priority="3" operator="notContains" text="YES">
+    <cfRule type="notContainsText" dxfId="3" priority="3" operator="notContains" text="YES">
       <formula>ISERROR(SEARCH("YES",M2))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="4" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",M2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O17:O18">
-    <cfRule type="cellIs" dxfId="12" priority="10" operator="between">
+  <conditionalFormatting sqref="O15:O16">
+    <cfRule type="containsBlanks" dxfId="16" priority="1">
+      <formula>LEN(TRIM(O15))=0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="10" operator="between">
       <formula>1</formula>
       <formula>4</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O17:O18">
-    <cfRule type="containsBlanks" dxfId="11" priority="1">
-      <formula>LEN(TRIM(O17))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O17:O18">
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH("X",O17)))</formula>
+    <cfRule type="containsText" dxfId="14" priority="11" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",O15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1 P4">
-    <cfRule type="cellIs" dxfId="9" priority="32" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="32" operator="between">
       <formula>1</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="33" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="0" priority="33" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",P1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q2">
-    <cfRule type="duplicateValues" dxfId="7" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1">
-    <cfRule type="duplicateValues" dxfId="6" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="29"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
@@ -59458,10 +59333,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L1 A1:K251">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="11" priority="1">
       <formula>$K1=FALSE</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="9">
+    <cfRule type="expression" dxfId="10" priority="9">
       <formula>$J1=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -67406,10 +67281,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J1:J253 J257 J259:J1048576">
-    <cfRule type="containsText" dxfId="3" priority="12" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="13" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="8" priority="13" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -67426,10 +67301,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M17">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",M17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",M17)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added more twin study data, removed several wrongly identified studies.
</commit_message>
<xml_diff>
--- a/Literature/Literature.xlsx
+++ b/Literature/Literature.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hso20\OneDrive\Plocha\IES\Diploma-Thesis\Literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5790807-DFDD-4C9F-AECC-2EE0BADB10E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A10534B-7646-4323-870B-F2A3E6131FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Query literature" sheetId="5" r:id="rId1"/>
@@ -694,7 +694,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10224" uniqueCount="5355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10199" uniqueCount="5349">
   <si>
     <t>Number</t>
   </si>
@@ -15991,24 +15991,6 @@
   </si>
   <si>
     <t>Behrman, Jere R., and Mark R. Rosenzweig. "“Ability” biases in schooling returns and twins: a test and new estimates." Economics of education review 18, no. 2 (1999): 159-167.</t>
-  </si>
-  <si>
-    <t>Gensowski, Miriam. "Personality, IQ, and lifetime earnings." Labour Economics 51 (2018): 170-183.</t>
-  </si>
-  <si>
-    <t>1AmpL352mVcJ</t>
-  </si>
-  <si>
-    <t>https://www.econstor.eu/bitstream/10419/99046/1/dp8235.pdf</t>
-  </si>
-  <si>
-    <t>Gensowski (2018)</t>
-  </si>
-  <si>
-    <t>Gensowski</t>
-  </si>
-  <si>
-    <t>Personality, IQ, and lifetime earnings</t>
   </si>
   <si>
     <t>Nakamuro, Makiko, and Tomohiko Inui. "Estimating the Returns to Education Using a Sample of Twins–The case of Japan." In RIETI Discussion Paper Series 12-E-076. 2012.</t>
@@ -17149,48 +17131,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFAACAC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAACAC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBA8CDC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFAACAC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
@@ -17274,6 +17214,41 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAACAC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAACAC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBA8CDC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <color theme="4" tint="-0.24994659260841701"/>
@@ -17303,6 +17278,13 @@
       <fill>
         <patternFill>
           <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFAACAC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -17898,27 +17880,27 @@
         <v>962</v>
       </c>
       <c r="N1" s="24" t="s">
+        <v>5113</v>
+      </c>
+      <c r="O1" s="25" t="s">
+        <v>5111</v>
+      </c>
+      <c r="P1" s="5" t="s">
         <v>5119</v>
-      </c>
-      <c r="O1" s="25" t="s">
-        <v>5117</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>5125</v>
       </c>
       <c r="Q1" s="28" t="s">
         <v>5037</v>
       </c>
       <c r="R1" s="29">
         <f>COUNTIFS($M:$M, "YES", $F:$F, "&lt;&gt;") + Twins!R1</f>
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="T1" s="28" t="s">
         <v>5038</v>
       </c>
       <c r="U1" s="29">
         <f>COUNTIF($L$2:$L$575, "&lt;&gt; ") +Twins!U1</f>
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="V1" s="31"/>
       <c r="W1" s="31"/>
@@ -18079,7 +18061,7 @@
         <v>574</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>5123</v>
+        <v>5117</v>
       </c>
       <c r="U4">
         <f>COUNTIFS($M:$M, "YES", $L:$L, "&lt;&gt;PRIMARY STUDY", $P:$P, "&lt;&gt;Twins")</f>
@@ -18140,7 +18122,7 @@
         <v>574</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>5120</v>
+        <v>5114</v>
       </c>
       <c r="U5" s="37">
         <f>COUNTIFS($N:$N, "YES", $F:$F, "&lt;&gt;")</f>
@@ -18248,7 +18230,7 @@
         <v>5028</v>
       </c>
       <c r="P7" t="s">
-        <v>5349</v>
+        <v>5343</v>
       </c>
       <c r="Q7" s="2" t="s">
         <v>904</v>
@@ -18449,10 +18431,10 @@
         <v>1</v>
       </c>
       <c r="P11" t="s">
-        <v>5124</v>
+        <v>5118</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>5118</v>
+        <v>5112</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
@@ -18505,7 +18487,7 @@
         <v>1</v>
       </c>
       <c r="R12" t="s">
-        <v>5121</v>
+        <v>5115</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
@@ -18558,7 +18540,7 @@
         <v>2</v>
       </c>
       <c r="R13" t="s">
-        <v>5122</v>
+        <v>5116</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
@@ -19811,7 +19793,7 @@
         <v>1</v>
       </c>
       <c r="P38" t="s">
-        <v>5124</v>
+        <v>5118</v>
       </c>
       <c r="R38" t="s">
         <v>904</v>
@@ -19964,7 +19946,7 @@
         <v>2</v>
       </c>
       <c r="P41" t="s">
-        <v>5135</v>
+        <v>5129</v>
       </c>
       <c r="R41" t="s">
         <v>904</v>
@@ -20767,7 +20749,7 @@
         <v>2</v>
       </c>
       <c r="P57" t="s">
-        <v>5127</v>
+        <v>5121</v>
       </c>
       <c r="R57" t="s">
         <v>904</v>
@@ -22420,7 +22402,7 @@
         <v>1</v>
       </c>
       <c r="P90" t="s">
-        <v>5128</v>
+        <v>5122</v>
       </c>
       <c r="R90" t="s">
         <v>904</v>
@@ -22431,7 +22413,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>5129</v>
+        <v>5123</v>
       </c>
       <c r="C91" t="s">
         <v>4015</v>
@@ -23423,7 +23405,7 @@
         <v>1</v>
       </c>
       <c r="P110" t="s">
-        <v>5130</v>
+        <v>5124</v>
       </c>
       <c r="R110" t="s">
         <v>904</v>
@@ -23876,7 +23858,7 @@
         <v>4</v>
       </c>
       <c r="P119" t="s">
-        <v>5131</v>
+        <v>5125</v>
       </c>
       <c r="R119" t="s">
         <v>904</v>
@@ -25170,7 +25152,7 @@
         <v>1765</v>
       </c>
       <c r="L145" t="s">
-        <v>5132</v>
+        <v>5126</v>
       </c>
       <c r="M145" t="s">
         <v>966</v>
@@ -25190,7 +25172,7 @@
         <v>145</v>
       </c>
       <c r="B146" t="s">
-        <v>5133</v>
+        <v>5127</v>
       </c>
       <c r="C146" t="s">
         <v>4080</v>
@@ -25202,7 +25184,7 @@
         <v>1766</v>
       </c>
       <c r="F146" t="s">
-        <v>5134</v>
+        <v>5128</v>
       </c>
       <c r="G146" t="s">
         <v>1768</v>
@@ -25393,7 +25375,7 @@
         <v>149</v>
       </c>
       <c r="B150" t="s">
-        <v>5136</v>
+        <v>5130</v>
       </c>
       <c r="C150" t="s">
         <v>4085</v>
@@ -25402,13 +25384,13 @@
         <v>2012</v>
       </c>
       <c r="E150" t="s">
-        <v>5137</v>
+        <v>5131</v>
       </c>
       <c r="F150" t="s">
-        <v>5138</v>
+        <v>5132</v>
       </c>
       <c r="G150" t="s">
-        <v>5139</v>
+        <v>5133</v>
       </c>
       <c r="H150">
         <v>0</v>
@@ -27297,7 +27279,7 @@
         <v>1</v>
       </c>
       <c r="P187" t="s">
-        <v>5124</v>
+        <v>5118</v>
       </c>
       <c r="R187" t="s">
         <v>904</v>
@@ -44598,16 +44580,16 @@
         <v>3907</v>
       </c>
       <c r="H1" s="23" t="s">
-        <v>5140</v>
+        <v>5134</v>
       </c>
       <c r="I1" s="23" t="s">
-        <v>5141</v>
+        <v>5135</v>
       </c>
       <c r="J1" s="23" t="s">
-        <v>5142</v>
+        <v>5136</v>
       </c>
       <c r="K1" s="23" t="s">
-        <v>5143</v>
+        <v>5137</v>
       </c>
       <c r="L1" s="23" t="s">
         <v>3902</v>
@@ -44628,13 +44610,13 @@
         <v>962</v>
       </c>
       <c r="R1" s="24" t="s">
+        <v>5113</v>
+      </c>
+      <c r="S1" s="25" t="s">
+        <v>5111</v>
+      </c>
+      <c r="T1" s="39" t="s">
         <v>5119</v>
-      </c>
-      <c r="S1" s="25" t="s">
-        <v>5117</v>
-      </c>
-      <c r="T1" s="39" t="s">
-        <v>5125</v>
       </c>
       <c r="U1" s="28" t="s">
         <v>5037</v>
@@ -44660,7 +44642,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>5148</v>
+        <v>5142</v>
       </c>
       <c r="C2" s="34" t="s">
         <v>4157</v>
@@ -44669,10 +44651,10 @@
         <v>2010</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>5149</v>
+        <v>5143</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>5150</v>
+        <v>5144</v>
       </c>
       <c r="G2" s="34" t="s">
         <v>5028</v>
@@ -44684,10 +44666,10 @@
         <v>1</v>
       </c>
       <c r="J2" s="34" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K2" s="34" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L2" s="34">
         <v>289</v>
@@ -44726,34 +44708,34 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5151</v>
+        <v>5145</v>
       </c>
       <c r="C3" t="s">
-        <v>5152</v>
+        <v>5146</v>
       </c>
       <c r="D3">
         <v>2000</v>
       </c>
       <c r="E3" t="s">
-        <v>5153</v>
+        <v>5147</v>
       </c>
       <c r="F3" t="s">
-        <v>5154</v>
+        <v>5148</v>
       </c>
       <c r="G3" t="s">
         <v>5028</v>
       </c>
       <c r="H3" t="s">
-        <v>5328</v>
+        <v>5322</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K3" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L3">
         <v>1486</v>
@@ -44768,7 +44750,7 @@
         <v>5028</v>
       </c>
       <c r="P3" t="s">
-        <v>5344</v>
+        <v>5338</v>
       </c>
       <c r="Q3" t="s">
         <v>963</v>
@@ -44794,10 +44776,10 @@
         <v>1995</v>
       </c>
       <c r="E4" t="s">
-        <v>5155</v>
+        <v>5149</v>
       </c>
       <c r="F4" t="s">
-        <v>5156</v>
+        <v>5150</v>
       </c>
       <c r="G4" t="s">
         <v>5028</v>
@@ -44809,10 +44791,10 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K4" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L4">
         <v>321</v>
@@ -44844,34 +44826,34 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5157</v>
+        <v>5151</v>
       </c>
       <c r="C5" t="s">
-        <v>5158</v>
+        <v>5152</v>
       </c>
       <c r="D5">
         <v>1991</v>
       </c>
       <c r="E5" t="s">
-        <v>5159</v>
+        <v>5153</v>
       </c>
       <c r="F5" t="s">
-        <v>5160</v>
+        <v>5154</v>
       </c>
       <c r="G5" t="s">
         <v>5028</v>
       </c>
       <c r="H5" t="s">
-        <v>5329</v>
+        <v>5323</v>
       </c>
       <c r="I5" t="b">
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K5" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L5">
         <v>3590</v>
@@ -44903,19 +44885,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>5161</v>
+        <v>5155</v>
       </c>
       <c r="C6" t="s">
-        <v>5162</v>
+        <v>5156</v>
       </c>
       <c r="D6">
         <v>2005</v>
       </c>
       <c r="E6" t="s">
-        <v>5163</v>
+        <v>5157</v>
       </c>
       <c r="F6" t="s">
-        <v>5164</v>
+        <v>5158</v>
       </c>
       <c r="G6" t="s">
         <v>5028</v>
@@ -44927,10 +44909,10 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K6" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L6">
         <v>1510</v>
@@ -44957,10 +44939,10 @@
         <v>5028</v>
       </c>
       <c r="T6" t="s">
-        <v>5342</v>
+        <v>5336</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>5123</v>
+        <v>5117</v>
       </c>
       <c r="V6">
         <f>COUNTIF($P:$P, "YES")</f>
@@ -44972,34 +44954,34 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>5165</v>
+        <v>5159</v>
       </c>
       <c r="C7" t="s">
-        <v>5166</v>
+        <v>5160</v>
       </c>
       <c r="D7">
         <v>2002</v>
       </c>
       <c r="E7" t="s">
-        <v>5167</v>
+        <v>5161</v>
       </c>
       <c r="F7" t="s">
-        <v>5168</v>
+        <v>5162</v>
       </c>
       <c r="G7" t="s">
         <v>5028</v>
       </c>
       <c r="H7" t="s">
-        <v>5330</v>
+        <v>5324</v>
       </c>
       <c r="I7" t="b">
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K7" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L7">
         <v>321</v>
@@ -45026,7 +45008,7 @@
         <v>1</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>5120</v>
+        <v>5114</v>
       </c>
       <c r="V7">
         <f>COUNTIFS($R:$R, "YES", $F:$F, "&lt;&gt;")</f>
@@ -45047,10 +45029,10 @@
         <v>1998</v>
       </c>
       <c r="E8" t="s">
-        <v>5169</v>
+        <v>5163</v>
       </c>
       <c r="F8" t="s">
-        <v>5170</v>
+        <v>5164</v>
       </c>
       <c r="G8" t="s">
         <v>5028</v>
@@ -45062,10 +45044,10 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K8" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L8">
         <v>588</v>
@@ -45097,34 +45079,34 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>5171</v>
+        <v>5165</v>
       </c>
       <c r="C9" t="s">
-        <v>5172</v>
+        <v>5166</v>
       </c>
       <c r="D9">
         <v>2014</v>
       </c>
       <c r="E9" t="s">
-        <v>5173</v>
+        <v>5167</v>
       </c>
       <c r="F9" t="s">
-        <v>5174</v>
+        <v>5168</v>
       </c>
       <c r="G9" t="s">
         <v>5028</v>
       </c>
       <c r="H9" t="s">
-        <v>5331</v>
+        <v>5325</v>
       </c>
       <c r="I9" t="b">
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K9" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L9">
         <v>73</v>
@@ -45156,34 +45138,34 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>5175</v>
+        <v>5169</v>
       </c>
       <c r="C10" t="s">
-        <v>5176</v>
+        <v>5170</v>
       </c>
       <c r="D10">
         <v>2018</v>
       </c>
       <c r="E10" t="s">
-        <v>5177</v>
+        <v>5171</v>
       </c>
       <c r="F10" t="s">
-        <v>5178</v>
+        <v>5172</v>
       </c>
       <c r="G10" t="s">
         <v>5028</v>
       </c>
       <c r="H10" t="s">
-        <v>5332</v>
+        <v>5326</v>
       </c>
       <c r="I10" t="b">
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K10" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L10">
         <v>74</v>
@@ -45198,7 +45180,7 @@
         <v>5028</v>
       </c>
       <c r="P10" t="s">
-        <v>5343</v>
+        <v>5337</v>
       </c>
       <c r="Q10" t="s">
         <v>963</v>
@@ -45215,19 +45197,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>5179</v>
+        <v>5173</v>
       </c>
       <c r="C11" t="s">
-        <v>5180</v>
+        <v>5174</v>
       </c>
       <c r="D11">
         <v>2014</v>
       </c>
       <c r="E11" t="s">
-        <v>5181</v>
+        <v>5175</v>
       </c>
       <c r="F11" t="s">
-        <v>5182</v>
+        <v>5176</v>
       </c>
       <c r="G11" t="s">
         <v>5028</v>
@@ -45239,10 +45221,10 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K11" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L11">
         <v>17</v>
@@ -45274,7 +45256,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>5183</v>
+        <v>5177</v>
       </c>
       <c r="C12" t="s">
         <v>3928</v>
@@ -45283,25 +45265,25 @@
         <v>1995</v>
       </c>
       <c r="E12" t="s">
-        <v>5184</v>
+        <v>5178</v>
       </c>
       <c r="F12" t="s">
-        <v>5185</v>
+        <v>5179</v>
       </c>
       <c r="G12" t="s">
         <v>5028</v>
       </c>
       <c r="H12" t="s">
-        <v>5333</v>
+        <v>5327</v>
       </c>
       <c r="I12" t="b">
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K12" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L12">
         <v>1789</v>
@@ -45333,7 +45315,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>5186</v>
+        <v>5180</v>
       </c>
       <c r="C13" t="s">
         <v>3928</v>
@@ -45342,25 +45324,25 @@
         <v>2001</v>
       </c>
       <c r="E13" t="s">
-        <v>5187</v>
+        <v>5181</v>
       </c>
       <c r="F13" t="s">
-        <v>5188</v>
+        <v>5182</v>
       </c>
       <c r="G13" t="s">
         <v>5028</v>
       </c>
       <c r="H13" t="s">
-        <v>5330</v>
+        <v>5324</v>
       </c>
       <c r="I13" t="b">
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K13" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L13">
         <v>2928</v>
@@ -45375,7 +45357,7 @@
         <v>5028</v>
       </c>
       <c r="P13" t="s">
-        <v>5345</v>
+        <v>5339</v>
       </c>
       <c r="Q13" t="s">
         <v>963</v>
@@ -45387,7 +45369,7 @@
         <v>1</v>
       </c>
       <c r="T13" t="s">
-        <v>5346</v>
+        <v>5340</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
@@ -45395,7 +45377,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>5189</v>
+        <v>5183</v>
       </c>
       <c r="C14" t="s">
         <v>4356</v>
@@ -45404,25 +45386,25 @@
         <v>2011</v>
       </c>
       <c r="E14" t="s">
-        <v>5190</v>
+        <v>5184</v>
       </c>
       <c r="F14" t="s">
-        <v>5191</v>
+        <v>5185</v>
       </c>
       <c r="G14" t="s">
         <v>5028</v>
       </c>
       <c r="H14" t="s">
-        <v>5334</v>
+        <v>5328</v>
       </c>
       <c r="I14" t="b">
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K14" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L14">
         <v>783</v>
@@ -45454,34 +45436,34 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>5192</v>
+        <v>5186</v>
       </c>
       <c r="C15" t="s">
-        <v>5193</v>
+        <v>5187</v>
       </c>
       <c r="D15">
         <v>2019</v>
       </c>
       <c r="E15" t="s">
-        <v>5194</v>
+        <v>5188</v>
       </c>
       <c r="F15" t="s">
-        <v>5195</v>
+        <v>5189</v>
       </c>
       <c r="G15" t="s">
         <v>5028</v>
       </c>
       <c r="H15" t="s">
-        <v>5335</v>
+        <v>5329</v>
       </c>
       <c r="I15" t="b">
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K15" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L15">
         <v>141</v>
@@ -45508,7 +45490,7 @@
         <v>5028</v>
       </c>
       <c r="T15" t="s">
-        <v>5347</v>
+        <v>5341</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
@@ -45525,10 +45507,10 @@
         <v>1998</v>
       </c>
       <c r="E16" t="s">
-        <v>5196</v>
+        <v>5190</v>
       </c>
       <c r="F16" t="s">
-        <v>5197</v>
+        <v>5191</v>
       </c>
       <c r="G16" t="s">
         <v>5028</v>
@@ -45540,10 +45522,10 @@
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K16" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L16">
         <v>284</v>
@@ -45575,34 +45557,34 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>5198</v>
+        <v>5192</v>
       </c>
       <c r="C17" t="s">
-        <v>5199</v>
+        <v>5193</v>
       </c>
       <c r="D17">
         <v>2010</v>
       </c>
       <c r="E17" t="s">
-        <v>5200</v>
+        <v>5194</v>
       </c>
       <c r="F17" t="s">
-        <v>5201</v>
+        <v>5195</v>
       </c>
       <c r="G17" t="s">
         <v>5028</v>
       </c>
       <c r="H17" t="s">
-        <v>5336</v>
+        <v>5330</v>
       </c>
       <c r="I17" t="b">
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K17" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L17">
         <v>252</v>
@@ -45634,19 +45616,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>5202</v>
+        <v>5196</v>
       </c>
       <c r="C18" t="s">
-        <v>5203</v>
+        <v>5197</v>
       </c>
       <c r="D18">
         <v>1991</v>
       </c>
       <c r="E18" t="s">
-        <v>5204</v>
+        <v>5198</v>
       </c>
       <c r="F18" t="s">
-        <v>5205</v>
+        <v>5199</v>
       </c>
       <c r="G18" t="s">
         <v>5028</v>
@@ -45658,10 +45640,10 @@
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K18" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L18">
         <v>88</v>
@@ -45702,10 +45684,10 @@
         <v>2001</v>
       </c>
       <c r="E19" t="s">
-        <v>5206</v>
+        <v>5200</v>
       </c>
       <c r="F19" t="s">
-        <v>5207</v>
+        <v>5201</v>
       </c>
       <c r="G19" t="s">
         <v>5028</v>
@@ -45717,10 +45699,10 @@
         <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K19" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L19">
         <v>2852</v>
@@ -45761,10 +45743,10 @@
         <v>2002</v>
       </c>
       <c r="E20" t="s">
-        <v>5208</v>
+        <v>5202</v>
       </c>
       <c r="F20" t="s">
-        <v>5209</v>
+        <v>5203</v>
       </c>
       <c r="G20" t="s">
         <v>5028</v>
@@ -45776,10 +45758,10 @@
         <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K20" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L20">
         <v>386</v>
@@ -45811,34 +45793,34 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>5210</v>
+        <v>5204</v>
       </c>
       <c r="C21" t="s">
-        <v>5211</v>
+        <v>5205</v>
       </c>
       <c r="D21">
         <v>2008</v>
       </c>
       <c r="E21" t="s">
-        <v>5212</v>
+        <v>5206</v>
       </c>
       <c r="F21" t="s">
-        <v>5213</v>
+        <v>5207</v>
       </c>
       <c r="G21" t="s">
         <v>5028</v>
       </c>
       <c r="H21" t="s">
-        <v>5337</v>
+        <v>5331</v>
       </c>
       <c r="I21" t="b">
         <v>1</v>
       </c>
       <c r="J21" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K21" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L21">
         <v>494</v>
@@ -45870,19 +45852,19 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>5214</v>
+        <v>5208</v>
       </c>
       <c r="C22" t="s">
-        <v>5215</v>
+        <v>5209</v>
       </c>
       <c r="D22">
         <v>2000</v>
       </c>
       <c r="E22" t="s">
-        <v>5216</v>
+        <v>5210</v>
       </c>
       <c r="F22" t="s">
-        <v>5217</v>
+        <v>5211</v>
       </c>
       <c r="G22" t="s">
         <v>5028</v>
@@ -45894,10 +45876,10 @@
         <v>1</v>
       </c>
       <c r="J22" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K22" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L22">
         <v>101</v>
@@ -45929,34 +45911,34 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>5218</v>
+        <v>5212</v>
       </c>
       <c r="C23" t="s">
-        <v>5219</v>
+        <v>5213</v>
       </c>
       <c r="D23">
         <v>2019</v>
       </c>
       <c r="E23" t="s">
-        <v>5220</v>
+        <v>5214</v>
       </c>
       <c r="F23" t="s">
-        <v>5221</v>
+        <v>5215</v>
       </c>
       <c r="G23" t="s">
         <v>5028</v>
       </c>
       <c r="H23" t="s">
-        <v>5332</v>
+        <v>5326</v>
       </c>
       <c r="I23" t="b">
         <v>1</v>
       </c>
       <c r="J23" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K23" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L23">
         <v>92</v>
@@ -45983,7 +45965,7 @@
         <v>5028</v>
       </c>
       <c r="T23" t="s">
-        <v>5348</v>
+        <v>5342</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
@@ -45991,19 +45973,19 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>5222</v>
+        <v>5216</v>
       </c>
       <c r="C24" t="s">
-        <v>5223</v>
+        <v>5217</v>
       </c>
       <c r="D24">
         <v>2005</v>
       </c>
       <c r="E24" t="s">
-        <v>5224</v>
+        <v>5218</v>
       </c>
       <c r="F24" t="s">
-        <v>5225</v>
+        <v>5219</v>
       </c>
       <c r="G24" t="s">
         <v>5028</v>
@@ -46015,10 +45997,10 @@
         <v>1</v>
       </c>
       <c r="J24" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K24" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L24">
         <v>171</v>
@@ -46050,34 +46032,34 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>5226</v>
+        <v>5220</v>
       </c>
       <c r="C25" t="s">
-        <v>5227</v>
+        <v>5221</v>
       </c>
       <c r="D25">
         <v>1995</v>
       </c>
       <c r="E25" t="s">
-        <v>5228</v>
+        <v>5222</v>
       </c>
       <c r="F25" t="s">
-        <v>5229</v>
+        <v>5223</v>
       </c>
       <c r="G25" t="s">
         <v>5028</v>
       </c>
       <c r="H25" t="s">
-        <v>5337</v>
+        <v>5331</v>
       </c>
       <c r="I25" t="b">
         <v>1</v>
       </c>
       <c r="J25" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K25" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L25">
         <v>662</v>
@@ -46109,7 +46091,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>5230</v>
+        <v>5224</v>
       </c>
       <c r="C26" t="s">
         <v>3930</v>
@@ -46118,10 +46100,10 @@
         <v>1995</v>
       </c>
       <c r="E26" t="s">
-        <v>5231</v>
+        <v>5225</v>
       </c>
       <c r="F26" t="s">
-        <v>5232</v>
+        <v>5226</v>
       </c>
       <c r="G26" t="s">
         <v>5028</v>
@@ -46133,10 +46115,10 @@
         <v>1</v>
       </c>
       <c r="J26" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K26" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L26">
         <v>888</v>
@@ -46168,7 +46150,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>5233</v>
+        <v>5227</v>
       </c>
       <c r="C27" t="s">
         <v>3930</v>
@@ -46177,10 +46159,10 @@
         <v>1999</v>
       </c>
       <c r="E27" t="s">
-        <v>5234</v>
+        <v>5228</v>
       </c>
       <c r="F27" t="s">
-        <v>5235</v>
+        <v>5229</v>
       </c>
       <c r="G27" t="s">
         <v>5028</v>
@@ -46192,10 +46174,10 @@
         <v>1</v>
       </c>
       <c r="J27" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K27" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L27">
         <v>100</v>
@@ -46236,25 +46218,25 @@
         <v>2003</v>
       </c>
       <c r="E28" t="s">
-        <v>5236</v>
+        <v>5230</v>
       </c>
       <c r="F28" t="s">
-        <v>5237</v>
+        <v>5231</v>
       </c>
       <c r="G28" t="s">
         <v>5028</v>
       </c>
       <c r="H28" t="s">
-        <v>5332</v>
+        <v>5326</v>
       </c>
       <c r="I28" t="b">
         <v>1</v>
       </c>
       <c r="J28" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K28" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L28">
         <v>860</v>
@@ -46286,19 +46268,19 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>5238</v>
+        <v>5232</v>
       </c>
       <c r="C29" t="s">
-        <v>5239</v>
+        <v>5233</v>
       </c>
       <c r="D29">
         <v>2007</v>
       </c>
       <c r="E29" t="s">
-        <v>5240</v>
+        <v>5234</v>
       </c>
       <c r="F29" t="s">
-        <v>5241</v>
+        <v>5235</v>
       </c>
       <c r="G29" t="s">
         <v>5028</v>
@@ -46310,10 +46292,10 @@
         <v>1</v>
       </c>
       <c r="J29" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K29" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L29">
         <v>27</v>
@@ -46345,34 +46327,34 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>5242</v>
+        <v>5236</v>
       </c>
       <c r="C30" t="s">
-        <v>5243</v>
+        <v>5237</v>
       </c>
       <c r="D30">
         <v>2006</v>
       </c>
       <c r="E30" t="s">
-        <v>5244</v>
+        <v>5238</v>
       </c>
       <c r="F30" t="s">
-        <v>5245</v>
+        <v>5239</v>
       </c>
       <c r="G30" t="s">
         <v>5028</v>
       </c>
       <c r="H30" t="s">
-        <v>5338</v>
+        <v>5332</v>
       </c>
       <c r="I30" t="b">
         <v>1</v>
       </c>
       <c r="J30" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K30" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L30">
         <v>1427</v>
@@ -46399,7 +46381,7 @@
         <v>3</v>
       </c>
       <c r="T30" t="s">
-        <v>5350</v>
+        <v>5344</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
@@ -46407,34 +46389,34 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>5246</v>
+        <v>5240</v>
       </c>
       <c r="C31" t="s">
-        <v>5247</v>
+        <v>5241</v>
       </c>
       <c r="D31">
         <v>2011</v>
       </c>
       <c r="E31" t="s">
-        <v>5248</v>
+        <v>5242</v>
       </c>
       <c r="F31" t="s">
-        <v>5249</v>
+        <v>5243</v>
       </c>
       <c r="G31" t="s">
         <v>5028</v>
       </c>
       <c r="H31" t="s">
-        <v>5337</v>
+        <v>5331</v>
       </c>
       <c r="I31" t="b">
         <v>1</v>
       </c>
       <c r="J31" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K31" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L31">
         <v>80</v>
@@ -46466,19 +46448,19 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>5250</v>
+        <v>5244</v>
       </c>
       <c r="C32" t="s">
-        <v>5251</v>
+        <v>5245</v>
       </c>
       <c r="D32">
         <v>1999</v>
       </c>
       <c r="E32" t="s">
-        <v>5252</v>
+        <v>5246</v>
       </c>
       <c r="F32" t="s">
-        <v>5253</v>
+        <v>5247</v>
       </c>
       <c r="G32" t="s">
         <v>5028</v>
@@ -46490,10 +46472,10 @@
         <v>1</v>
       </c>
       <c r="J32" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K32" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L32">
         <v>182</v>
@@ -46525,34 +46507,34 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>5254</v>
+        <v>5248</v>
       </c>
       <c r="C33" t="s">
-        <v>5255</v>
+        <v>5249</v>
       </c>
       <c r="D33">
         <v>2004</v>
       </c>
       <c r="E33" t="s">
-        <v>5256</v>
+        <v>5250</v>
       </c>
       <c r="F33" t="s">
-        <v>5257</v>
+        <v>5251</v>
       </c>
       <c r="G33" t="s">
         <v>5028</v>
       </c>
       <c r="H33" t="s">
-        <v>5332</v>
+        <v>5326</v>
       </c>
       <c r="I33" t="b">
         <v>1</v>
       </c>
       <c r="J33" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K33" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L33">
         <v>389</v>
@@ -46593,10 +46575,10 @@
         <v>1999</v>
       </c>
       <c r="E34" t="s">
-        <v>5258</v>
+        <v>5252</v>
       </c>
       <c r="F34" t="s">
-        <v>5259</v>
+        <v>5253</v>
       </c>
       <c r="G34" t="s">
         <v>5028</v>
@@ -46608,10 +46590,10 @@
         <v>1</v>
       </c>
       <c r="J34" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K34" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L34">
         <v>177</v>
@@ -46626,7 +46608,7 @@
         <v>5028</v>
       </c>
       <c r="P34" t="s">
-        <v>5351</v>
+        <v>5345</v>
       </c>
       <c r="Q34" t="s">
         <v>963</v>
@@ -46652,10 +46634,10 @@
         <v>2001</v>
       </c>
       <c r="E35" t="s">
-        <v>5260</v>
+        <v>5254</v>
       </c>
       <c r="F35" t="s">
-        <v>5261</v>
+        <v>5255</v>
       </c>
       <c r="G35" t="s">
         <v>5028</v>
@@ -46667,10 +46649,10 @@
         <v>1</v>
       </c>
       <c r="J35" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K35" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L35">
         <v>217</v>
@@ -46702,19 +46684,19 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>5262</v>
+        <v>5256</v>
       </c>
       <c r="C36" t="s">
-        <v>5263</v>
+        <v>5257</v>
       </c>
       <c r="D36">
         <v>1993</v>
       </c>
       <c r="E36" t="s">
-        <v>5264</v>
+        <v>5258</v>
       </c>
       <c r="F36" t="s">
-        <v>5265</v>
+        <v>5259</v>
       </c>
       <c r="G36" t="s">
         <v>5028</v>
@@ -46726,10 +46708,10 @@
         <v>1</v>
       </c>
       <c r="J36" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K36" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L36">
         <v>1442</v>
@@ -46770,10 +46752,10 @@
         <v>2006</v>
       </c>
       <c r="E37" t="s">
-        <v>5266</v>
+        <v>5260</v>
       </c>
       <c r="F37" t="s">
-        <v>5267</v>
+        <v>5261</v>
       </c>
       <c r="G37" t="s">
         <v>5028</v>
@@ -46785,10 +46767,10 @@
         <v>1</v>
       </c>
       <c r="J37" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K37" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L37">
         <v>254</v>
@@ -46829,10 +46811,10 @@
         <v>1998</v>
       </c>
       <c r="E38" t="s">
-        <v>5268</v>
+        <v>5262</v>
       </c>
       <c r="F38" t="s">
-        <v>5269</v>
+        <v>5263</v>
       </c>
       <c r="G38" t="s">
         <v>5028</v>
@@ -46844,10 +46826,10 @@
         <v>1</v>
       </c>
       <c r="J38" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K38" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L38">
         <v>301</v>
@@ -46888,25 +46870,25 @@
         <v>2001</v>
       </c>
       <c r="E39" t="s">
-        <v>5270</v>
+        <v>5264</v>
       </c>
       <c r="F39" t="s">
-        <v>5271</v>
+        <v>5265</v>
       </c>
       <c r="G39" t="s">
         <v>5028</v>
       </c>
       <c r="H39" t="s">
-        <v>5339</v>
+        <v>5333</v>
       </c>
       <c r="I39" t="b">
         <v>1</v>
       </c>
       <c r="J39" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K39" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L39">
         <v>293</v>
@@ -46921,7 +46903,7 @@
         <v>5028</v>
       </c>
       <c r="P39" t="s">
-        <v>5353</v>
+        <v>5347</v>
       </c>
       <c r="Q39" t="s">
         <v>963</v>
@@ -46947,25 +46929,25 @@
         <v>2008</v>
       </c>
       <c r="E40" t="s">
-        <v>5272</v>
+        <v>5266</v>
       </c>
       <c r="F40" t="s">
-        <v>5273</v>
+        <v>5267</v>
       </c>
       <c r="G40" t="s">
         <v>5028</v>
       </c>
       <c r="H40" t="s">
-        <v>5337</v>
+        <v>5331</v>
       </c>
       <c r="I40" t="b">
         <v>1</v>
       </c>
       <c r="J40" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K40" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L40">
         <v>153</v>
@@ -46997,19 +46979,19 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>5274</v>
+        <v>5268</v>
       </c>
       <c r="C41" t="s">
-        <v>5275</v>
+        <v>5269</v>
       </c>
       <c r="D41">
         <v>2001</v>
       </c>
       <c r="E41" t="s">
-        <v>5276</v>
+        <v>5270</v>
       </c>
       <c r="F41" t="s">
-        <v>5277</v>
+        <v>5271</v>
       </c>
       <c r="G41" t="s">
         <v>5028</v>
@@ -47021,10 +47003,10 @@
         <v>1</v>
       </c>
       <c r="J41" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K41" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L41">
         <v>188</v>
@@ -47056,34 +47038,34 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>5278</v>
+        <v>5272</v>
       </c>
       <c r="C42" t="s">
-        <v>5279</v>
+        <v>5273</v>
       </c>
       <c r="D42">
         <v>2004</v>
       </c>
       <c r="E42" t="s">
-        <v>5280</v>
+        <v>5274</v>
       </c>
       <c r="F42" t="s">
-        <v>5281</v>
+        <v>5275</v>
       </c>
       <c r="G42" t="s">
         <v>5028</v>
       </c>
       <c r="H42" t="s">
-        <v>5332</v>
+        <v>5326</v>
       </c>
       <c r="I42" t="b">
         <v>1</v>
       </c>
       <c r="J42" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K42" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L42">
         <v>93</v>
@@ -47124,25 +47106,25 @@
         <v>1995</v>
       </c>
       <c r="E43" t="s">
-        <v>5282</v>
+        <v>5276</v>
       </c>
       <c r="F43" t="s">
-        <v>5283</v>
+        <v>5277</v>
       </c>
       <c r="G43" t="s">
         <v>5028</v>
       </c>
       <c r="H43" t="s">
-        <v>5340</v>
+        <v>5334</v>
       </c>
       <c r="I43" t="b">
         <v>1</v>
       </c>
       <c r="J43" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K43" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L43">
         <v>372</v>
@@ -47157,7 +47139,7 @@
         <v>5028</v>
       </c>
       <c r="P43" t="s">
-        <v>5351</v>
+        <v>5345</v>
       </c>
       <c r="Q43" t="s">
         <v>963</v>
@@ -47169,7 +47151,7 @@
         <v>5028</v>
       </c>
       <c r="T43" t="s">
-        <v>5354</v>
+        <v>5348</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
@@ -47177,19 +47159,19 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>5284</v>
+        <v>5278</v>
       </c>
       <c r="C44" t="s">
-        <v>5285</v>
+        <v>5279</v>
       </c>
       <c r="D44">
         <v>2004</v>
       </c>
       <c r="E44" t="s">
-        <v>5286</v>
+        <v>5280</v>
       </c>
       <c r="F44" t="s">
-        <v>5287</v>
+        <v>5281</v>
       </c>
       <c r="G44" t="s">
         <v>5028</v>
@@ -47201,10 +47183,10 @@
         <v>1</v>
       </c>
       <c r="J44" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K44" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L44">
         <v>1830</v>
@@ -47236,19 +47218,19 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>5288</v>
+        <v>5282</v>
       </c>
       <c r="C45" t="s">
-        <v>5289</v>
+        <v>5283</v>
       </c>
       <c r="D45">
         <v>2005</v>
       </c>
       <c r="E45" t="s">
-        <v>5290</v>
+        <v>5284</v>
       </c>
       <c r="F45" t="s">
-        <v>5291</v>
+        <v>5285</v>
       </c>
       <c r="G45" t="s">
         <v>5028</v>
@@ -47260,10 +47242,10 @@
         <v>1</v>
       </c>
       <c r="J45" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K45" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L45">
         <v>345</v>
@@ -47295,34 +47277,34 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>5292</v>
+        <v>5286</v>
       </c>
       <c r="C46" t="s">
-        <v>5293</v>
+        <v>5287</v>
       </c>
       <c r="D46">
         <v>2006</v>
       </c>
       <c r="E46" t="s">
-        <v>5294</v>
+        <v>5288</v>
       </c>
       <c r="F46" t="s">
-        <v>5295</v>
+        <v>5289</v>
       </c>
       <c r="G46" t="s">
         <v>5028</v>
       </c>
       <c r="H46" t="s">
-        <v>5341</v>
+        <v>5335</v>
       </c>
       <c r="I46" t="b">
         <v>1</v>
       </c>
       <c r="J46" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K46" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L46">
         <v>1005</v>
@@ -47337,7 +47319,7 @@
         <v>5028</v>
       </c>
       <c r="P46" t="s">
-        <v>5343</v>
+        <v>5337</v>
       </c>
       <c r="Q46" t="s">
         <v>963</v>
@@ -47354,19 +47336,19 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>5296</v>
+        <v>5290</v>
       </c>
       <c r="C47" t="s">
-        <v>5297</v>
+        <v>5291</v>
       </c>
       <c r="D47">
         <v>2006</v>
       </c>
       <c r="E47" t="s">
-        <v>5298</v>
+        <v>5292</v>
       </c>
       <c r="F47" t="s">
-        <v>5299</v>
+        <v>5293</v>
       </c>
       <c r="G47" t="s">
         <v>5028</v>
@@ -47378,10 +47360,10 @@
         <v>1</v>
       </c>
       <c r="J47" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K47" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L47">
         <v>596</v>
@@ -47396,7 +47378,7 @@
         <v>5028</v>
       </c>
       <c r="P47" t="s">
-        <v>5343</v>
+        <v>5337</v>
       </c>
       <c r="Q47" t="s">
         <v>963</v>
@@ -47413,19 +47395,19 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>5300</v>
+        <v>5294</v>
       </c>
       <c r="C48" t="s">
-        <v>5301</v>
+        <v>5295</v>
       </c>
       <c r="D48">
         <v>2005</v>
       </c>
       <c r="E48" t="s">
-        <v>5302</v>
+        <v>5296</v>
       </c>
       <c r="F48" t="s">
-        <v>5144</v>
+        <v>5138</v>
       </c>
       <c r="G48" t="s">
         <v>5028</v>
@@ -47437,10 +47419,10 @@
         <v>1</v>
       </c>
       <c r="J48" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K48" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L48">
         <v>386</v>
@@ -47481,25 +47463,25 @@
         <v>1982</v>
       </c>
       <c r="E49" t="s">
-        <v>5303</v>
+        <v>5297</v>
       </c>
       <c r="F49" t="s">
-        <v>5145</v>
+        <v>5139</v>
       </c>
       <c r="G49" t="s">
         <v>5028</v>
       </c>
       <c r="H49" t="s">
-        <v>5340</v>
+        <v>5334</v>
       </c>
       <c r="I49" t="b">
         <v>1</v>
       </c>
       <c r="J49" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K49" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L49">
         <v>55</v>
@@ -47540,10 +47522,10 @@
         <v>1985</v>
       </c>
       <c r="E50" t="s">
-        <v>5304</v>
+        <v>5298</v>
       </c>
       <c r="F50" t="s">
-        <v>5146</v>
+        <v>5140</v>
       </c>
       <c r="G50" t="s">
         <v>5028</v>
@@ -47555,10 +47537,10 @@
         <v>1</v>
       </c>
       <c r="J50" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K50" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L50">
         <v>2143</v>
@@ -47590,7 +47572,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>5305</v>
+        <v>5299</v>
       </c>
       <c r="C51" t="s">
         <v>674</v>
@@ -47599,10 +47581,10 @@
         <v>1979</v>
       </c>
       <c r="E51" t="s">
-        <v>5306</v>
+        <v>5300</v>
       </c>
       <c r="F51" t="s">
-        <v>5147</v>
+        <v>5141</v>
       </c>
       <c r="G51" t="s">
         <v>5028</v>
@@ -47614,10 +47596,10 @@
         <v>1</v>
       </c>
       <c r="J51" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K51" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L51">
         <v>251</v>
@@ -47649,19 +47631,19 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>5307</v>
+        <v>5301</v>
       </c>
       <c r="C52" t="s">
-        <v>5308</v>
+        <v>5302</v>
       </c>
       <c r="D52">
         <v>1997</v>
       </c>
       <c r="E52" t="s">
-        <v>5309</v>
+        <v>5303</v>
       </c>
       <c r="F52" t="s">
-        <v>5310</v>
+        <v>5304</v>
       </c>
       <c r="G52" t="s">
         <v>5028</v>
@@ -47673,10 +47655,10 @@
         <v>1</v>
       </c>
       <c r="J52" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K52" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L52">
         <v>9699</v>
@@ -47708,34 +47690,34 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>5311</v>
+        <v>5305</v>
       </c>
       <c r="C53" t="s">
-        <v>5312</v>
+        <v>5306</v>
       </c>
       <c r="D53">
         <v>2014</v>
       </c>
       <c r="E53" t="s">
-        <v>5313</v>
+        <v>5307</v>
       </c>
       <c r="F53" t="s">
-        <v>5314</v>
+        <v>5308</v>
       </c>
       <c r="G53" t="s">
         <v>5028</v>
       </c>
       <c r="H53" t="s">
-        <v>5330</v>
+        <v>5324</v>
       </c>
       <c r="I53" t="b">
         <v>1</v>
       </c>
       <c r="J53" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K53" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L53">
         <v>264</v>
@@ -47767,19 +47749,19 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>5315</v>
+        <v>5309</v>
       </c>
       <c r="C54" t="s">
-        <v>5316</v>
+        <v>5310</v>
       </c>
       <c r="D54">
         <v>2001</v>
       </c>
       <c r="E54" t="s">
-        <v>5317</v>
+        <v>5311</v>
       </c>
       <c r="F54" t="s">
-        <v>5318</v>
+        <v>5312</v>
       </c>
       <c r="G54" t="s">
         <v>5028</v>
@@ -47791,10 +47773,10 @@
         <v>1</v>
       </c>
       <c r="J54" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K54" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L54">
         <v>261</v>
@@ -47826,19 +47808,19 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>5319</v>
+        <v>5313</v>
       </c>
       <c r="C55" t="s">
-        <v>5320</v>
+        <v>5314</v>
       </c>
       <c r="D55">
         <v>1999</v>
       </c>
       <c r="E55" t="s">
-        <v>5321</v>
+        <v>5315</v>
       </c>
       <c r="F55" t="s">
-        <v>5322</v>
+        <v>5316</v>
       </c>
       <c r="G55" t="s">
         <v>5028</v>
@@ -47850,10 +47832,10 @@
         <v>1</v>
       </c>
       <c r="J55" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K55" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L55">
         <v>423</v>
@@ -47885,19 +47867,19 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>5323</v>
+        <v>5317</v>
       </c>
       <c r="C56" t="s">
-        <v>5324</v>
+        <v>5318</v>
       </c>
       <c r="D56">
         <v>2011</v>
       </c>
       <c r="E56" t="s">
-        <v>5325</v>
+        <v>5319</v>
       </c>
       <c r="F56" t="s">
-        <v>5326</v>
+        <v>5320</v>
       </c>
       <c r="G56" t="s">
         <v>5028</v>
@@ -47909,10 +47891,10 @@
         <v>1</v>
       </c>
       <c r="J56" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="K56" t="s">
-        <v>5327</v>
+        <v>5321</v>
       </c>
       <c r="L56">
         <v>197</v>
@@ -49544,10 +49526,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:Y16"/>
+  <dimension ref="A1:Y14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49599,24 +49581,24 @@
         <v>962</v>
       </c>
       <c r="O1" s="23" t="s">
+        <v>5113</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>5119</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>5125</v>
       </c>
       <c r="Q1" s="28" t="s">
         <v>5037</v>
       </c>
       <c r="R1" s="29">
         <f>COUNTIFS($N:$N, "YES", $F:$F, "&lt;&gt;")</f>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="T1" s="28" t="s">
         <v>5038</v>
       </c>
       <c r="U1" s="29">
-        <f>COUNTIF($M$2:$M$569, "YES")</f>
-        <v>15</v>
+        <f>COUNTIF($M$2:$M$567, "YES")</f>
+        <v>13</v>
       </c>
       <c r="V1" s="31"/>
       <c r="W1" s="31"/>
@@ -49873,11 +49855,11 @@
         <v>966</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>5123</v>
+        <v>5117</v>
       </c>
       <c r="R6">
         <f>COUNTIFS($N:$N, "YES", $M:$M, "&lt;&gt;PRIMARY STUDY")</f>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="W6" t="s">
         <v>5075</v>
@@ -49930,7 +49912,7 @@
         <v>966</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>5120</v>
+        <v>5114</v>
       </c>
       <c r="R7">
         <f>COUNTIFS($O:$O, "YES", $F:$F, "&lt;&gt;")</f>
@@ -50039,7 +50021,7 @@
         <v>5103</v>
       </c>
       <c r="D10">
-        <v>2018</v>
+        <v>2012</v>
       </c>
       <c r="E10" t="s">
         <v>5104</v>
@@ -50051,7 +50033,7 @@
         <v>5029</v>
       </c>
       <c r="H10">
-        <v>181</v>
+        <v>18</v>
       </c>
       <c r="I10" t="s">
         <v>5100</v>
@@ -50080,37 +50062,37 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>5108</v>
+        <v>5109</v>
       </c>
       <c r="C11" t="s">
-        <v>5109</v>
+        <v>5106</v>
       </c>
       <c r="D11">
-        <v>2012</v>
+        <v>2020</v>
       </c>
       <c r="E11" t="s">
         <v>5110</v>
       </c>
       <c r="F11" t="s">
-        <v>5105</v>
+        <v>5107</v>
       </c>
       <c r="G11" t="s">
         <v>5029</v>
       </c>
       <c r="H11">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="I11" t="s">
-        <v>5106</v>
+        <v>5108</v>
       </c>
       <c r="J11" t="s">
-        <v>5107</v>
+        <v>5105</v>
       </c>
       <c r="K11" t="s">
-        <v>5107</v>
+        <v>5105</v>
       </c>
       <c r="L11" t="s">
-        <v>5108</v>
+        <v>5109</v>
       </c>
       <c r="M11" t="s">
         <v>963</v>
@@ -50127,37 +50109,37 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>5115</v>
+        <v>3935</v>
       </c>
       <c r="C12" t="s">
-        <v>5112</v>
+        <v>3936</v>
       </c>
       <c r="D12">
-        <v>2020</v>
+        <v>2005</v>
       </c>
       <c r="E12" t="s">
-        <v>5116</v>
+        <v>1072</v>
       </c>
       <c r="F12" t="s">
-        <v>5113</v>
+        <v>970</v>
       </c>
       <c r="G12" t="s">
-        <v>5029</v>
+        <v>1074</v>
       </c>
       <c r="H12">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="I12" t="s">
-        <v>5114</v>
+        <v>1073</v>
       </c>
       <c r="J12" t="s">
-        <v>5111</v>
+        <v>1075</v>
       </c>
       <c r="K12" t="s">
-        <v>5111</v>
+        <v>1075</v>
       </c>
       <c r="L12" t="s">
-        <v>5115</v>
+        <v>3935</v>
       </c>
       <c r="M12" t="s">
         <v>963</v>
@@ -50167,6 +50149,9 @@
       </c>
       <c r="O12" s="7" t="s">
         <v>966</v>
+      </c>
+      <c r="P12" t="s">
+        <v>5120</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
@@ -50174,37 +50159,37 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>3935</v>
+        <v>4127</v>
       </c>
       <c r="C13" t="s">
-        <v>3936</v>
+        <v>4128</v>
       </c>
       <c r="D13">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="E13" t="s">
-        <v>1072</v>
+        <v>1957</v>
       </c>
       <c r="F13" t="s">
-        <v>970</v>
+        <v>1962</v>
       </c>
       <c r="G13" t="s">
-        <v>1074</v>
+        <v>1959</v>
       </c>
       <c r="H13">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="I13" t="s">
-        <v>1073</v>
+        <v>1958</v>
       </c>
       <c r="J13" t="s">
-        <v>1075</v>
+        <v>1960</v>
       </c>
       <c r="K13" t="s">
-        <v>1075</v>
+        <v>1961</v>
       </c>
       <c r="L13" t="s">
-        <v>3935</v>
+        <v>4127</v>
       </c>
       <c r="M13" t="s">
         <v>963</v>
@@ -50216,7 +50201,7 @@
         <v>966</v>
       </c>
       <c r="P13" t="s">
-        <v>5126</v>
+        <v>5120</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
@@ -50224,37 +50209,37 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>3965</v>
+        <v>399</v>
       </c>
       <c r="C14" t="s">
-        <v>3966</v>
+        <v>400</v>
       </c>
       <c r="D14">
-        <v>2003</v>
+        <v>1999</v>
       </c>
       <c r="E14" t="s">
-        <v>1211</v>
+        <v>5252</v>
       </c>
       <c r="F14" t="s">
-        <v>4598</v>
+        <v>5253</v>
       </c>
       <c r="G14" t="s">
-        <v>1213</v>
+        <v>5028</v>
       </c>
       <c r="H14">
-        <v>265</v>
+        <v>177</v>
       </c>
       <c r="I14" t="s">
-        <v>1212</v>
+        <v>5028</v>
       </c>
       <c r="J14" t="s">
-        <v>1214</v>
+        <v>5028</v>
       </c>
       <c r="K14" t="s">
-        <v>1215</v>
+        <v>5028</v>
       </c>
       <c r="L14" t="s">
-        <v>3965</v>
+        <v>399</v>
       </c>
       <c r="M14" t="s">
         <v>963</v>
@@ -50266,107 +50251,7 @@
         <v>966</v>
       </c>
       <c r="P14" t="s">
-        <v>5126</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>4127</v>
-      </c>
-      <c r="C15" t="s">
-        <v>4128</v>
-      </c>
-      <c r="D15">
-        <v>2004</v>
-      </c>
-      <c r="E15" t="s">
-        <v>1957</v>
-      </c>
-      <c r="F15" t="s">
-        <v>1962</v>
-      </c>
-      <c r="G15" t="s">
-        <v>1959</v>
-      </c>
-      <c r="H15">
-        <v>19</v>
-      </c>
-      <c r="I15" t="s">
-        <v>1958</v>
-      </c>
-      <c r="J15" t="s">
-        <v>1960</v>
-      </c>
-      <c r="K15" t="s">
-        <v>1961</v>
-      </c>
-      <c r="L15" t="s">
-        <v>4127</v>
-      </c>
-      <c r="M15" t="s">
-        <v>963</v>
-      </c>
-      <c r="N15" t="s">
-        <v>963</v>
-      </c>
-      <c r="O15" s="7" t="s">
-        <v>966</v>
-      </c>
-      <c r="P15" t="s">
-        <v>5126</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>399</v>
-      </c>
-      <c r="C16" t="s">
-        <v>400</v>
-      </c>
-      <c r="D16">
-        <v>1999</v>
-      </c>
-      <c r="E16" t="s">
-        <v>5258</v>
-      </c>
-      <c r="F16" t="s">
-        <v>5259</v>
-      </c>
-      <c r="G16" t="s">
-        <v>5028</v>
-      </c>
-      <c r="H16">
-        <v>177</v>
-      </c>
-      <c r="I16" t="s">
-        <v>5028</v>
-      </c>
-      <c r="J16" t="s">
-        <v>5028</v>
-      </c>
-      <c r="K16" t="s">
-        <v>5028</v>
-      </c>
-      <c r="L16" t="s">
-        <v>399</v>
-      </c>
-      <c r="M16" t="s">
-        <v>963</v>
-      </c>
-      <c r="N16" t="s">
-        <v>963</v>
-      </c>
-      <c r="O16" s="7" t="s">
-        <v>966</v>
-      </c>
-      <c r="P16" t="s">
-        <v>5352</v>
+        <v>5346</v>
       </c>
     </row>
   </sheetData>
@@ -50374,10 +50259,10 @@
   <conditionalFormatting sqref="B1:B2">
     <cfRule type="duplicateValues" dxfId="24" priority="30"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15">
+  <conditionalFormatting sqref="B13">
     <cfRule type="duplicateValues" dxfId="23" priority="20"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B16">
+  <conditionalFormatting sqref="B14">
     <cfRule type="duplicateValues" dxfId="22" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F2">
@@ -50385,62 +50270,62 @@
       <formula>LEN(TRIM(F1))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F15:F16">
+  <conditionalFormatting sqref="F13:F14">
     <cfRule type="containsBlanks" dxfId="20" priority="15">
-      <formula>LEN(TRIM(F15))=0</formula>
+      <formula>LEN(TRIM(F13))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H17:H1048576 H1:H14">
-    <cfRule type="containsBlanks" dxfId="5" priority="38">
+  <conditionalFormatting sqref="H1:H12 H15:H1048576">
+    <cfRule type="containsBlanks" dxfId="19" priority="38">
       <formula>LEN(TRIM(H1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2">
-    <cfRule type="duplicateValues" dxfId="19" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="28"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L15">
-    <cfRule type="duplicateValues" dxfId="18" priority="16"/>
+  <conditionalFormatting sqref="L13">
+    <cfRule type="duplicateValues" dxfId="17" priority="16"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L16">
-    <cfRule type="duplicateValues" dxfId="17" priority="5"/>
+  <conditionalFormatting sqref="L14">
+    <cfRule type="duplicateValues" dxfId="16" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:O16">
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="PRIMARY STUDY">
+  <conditionalFormatting sqref="M2:O14">
+    <cfRule type="containsText" dxfId="15" priority="2" operator="containsText" text="PRIMARY STUDY">
       <formula>NOT(ISERROR(SEARCH("PRIMARY STUDY",M2)))</formula>
     </cfRule>
-    <cfRule type="notContainsText" dxfId="3" priority="3" operator="notContains" text="YES">
+    <cfRule type="notContainsText" dxfId="14" priority="3" operator="notContains" text="YES">
       <formula>ISERROR(SEARCH("YES",M2))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="13" priority="4" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",M2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O15:O16">
-    <cfRule type="containsBlanks" dxfId="16" priority="1">
-      <formula>LEN(TRIM(O15))=0</formula>
+  <conditionalFormatting sqref="O13:O14">
+    <cfRule type="containsBlanks" dxfId="12" priority="1">
+      <formula>LEN(TRIM(O13))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="between">
       <formula>1</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="11" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH("X",O15)))</formula>
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="X">
+      <formula>NOT(ISERROR(SEARCH("X",O13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P1 P4">
-    <cfRule type="cellIs" dxfId="1" priority="32" operator="between">
+    <cfRule type="cellIs" dxfId="9" priority="32" operator="between">
       <formula>1</formula>
       <formula>4</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="33" operator="containsText" text="X">
+    <cfRule type="containsText" dxfId="8" priority="33" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH("X",P1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:Q2">
-    <cfRule type="duplicateValues" dxfId="13" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="T1">
-    <cfRule type="duplicateValues" dxfId="12" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="29"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
@@ -59333,10 +59218,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L1 A1:K251">
-    <cfRule type="expression" dxfId="11" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>$K1=FALSE</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="9">
+    <cfRule type="expression" dxfId="4" priority="9">
       <formula>$J1=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -67281,10 +67166,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J1:J253 J257 J259:J1048576">
-    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="3" priority="12" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",J1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="13" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="2" priority="13" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",J1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -67301,10 +67186,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M17">
-    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="FALSE">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",M17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",M17)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added even more twin data, updated the literature file
</commit_message>
<xml_diff>
--- a/Literature/Literature.xlsx
+++ b/Literature/Literature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hso20\OneDrive\Plocha\IES\Diploma-Thesis\Literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A10534B-7646-4323-870B-F2A3E6131FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCFE65CD-E19A-4410-A372-5CAA4820C354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -694,7 +694,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10199" uniqueCount="5349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10210" uniqueCount="5354">
   <si>
     <t>Number</t>
   </si>
@@ -15894,9 +15894,6 @@
     <t>Further estimates of the economic return to schooling from a new sample of twins</t>
   </si>
   <si>
-    <t>Check whether indeed 1</t>
-  </si>
-  <si>
     <t>Dude, 354 pages, how can you even write that. Look for 2013 or 2015 by the same author - more concise publications with the same approach.</t>
   </si>
   <si>
@@ -16741,6 +16738,24 @@
   </si>
   <si>
     <t>Already identified during twins snowballing</t>
+  </si>
+  <si>
+    <t>Blanchflower &amp; Elias (1999)</t>
+  </si>
+  <si>
+    <t>Blanchflower &amp; Elias</t>
+  </si>
+  <si>
+    <t>Blanchflower, David, and Peter Elias. "Ability, schooling and earnings: Are twins different?." Unpublished manuscript, Warwick University (1999).</t>
+  </si>
+  <si>
+    <t>Ability, schooling and earnings: Are twins different?</t>
+  </si>
+  <si>
+    <t>http://perso.univ-lemans.fr/~mtensao/article/Twins.pdf</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0927537198000141</t>
   </si>
 </sst>
 </file>
@@ -17075,7 +17090,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -17122,6 +17137,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -17880,27 +17896,27 @@
         <v>962</v>
       </c>
       <c r="N1" s="24" t="s">
-        <v>5113</v>
+        <v>5112</v>
       </c>
       <c r="O1" s="25" t="s">
-        <v>5111</v>
+        <v>5110</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>5119</v>
+        <v>5118</v>
       </c>
       <c r="Q1" s="28" t="s">
         <v>5037</v>
       </c>
       <c r="R1" s="29">
         <f>COUNTIFS($M:$M, "YES", $F:$F, "&lt;&gt;") + Twins!R1</f>
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="T1" s="28" t="s">
         <v>5038</v>
       </c>
       <c r="U1" s="29">
         <f>COUNTIF($L$2:$L$575, "&lt;&gt; ") +Twins!U1</f>
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="V1" s="31"/>
       <c r="W1" s="31"/>
@@ -18061,7 +18077,7 @@
         <v>574</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>5117</v>
+        <v>5116</v>
       </c>
       <c r="U4">
         <f>COUNTIFS($M:$M, "YES", $L:$L, "&lt;&gt;PRIMARY STUDY", $P:$P, "&lt;&gt;Twins")</f>
@@ -18122,7 +18138,7 @@
         <v>574</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>5114</v>
+        <v>5113</v>
       </c>
       <c r="U5" s="37">
         <f>COUNTIFS($N:$N, "YES", $F:$F, "&lt;&gt;")</f>
@@ -18230,7 +18246,7 @@
         <v>5028</v>
       </c>
       <c r="P7" t="s">
-        <v>5343</v>
+        <v>5342</v>
       </c>
       <c r="Q7" s="2" t="s">
         <v>904</v>
@@ -18431,10 +18447,10 @@
         <v>1</v>
       </c>
       <c r="P11" t="s">
-        <v>5118</v>
+        <v>5117</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>5112</v>
+        <v>5111</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
@@ -18487,7 +18503,7 @@
         <v>1</v>
       </c>
       <c r="R12" t="s">
-        <v>5115</v>
+        <v>5114</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
@@ -18540,7 +18556,7 @@
         <v>2</v>
       </c>
       <c r="R13" t="s">
-        <v>5116</v>
+        <v>5115</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
@@ -19793,7 +19809,7 @@
         <v>1</v>
       </c>
       <c r="P38" t="s">
-        <v>5118</v>
+        <v>5117</v>
       </c>
       <c r="R38" t="s">
         <v>904</v>
@@ -19946,7 +19962,7 @@
         <v>2</v>
       </c>
       <c r="P41" t="s">
-        <v>5129</v>
+        <v>5128</v>
       </c>
       <c r="R41" t="s">
         <v>904</v>
@@ -20749,7 +20765,7 @@
         <v>2</v>
       </c>
       <c r="P57" t="s">
-        <v>5121</v>
+        <v>5120</v>
       </c>
       <c r="R57" t="s">
         <v>904</v>
@@ -22402,7 +22418,7 @@
         <v>1</v>
       </c>
       <c r="P90" t="s">
-        <v>5122</v>
+        <v>5121</v>
       </c>
       <c r="R90" t="s">
         <v>904</v>
@@ -22413,7 +22429,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>5123</v>
+        <v>5122</v>
       </c>
       <c r="C91" t="s">
         <v>4015</v>
@@ -23405,7 +23421,7 @@
         <v>1</v>
       </c>
       <c r="P110" t="s">
-        <v>5124</v>
+        <v>5123</v>
       </c>
       <c r="R110" t="s">
         <v>904</v>
@@ -23858,7 +23874,7 @@
         <v>4</v>
       </c>
       <c r="P119" t="s">
-        <v>5125</v>
+        <v>5124</v>
       </c>
       <c r="R119" t="s">
         <v>904</v>
@@ -25152,7 +25168,7 @@
         <v>1765</v>
       </c>
       <c r="L145" t="s">
-        <v>5126</v>
+        <v>5125</v>
       </c>
       <c r="M145" t="s">
         <v>966</v>
@@ -25172,7 +25188,7 @@
         <v>145</v>
       </c>
       <c r="B146" t="s">
-        <v>5127</v>
+        <v>5126</v>
       </c>
       <c r="C146" t="s">
         <v>4080</v>
@@ -25184,7 +25200,7 @@
         <v>1766</v>
       </c>
       <c r="F146" t="s">
-        <v>5128</v>
+        <v>5127</v>
       </c>
       <c r="G146" t="s">
         <v>1768</v>
@@ -25375,7 +25391,7 @@
         <v>149</v>
       </c>
       <c r="B150" t="s">
-        <v>5130</v>
+        <v>5129</v>
       </c>
       <c r="C150" t="s">
         <v>4085</v>
@@ -25384,13 +25400,13 @@
         <v>2012</v>
       </c>
       <c r="E150" t="s">
+        <v>5130</v>
+      </c>
+      <c r="F150" t="s">
         <v>5131</v>
       </c>
-      <c r="F150" t="s">
+      <c r="G150" t="s">
         <v>5132</v>
-      </c>
-      <c r="G150" t="s">
-        <v>5133</v>
       </c>
       <c r="H150">
         <v>0</v>
@@ -27279,7 +27295,7 @@
         <v>1</v>
       </c>
       <c r="P187" t="s">
-        <v>5118</v>
+        <v>5117</v>
       </c>
       <c r="R187" t="s">
         <v>904</v>
@@ -27382,7 +27398,7 @@
         <v>1</v>
       </c>
       <c r="P189" t="s">
-        <v>5067</v>
+        <v>5066</v>
       </c>
       <c r="R189" t="s">
         <v>904</v>
@@ -27435,7 +27451,7 @@
         <v>5028</v>
       </c>
       <c r="P190" t="s">
-        <v>5068</v>
+        <v>5067</v>
       </c>
       <c r="R190" t="s">
         <v>904</v>
@@ -29668,7 +29684,7 @@
         <v>239</v>
       </c>
       <c r="B240" t="s">
-        <v>5069</v>
+        <v>5068</v>
       </c>
       <c r="C240" t="s">
         <v>4786</v>
@@ -44580,16 +44596,16 @@
         <v>3907</v>
       </c>
       <c r="H1" s="23" t="s">
+        <v>5133</v>
+      </c>
+      <c r="I1" s="23" t="s">
         <v>5134</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="J1" s="23" t="s">
         <v>5135</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="K1" s="23" t="s">
         <v>5136</v>
-      </c>
-      <c r="K1" s="23" t="s">
-        <v>5137</v>
       </c>
       <c r="L1" s="23" t="s">
         <v>3902</v>
@@ -44610,13 +44626,13 @@
         <v>962</v>
       </c>
       <c r="R1" s="24" t="s">
-        <v>5113</v>
+        <v>5112</v>
       </c>
       <c r="S1" s="25" t="s">
-        <v>5111</v>
+        <v>5110</v>
       </c>
       <c r="T1" s="39" t="s">
-        <v>5119</v>
+        <v>5118</v>
       </c>
       <c r="U1" s="28" t="s">
         <v>5037</v>
@@ -44642,7 +44658,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>5142</v>
+        <v>5141</v>
       </c>
       <c r="C2" s="34" t="s">
         <v>4157</v>
@@ -44651,10 +44667,10 @@
         <v>2010</v>
       </c>
       <c r="E2" s="34" t="s">
+        <v>5142</v>
+      </c>
+      <c r="F2" s="34" t="s">
         <v>5143</v>
-      </c>
-      <c r="F2" s="34" t="s">
-        <v>5144</v>
       </c>
       <c r="G2" s="34" t="s">
         <v>5028</v>
@@ -44666,10 +44682,10 @@
         <v>1</v>
       </c>
       <c r="J2" s="34" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K2" s="34" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L2" s="34">
         <v>289</v>
@@ -44708,34 +44724,34 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>5144</v>
+      </c>
+      <c r="C3" t="s">
         <v>5145</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5146</v>
       </c>
       <c r="D3">
         <v>2000</v>
       </c>
       <c r="E3" t="s">
+        <v>5146</v>
+      </c>
+      <c r="F3" t="s">
         <v>5147</v>
       </c>
-      <c r="F3" t="s">
-        <v>5148</v>
-      </c>
       <c r="G3" t="s">
         <v>5028</v>
       </c>
       <c r="H3" t="s">
-        <v>5322</v>
+        <v>5321</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K3" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L3">
         <v>1486</v>
@@ -44750,7 +44766,7 @@
         <v>5028</v>
       </c>
       <c r="P3" t="s">
-        <v>5338</v>
+        <v>5337</v>
       </c>
       <c r="Q3" t="s">
         <v>963</v>
@@ -44776,10 +44792,10 @@
         <v>1995</v>
       </c>
       <c r="E4" t="s">
+        <v>5148</v>
+      </c>
+      <c r="F4" t="s">
         <v>5149</v>
-      </c>
-      <c r="F4" t="s">
-        <v>5150</v>
       </c>
       <c r="G4" t="s">
         <v>5028</v>
@@ -44791,10 +44807,10 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K4" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L4">
         <v>321</v>
@@ -44826,34 +44842,34 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>5150</v>
+      </c>
+      <c r="C5" t="s">
         <v>5151</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5152</v>
       </c>
       <c r="D5">
         <v>1991</v>
       </c>
       <c r="E5" t="s">
+        <v>5152</v>
+      </c>
+      <c r="F5" t="s">
         <v>5153</v>
       </c>
-      <c r="F5" t="s">
-        <v>5154</v>
-      </c>
       <c r="G5" t="s">
         <v>5028</v>
       </c>
       <c r="H5" t="s">
-        <v>5323</v>
+        <v>5322</v>
       </c>
       <c r="I5" t="b">
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K5" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L5">
         <v>3590</v>
@@ -44885,19 +44901,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>5154</v>
+      </c>
+      <c r="C6" t="s">
         <v>5155</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5156</v>
       </c>
       <c r="D6">
         <v>2005</v>
       </c>
       <c r="E6" t="s">
+        <v>5156</v>
+      </c>
+      <c r="F6" t="s">
         <v>5157</v>
-      </c>
-      <c r="F6" t="s">
-        <v>5158</v>
       </c>
       <c r="G6" t="s">
         <v>5028</v>
@@ -44909,10 +44925,10 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K6" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L6">
         <v>1510</v>
@@ -44939,10 +44955,10 @@
         <v>5028</v>
       </c>
       <c r="T6" t="s">
-        <v>5336</v>
+        <v>5335</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>5117</v>
+        <v>5116</v>
       </c>
       <c r="V6">
         <f>COUNTIF($P:$P, "YES")</f>
@@ -44954,34 +44970,34 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>5158</v>
+      </c>
+      <c r="C7" t="s">
         <v>5159</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5160</v>
       </c>
       <c r="D7">
         <v>2002</v>
       </c>
       <c r="E7" t="s">
+        <v>5160</v>
+      </c>
+      <c r="F7" t="s">
         <v>5161</v>
       </c>
-      <c r="F7" t="s">
-        <v>5162</v>
-      </c>
       <c r="G7" t="s">
         <v>5028</v>
       </c>
       <c r="H7" t="s">
-        <v>5324</v>
+        <v>5323</v>
       </c>
       <c r="I7" t="b">
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K7" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L7">
         <v>321</v>
@@ -45008,7 +45024,7 @@
         <v>1</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>5114</v>
+        <v>5113</v>
       </c>
       <c r="V7">
         <f>COUNTIFS($R:$R, "YES", $F:$F, "&lt;&gt;")</f>
@@ -45029,10 +45045,10 @@
         <v>1998</v>
       </c>
       <c r="E8" t="s">
+        <v>5162</v>
+      </c>
+      <c r="F8" t="s">
         <v>5163</v>
-      </c>
-      <c r="F8" t="s">
-        <v>5164</v>
       </c>
       <c r="G8" t="s">
         <v>5028</v>
@@ -45044,10 +45060,10 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K8" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L8">
         <v>588</v>
@@ -45079,34 +45095,34 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>5164</v>
+      </c>
+      <c r="C9" t="s">
         <v>5165</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5166</v>
       </c>
       <c r="D9">
         <v>2014</v>
       </c>
       <c r="E9" t="s">
+        <v>5166</v>
+      </c>
+      <c r="F9" t="s">
         <v>5167</v>
       </c>
-      <c r="F9" t="s">
-        <v>5168</v>
-      </c>
       <c r="G9" t="s">
         <v>5028</v>
       </c>
       <c r="H9" t="s">
-        <v>5325</v>
+        <v>5324</v>
       </c>
       <c r="I9" t="b">
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K9" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L9">
         <v>73</v>
@@ -45138,34 +45154,34 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>5168</v>
+      </c>
+      <c r="C10" t="s">
         <v>5169</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5170</v>
       </c>
       <c r="D10">
         <v>2018</v>
       </c>
       <c r="E10" t="s">
+        <v>5170</v>
+      </c>
+      <c r="F10" t="s">
         <v>5171</v>
       </c>
-      <c r="F10" t="s">
-        <v>5172</v>
-      </c>
       <c r="G10" t="s">
         <v>5028</v>
       </c>
       <c r="H10" t="s">
-        <v>5326</v>
+        <v>5325</v>
       </c>
       <c r="I10" t="b">
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K10" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L10">
         <v>74</v>
@@ -45180,7 +45196,7 @@
         <v>5028</v>
       </c>
       <c r="P10" t="s">
-        <v>5337</v>
+        <v>5336</v>
       </c>
       <c r="Q10" t="s">
         <v>963</v>
@@ -45197,19 +45213,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>5172</v>
+      </c>
+      <c r="C11" t="s">
         <v>5173</v>
-      </c>
-      <c r="C11" t="s">
-        <v>5174</v>
       </c>
       <c r="D11">
         <v>2014</v>
       </c>
       <c r="E11" t="s">
+        <v>5174</v>
+      </c>
+      <c r="F11" t="s">
         <v>5175</v>
-      </c>
-      <c r="F11" t="s">
-        <v>5176</v>
       </c>
       <c r="G11" t="s">
         <v>5028</v>
@@ -45221,10 +45237,10 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K11" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L11">
         <v>17</v>
@@ -45256,7 +45272,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>5177</v>
+        <v>5176</v>
       </c>
       <c r="C12" t="s">
         <v>3928</v>
@@ -45265,25 +45281,25 @@
         <v>1995</v>
       </c>
       <c r="E12" t="s">
+        <v>5177</v>
+      </c>
+      <c r="F12" t="s">
         <v>5178</v>
       </c>
-      <c r="F12" t="s">
-        <v>5179</v>
-      </c>
       <c r="G12" t="s">
         <v>5028</v>
       </c>
       <c r="H12" t="s">
-        <v>5327</v>
+        <v>5326</v>
       </c>
       <c r="I12" t="b">
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K12" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L12">
         <v>1789</v>
@@ -45315,7 +45331,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>5180</v>
+        <v>5179</v>
       </c>
       <c r="C13" t="s">
         <v>3928</v>
@@ -45324,25 +45340,25 @@
         <v>2001</v>
       </c>
       <c r="E13" t="s">
+        <v>5180</v>
+      </c>
+      <c r="F13" t="s">
         <v>5181</v>
       </c>
-      <c r="F13" t="s">
-        <v>5182</v>
-      </c>
       <c r="G13" t="s">
         <v>5028</v>
       </c>
       <c r="H13" t="s">
-        <v>5324</v>
+        <v>5323</v>
       </c>
       <c r="I13" t="b">
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K13" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L13">
         <v>2928</v>
@@ -45357,7 +45373,7 @@
         <v>5028</v>
       </c>
       <c r="P13" t="s">
-        <v>5339</v>
+        <v>5338</v>
       </c>
       <c r="Q13" t="s">
         <v>963</v>
@@ -45369,7 +45385,7 @@
         <v>1</v>
       </c>
       <c r="T13" t="s">
-        <v>5340</v>
+        <v>5339</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.25">
@@ -45377,7 +45393,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>5183</v>
+        <v>5182</v>
       </c>
       <c r="C14" t="s">
         <v>4356</v>
@@ -45386,25 +45402,25 @@
         <v>2011</v>
       </c>
       <c r="E14" t="s">
+        <v>5183</v>
+      </c>
+      <c r="F14" t="s">
         <v>5184</v>
       </c>
-      <c r="F14" t="s">
-        <v>5185</v>
-      </c>
       <c r="G14" t="s">
         <v>5028</v>
       </c>
       <c r="H14" t="s">
-        <v>5328</v>
+        <v>5327</v>
       </c>
       <c r="I14" t="b">
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K14" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L14">
         <v>783</v>
@@ -45436,34 +45452,34 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>5185</v>
+      </c>
+      <c r="C15" t="s">
         <v>5186</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5187</v>
       </c>
       <c r="D15">
         <v>2019</v>
       </c>
       <c r="E15" t="s">
+        <v>5187</v>
+      </c>
+      <c r="F15" t="s">
         <v>5188</v>
       </c>
-      <c r="F15" t="s">
-        <v>5189</v>
-      </c>
       <c r="G15" t="s">
         <v>5028</v>
       </c>
       <c r="H15" t="s">
-        <v>5329</v>
+        <v>5328</v>
       </c>
       <c r="I15" t="b">
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K15" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L15">
         <v>141</v>
@@ -45490,7 +45506,7 @@
         <v>5028</v>
       </c>
       <c r="T15" t="s">
-        <v>5341</v>
+        <v>5340</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
@@ -45507,10 +45523,10 @@
         <v>1998</v>
       </c>
       <c r="E16" t="s">
+        <v>5189</v>
+      </c>
+      <c r="F16" t="s">
         <v>5190</v>
-      </c>
-      <c r="F16" t="s">
-        <v>5191</v>
       </c>
       <c r="G16" t="s">
         <v>5028</v>
@@ -45522,10 +45538,10 @@
         <v>1</v>
       </c>
       <c r="J16" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K16" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L16">
         <v>284</v>
@@ -45557,34 +45573,34 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>5191</v>
+      </c>
+      <c r="C17" t="s">
         <v>5192</v>
-      </c>
-      <c r="C17" t="s">
-        <v>5193</v>
       </c>
       <c r="D17">
         <v>2010</v>
       </c>
       <c r="E17" t="s">
+        <v>5193</v>
+      </c>
+      <c r="F17" t="s">
         <v>5194</v>
       </c>
-      <c r="F17" t="s">
-        <v>5195</v>
-      </c>
       <c r="G17" t="s">
         <v>5028</v>
       </c>
       <c r="H17" t="s">
-        <v>5330</v>
+        <v>5329</v>
       </c>
       <c r="I17" t="b">
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K17" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L17">
         <v>252</v>
@@ -45616,19 +45632,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>5195</v>
+      </c>
+      <c r="C18" t="s">
         <v>5196</v>
-      </c>
-      <c r="C18" t="s">
-        <v>5197</v>
       </c>
       <c r="D18">
         <v>1991</v>
       </c>
       <c r="E18" t="s">
+        <v>5197</v>
+      </c>
+      <c r="F18" t="s">
         <v>5198</v>
-      </c>
-      <c r="F18" t="s">
-        <v>5199</v>
       </c>
       <c r="G18" t="s">
         <v>5028</v>
@@ -45640,10 +45656,10 @@
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K18" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L18">
         <v>88</v>
@@ -45684,10 +45700,10 @@
         <v>2001</v>
       </c>
       <c r="E19" t="s">
+        <v>5199</v>
+      </c>
+      <c r="F19" t="s">
         <v>5200</v>
-      </c>
-      <c r="F19" t="s">
-        <v>5201</v>
       </c>
       <c r="G19" t="s">
         <v>5028</v>
@@ -45699,10 +45715,10 @@
         <v>1</v>
       </c>
       <c r="J19" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K19" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L19">
         <v>2852</v>
@@ -45743,10 +45759,10 @@
         <v>2002</v>
       </c>
       <c r="E20" t="s">
+        <v>5201</v>
+      </c>
+      <c r="F20" t="s">
         <v>5202</v>
-      </c>
-      <c r="F20" t="s">
-        <v>5203</v>
       </c>
       <c r="G20" t="s">
         <v>5028</v>
@@ -45758,10 +45774,10 @@
         <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K20" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L20">
         <v>386</v>
@@ -45793,34 +45809,34 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>5203</v>
+      </c>
+      <c r="C21" t="s">
         <v>5204</v>
-      </c>
-      <c r="C21" t="s">
-        <v>5205</v>
       </c>
       <c r="D21">
         <v>2008</v>
       </c>
       <c r="E21" t="s">
+        <v>5205</v>
+      </c>
+      <c r="F21" t="s">
         <v>5206</v>
       </c>
-      <c r="F21" t="s">
-        <v>5207</v>
-      </c>
       <c r="G21" t="s">
         <v>5028</v>
       </c>
       <c r="H21" t="s">
-        <v>5331</v>
+        <v>5330</v>
       </c>
       <c r="I21" t="b">
         <v>1</v>
       </c>
       <c r="J21" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K21" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L21">
         <v>494</v>
@@ -45852,19 +45868,19 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>5207</v>
+      </c>
+      <c r="C22" t="s">
         <v>5208</v>
-      </c>
-      <c r="C22" t="s">
-        <v>5209</v>
       </c>
       <c r="D22">
         <v>2000</v>
       </c>
       <c r="E22" t="s">
+        <v>5209</v>
+      </c>
+      <c r="F22" t="s">
         <v>5210</v>
-      </c>
-      <c r="F22" t="s">
-        <v>5211</v>
       </c>
       <c r="G22" t="s">
         <v>5028</v>
@@ -45876,10 +45892,10 @@
         <v>1</v>
       </c>
       <c r="J22" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K22" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L22">
         <v>101</v>
@@ -45911,34 +45927,34 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>5211</v>
+      </c>
+      <c r="C23" t="s">
         <v>5212</v>
-      </c>
-      <c r="C23" t="s">
-        <v>5213</v>
       </c>
       <c r="D23">
         <v>2019</v>
       </c>
       <c r="E23" t="s">
+        <v>5213</v>
+      </c>
+      <c r="F23" t="s">
         <v>5214</v>
       </c>
-      <c r="F23" t="s">
-        <v>5215</v>
-      </c>
       <c r="G23" t="s">
         <v>5028</v>
       </c>
       <c r="H23" t="s">
-        <v>5326</v>
+        <v>5325</v>
       </c>
       <c r="I23" t="b">
         <v>1</v>
       </c>
       <c r="J23" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K23" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L23">
         <v>92</v>
@@ -45965,7 +45981,7 @@
         <v>5028</v>
       </c>
       <c r="T23" t="s">
-        <v>5342</v>
+        <v>5341</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
@@ -45973,19 +45989,19 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>5215</v>
+      </c>
+      <c r="C24" t="s">
         <v>5216</v>
-      </c>
-      <c r="C24" t="s">
-        <v>5217</v>
       </c>
       <c r="D24">
         <v>2005</v>
       </c>
       <c r="E24" t="s">
+        <v>5217</v>
+      </c>
+      <c r="F24" t="s">
         <v>5218</v>
-      </c>
-      <c r="F24" t="s">
-        <v>5219</v>
       </c>
       <c r="G24" t="s">
         <v>5028</v>
@@ -45997,10 +46013,10 @@
         <v>1</v>
       </c>
       <c r="J24" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K24" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L24">
         <v>171</v>
@@ -46032,34 +46048,34 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>5219</v>
+      </c>
+      <c r="C25" t="s">
         <v>5220</v>
-      </c>
-      <c r="C25" t="s">
-        <v>5221</v>
       </c>
       <c r="D25">
         <v>1995</v>
       </c>
       <c r="E25" t="s">
+        <v>5221</v>
+      </c>
+      <c r="F25" t="s">
         <v>5222</v>
       </c>
-      <c r="F25" t="s">
-        <v>5223</v>
-      </c>
       <c r="G25" t="s">
         <v>5028</v>
       </c>
       <c r="H25" t="s">
-        <v>5331</v>
+        <v>5330</v>
       </c>
       <c r="I25" t="b">
         <v>1</v>
       </c>
       <c r="J25" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K25" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L25">
         <v>662</v>
@@ -46091,7 +46107,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>5224</v>
+        <v>5223</v>
       </c>
       <c r="C26" t="s">
         <v>3930</v>
@@ -46100,10 +46116,10 @@
         <v>1995</v>
       </c>
       <c r="E26" t="s">
+        <v>5224</v>
+      </c>
+      <c r="F26" t="s">
         <v>5225</v>
-      </c>
-      <c r="F26" t="s">
-        <v>5226</v>
       </c>
       <c r="G26" t="s">
         <v>5028</v>
@@ -46115,10 +46131,10 @@
         <v>1</v>
       </c>
       <c r="J26" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K26" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L26">
         <v>888</v>
@@ -46150,7 +46166,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>5227</v>
+        <v>5226</v>
       </c>
       <c r="C27" t="s">
         <v>3930</v>
@@ -46159,10 +46175,10 @@
         <v>1999</v>
       </c>
       <c r="E27" t="s">
+        <v>5227</v>
+      </c>
+      <c r="F27" t="s">
         <v>5228</v>
-      </c>
-      <c r="F27" t="s">
-        <v>5229</v>
       </c>
       <c r="G27" t="s">
         <v>5028</v>
@@ -46174,10 +46190,10 @@
         <v>1</v>
       </c>
       <c r="J27" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K27" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L27">
         <v>100</v>
@@ -46218,25 +46234,25 @@
         <v>2003</v>
       </c>
       <c r="E28" t="s">
+        <v>5229</v>
+      </c>
+      <c r="F28" t="s">
         <v>5230</v>
       </c>
-      <c r="F28" t="s">
-        <v>5231</v>
-      </c>
       <c r="G28" t="s">
         <v>5028</v>
       </c>
       <c r="H28" t="s">
-        <v>5326</v>
+        <v>5325</v>
       </c>
       <c r="I28" t="b">
         <v>1</v>
       </c>
       <c r="J28" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K28" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L28">
         <v>860</v>
@@ -46268,19 +46284,19 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
+        <v>5231</v>
+      </c>
+      <c r="C29" t="s">
         <v>5232</v>
-      </c>
-      <c r="C29" t="s">
-        <v>5233</v>
       </c>
       <c r="D29">
         <v>2007</v>
       </c>
       <c r="E29" t="s">
+        <v>5233</v>
+      </c>
+      <c r="F29" t="s">
         <v>5234</v>
-      </c>
-      <c r="F29" t="s">
-        <v>5235</v>
       </c>
       <c r="G29" t="s">
         <v>5028</v>
@@ -46292,10 +46308,10 @@
         <v>1</v>
       </c>
       <c r="J29" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K29" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L29">
         <v>27</v>
@@ -46327,34 +46343,34 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
+        <v>5235</v>
+      </c>
+      <c r="C30" t="s">
         <v>5236</v>
-      </c>
-      <c r="C30" t="s">
-        <v>5237</v>
       </c>
       <c r="D30">
         <v>2006</v>
       </c>
       <c r="E30" t="s">
+        <v>5237</v>
+      </c>
+      <c r="F30" t="s">
         <v>5238</v>
       </c>
-      <c r="F30" t="s">
-        <v>5239</v>
-      </c>
       <c r="G30" t="s">
         <v>5028</v>
       </c>
       <c r="H30" t="s">
-        <v>5332</v>
+        <v>5331</v>
       </c>
       <c r="I30" t="b">
         <v>1</v>
       </c>
       <c r="J30" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K30" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L30">
         <v>1427</v>
@@ -46381,7 +46397,7 @@
         <v>3</v>
       </c>
       <c r="T30" t="s">
-        <v>5344</v>
+        <v>5343</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
@@ -46389,34 +46405,34 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
+        <v>5239</v>
+      </c>
+      <c r="C31" t="s">
         <v>5240</v>
-      </c>
-      <c r="C31" t="s">
-        <v>5241</v>
       </c>
       <c r="D31">
         <v>2011</v>
       </c>
       <c r="E31" t="s">
+        <v>5241</v>
+      </c>
+      <c r="F31" t="s">
         <v>5242</v>
       </c>
-      <c r="F31" t="s">
-        <v>5243</v>
-      </c>
       <c r="G31" t="s">
         <v>5028</v>
       </c>
       <c r="H31" t="s">
-        <v>5331</v>
+        <v>5330</v>
       </c>
       <c r="I31" t="b">
         <v>1</v>
       </c>
       <c r="J31" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K31" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L31">
         <v>80</v>
@@ -46448,19 +46464,19 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
+        <v>5243</v>
+      </c>
+      <c r="C32" t="s">
         <v>5244</v>
-      </c>
-      <c r="C32" t="s">
-        <v>5245</v>
       </c>
       <c r="D32">
         <v>1999</v>
       </c>
       <c r="E32" t="s">
+        <v>5245</v>
+      </c>
+      <c r="F32" t="s">
         <v>5246</v>
-      </c>
-      <c r="F32" t="s">
-        <v>5247</v>
       </c>
       <c r="G32" t="s">
         <v>5028</v>
@@ -46472,10 +46488,10 @@
         <v>1</v>
       </c>
       <c r="J32" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K32" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L32">
         <v>182</v>
@@ -46507,34 +46523,34 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
+        <v>5247</v>
+      </c>
+      <c r="C33" t="s">
         <v>5248</v>
-      </c>
-      <c r="C33" t="s">
-        <v>5249</v>
       </c>
       <c r="D33">
         <v>2004</v>
       </c>
       <c r="E33" t="s">
+        <v>5249</v>
+      </c>
+      <c r="F33" t="s">
         <v>5250</v>
       </c>
-      <c r="F33" t="s">
-        <v>5251</v>
-      </c>
       <c r="G33" t="s">
         <v>5028</v>
       </c>
       <c r="H33" t="s">
-        <v>5326</v>
+        <v>5325</v>
       </c>
       <c r="I33" t="b">
         <v>1</v>
       </c>
       <c r="J33" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K33" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L33">
         <v>389</v>
@@ -46575,10 +46591,10 @@
         <v>1999</v>
       </c>
       <c r="E34" t="s">
+        <v>5251</v>
+      </c>
+      <c r="F34" t="s">
         <v>5252</v>
-      </c>
-      <c r="F34" t="s">
-        <v>5253</v>
       </c>
       <c r="G34" t="s">
         <v>5028</v>
@@ -46590,10 +46606,10 @@
         <v>1</v>
       </c>
       <c r="J34" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K34" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L34">
         <v>177</v>
@@ -46608,7 +46624,7 @@
         <v>5028</v>
       </c>
       <c r="P34" t="s">
-        <v>5345</v>
+        <v>5344</v>
       </c>
       <c r="Q34" t="s">
         <v>963</v>
@@ -46634,10 +46650,10 @@
         <v>2001</v>
       </c>
       <c r="E35" t="s">
+        <v>5253</v>
+      </c>
+      <c r="F35" t="s">
         <v>5254</v>
-      </c>
-      <c r="F35" t="s">
-        <v>5255</v>
       </c>
       <c r="G35" t="s">
         <v>5028</v>
@@ -46649,10 +46665,10 @@
         <v>1</v>
       </c>
       <c r="J35" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K35" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L35">
         <v>217</v>
@@ -46684,19 +46700,19 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
+        <v>5255</v>
+      </c>
+      <c r="C36" t="s">
         <v>5256</v>
-      </c>
-      <c r="C36" t="s">
-        <v>5257</v>
       </c>
       <c r="D36">
         <v>1993</v>
       </c>
       <c r="E36" t="s">
+        <v>5257</v>
+      </c>
+      <c r="F36" t="s">
         <v>5258</v>
-      </c>
-      <c r="F36" t="s">
-        <v>5259</v>
       </c>
       <c r="G36" t="s">
         <v>5028</v>
@@ -46708,10 +46724,10 @@
         <v>1</v>
       </c>
       <c r="J36" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K36" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L36">
         <v>1442</v>
@@ -46752,10 +46768,10 @@
         <v>2006</v>
       </c>
       <c r="E37" t="s">
+        <v>5259</v>
+      </c>
+      <c r="F37" t="s">
         <v>5260</v>
-      </c>
-      <c r="F37" t="s">
-        <v>5261</v>
       </c>
       <c r="G37" t="s">
         <v>5028</v>
@@ -46767,10 +46783,10 @@
         <v>1</v>
       </c>
       <c r="J37" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K37" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L37">
         <v>254</v>
@@ -46811,10 +46827,10 @@
         <v>1998</v>
       </c>
       <c r="E38" t="s">
+        <v>5261</v>
+      </c>
+      <c r="F38" t="s">
         <v>5262</v>
-      </c>
-      <c r="F38" t="s">
-        <v>5263</v>
       </c>
       <c r="G38" t="s">
         <v>5028</v>
@@ -46826,10 +46842,10 @@
         <v>1</v>
       </c>
       <c r="J38" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K38" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L38">
         <v>301</v>
@@ -46870,25 +46886,25 @@
         <v>2001</v>
       </c>
       <c r="E39" t="s">
+        <v>5263</v>
+      </c>
+      <c r="F39" t="s">
         <v>5264</v>
       </c>
-      <c r="F39" t="s">
-        <v>5265</v>
-      </c>
       <c r="G39" t="s">
         <v>5028</v>
       </c>
       <c r="H39" t="s">
-        <v>5333</v>
+        <v>5332</v>
       </c>
       <c r="I39" t="b">
         <v>1</v>
       </c>
       <c r="J39" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K39" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L39">
         <v>293</v>
@@ -46903,7 +46919,7 @@
         <v>5028</v>
       </c>
       <c r="P39" t="s">
-        <v>5347</v>
+        <v>5346</v>
       </c>
       <c r="Q39" t="s">
         <v>963</v>
@@ -46929,25 +46945,25 @@
         <v>2008</v>
       </c>
       <c r="E40" t="s">
+        <v>5265</v>
+      </c>
+      <c r="F40" t="s">
         <v>5266</v>
       </c>
-      <c r="F40" t="s">
-        <v>5267</v>
-      </c>
       <c r="G40" t="s">
         <v>5028</v>
       </c>
       <c r="H40" t="s">
-        <v>5331</v>
+        <v>5330</v>
       </c>
       <c r="I40" t="b">
         <v>1</v>
       </c>
       <c r="J40" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K40" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L40">
         <v>153</v>
@@ -46979,19 +46995,19 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
+        <v>5267</v>
+      </c>
+      <c r="C41" t="s">
         <v>5268</v>
-      </c>
-      <c r="C41" t="s">
-        <v>5269</v>
       </c>
       <c r="D41">
         <v>2001</v>
       </c>
       <c r="E41" t="s">
+        <v>5269</v>
+      </c>
+      <c r="F41" t="s">
         <v>5270</v>
-      </c>
-      <c r="F41" t="s">
-        <v>5271</v>
       </c>
       <c r="G41" t="s">
         <v>5028</v>
@@ -47003,10 +47019,10 @@
         <v>1</v>
       </c>
       <c r="J41" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K41" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L41">
         <v>188</v>
@@ -47038,34 +47054,34 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
+        <v>5271</v>
+      </c>
+      <c r="C42" t="s">
         <v>5272</v>
-      </c>
-      <c r="C42" t="s">
-        <v>5273</v>
       </c>
       <c r="D42">
         <v>2004</v>
       </c>
       <c r="E42" t="s">
+        <v>5273</v>
+      </c>
+      <c r="F42" t="s">
         <v>5274</v>
       </c>
-      <c r="F42" t="s">
-        <v>5275</v>
-      </c>
       <c r="G42" t="s">
         <v>5028</v>
       </c>
       <c r="H42" t="s">
-        <v>5326</v>
+        <v>5325</v>
       </c>
       <c r="I42" t="b">
         <v>1</v>
       </c>
       <c r="J42" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K42" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L42">
         <v>93</v>
@@ -47097,7 +47113,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>5072</v>
+        <v>5071</v>
       </c>
       <c r="C43" t="s">
         <v>4128</v>
@@ -47106,25 +47122,25 @@
         <v>1995</v>
       </c>
       <c r="E43" t="s">
+        <v>5275</v>
+      </c>
+      <c r="F43" t="s">
         <v>5276</v>
       </c>
-      <c r="F43" t="s">
-        <v>5277</v>
-      </c>
       <c r="G43" t="s">
         <v>5028</v>
       </c>
       <c r="H43" t="s">
-        <v>5334</v>
+        <v>5333</v>
       </c>
       <c r="I43" t="b">
         <v>1</v>
       </c>
       <c r="J43" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K43" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L43">
         <v>372</v>
@@ -47139,7 +47155,7 @@
         <v>5028</v>
       </c>
       <c r="P43" t="s">
-        <v>5345</v>
+        <v>5344</v>
       </c>
       <c r="Q43" t="s">
         <v>963</v>
@@ -47151,7 +47167,7 @@
         <v>5028</v>
       </c>
       <c r="T43" t="s">
-        <v>5348</v>
+        <v>5347</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
@@ -47159,19 +47175,19 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
+        <v>5277</v>
+      </c>
+      <c r="C44" t="s">
         <v>5278</v>
-      </c>
-      <c r="C44" t="s">
-        <v>5279</v>
       </c>
       <c r="D44">
         <v>2004</v>
       </c>
       <c r="E44" t="s">
+        <v>5279</v>
+      </c>
+      <c r="F44" t="s">
         <v>5280</v>
-      </c>
-      <c r="F44" t="s">
-        <v>5281</v>
       </c>
       <c r="G44" t="s">
         <v>5028</v>
@@ -47183,10 +47199,10 @@
         <v>1</v>
       </c>
       <c r="J44" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K44" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L44">
         <v>1830</v>
@@ -47218,19 +47234,19 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
+        <v>5281</v>
+      </c>
+      <c r="C45" t="s">
         <v>5282</v>
-      </c>
-      <c r="C45" t="s">
-        <v>5283</v>
       </c>
       <c r="D45">
         <v>2005</v>
       </c>
       <c r="E45" t="s">
+        <v>5283</v>
+      </c>
+      <c r="F45" t="s">
         <v>5284</v>
-      </c>
-      <c r="F45" t="s">
-        <v>5285</v>
       </c>
       <c r="G45" t="s">
         <v>5028</v>
@@ -47242,10 +47258,10 @@
         <v>1</v>
       </c>
       <c r="J45" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K45" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L45">
         <v>345</v>
@@ -47277,34 +47293,34 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
+        <v>5285</v>
+      </c>
+      <c r="C46" t="s">
         <v>5286</v>
-      </c>
-      <c r="C46" t="s">
-        <v>5287</v>
       </c>
       <c r="D46">
         <v>2006</v>
       </c>
       <c r="E46" t="s">
+        <v>5287</v>
+      </c>
+      <c r="F46" t="s">
         <v>5288</v>
       </c>
-      <c r="F46" t="s">
-        <v>5289</v>
-      </c>
       <c r="G46" t="s">
         <v>5028</v>
       </c>
       <c r="H46" t="s">
-        <v>5335</v>
+        <v>5334</v>
       </c>
       <c r="I46" t="b">
         <v>1</v>
       </c>
       <c r="J46" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K46" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L46">
         <v>1005</v>
@@ -47319,7 +47335,7 @@
         <v>5028</v>
       </c>
       <c r="P46" t="s">
-        <v>5337</v>
+        <v>5336</v>
       </c>
       <c r="Q46" t="s">
         <v>963</v>
@@ -47336,19 +47352,19 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
+        <v>5289</v>
+      </c>
+      <c r="C47" t="s">
         <v>5290</v>
-      </c>
-      <c r="C47" t="s">
-        <v>5291</v>
       </c>
       <c r="D47">
         <v>2006</v>
       </c>
       <c r="E47" t="s">
+        <v>5291</v>
+      </c>
+      <c r="F47" t="s">
         <v>5292</v>
-      </c>
-      <c r="F47" t="s">
-        <v>5293</v>
       </c>
       <c r="G47" t="s">
         <v>5028</v>
@@ -47360,10 +47376,10 @@
         <v>1</v>
       </c>
       <c r="J47" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K47" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L47">
         <v>596</v>
@@ -47378,7 +47394,7 @@
         <v>5028</v>
       </c>
       <c r="P47" t="s">
-        <v>5337</v>
+        <v>5336</v>
       </c>
       <c r="Q47" t="s">
         <v>963</v>
@@ -47395,19 +47411,19 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
+        <v>5293</v>
+      </c>
+      <c r="C48" t="s">
         <v>5294</v>
-      </c>
-      <c r="C48" t="s">
-        <v>5295</v>
       </c>
       <c r="D48">
         <v>2005</v>
       </c>
       <c r="E48" t="s">
-        <v>5296</v>
+        <v>5295</v>
       </c>
       <c r="F48" t="s">
-        <v>5138</v>
+        <v>5137</v>
       </c>
       <c r="G48" t="s">
         <v>5028</v>
@@ -47419,10 +47435,10 @@
         <v>1</v>
       </c>
       <c r="J48" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K48" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L48">
         <v>386</v>
@@ -47463,25 +47479,25 @@
         <v>1982</v>
       </c>
       <c r="E49" t="s">
-        <v>5297</v>
+        <v>5296</v>
       </c>
       <c r="F49" t="s">
-        <v>5139</v>
+        <v>5138</v>
       </c>
       <c r="G49" t="s">
         <v>5028</v>
       </c>
       <c r="H49" t="s">
-        <v>5334</v>
+        <v>5333</v>
       </c>
       <c r="I49" t="b">
         <v>1</v>
       </c>
       <c r="J49" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K49" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L49">
         <v>55</v>
@@ -47522,10 +47538,10 @@
         <v>1985</v>
       </c>
       <c r="E50" t="s">
-        <v>5298</v>
+        <v>5297</v>
       </c>
       <c r="F50" t="s">
-        <v>5140</v>
+        <v>5139</v>
       </c>
       <c r="G50" t="s">
         <v>5028</v>
@@ -47537,10 +47553,10 @@
         <v>1</v>
       </c>
       <c r="J50" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K50" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L50">
         <v>2143</v>
@@ -47572,7 +47588,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>5299</v>
+        <v>5298</v>
       </c>
       <c r="C51" t="s">
         <v>674</v>
@@ -47581,10 +47597,10 @@
         <v>1979</v>
       </c>
       <c r="E51" t="s">
-        <v>5300</v>
+        <v>5299</v>
       </c>
       <c r="F51" t="s">
-        <v>5141</v>
+        <v>5140</v>
       </c>
       <c r="G51" t="s">
         <v>5028</v>
@@ -47596,10 +47612,10 @@
         <v>1</v>
       </c>
       <c r="J51" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K51" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L51">
         <v>251</v>
@@ -47631,19 +47647,19 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
+        <v>5300</v>
+      </c>
+      <c r="C52" t="s">
         <v>5301</v>
-      </c>
-      <c r="C52" t="s">
-        <v>5302</v>
       </c>
       <c r="D52">
         <v>1997</v>
       </c>
       <c r="E52" t="s">
+        <v>5302</v>
+      </c>
+      <c r="F52" t="s">
         <v>5303</v>
-      </c>
-      <c r="F52" t="s">
-        <v>5304</v>
       </c>
       <c r="G52" t="s">
         <v>5028</v>
@@ -47655,10 +47671,10 @@
         <v>1</v>
       </c>
       <c r="J52" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K52" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L52">
         <v>9699</v>
@@ -47690,34 +47706,34 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
+        <v>5304</v>
+      </c>
+      <c r="C53" t="s">
         <v>5305</v>
-      </c>
-      <c r="C53" t="s">
-        <v>5306</v>
       </c>
       <c r="D53">
         <v>2014</v>
       </c>
       <c r="E53" t="s">
+        <v>5306</v>
+      </c>
+      <c r="F53" t="s">
         <v>5307</v>
       </c>
-      <c r="F53" t="s">
-        <v>5308</v>
-      </c>
       <c r="G53" t="s">
         <v>5028</v>
       </c>
       <c r="H53" t="s">
-        <v>5324</v>
+        <v>5323</v>
       </c>
       <c r="I53" t="b">
         <v>1</v>
       </c>
       <c r="J53" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K53" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L53">
         <v>264</v>
@@ -47749,19 +47765,19 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
+        <v>5308</v>
+      </c>
+      <c r="C54" t="s">
         <v>5309</v>
-      </c>
-      <c r="C54" t="s">
-        <v>5310</v>
       </c>
       <c r="D54">
         <v>2001</v>
       </c>
       <c r="E54" t="s">
+        <v>5310</v>
+      </c>
+      <c r="F54" t="s">
         <v>5311</v>
-      </c>
-      <c r="F54" t="s">
-        <v>5312</v>
       </c>
       <c r="G54" t="s">
         <v>5028</v>
@@ -47773,10 +47789,10 @@
         <v>1</v>
       </c>
       <c r="J54" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K54" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L54">
         <v>261</v>
@@ -47808,19 +47824,19 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
+        <v>5312</v>
+      </c>
+      <c r="C55" t="s">
         <v>5313</v>
-      </c>
-      <c r="C55" t="s">
-        <v>5314</v>
       </c>
       <c r="D55">
         <v>1999</v>
       </c>
       <c r="E55" t="s">
+        <v>5314</v>
+      </c>
+      <c r="F55" t="s">
         <v>5315</v>
-      </c>
-      <c r="F55" t="s">
-        <v>5316</v>
       </c>
       <c r="G55" t="s">
         <v>5028</v>
@@ -47832,10 +47848,10 @@
         <v>1</v>
       </c>
       <c r="J55" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K55" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L55">
         <v>423</v>
@@ -47867,19 +47883,19 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
+        <v>5316</v>
+      </c>
+      <c r="C56" t="s">
         <v>5317</v>
-      </c>
-      <c r="C56" t="s">
-        <v>5318</v>
       </c>
       <c r="D56">
         <v>2011</v>
       </c>
       <c r="E56" t="s">
+        <v>5318</v>
+      </c>
+      <c r="F56" t="s">
         <v>5319</v>
-      </c>
-      <c r="F56" t="s">
-        <v>5320</v>
       </c>
       <c r="G56" t="s">
         <v>5028</v>
@@ -47891,10 +47907,10 @@
         <v>1</v>
       </c>
       <c r="J56" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="K56" t="s">
-        <v>5321</v>
+        <v>5320</v>
       </c>
       <c r="L56">
         <v>197</v>
@@ -49526,10 +49542,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:Y14"/>
+  <dimension ref="A1:Y15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49581,24 +49597,24 @@
         <v>962</v>
       </c>
       <c r="O1" s="23" t="s">
-        <v>5113</v>
+        <v>5112</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>5119</v>
+        <v>5118</v>
       </c>
       <c r="Q1" s="28" t="s">
         <v>5037</v>
       </c>
       <c r="R1" s="29">
         <f>COUNTIFS($N:$N, "YES", $F:$F, "&lt;&gt;")</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="T1" s="28" t="s">
         <v>5038</v>
       </c>
       <c r="U1" s="29">
         <f>COUNTIF($M$2:$M$567, "YES")</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="V1" s="31"/>
       <c r="W1" s="31"/>
@@ -49649,7 +49665,7 @@
         <v>963</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
       <c r="R2" t="s">
         <v>904</v>
@@ -49702,7 +49718,7 @@
         <v>963</v>
       </c>
       <c r="O3" s="7" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
       <c r="W3" t="s">
         <v>5047</v>
@@ -49752,10 +49768,7 @@
         <v>963</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>966</v>
-      </c>
-      <c r="P4" t="s">
-        <v>5066</v>
+        <v>963</v>
       </c>
       <c r="W4" t="s">
         <v>5048</v>
@@ -49766,19 +49779,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5070</v>
+        <v>5069</v>
       </c>
       <c r="C5" t="s">
-        <v>5078</v>
+        <v>5077</v>
       </c>
       <c r="D5">
         <v>2003</v>
       </c>
       <c r="E5" t="s">
+        <v>5080</v>
+      </c>
+      <c r="F5" t="s">
         <v>5081</v>
-      </c>
-      <c r="F5" t="s">
-        <v>5082</v>
       </c>
       <c r="G5" t="s">
         <v>5029</v>
@@ -49787,16 +49800,16 @@
         <v>158</v>
       </c>
       <c r="I5" t="s">
+        <v>5075</v>
+      </c>
+      <c r="J5" t="s">
         <v>5076</v>
       </c>
-      <c r="J5" t="s">
-        <v>5077</v>
-      </c>
       <c r="K5" t="s">
-        <v>5077</v>
+        <v>5076</v>
       </c>
       <c r="L5" t="s">
-        <v>5070</v>
+        <v>5069</v>
       </c>
       <c r="M5" t="s">
         <v>963</v>
@@ -49805,7 +49818,7 @@
         <v>963</v>
       </c>
       <c r="O5" s="7" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
@@ -49813,19 +49826,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>5071</v>
+        <v>5070</v>
       </c>
       <c r="C6" t="s">
-        <v>5079</v>
+        <v>5078</v>
       </c>
       <c r="D6">
         <v>2012</v>
       </c>
       <c r="E6" t="s">
-        <v>5084</v>
+        <v>5083</v>
       </c>
       <c r="F6" t="s">
-        <v>5083</v>
+        <v>5082</v>
       </c>
       <c r="G6" t="s">
         <v>5029</v>
@@ -49834,16 +49847,16 @@
         <v>176</v>
       </c>
       <c r="I6" t="s">
+        <v>5084</v>
+      </c>
+      <c r="J6" t="s">
         <v>5085</v>
       </c>
-      <c r="J6" t="s">
-        <v>5086</v>
-      </c>
       <c r="K6" t="s">
-        <v>5086</v>
+        <v>5085</v>
       </c>
       <c r="L6" t="s">
-        <v>5071</v>
+        <v>5070</v>
       </c>
       <c r="M6" t="s">
         <v>963</v>
@@ -49852,17 +49865,17 @@
         <v>963</v>
       </c>
       <c r="O6" s="7" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>5117</v>
+        <v>5116</v>
       </c>
       <c r="R6">
         <f>COUNTIFS($N:$N, "YES", $M:$M, "&lt;&gt;PRIMARY STUDY")</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="W6" t="s">
-        <v>5075</v>
+        <v>5074</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
@@ -49870,7 +49883,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>5072</v>
+        <v>5071</v>
       </c>
       <c r="C7" t="s">
         <v>4128</v>
@@ -49879,10 +49892,10 @@
         <v>1995</v>
       </c>
       <c r="E7" t="s">
+        <v>5086</v>
+      </c>
+      <c r="F7" t="s">
         <v>5087</v>
-      </c>
-      <c r="F7" t="s">
-        <v>5088</v>
       </c>
       <c r="G7" t="s">
         <v>5029</v>
@@ -49891,16 +49904,16 @@
         <v>372</v>
       </c>
       <c r="I7" t="s">
+        <v>5088</v>
+      </c>
+      <c r="J7" t="s">
         <v>5089</v>
       </c>
-      <c r="J7" t="s">
-        <v>5090</v>
-      </c>
       <c r="K7" t="s">
-        <v>5090</v>
+        <v>5089</v>
       </c>
       <c r="L7" t="s">
-        <v>5072</v>
+        <v>5071</v>
       </c>
       <c r="M7" t="s">
         <v>963</v>
@@ -49909,14 +49922,14 @@
         <v>963</v>
       </c>
       <c r="O7" s="7" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>5114</v>
+        <v>5113</v>
       </c>
       <c r="R7">
         <f>COUNTIFS($O:$O, "YES", $F:$F, "&lt;&gt;")</f>
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
@@ -49924,7 +49937,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>5073</v>
+        <v>5072</v>
       </c>
       <c r="C8" t="s">
         <v>4077</v>
@@ -49933,10 +49946,10 @@
         <v>1994</v>
       </c>
       <c r="E8" t="s">
-        <v>5094</v>
+        <v>5093</v>
       </c>
       <c r="F8" t="s">
-        <v>5093</v>
+        <v>5092</v>
       </c>
       <c r="G8" t="s">
         <v>5029</v>
@@ -49945,13 +49958,13 @@
         <v>616</v>
       </c>
       <c r="I8" t="s">
+        <v>5090</v>
+      </c>
+      <c r="J8" t="s">
         <v>5091</v>
       </c>
-      <c r="J8" t="s">
-        <v>5092</v>
-      </c>
       <c r="L8" t="s">
-        <v>5073</v>
+        <v>5072</v>
       </c>
       <c r="M8" t="s">
         <v>963</v>
@@ -49960,7 +49973,7 @@
         <v>963</v>
       </c>
       <c r="O8" s="7" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
@@ -49968,19 +49981,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>5074</v>
+        <v>5073</v>
       </c>
       <c r="C9" t="s">
-        <v>5080</v>
+        <v>5079</v>
       </c>
       <c r="D9">
         <v>1999</v>
       </c>
       <c r="E9" t="s">
+        <v>5096</v>
+      </c>
+      <c r="F9" t="s">
         <v>5097</v>
-      </c>
-      <c r="F9" t="s">
-        <v>5098</v>
       </c>
       <c r="G9" t="s">
         <v>5029</v>
@@ -49989,16 +50002,16 @@
         <v>196</v>
       </c>
       <c r="I9" t="s">
+        <v>5094</v>
+      </c>
+      <c r="J9" t="s">
         <v>5095</v>
       </c>
-      <c r="J9" t="s">
-        <v>5096</v>
-      </c>
       <c r="K9" t="s">
-        <v>5096</v>
+        <v>5095</v>
       </c>
       <c r="L9" t="s">
-        <v>5074</v>
+        <v>5073</v>
       </c>
       <c r="M9" t="s">
         <v>963</v>
@@ -50007,7 +50020,7 @@
         <v>963</v>
       </c>
       <c r="O9" s="7" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
@@ -50015,19 +50028,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>5101</v>
+      </c>
+      <c r="C10" t="s">
         <v>5102</v>
-      </c>
-      <c r="C10" t="s">
-        <v>5103</v>
       </c>
       <c r="D10">
         <v>2012</v>
       </c>
       <c r="E10" t="s">
-        <v>5104</v>
+        <v>5103</v>
       </c>
       <c r="F10" t="s">
-        <v>5099</v>
+        <v>5098</v>
       </c>
       <c r="G10" t="s">
         <v>5029</v>
@@ -50036,16 +50049,16 @@
         <v>18</v>
       </c>
       <c r="I10" t="s">
+        <v>5099</v>
+      </c>
+      <c r="J10" t="s">
         <v>5100</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
+        <v>5100</v>
+      </c>
+      <c r="L10" t="s">
         <v>5101</v>
-      </c>
-      <c r="K10" t="s">
-        <v>5101</v>
-      </c>
-      <c r="L10" t="s">
-        <v>5102</v>
       </c>
       <c r="M10" t="s">
         <v>963</v>
@@ -50054,7 +50067,7 @@
         <v>963</v>
       </c>
       <c r="O10" s="7" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
@@ -50062,19 +50075,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>5109</v>
+        <v>5108</v>
       </c>
       <c r="C11" t="s">
-        <v>5106</v>
+        <v>5105</v>
       </c>
       <c r="D11">
         <v>2020</v>
       </c>
       <c r="E11" t="s">
-        <v>5110</v>
+        <v>5109</v>
       </c>
       <c r="F11" t="s">
-        <v>5107</v>
+        <v>5106</v>
       </c>
       <c r="G11" t="s">
         <v>5029</v>
@@ -50083,16 +50096,16 @@
         <v>11</v>
       </c>
       <c r="I11" t="s">
+        <v>5107</v>
+      </c>
+      <c r="J11" t="s">
+        <v>5104</v>
+      </c>
+      <c r="K11" t="s">
+        <v>5104</v>
+      </c>
+      <c r="L11" t="s">
         <v>5108</v>
-      </c>
-      <c r="J11" t="s">
-        <v>5105</v>
-      </c>
-      <c r="K11" t="s">
-        <v>5105</v>
-      </c>
-      <c r="L11" t="s">
-        <v>5109</v>
       </c>
       <c r="M11" t="s">
         <v>963</v>
@@ -50101,7 +50114,7 @@
         <v>963</v>
       </c>
       <c r="O11" s="7" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
@@ -50148,10 +50161,10 @@
         <v>963</v>
       </c>
       <c r="O12" s="7" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
       <c r="P12" t="s">
-        <v>5120</v>
+        <v>5119</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
@@ -50198,10 +50211,10 @@
         <v>963</v>
       </c>
       <c r="O13" s="7" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
       <c r="P13" t="s">
-        <v>5120</v>
+        <v>5119</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
@@ -50218,10 +50231,10 @@
         <v>1999</v>
       </c>
       <c r="E14" t="s">
+        <v>5251</v>
+      </c>
+      <c r="F14" t="s">
         <v>5252</v>
-      </c>
-      <c r="F14" t="s">
-        <v>5253</v>
       </c>
       <c r="G14" t="s">
         <v>5028</v>
@@ -50233,7 +50246,7 @@
         <v>5028</v>
       </c>
       <c r="J14" t="s">
-        <v>5028</v>
+        <v>5353</v>
       </c>
       <c r="K14" t="s">
         <v>5028</v>
@@ -50248,10 +50261,57 @@
         <v>963</v>
       </c>
       <c r="O14" s="7" t="s">
+        <v>963</v>
+      </c>
+      <c r="P14" t="s">
+        <v>5345</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5348</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5349</v>
+      </c>
+      <c r="D15">
+        <v>1999</v>
+      </c>
+      <c r="E15" t="s">
+        <v>5351</v>
+      </c>
+      <c r="F15" t="s">
+        <v>5350</v>
+      </c>
+      <c r="G15" t="s">
+        <v>5028</v>
+      </c>
+      <c r="H15">
+        <v>17</v>
+      </c>
+      <c r="I15" t="s">
+        <v>5028</v>
+      </c>
+      <c r="J15" t="s">
+        <v>5352</v>
+      </c>
+      <c r="K15" t="s">
+        <v>5352</v>
+      </c>
+      <c r="L15" t="s">
+        <v>5348</v>
+      </c>
+      <c r="M15" t="s">
+        <v>963</v>
+      </c>
+      <c r="N15" t="s">
+        <v>963</v>
+      </c>
+      <c r="O15" s="40" t="s">
         <v>966</v>
-      </c>
-      <c r="P14" t="s">
-        <v>5346</v>
       </c>
     </row>
   </sheetData>
@@ -50289,7 +50349,7 @@
   <conditionalFormatting sqref="L14">
     <cfRule type="duplicateValues" dxfId="16" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:O14">
+  <conditionalFormatting sqref="M2:O15">
     <cfRule type="containsText" dxfId="15" priority="2" operator="containsText" text="PRIMARY STUDY">
       <formula>NOT(ISERROR(SEARCH("PRIMARY STUDY",M2)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Finished the twin study list (17 studies), restructured several folders
</commit_message>
<xml_diff>
--- a/Literature/Literature.xlsx
+++ b/Literature/Literature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hso20\OneDrive\Plocha\IES\Diploma-Thesis\Literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCFE65CD-E19A-4410-A372-5CAA4820C354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEBEDF9D-1FC4-4ED0-9EA8-B3FAAF4AC43E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -511,7 +511,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -537,7 +537,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -564,7 +564,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
         <r>
           <rPr>
@@ -590,7 +590,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
       <text>
         <r>
           <rPr>
@@ -616,7 +616,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000006000000}">
+    <comment ref="P6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000006000000}">
       <text>
         <r>
           <rPr>
@@ -694,7 +694,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10210" uniqueCount="5354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10228" uniqueCount="5367">
   <si>
     <t>Number</t>
   </si>
@@ -16756,6 +16756,45 @@
   </si>
   <si>
     <t>https://www.sciencedirect.com/science/article/pii/S0927537198000141</t>
+  </si>
+  <si>
+    <t>Bingley, Paul, Kaare Christensen, and Ian Walker. "Twin-based estimates of the returns to education: Evidence from the population of Danish twins." unpublished paper (2005).</t>
+  </si>
+  <si>
+    <t>Bingley et al. (2005)</t>
+  </si>
+  <si>
+    <t>Twin-based estimates of the returns to education: Evidence from the population of Danish twins</t>
+  </si>
+  <si>
+    <t>http://www.warwick.ac.uk/fac/soc/economics/staff/academic/walker/current_research/twins2_130905.pdf</t>
+  </si>
+  <si>
+    <t>Bingley, Paul, Kaare Christensen, and Ian Walker. "The returns to observed and unobserved skills over time: Evidence from a panel of the population of danish twins." Danish National Institute for Social Research (2009).</t>
+  </si>
+  <si>
+    <t>Bingley et al.</t>
+  </si>
+  <si>
+    <t>Bingley et al. (2009)</t>
+  </si>
+  <si>
+    <t>The returns to observed and unobserved skills over time: Evidence from a panel of the population of danish twins</t>
+  </si>
+  <si>
+    <t>https://citeseerx.ist.psu.edu/document?repid=rep1&amp;type=pdf&amp;doi=433cabc29ff5522c0c57c251f78124d6f4cb7ec6</t>
+  </si>
+  <si>
+    <t>Isacsson, Gunnar. "Estimating the economic return to educational levels using data on twins." Journal of Applied Econometrics 19, no. 1 (2004): 99-119.</t>
+  </si>
+  <si>
+    <t>Isacsson (2004)</t>
+  </si>
+  <si>
+    <t>Estimating the economic return to educational levels using data on twins</t>
+  </si>
+  <si>
+    <t>https://onlinelibrary.wiley.com/doi/abs/10.1002/jae.724</t>
   </si>
 </sst>
 </file>
@@ -17090,7 +17129,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -17137,7 +17176,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -17832,8 +17870,8 @@
   <dimension ref="A1:Y575"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17908,15 +17946,15 @@
         <v>5037</v>
       </c>
       <c r="R1" s="29">
-        <f>COUNTIFS($M:$M, "YES", $F:$F, "&lt;&gt;") + Twins!R1</f>
-        <v>93</v>
+        <f>COUNTIFS($M:$M, "YES", $F:$F, "&lt;&gt;") + Twins!Q1</f>
+        <v>96</v>
       </c>
       <c r="T1" s="28" t="s">
         <v>5038</v>
       </c>
       <c r="U1" s="29">
-        <f>COUNTIF($L$2:$L$575, "&lt;&gt; ") +Twins!U1</f>
-        <v>239</v>
+        <f>COUNTIF($L$2:$L$575, "&lt;&gt; ") +Twins!T1</f>
+        <v>242</v>
       </c>
       <c r="V1" s="31"/>
       <c r="W1" s="31"/>
@@ -44554,7 +44592,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49542,10 +49580,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:Y15"/>
+  <dimension ref="A1:X18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49553,7 +49591,7 @@
     <col min="2" max="2" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -49573,55 +49611,52 @@
         <v>3903</v>
       </c>
       <c r="G1" s="23" t="s">
-        <v>3907</v>
+        <v>3902</v>
       </c>
       <c r="H1" s="23" t="s">
-        <v>3902</v>
+        <v>3906</v>
       </c>
       <c r="I1" s="23" t="s">
-        <v>3906</v>
+        <v>3904</v>
       </c>
       <c r="J1" s="23" t="s">
-        <v>3904</v>
-      </c>
-      <c r="K1" s="23" t="s">
         <v>3905</v>
       </c>
+      <c r="K1" s="24" t="s">
+        <v>7</v>
+      </c>
       <c r="L1" s="24" t="s">
-        <v>7</v>
+        <v>965</v>
       </c>
       <c r="M1" s="24" t="s">
-        <v>965</v>
-      </c>
-      <c r="N1" s="24" t="s">
         <v>962</v>
       </c>
-      <c r="O1" s="23" t="s">
+      <c r="N1" s="23" t="s">
         <v>5112</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>5118</v>
       </c>
-      <c r="Q1" s="28" t="s">
+      <c r="P1" s="28" t="s">
         <v>5037</v>
       </c>
-      <c r="R1" s="29">
-        <f>COUNTIFS($N:$N, "YES", $F:$F, "&lt;&gt;")</f>
-        <v>14</v>
-      </c>
-      <c r="T1" s="28" t="s">
+      <c r="Q1" s="29">
+        <f>COUNTIFS($M:$M, "YES", $F:$F, "&lt;&gt;")</f>
+        <v>17</v>
+      </c>
+      <c r="S1" s="28" t="s">
         <v>5038</v>
       </c>
-      <c r="U1" s="29">
-        <f>COUNTIF($M$2:$M$567, "YES")</f>
-        <v>14</v>
-      </c>
+      <c r="T1" s="29">
+        <f>COUNTIF($L$2:$L$567, "YES")</f>
+        <v>17</v>
+      </c>
+      <c r="U1" s="31"/>
       <c r="V1" s="31"/>
       <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="30"/>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X1" s="30"/>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -49640,41 +49675,38 @@
       <c r="F2" t="s">
         <v>5049</v>
       </c>
-      <c r="G2" t="s">
-        <v>5029</v>
-      </c>
-      <c r="H2">
+      <c r="G2">
         <v>908</v>
       </c>
+      <c r="H2" t="s">
+        <v>5053</v>
+      </c>
       <c r="I2" t="s">
-        <v>5053</v>
+        <v>5052</v>
       </c>
       <c r="J2" t="s">
         <v>5052</v>
       </c>
       <c r="K2" t="s">
-        <v>5052</v>
+        <v>5051</v>
       </c>
       <c r="L2" t="s">
-        <v>5051</v>
+        <v>963</v>
       </c>
       <c r="M2" t="s">
         <v>963</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" s="7" t="s">
         <v>963</v>
       </c>
-      <c r="O2" s="7" t="s">
-        <v>963</v>
-      </c>
-      <c r="R2" t="s">
-        <v>904</v>
-      </c>
-      <c r="W2" t="s">
+      <c r="Q2" t="s">
+        <v>904</v>
+      </c>
+      <c r="V2" t="s">
         <v>5046</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -49693,38 +49725,35 @@
       <c r="F3" t="s">
         <v>5054</v>
       </c>
-      <c r="G3" t="s">
-        <v>5029</v>
-      </c>
-      <c r="H3">
+      <c r="G3">
         <v>1812</v>
       </c>
+      <c r="H3" t="s">
+        <v>5055</v>
+      </c>
       <c r="I3" t="s">
-        <v>5055</v>
+        <v>5056</v>
       </c>
       <c r="J3" t="s">
         <v>5056</v>
       </c>
       <c r="K3" t="s">
-        <v>5056</v>
+        <v>5060</v>
       </c>
       <c r="L3" t="s">
-        <v>5060</v>
+        <v>963</v>
       </c>
       <c r="M3" t="s">
         <v>963</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" s="7" t="s">
         <v>963</v>
       </c>
-      <c r="O3" s="7" t="s">
-        <v>963</v>
-      </c>
-      <c r="W3" t="s">
+      <c r="V3" t="s">
         <v>5047</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -49743,38 +49772,35 @@
       <c r="F4" t="s">
         <v>5061</v>
       </c>
-      <c r="G4" t="s">
-        <v>5029</v>
-      </c>
-      <c r="H4">
+      <c r="G4">
         <v>188</v>
       </c>
+      <c r="H4" t="s">
+        <v>5062</v>
+      </c>
       <c r="I4" t="s">
-        <v>5062</v>
+        <v>5064</v>
       </c>
       <c r="J4" t="s">
-        <v>5064</v>
+        <v>5063</v>
       </c>
       <c r="K4" t="s">
-        <v>5063</v>
+        <v>727</v>
       </c>
       <c r="L4" t="s">
-        <v>727</v>
+        <v>963</v>
       </c>
       <c r="M4" t="s">
         <v>963</v>
       </c>
-      <c r="N4" t="s">
+      <c r="N4" s="7" t="s">
         <v>963</v>
       </c>
-      <c r="O4" s="7" t="s">
-        <v>963</v>
-      </c>
-      <c r="W4" t="s">
+      <c r="V4" t="s">
         <v>5048</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -49793,35 +49819,32 @@
       <c r="F5" t="s">
         <v>5081</v>
       </c>
-      <c r="G5" t="s">
-        <v>5029</v>
-      </c>
-      <c r="H5">
+      <c r="G5">
         <v>158</v>
       </c>
+      <c r="H5" t="s">
+        <v>5075</v>
+      </c>
       <c r="I5" t="s">
-        <v>5075</v>
+        <v>5076</v>
       </c>
       <c r="J5" t="s">
         <v>5076</v>
       </c>
       <c r="K5" t="s">
-        <v>5076</v>
+        <v>5069</v>
       </c>
       <c r="L5" t="s">
-        <v>5069</v>
+        <v>963</v>
       </c>
       <c r="M5" t="s">
         <v>963</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" s="7" t="s">
         <v>963</v>
       </c>
-      <c r="O5" s="7" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -49840,45 +49863,42 @@
       <c r="F6" t="s">
         <v>5082</v>
       </c>
-      <c r="G6" t="s">
-        <v>5029</v>
-      </c>
-      <c r="H6">
+      <c r="G6">
         <v>176</v>
       </c>
+      <c r="H6" t="s">
+        <v>5084</v>
+      </c>
       <c r="I6" t="s">
-        <v>5084</v>
+        <v>5085</v>
       </c>
       <c r="J6" t="s">
         <v>5085</v>
       </c>
       <c r="K6" t="s">
-        <v>5085</v>
+        <v>5070</v>
       </c>
       <c r="L6" t="s">
-        <v>5070</v>
+        <v>963</v>
       </c>
       <c r="M6" t="s">
         <v>963</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N6" s="7" t="s">
         <v>963</v>
       </c>
-      <c r="O6" s="7" t="s">
-        <v>963</v>
-      </c>
-      <c r="Q6" s="2" t="s">
+      <c r="P6" s="2" t="s">
         <v>5116</v>
       </c>
-      <c r="R6">
-        <f>COUNTIFS($N:$N, "YES", $M:$M, "&lt;&gt;PRIMARY STUDY")</f>
-        <v>14</v>
-      </c>
-      <c r="W6" t="s">
+      <c r="Q6">
+        <f>COUNTIFS($M:$M, "YES", $L:$L, "&lt;&gt;PRIMARY STUDY")</f>
+        <v>17</v>
+      </c>
+      <c r="V6" t="s">
         <v>5074</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -49897,42 +49917,39 @@
       <c r="F7" t="s">
         <v>5087</v>
       </c>
-      <c r="G7" t="s">
-        <v>5029</v>
-      </c>
-      <c r="H7">
+      <c r="G7">
         <v>372</v>
       </c>
+      <c r="H7" t="s">
+        <v>5088</v>
+      </c>
       <c r="I7" t="s">
-        <v>5088</v>
+        <v>5089</v>
       </c>
       <c r="J7" t="s">
         <v>5089</v>
       </c>
       <c r="K7" t="s">
-        <v>5089</v>
+        <v>5071</v>
       </c>
       <c r="L7" t="s">
-        <v>5071</v>
+        <v>963</v>
       </c>
       <c r="M7" t="s">
         <v>963</v>
       </c>
-      <c r="N7" t="s">
+      <c r="N7" s="7" t="s">
         <v>963</v>
       </c>
-      <c r="O7" s="7" t="s">
-        <v>963</v>
-      </c>
-      <c r="Q7" s="2" t="s">
+      <c r="P7" s="2" t="s">
         <v>5113</v>
       </c>
-      <c r="R7">
-        <f>COUNTIFS($O:$O, "YES", $F:$F, "&lt;&gt;")</f>
+      <c r="Q7">
+        <f>COUNTIFS($N:$N, "YES", $F:$F, "&lt;&gt;")</f>
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -49951,32 +49968,29 @@
       <c r="F8" t="s">
         <v>5092</v>
       </c>
-      <c r="G8" t="s">
-        <v>5029</v>
-      </c>
-      <c r="H8">
+      <c r="G8">
         <v>616</v>
       </c>
+      <c r="H8" t="s">
+        <v>5090</v>
+      </c>
       <c r="I8" t="s">
-        <v>5090</v>
-      </c>
-      <c r="J8" t="s">
         <v>5091</v>
       </c>
+      <c r="K8" t="s">
+        <v>5072</v>
+      </c>
       <c r="L8" t="s">
-        <v>5072</v>
+        <v>963</v>
       </c>
       <c r="M8" t="s">
         <v>963</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N8" s="7" t="s">
         <v>963</v>
       </c>
-      <c r="O8" s="7" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -49995,35 +50009,32 @@
       <c r="F9" t="s">
         <v>5097</v>
       </c>
-      <c r="G9" t="s">
-        <v>5029</v>
-      </c>
-      <c r="H9">
+      <c r="G9">
         <v>196</v>
       </c>
+      <c r="H9" t="s">
+        <v>5094</v>
+      </c>
       <c r="I9" t="s">
-        <v>5094</v>
+        <v>5095</v>
       </c>
       <c r="J9" t="s">
         <v>5095</v>
       </c>
       <c r="K9" t="s">
-        <v>5095</v>
+        <v>5073</v>
       </c>
       <c r="L9" t="s">
-        <v>5073</v>
+        <v>963</v>
       </c>
       <c r="M9" t="s">
         <v>963</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N9" s="7" t="s">
         <v>963</v>
       </c>
-      <c r="O9" s="7" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -50042,35 +50053,32 @@
       <c r="F10" t="s">
         <v>5098</v>
       </c>
-      <c r="G10" t="s">
-        <v>5029</v>
-      </c>
-      <c r="H10">
+      <c r="G10">
         <v>18</v>
       </c>
+      <c r="H10" t="s">
+        <v>5099</v>
+      </c>
       <c r="I10" t="s">
-        <v>5099</v>
+        <v>5100</v>
       </c>
       <c r="J10" t="s">
         <v>5100</v>
       </c>
       <c r="K10" t="s">
-        <v>5100</v>
+        <v>5101</v>
       </c>
       <c r="L10" t="s">
-        <v>5101</v>
+        <v>963</v>
       </c>
       <c r="M10" t="s">
         <v>963</v>
       </c>
-      <c r="N10" t="s">
+      <c r="N10" s="7" t="s">
         <v>963</v>
       </c>
-      <c r="O10" s="7" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -50089,35 +50097,32 @@
       <c r="F11" t="s">
         <v>5106</v>
       </c>
-      <c r="G11" t="s">
-        <v>5029</v>
-      </c>
-      <c r="H11">
+      <c r="G11">
         <v>11</v>
       </c>
+      <c r="H11" t="s">
+        <v>5107</v>
+      </c>
       <c r="I11" t="s">
-        <v>5107</v>
+        <v>5104</v>
       </c>
       <c r="J11" t="s">
         <v>5104</v>
       </c>
       <c r="K11" t="s">
-        <v>5104</v>
+        <v>5108</v>
       </c>
       <c r="L11" t="s">
-        <v>5108</v>
+        <v>963</v>
       </c>
       <c r="M11" t="s">
         <v>963</v>
       </c>
-      <c r="N11" t="s">
+      <c r="N11" s="7" t="s">
         <v>963</v>
       </c>
-      <c r="O11" s="7" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -50136,38 +50141,35 @@
       <c r="F12" t="s">
         <v>970</v>
       </c>
-      <c r="G12" t="s">
-        <v>1074</v>
-      </c>
-      <c r="H12">
-        <v>1</v>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>1073</v>
       </c>
       <c r="I12" t="s">
-        <v>1073</v>
+        <v>1075</v>
       </c>
       <c r="J12" t="s">
         <v>1075</v>
       </c>
       <c r="K12" t="s">
-        <v>1075</v>
+        <v>3935</v>
       </c>
       <c r="L12" t="s">
-        <v>3935</v>
+        <v>963</v>
       </c>
       <c r="M12" t="s">
         <v>963</v>
       </c>
-      <c r="N12" t="s">
+      <c r="N12" s="7" t="s">
         <v>963</v>
       </c>
-      <c r="O12" s="7" t="s">
-        <v>963</v>
-      </c>
-      <c r="P12" t="s">
+      <c r="O12" t="s">
         <v>5119</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -50186,38 +50188,35 @@
       <c r="F13" t="s">
         <v>1962</v>
       </c>
-      <c r="G13" t="s">
-        <v>1959</v>
-      </c>
-      <c r="H13">
+      <c r="G13">
         <v>19</v>
       </c>
+      <c r="H13" t="s">
+        <v>1958</v>
+      </c>
       <c r="I13" t="s">
-        <v>1958</v>
+        <v>1960</v>
       </c>
       <c r="J13" t="s">
-        <v>1960</v>
+        <v>1961</v>
       </c>
       <c r="K13" t="s">
-        <v>1961</v>
+        <v>4127</v>
       </c>
       <c r="L13" t="s">
-        <v>4127</v>
+        <v>963</v>
       </c>
       <c r="M13" t="s">
         <v>963</v>
       </c>
-      <c r="N13" t="s">
+      <c r="N13" s="7" t="s">
         <v>963</v>
       </c>
-      <c r="O13" s="7" t="s">
-        <v>963</v>
-      </c>
-      <c r="P13" t="s">
+      <c r="O13" t="s">
         <v>5119</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -50236,38 +50235,35 @@
       <c r="F14" t="s">
         <v>5252</v>
       </c>
-      <c r="G14" t="s">
-        <v>5028</v>
-      </c>
-      <c r="H14">
+      <c r="G14">
         <v>177</v>
       </c>
+      <c r="H14" t="s">
+        <v>5028</v>
+      </c>
       <c r="I14" t="s">
-        <v>5028</v>
+        <v>5353</v>
       </c>
       <c r="J14" t="s">
-        <v>5353</v>
+        <v>5028</v>
       </c>
       <c r="K14" t="s">
-        <v>5028</v>
+        <v>399</v>
       </c>
       <c r="L14" t="s">
-        <v>399</v>
+        <v>963</v>
       </c>
       <c r="M14" t="s">
         <v>963</v>
       </c>
-      <c r="N14" t="s">
+      <c r="N14" s="7" t="s">
         <v>963</v>
       </c>
-      <c r="O14" s="7" t="s">
-        <v>963</v>
-      </c>
-      <c r="P14" t="s">
+      <c r="O14" t="s">
         <v>5345</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -50286,31 +50282,160 @@
       <c r="F15" t="s">
         <v>5350</v>
       </c>
-      <c r="G15" t="s">
-        <v>5028</v>
-      </c>
-      <c r="H15">
+      <c r="G15">
         <v>17</v>
       </c>
+      <c r="H15" t="s">
+        <v>5028</v>
+      </c>
       <c r="I15" t="s">
-        <v>5028</v>
+        <v>5352</v>
       </c>
       <c r="J15" t="s">
         <v>5352</v>
       </c>
       <c r="K15" t="s">
-        <v>5352</v>
+        <v>5348</v>
       </c>
       <c r="L15" t="s">
-        <v>5348</v>
+        <v>963</v>
       </c>
       <c r="M15" t="s">
         <v>963</v>
       </c>
-      <c r="N15" t="s">
+      <c r="N15" s="7" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5355</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5359</v>
+      </c>
+      <c r="D16">
+        <v>2005</v>
+      </c>
+      <c r="E16" t="s">
+        <v>5356</v>
+      </c>
+      <c r="F16" t="s">
+        <v>5354</v>
+      </c>
+      <c r="G16">
+        <v>19</v>
+      </c>
+      <c r="H16" t="s">
+        <v>5028</v>
+      </c>
+      <c r="I16" t="s">
+        <v>5357</v>
+      </c>
+      <c r="J16" t="s">
+        <v>5357</v>
+      </c>
+      <c r="K16" t="s">
+        <v>5355</v>
+      </c>
+      <c r="L16" t="s">
         <v>963</v>
       </c>
-      <c r="O15" s="40" t="s">
+      <c r="M16" t="s">
+        <v>963</v>
+      </c>
+      <c r="N16" s="7" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5360</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5359</v>
+      </c>
+      <c r="D17">
+        <v>2009</v>
+      </c>
+      <c r="E17" t="s">
+        <v>5361</v>
+      </c>
+      <c r="F17" t="s">
+        <v>5358</v>
+      </c>
+      <c r="G17">
+        <v>8</v>
+      </c>
+      <c r="H17" t="s">
+        <v>5028</v>
+      </c>
+      <c r="I17" t="s">
+        <v>5362</v>
+      </c>
+      <c r="J17" t="s">
+        <v>5357</v>
+      </c>
+      <c r="K17" t="s">
+        <v>5360</v>
+      </c>
+      <c r="L17" t="s">
+        <v>963</v>
+      </c>
+      <c r="M17" t="s">
+        <v>963</v>
+      </c>
+      <c r="N17" s="7" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5364</v>
+      </c>
+      <c r="C18" t="s">
+        <v>400</v>
+      </c>
+      <c r="D18">
+        <v>2004</v>
+      </c>
+      <c r="E18" t="s">
+        <v>5365</v>
+      </c>
+      <c r="F18" t="s">
+        <v>5363</v>
+      </c>
+      <c r="G18">
+        <v>85</v>
+      </c>
+      <c r="H18" t="s">
+        <v>5028</v>
+      </c>
+      <c r="I18" t="s">
+        <v>5366</v>
+      </c>
+      <c r="J18" t="s">
+        <v>5366</v>
+      </c>
+      <c r="K18" t="s">
+        <v>5364</v>
+      </c>
+      <c r="L18" t="s">
+        <v>963</v>
+      </c>
+      <c r="M18" t="s">
+        <v>963</v>
+      </c>
+      <c r="N18" s="7" t="s">
         <v>966</v>
       </c>
     </row>
@@ -50335,56 +50460,56 @@
       <formula>LEN(TRIM(F13))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H12 H15:H1048576">
+  <conditionalFormatting sqref="G1:G12 G15:G1048576 H16:H18">
     <cfRule type="containsBlanks" dxfId="19" priority="38">
-      <formula>LEN(TRIM(H1))=0</formula>
+      <formula>LEN(TRIM(G1))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2">
+  <conditionalFormatting sqref="K2">
     <cfRule type="duplicateValues" dxfId="18" priority="28"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L13">
+  <conditionalFormatting sqref="K13">
     <cfRule type="duplicateValues" dxfId="17" priority="16"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L14">
+  <conditionalFormatting sqref="K14">
     <cfRule type="duplicateValues" dxfId="16" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:O15">
+  <conditionalFormatting sqref="L2:N18">
     <cfRule type="containsText" dxfId="15" priority="2" operator="containsText" text="PRIMARY STUDY">
-      <formula>NOT(ISERROR(SEARCH("PRIMARY STUDY",M2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("PRIMARY STUDY",L2)))</formula>
     </cfRule>
     <cfRule type="notContainsText" dxfId="14" priority="3" operator="notContains" text="YES">
-      <formula>ISERROR(SEARCH("YES",M2))</formula>
+      <formula>ISERROR(SEARCH("YES",L2))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="13" priority="4" operator="containsText" text="YES">
-      <formula>NOT(ISERROR(SEARCH("YES",M2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("YES",L2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O13:O14">
+  <conditionalFormatting sqref="N13:N14">
     <cfRule type="containsBlanks" dxfId="12" priority="1">
-      <formula>LEN(TRIM(O13))=0</formula>
+      <formula>LEN(TRIM(N13))=0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="11" priority="10" operator="between">
       <formula>1</formula>
       <formula>4</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH("X",O13)))</formula>
+      <formula>NOT(ISERROR(SEARCH("X",N13)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P1 P4">
+  <conditionalFormatting sqref="O1 O4">
     <cfRule type="cellIs" dxfId="9" priority="32" operator="between">
       <formula>1</formula>
       <formula>4</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="8" priority="33" operator="containsText" text="X">
-      <formula>NOT(ISERROR(SEARCH("X",P1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("X",O1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q1:Q2">
+  <conditionalFormatting sqref="P1:P2">
     <cfRule type="duplicateValues" dxfId="7" priority="31"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T1">
+  <conditionalFormatting sqref="S1">
     <cfRule type="duplicateValues" dxfId="6" priority="29"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
All 16 studies collected, twin data set provisionally complete
</commit_message>
<xml_diff>
--- a/Literature/Literature.xlsx
+++ b/Literature/Literature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hso20\OneDrive\Plocha\IES\Diploma-Thesis\Literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEBEDF9D-1FC4-4ED0-9EA8-B3FAAF4AC43E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C65A8C-66B5-4771-9241-59B1B934700C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -694,7 +694,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10228" uniqueCount="5367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10217" uniqueCount="5364">
   <si>
     <t>Number</t>
   </si>
@@ -16756,15 +16756,6 @@
   </si>
   <si>
     <t>https://www.sciencedirect.com/science/article/pii/S0927537198000141</t>
-  </si>
-  <si>
-    <t>Bingley, Paul, Kaare Christensen, and Ian Walker. "Twin-based estimates of the returns to education: Evidence from the population of Danish twins." unpublished paper (2005).</t>
-  </si>
-  <si>
-    <t>Bingley et al. (2005)</t>
-  </si>
-  <si>
-    <t>Twin-based estimates of the returns to education: Evidence from the population of Danish twins</t>
   </si>
   <si>
     <t>http://www.warwick.ac.uk/fac/soc/economics/staff/academic/walker/current_research/twins2_130905.pdf</t>
@@ -17947,14 +17938,14 @@
       </c>
       <c r="R1" s="29">
         <f>COUNTIFS($M:$M, "YES", $F:$F, "&lt;&gt;") + Twins!Q1</f>
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="T1" s="28" t="s">
         <v>5038</v>
       </c>
       <c r="U1" s="29">
         <f>COUNTIF($L$2:$L$575, "&lt;&gt; ") +Twins!T1</f>
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="V1" s="31"/>
       <c r="W1" s="31"/>
@@ -49580,10 +49571,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:X18"/>
+  <dimension ref="A1:X17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49642,14 +49633,14 @@
       </c>
       <c r="Q1" s="29">
         <f>COUNTIFS($M:$M, "YES", $F:$F, "&lt;&gt;")</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="S1" s="28" t="s">
         <v>5038</v>
       </c>
       <c r="T1" s="29">
-        <f>COUNTIF($L$2:$L$567, "YES")</f>
-        <v>17</v>
+        <f>COUNTIF($L$2:$L$566, "YES")</f>
+        <v>16</v>
       </c>
       <c r="U1" s="31"/>
       <c r="V1" s="31"/>
@@ -49892,7 +49883,7 @@
       </c>
       <c r="Q6">
         <f>COUNTIFS($M:$M, "YES", $L:$L, "&lt;&gt;PRIMARY STUDY")</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="V6" t="s">
         <v>5074</v>
@@ -49946,7 +49937,7 @@
       </c>
       <c r="Q7">
         <f>COUNTIFS($N:$N, "YES", $F:$F, "&lt;&gt;")</f>
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
@@ -50304,7 +50295,7 @@
         <v>963</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
@@ -50312,34 +50303,34 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>5357</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5356</v>
+      </c>
+      <c r="D16">
+        <v>2009</v>
+      </c>
+      <c r="E16" t="s">
+        <v>5358</v>
+      </c>
+      <c r="F16" t="s">
         <v>5355</v>
       </c>
-      <c r="C16" t="s">
+      <c r="G16">
+        <v>8</v>
+      </c>
+      <c r="H16" t="s">
+        <v>5028</v>
+      </c>
+      <c r="I16" t="s">
         <v>5359</v>
       </c>
-      <c r="D16">
-        <v>2005</v>
-      </c>
-      <c r="E16" t="s">
-        <v>5356</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="J16" t="s">
         <v>5354</v>
       </c>
-      <c r="G16">
-        <v>19</v>
-      </c>
-      <c r="H16" t="s">
-        <v>5028</v>
-      </c>
-      <c r="I16" t="s">
+      <c r="K16" t="s">
         <v>5357</v>
-      </c>
-      <c r="J16" t="s">
-        <v>5357</v>
-      </c>
-      <c r="K16" t="s">
-        <v>5355</v>
       </c>
       <c r="L16" t="s">
         <v>963</v>
@@ -50348,7 +50339,7 @@
         <v>963</v>
       </c>
       <c r="N16" s="7" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -50356,34 +50347,34 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>5361</v>
+      </c>
+      <c r="C17" t="s">
+        <v>400</v>
+      </c>
+      <c r="D17">
+        <v>2004</v>
+      </c>
+      <c r="E17" t="s">
+        <v>5362</v>
+      </c>
+      <c r="F17" t="s">
         <v>5360</v>
       </c>
-      <c r="C17" t="s">
-        <v>5359</v>
-      </c>
-      <c r="D17">
-        <v>2009</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="G17">
+        <v>85</v>
+      </c>
+      <c r="H17" t="s">
+        <v>5028</v>
+      </c>
+      <c r="I17" t="s">
+        <v>5363</v>
+      </c>
+      <c r="J17" t="s">
+        <v>5363</v>
+      </c>
+      <c r="K17" t="s">
         <v>5361</v>
-      </c>
-      <c r="F17" t="s">
-        <v>5358</v>
-      </c>
-      <c r="G17">
-        <v>8</v>
-      </c>
-      <c r="H17" t="s">
-        <v>5028</v>
-      </c>
-      <c r="I17" t="s">
-        <v>5362</v>
-      </c>
-      <c r="J17" t="s">
-        <v>5357</v>
-      </c>
-      <c r="K17" t="s">
-        <v>5360</v>
       </c>
       <c r="L17" t="s">
         <v>963</v>
@@ -50392,50 +50383,6 @@
         <v>963</v>
       </c>
       <c r="N17" s="7" t="s">
-        <v>966</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>5364</v>
-      </c>
-      <c r="C18" t="s">
-        <v>400</v>
-      </c>
-      <c r="D18">
-        <v>2004</v>
-      </c>
-      <c r="E18" t="s">
-        <v>5365</v>
-      </c>
-      <c r="F18" t="s">
-        <v>5363</v>
-      </c>
-      <c r="G18">
-        <v>85</v>
-      </c>
-      <c r="H18" t="s">
-        <v>5028</v>
-      </c>
-      <c r="I18" t="s">
-        <v>5366</v>
-      </c>
-      <c r="J18" t="s">
-        <v>5366</v>
-      </c>
-      <c r="K18" t="s">
-        <v>5364</v>
-      </c>
-      <c r="L18" t="s">
-        <v>963</v>
-      </c>
-      <c r="M18" t="s">
-        <v>963</v>
-      </c>
-      <c r="N18" s="7" t="s">
         <v>966</v>
       </c>
     </row>
@@ -50460,7 +50407,7 @@
       <formula>LEN(TRIM(F13))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G12 G15:G1048576 H16:H18">
+  <conditionalFormatting sqref="G1:G12 G15:G1048576 H16:H17">
     <cfRule type="containsBlanks" dxfId="19" priority="38">
       <formula>LEN(TRIM(G1))=0</formula>
     </cfRule>
@@ -50474,7 +50421,7 @@
   <conditionalFormatting sqref="K14">
     <cfRule type="duplicateValues" dxfId="16" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:N18">
+  <conditionalFormatting sqref="L2:N17">
     <cfRule type="containsText" dxfId="15" priority="2" operator="containsText" text="PRIMARY STUDY">
       <formula>NOT(ISERROR(SEARCH("PRIMARY STUDY",L2)))</formula>
     </cfRule>
@@ -50485,7 +50432,7 @@
       <formula>NOT(ISERROR(SEARCH("YES",L2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N13:N14">
+  <conditionalFormatting sqref="N13:N16">
     <cfRule type="containsBlanks" dxfId="12" priority="1">
       <formula>LEN(TRIM(N13))=0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Removed redundant summary statistics from main data (pcc, CI, se_pcc,...)
</commit_message>
<xml_diff>
--- a/Literature/Literature.xlsx
+++ b/Literature/Literature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hso20\OneDrive\Plocha\IES\Diploma-Thesis\Literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C65A8C-66B5-4771-9241-59B1B934700C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0768EEC-B02F-4659-B62D-94FE0182A6D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49574,7 +49574,7 @@
   <dimension ref="A1:X17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49937,7 +49937,7 @@
       </c>
       <c r="Q7">
         <f>COUNTIFS($N:$N, "YES", $F:$F, "&lt;&gt;")</f>
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
@@ -50383,7 +50383,7 @@
         <v>963</v>
       </c>
       <c r="N17" s="7" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
     </row>
   </sheetData>
@@ -50432,7 +50432,7 @@
       <formula>NOT(ISERROR(SEARCH("YES",L2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N13:N16">
+  <conditionalFormatting sqref="N13:N17">
     <cfRule type="containsBlanks" dxfId="12" priority="1">
       <formula>LEN(TRIM(N13))=0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Grammar checked the rest of the thesis text, polished up several graphs
</commit_message>
<xml_diff>
--- a/Literature/Literature.xlsx
+++ b/Literature/Literature.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hso20\OneDrive\Plocha\IES\Diploma-Thesis\Literature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0768EEC-B02F-4659-B62D-94FE0182A6D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDBD65D0-271D-492E-BFAA-46BC06C8D015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Query literature" sheetId="5" r:id="rId1"/>
@@ -694,7 +694,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10217" uniqueCount="5364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10218" uniqueCount="5365">
   <si>
     <t>Number</t>
   </si>
@@ -16786,6 +16786,9 @@
   </si>
   <si>
     <t>https://onlinelibrary.wiley.com/doi/abs/10.1002/jae.724</t>
+  </si>
+  <si>
+    <t>Relevant:</t>
   </si>
 </sst>
 </file>
@@ -17860,9 +17863,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Y575"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18279,6 +18282,13 @@
       </c>
       <c r="Q7" s="2" t="s">
         <v>904</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>5364</v>
+      </c>
+      <c r="U7">
+        <f>COUNTIF(L:L,"YES") + COUNTIF(L:L,"INSUFFICIENT DATA")</f>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
@@ -49573,7 +49583,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:X17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>

</xml_diff>